<commit_message>
update rnn results analysis
</commit_message>
<xml_diff>
--- a/results_analysis/compare_with_ibes/#compare_all.xlsx
+++ b/results_analysis/compare_with_ibes/#compare_all.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
   <si>
     <t>consensus_mae</t>
   </si>
@@ -34,6 +34,15 @@
   </si>
   <si>
     <t>ibes_2|fwdepsqcut|ibes_new industry_only ws -indi space3</t>
+  </si>
+  <si>
+    <t>ibes_1|fwdepsqcut|cnn_rnn｜all</t>
+  </si>
+  <si>
+    <t>ibes_1|fwdepsqcut-industry_code|cnn_rnn｜all</t>
+  </si>
+  <si>
+    <t>ibes_1|fwdepsqcut-sector_code|cnn_rnn｜all</t>
   </si>
   <si>
     <t>ibes_1|fwdepsqcut|dense2｜all x 0 -fix space</t>
@@ -436,7 +445,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -489,13 +498,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.008861431855592515</v>
+        <v>0.008755819147523276</v>
       </c>
       <c r="C4">
-        <v>0.009338113103833704</v>
+        <v>0.009324414666975152</v>
       </c>
       <c r="D4">
-        <v>15176</v>
+        <v>10738</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -503,13 +512,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.008875614826370663</v>
+        <v>0.008480565232120381</v>
       </c>
       <c r="C5">
-        <v>0.008557495853986283</v>
+        <v>0.008767403629820283</v>
       </c>
       <c r="D5">
-        <v>15176</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -517,13 +526,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0.008861431855592515</v>
+        <v>0.008737944380384322</v>
       </c>
       <c r="C6">
-        <v>0.008655596509046039</v>
+        <v>0.009069548311264761</v>
       </c>
       <c r="D6">
-        <v>15176</v>
+        <v>10685</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -534,7 +543,7 @@
         <v>0.008861431855592515</v>
       </c>
       <c r="C7">
-        <v>0.008658869869704775</v>
+        <v>0.009338113103833704</v>
       </c>
       <c r="D7">
         <v>15176</v>
@@ -545,10 +554,10 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>0.008861431855592515</v>
+        <v>0.008875614826370663</v>
       </c>
       <c r="C8">
-        <v>0.008630337442592475</v>
+        <v>0.008557495853986283</v>
       </c>
       <c r="D8">
         <v>15176</v>
@@ -559,10 +568,10 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>0.008828774570773384</v>
+        <v>0.008861431855592515</v>
       </c>
       <c r="C9">
-        <v>0.007811737484649521</v>
+        <v>0.008655596509046039</v>
       </c>
       <c r="D9">
         <v>15176</v>
@@ -573,10 +582,10 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>0.008828774570773384</v>
+        <v>0.008861431855592515</v>
       </c>
       <c r="C10">
-        <v>0.009833523580700576</v>
+        <v>0.008658869869704775</v>
       </c>
       <c r="D10">
         <v>15176</v>
@@ -590,7 +599,7 @@
         <v>0.008861431855592515</v>
       </c>
       <c r="C11">
-        <v>0.009476279475976703</v>
+        <v>0.008630337442592475</v>
       </c>
       <c r="D11">
         <v>15176</v>
@@ -601,10 +610,10 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>0.008861431855592515</v>
+        <v>0.008828774570773384</v>
       </c>
       <c r="C12">
-        <v>0.009848581092865606</v>
+        <v>0.007811737484649521</v>
       </c>
       <c r="D12">
         <v>15176</v>
@@ -615,12 +624,54 @@
         <v>15</v>
       </c>
       <c r="B13">
+        <v>0.008828774570773384</v>
+      </c>
+      <c r="C13">
+        <v>0.009833523580700576</v>
+      </c>
+      <c r="D13">
+        <v>15176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
         <v>0.008861431855592515</v>
       </c>
-      <c r="C13">
+      <c r="C14">
+        <v>0.009476279475976703</v>
+      </c>
+      <c r="D14">
+        <v>15176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>0.008861431855592515</v>
+      </c>
+      <c r="C15">
+        <v>0.009848581092865606</v>
+      </c>
+      <c r="D15">
+        <v>15176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>0.008861431855592515</v>
+      </c>
+      <c r="C16">
         <v>0.01057408267989892</v>
       </c>
-      <c r="D13">
+      <c r="D16">
         <v>15176</v>
       </c>
     </row>
@@ -631,7 +682,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -642,10 +693,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -675,10 +726,10 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.0001975833946462478</v>
+        <v>0.0001959711547623701</v>
       </c>
       <c r="C4">
-        <v>0.0001881828907176001</v>
+        <v>0.0001845585823280265</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -686,10 +737,10 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.0002043910143630977</v>
+        <v>0.0001902011333966551</v>
       </c>
       <c r="C5">
-        <v>0.0001720965334955223</v>
+        <v>0.0001643412632725041</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -697,10 +748,10 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0.0001975833946462478</v>
+        <v>0.0001954134214635005</v>
       </c>
       <c r="C6">
-        <v>0.0001658971970851478</v>
+        <v>0.0001775504865366938</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -711,7 +762,7 @@
         <v>0.0001975833946462478</v>
       </c>
       <c r="C7">
-        <v>0.0001657197735352102</v>
+        <v>0.0001881828907176001</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -719,10 +770,10 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>0.0001975833946462478</v>
+        <v>0.0002043910143630977</v>
       </c>
       <c r="C8">
-        <v>0.0001649945689266668</v>
+        <v>0.0001720965334955223</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -730,10 +781,10 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>0.0002002415943724616</v>
+        <v>0.0001975833946462478</v>
       </c>
       <c r="C9">
-        <v>0.0001454923001376933</v>
+        <v>0.0001658971970851478</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -741,10 +792,10 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>0.0002002415943724616</v>
+        <v>0.0001975833946462478</v>
       </c>
       <c r="C10">
-        <v>0.0002242374076787091</v>
+        <v>0.0001657197735352102</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -755,7 +806,7 @@
         <v>0.0001975833946462478</v>
       </c>
       <c r="C11">
-        <v>0.0001902112594253567</v>
+        <v>0.0001649945689266668</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -763,10 +814,10 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>0.0001975833946462478</v>
+        <v>0.0002002415943724616</v>
       </c>
       <c r="C12">
-        <v>0.0002044223000088748</v>
+        <v>0.0001454923001376933</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -774,9 +825,42 @@
         <v>15</v>
       </c>
       <c r="B13">
+        <v>0.0002002415943724616</v>
+      </c>
+      <c r="C13">
+        <v>0.0002242374076787091</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
         <v>0.0001975833946462478</v>
       </c>
-      <c r="C13">
+      <c r="C14">
+        <v>0.0001902112594253567</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>0.0001975833946462478</v>
+      </c>
+      <c r="C15">
+        <v>0.0002044223000088748</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>0.0001975833946462478</v>
+      </c>
+      <c r="C16">
         <v>0.0002335431519097555</v>
       </c>
     </row>
@@ -787,7 +871,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -798,13 +882,13 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -840,13 +924,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.1445666443086192</v>
+        <v>0.1167952563634991</v>
       </c>
       <c r="C4">
-        <v>0.2636440167903586</v>
+        <v>0.2844903572053815</v>
       </c>
       <c r="D4">
-        <v>0.1852659380689607</v>
+        <v>0.1682295509836931</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -854,13 +938,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.1726321527164353</v>
+        <v>0.1948744524944567</v>
       </c>
       <c r="C5">
-        <v>0.2636440167903589</v>
+        <v>0.5386460971477394</v>
       </c>
       <c r="D5">
-        <v>0.3033591085848544</v>
+        <v>0.3043398469446008</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -868,13 +952,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0.1445666443086192</v>
+        <v>0.1109639479325829</v>
       </c>
       <c r="C6">
-        <v>0.2636440167903586</v>
+        <v>0.2723384459123704</v>
       </c>
       <c r="D6">
-        <v>0.2817514029636731</v>
+        <v>0.1922316163799704</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -888,7 +972,7 @@
         <v>0.2636440167903586</v>
       </c>
       <c r="D7">
-        <v>0.2825195546748713</v>
+        <v>0.1852659380689607</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -896,13 +980,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>0.1445666443086192</v>
+        <v>0.1726321527164353</v>
       </c>
       <c r="C8">
-        <v>0.2636440167903586</v>
+        <v>0.2636440167903589</v>
       </c>
       <c r="D8">
-        <v>0.2856593135243424</v>
+        <v>0.3033591085848544</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -910,13 +994,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>0.1712998665722781</v>
+        <v>0.1445666443086192</v>
       </c>
       <c r="C9">
         <v>0.2636440167903586</v>
       </c>
       <c r="D9">
-        <v>0.3978799014527122</v>
+        <v>0.2817514029636731</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -924,13 +1008,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>0.1712998665722781</v>
+        <v>0.1445666443086192</v>
       </c>
       <c r="C10">
         <v>0.2636440167903586</v>
       </c>
       <c r="D10">
-        <v>0.07199315783919602</v>
+        <v>0.2825195546748713</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -944,7 +1028,7 @@
         <v>0.2636440167903586</v>
       </c>
       <c r="D11">
-        <v>0.1764841563136554</v>
+        <v>0.2856593135243424</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -952,13 +1036,13 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>0.1445666443086192</v>
+        <v>0.1712998665722781</v>
       </c>
       <c r="C12">
         <v>0.2636440167903586</v>
       </c>
       <c r="D12">
-        <v>0.114957740310983</v>
+        <v>0.3978799014527122</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -966,12 +1050,54 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>0.1445666443086192</v>
+        <v>0.1712998665722781</v>
       </c>
       <c r="C13">
         <v>0.2636440167903586</v>
       </c>
       <c r="D13">
+        <v>0.07199315783919602</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>0.1445666443086192</v>
+      </c>
+      <c r="C14">
+        <v>0.2636440167903586</v>
+      </c>
+      <c r="D14">
+        <v>0.1764841563136554</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>0.1445666443086192</v>
+      </c>
+      <c r="C15">
+        <v>0.2636440167903586</v>
+      </c>
+      <c r="D15">
+        <v>0.114957740310983</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>0.1445666443086192</v>
+      </c>
+      <c r="C16">
+        <v>0.2636440167903586</v>
+      </c>
+      <c r="D16">
         <v>-0.01112040561197025</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update bug in rnn_eps
</commit_message>
<xml_diff>
--- a/results_analysis/compare_with_ibes/#compare_all.xlsx
+++ b/results_analysis/compare_with_ibes/#compare_all.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Clair/PycharmProjects/ai_value/results_analysis/compare_with_ibes/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA652C04-1AAF-1546-8301-FDE717049E2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="average_mae" sheetId="1" r:id="rId1"/>
     <sheet name="average_mse" sheetId="2" r:id="rId2"/>
     <sheet name="average_r2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" iterateDelta="9.9999999999994451E-4"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
   <si>
     <t>consensus_mae</t>
   </si>
@@ -54,6 +48,9 @@
     <t>ibes_6|fwdepsqcut|ibes_sector_only ws -indi space</t>
   </si>
   <si>
+    <t>ibes_2|ni|ibes_new industry_all x -mse</t>
+  </si>
+  <si>
     <t>ibes_1|fwdepsqcut|ibes_entire_only ws -smaller space</t>
   </si>
   <si>
@@ -94,58 +91,13 @@
   </si>
   <si>
     <t>lgbm_r2</t>
-  </si>
-  <si>
-    <t>lgbm | industy | with ibes as X</t>
-  </si>
-  <si>
-    <t>lgbm | industry</t>
-  </si>
-  <si>
-    <t>lgbm | sector</t>
-  </si>
-  <si>
-    <t>lgbm | aggregate | with sector code</t>
-  </si>
-  <si>
-    <t>lgbm | aggregate</t>
-  </si>
-  <si>
-    <t>lgbm | aggregate | with industry code</t>
-  </si>
-  <si>
-    <t>cnn_rnn|aggregate | with ibes as X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cnn_rnn|aggregate </t>
-  </si>
-  <si>
-    <t>dense |aggregate | with ibes as X</t>
-  </si>
-  <si>
-    <t>dense | aggregate</t>
-  </si>
-  <si>
-    <t>dense | industry</t>
-  </si>
-  <si>
-    <t>dense | aggregate | with industry code</t>
-  </si>
-  <si>
-    <t>dense | aggregate | larger space</t>
-  </si>
-  <si>
-    <t>rnn_eps | aggregate</t>
-  </si>
-  <si>
-    <t>dense | aggregate | with sector code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,16 +149,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -214,14 +160,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -268,7 +206,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -300,27 +238,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -352,24 +272,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -545,20 +447,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="237" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:D9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="57.83203125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -571,406 +468,428 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>24</v>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>8.8287745707733845E-3</v>
+        <v>0.008861431855592515</v>
       </c>
       <c r="C2">
-        <v>7.8117374846495211E-3</v>
+        <v>0.009885775671985323</v>
       </c>
       <c r="D2">
         <v>15176</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>25</v>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>8.8287745707733845E-3</v>
+        <v>0.008828774570773384</v>
       </c>
       <c r="C3">
-        <v>8.5533193098867016E-3</v>
+        <v>0.008553319309886702</v>
       </c>
       <c r="D3">
         <v>15176</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>26</v>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>8.8756148263706633E-3</v>
+        <v>0.00870510303297917</v>
       </c>
       <c r="C4">
-        <v>8.5574958539862828E-3</v>
+        <v>0.009208389006560668</v>
       </c>
       <c r="D4">
-        <v>15176</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>12746</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>8.8614318555925147E-3</v>
+        <v>0.008736590526442781</v>
       </c>
       <c r="C5">
-        <v>8.6555965090460395E-3</v>
+        <v>0.009050386758606433</v>
       </c>
       <c r="D5">
-        <v>15176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>12054</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>8.8614318555925147E-3</v>
+        <v>0.008861431855592515</v>
       </c>
       <c r="C6">
-        <v>8.6588698697047748E-3</v>
+        <v>0.009338113103833704</v>
       </c>
       <c r="D6">
         <v>15176</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>27</v>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>8.8614318555925147E-3</v>
+        <v>0.008875614826370663</v>
       </c>
       <c r="C7">
-        <v>8.6303374425924749E-3</v>
+        <v>0.008557495853986283</v>
       </c>
       <c r="D7">
         <v>15176</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>30</v>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>8.7365905264427807E-3</v>
+        <v>0.008828774570773384</v>
       </c>
       <c r="C8">
-        <v>9.0503867586064334E-3</v>
+        <v>0.008541934475696275</v>
       </c>
       <c r="D8">
-        <v>12054</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>15176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B9">
-        <v>8.7051030329791702E-3</v>
+        <v>0.008861431855592515</v>
       </c>
       <c r="C9">
-        <v>9.2083890065606678E-3</v>
+        <v>0.008655596509046039</v>
       </c>
       <c r="D9">
-        <v>12746</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>15176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>8.8614318555925147E-3</v>
+        <v>0.008861431855592515</v>
       </c>
       <c r="C10">
-        <v>9.3381131038337041E-3</v>
+        <v>0.008658869869704775</v>
       </c>
       <c r="D10">
         <v>15176</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>33</v>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B11">
-        <v>8.8614318555925147E-3</v>
+        <v>0.008861431855592515</v>
       </c>
       <c r="C11">
-        <v>9.4762794759767031E-3</v>
+        <v>0.008630337442592475</v>
       </c>
       <c r="D11">
         <v>15176</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>34</v>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B12">
-        <v>8.8287745707733845E-3</v>
+        <v>0.008828774570773384</v>
       </c>
       <c r="C12">
-        <v>9.8335235807005764E-3</v>
+        <v>0.007811737484649521</v>
       </c>
       <c r="D12">
         <v>15176</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>35</v>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>8.8614318555925147E-3</v>
+        <v>0.008828774570773384</v>
       </c>
       <c r="C13">
-        <v>9.8485810928656062E-3</v>
+        <v>0.009833523580700576</v>
       </c>
       <c r="D13">
         <v>15176</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>36</v>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B14">
-        <v>8.8614318555925147E-3</v>
+        <v>0.008861431855592515</v>
       </c>
       <c r="C14">
-        <v>9.8857756719853227E-3</v>
+        <v>0.009476279475976703</v>
       </c>
       <c r="D14">
         <v>15176</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>37</v>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>8.7378846049827007E-3</v>
+        <v>0.008861431855592515</v>
       </c>
       <c r="C15">
-        <v>9.9215284738299134E-3</v>
+        <v>0.009848581092865606</v>
       </c>
       <c r="D15">
+        <v>15176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>0.008861431855592515</v>
+      </c>
+      <c r="C16">
+        <v>0.01057408267989892</v>
+      </c>
+      <c r="D16">
+        <v>15176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>0.008737884604982701</v>
+      </c>
+      <c r="C17">
+        <v>0.009921528473829913</v>
+      </c>
+      <c r="D17">
         <v>6584</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16">
-        <v>8.8614318555925147E-3</v>
-      </c>
-      <c r="C16">
-        <v>1.057408267989892E-2</v>
-      </c>
-      <c r="D16">
-        <v>15176</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D16">
-    <sortCondition ref="C3"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>1.9758339464624779E-4</v>
+        <v>0.0001975833946462478</v>
       </c>
       <c r="C2">
-        <v>2.041352586055002E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.0002041352586055002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>2.002415943724616E-4</v>
+        <v>0.0002002415943724616</v>
       </c>
       <c r="C3">
-        <v>1.6887281030830169E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.0001688728103083017</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4">
-        <v>1.918729794254194E-4</v>
+        <v>0.0001918729794254194</v>
       </c>
       <c r="C4">
-        <v>1.801854361867948E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.0001801854361867948</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5">
-        <v>1.9447780436028151E-4</v>
+        <v>0.0001944778043602815</v>
       </c>
       <c r="C5">
-        <v>1.7650255848324041E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.0001765025584832404</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6">
-        <v>1.9758339464624779E-4</v>
+        <v>0.0001975833946462478</v>
       </c>
       <c r="C6">
-        <v>1.8818289071760011E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.0001881828907176001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7">
-        <v>2.0439101436309771E-4</v>
+        <v>0.0002043910143630977</v>
       </c>
       <c r="C7">
-        <v>1.7209653349552231E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.0001720965334955223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8">
-        <v>1.9758339464624779E-4</v>
+        <v>0.0002002415943724616</v>
       </c>
       <c r="C8">
-        <v>1.6589719708514779E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.0001662305676343938</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9">
-        <v>1.9758339464624779E-4</v>
+        <v>0.0001975833946462478</v>
       </c>
       <c r="C9">
-        <v>1.6571977353521019E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.0001658971970851478</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10">
-        <v>1.9758339464624779E-4</v>
+        <v>0.0001975833946462478</v>
       </c>
       <c r="C10">
-        <v>1.649945689266668E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.0001657197735352102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11">
-        <v>2.002415943724616E-4</v>
+        <v>0.0001975833946462478</v>
       </c>
       <c r="C11">
-        <v>1.4549230013769331E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.0001649945689266668</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B12">
-        <v>2.002415943724616E-4</v>
+        <v>0.0002002415943724616</v>
       </c>
       <c r="C12">
-        <v>2.2423740767870911E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.0001454923001376933</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B13">
-        <v>1.9758339464624779E-4</v>
+        <v>0.0002002415943724616</v>
       </c>
       <c r="C13">
-        <v>1.9021125942535671E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.0002242374076787091</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B14">
-        <v>1.9758339464624779E-4</v>
+        <v>0.0001975833946462478</v>
       </c>
       <c r="C14">
-        <v>2.0442230000887479E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.0001902112594253567</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B15">
-        <v>1.9758339464624779E-4</v>
+        <v>0.0001975833946462478</v>
       </c>
       <c r="C15">
-        <v>2.3354315190975551E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0.0002044223000088748</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B16">
-        <v>1.96008906973461E-4</v>
+        <v>0.0001975833946462478</v>
       </c>
       <c r="C16">
-        <v>2.2368564019773179E-4</v>
+        <v>0.0002335431519097555</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>0.000196008906973461</v>
+      </c>
+      <c r="C17">
+        <v>0.0002236856401977318</v>
       </c>
     </row>
   </sheetData>
@@ -979,56 +898,56 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.14456664430861921</v>
+        <v>0.1445666443086192</v>
       </c>
       <c r="C2">
-        <v>0.26364401679035859</v>
+        <v>0.2636440167903586</v>
       </c>
       <c r="D2">
         <v>0.1162004803264115</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.17129986657227811</v>
+        <v>0.1712998665722781</v>
       </c>
       <c r="C3">
-        <v>0.26364401679035859</v>
+        <v>0.2636440167903586</v>
       </c>
       <c r="D3">
-        <v>0.30111962565331002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.30111962565331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1036,13 +955,13 @@
         <v>0.1261272704213072</v>
       </c>
       <c r="C4">
-        <v>0.26014990209476591</v>
+        <v>0.2601499020947659</v>
       </c>
       <c r="D4">
-        <v>0.17935740914428339</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.1793574091442834</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1050,164 +969,178 @@
         <v>0.1185037215870294</v>
       </c>
       <c r="C5">
-        <v>0.26010602216186401</v>
+        <v>0.260106022161864</v>
       </c>
       <c r="D5">
-        <v>0.19997889247499279</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.1999788924749928</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0.14456664430861921</v>
+        <v>0.1445666443086192</v>
       </c>
       <c r="C6">
-        <v>0.26364401679035859</v>
+        <v>0.2636440167903586</v>
       </c>
       <c r="D6">
-        <v>0.18526593806896069</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.1852659380689607</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7">
-        <v>0.17263215271643531</v>
+        <v>0.1726321527164353</v>
       </c>
       <c r="C7">
-        <v>0.26364401679035893</v>
+        <v>0.2636440167903589</v>
       </c>
       <c r="D7">
-        <v>0.30335910858485438</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.3033591085848544</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B8">
-        <v>0.14456664430861921</v>
+        <v>0.1712998665722781</v>
       </c>
       <c r="C8">
-        <v>0.26364401679035859</v>
+        <v>0.2636440167903586</v>
       </c>
       <c r="D8">
-        <v>0.28175140296367313</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.3120545508534311</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9">
-        <v>0.14456664430861921</v>
+        <v>0.1445666443086192</v>
       </c>
       <c r="C9">
-        <v>0.26364401679035859</v>
+        <v>0.2636440167903586</v>
       </c>
       <c r="D9">
-        <v>0.28251955467487128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.2817514029636731</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10">
-        <v>0.14456664430861921</v>
+        <v>0.1445666443086192</v>
       </c>
       <c r="C10">
-        <v>0.26364401679035859</v>
+        <v>0.2636440167903586</v>
       </c>
       <c r="D10">
-        <v>0.28565931352434237</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.2825195546748713</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11">
-        <v>0.17129986657227811</v>
+        <v>0.1445666443086192</v>
       </c>
       <c r="C11">
-        <v>0.26364401679035859</v>
+        <v>0.2636440167903586</v>
       </c>
       <c r="D11">
-        <v>0.39787990145271218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.2856593135243424</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B12">
-        <v>0.17129986657227811</v>
+        <v>0.1712998665722781</v>
       </c>
       <c r="C12">
-        <v>0.26364401679035859</v>
+        <v>0.2636440167903586</v>
       </c>
       <c r="D12">
-        <v>7.199315783919602E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.3978799014527122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B13">
-        <v>0.14456664430861921</v>
+        <v>0.1712998665722781</v>
       </c>
       <c r="C13">
-        <v>0.26364401679035859</v>
+        <v>0.2636440167903586</v>
       </c>
       <c r="D13">
-        <v>0.17648415631365541</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.07199315783919602</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B14">
-        <v>0.14456664430861921</v>
+        <v>0.1445666443086192</v>
       </c>
       <c r="C14">
-        <v>0.26364401679035859</v>
+        <v>0.2636440167903586</v>
       </c>
       <c r="D14">
-        <v>0.11495774031098301</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.1764841563136554</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B15">
-        <v>0.14456664430861921</v>
+        <v>0.1445666443086192</v>
       </c>
       <c r="C15">
-        <v>0.26364401679035859</v>
+        <v>0.2636440167903586</v>
       </c>
       <c r="D15">
-        <v>-1.112040561197025E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.114957740310983</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B16">
+        <v>0.1445666443086192</v>
+      </c>
+      <c r="C16">
+        <v>0.2636440167903586</v>
+      </c>
+      <c r="D16">
+        <v>-0.01112040561197025</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
         <v>0.1037236563029756</v>
       </c>
-      <c r="C16">
-        <v>0.33127939154455122</v>
-      </c>
-      <c r="D16">
-        <v>-2.2831823459411149E-2</v>
+      <c r="C17">
+        <v>0.3312793915445512</v>
+      </c>
+      <c r="D17">
+        <v>-0.02283182345941115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update compare using old IBES data
</commit_message>
<xml_diff>
--- a/results_analysis/compare_with_ibes/#compare_all.xlsx
+++ b/results_analysis/compare_with_ibes/#compare_all.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>lgbm_mae</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>ibes_1|fwdepsqcut|dense2｜all x 0 -fix space</t>
+  </si>
+  <si>
+    <t>ibes_2|fwdepsqcut|ibes_industry_all x -exclude_stock</t>
   </si>
   <si>
     <t>ibes_6|fwdepsqcut|ibes_sector_only ws -indi space</t>
@@ -455,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -669,28 +672,28 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>0.008271263221934944</v>
+        <v>0.006723070191127427</v>
       </c>
       <c r="C8">
-        <v>0.008659154831887702</v>
+        <v>0.006502442371883452</v>
       </c>
       <c r="D8">
-        <v>0.000162539775585851</v>
+        <v>0.0001075952021389975</v>
       </c>
       <c r="E8">
-        <v>0.0001949633210112301</v>
+        <v>0.000110182239419974</v>
       </c>
       <c r="F8">
-        <v>0.2920577529107484</v>
+        <v>0.224562807151098</v>
       </c>
       <c r="G8">
-        <v>0.1508369500376733</v>
+        <v>0.2059180638254218</v>
       </c>
       <c r="H8">
-        <v>0.2583620952127688</v>
+        <v>0.301426345673243</v>
       </c>
       <c r="I8">
-        <v>14166</v>
+        <v>3343</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -698,22 +701,22 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <v>0.008305626259430711</v>
+        <v>0.008271263221934944</v>
       </c>
       <c r="C9">
-        <v>0.008635508151540194</v>
+        <v>0.008659154831887702</v>
       </c>
       <c r="D9">
-        <v>0.0001581971829802284</v>
+        <v>0.000162539775585851</v>
       </c>
       <c r="E9">
-        <v>0.0001921541471413092</v>
+        <v>0.0001949633210112301</v>
       </c>
       <c r="F9">
-        <v>0.3016074861881056</v>
+        <v>0.2920577529107484</v>
       </c>
       <c r="G9">
-        <v>0.15169780312604</v>
+        <v>0.1508369500376733</v>
       </c>
       <c r="H9">
         <v>0.2583620952127688</v>
@@ -727,25 +730,25 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <v>0.00844284418539723</v>
+        <v>0.008305626259430711</v>
       </c>
       <c r="C10">
-        <v>0.008687458498950898</v>
+        <v>0.008635508151540194</v>
       </c>
       <c r="D10">
-        <v>0.0001604772912864719</v>
+        <v>0.0001581971829802284</v>
       </c>
       <c r="E10">
-        <v>0.0001906209278749646</v>
+        <v>0.0001921541471413092</v>
       </c>
       <c r="F10">
-        <v>0.2644361756264868</v>
+        <v>0.3016074861881056</v>
       </c>
       <c r="G10">
-        <v>0.1262697819155144</v>
+        <v>0.15169780312604</v>
       </c>
       <c r="H10">
-        <v>0.2583620952127686</v>
+        <v>0.2583620952127688</v>
       </c>
       <c r="I10">
         <v>14166</v>
@@ -756,19 +759,19 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <v>0.008443125284138316</v>
+        <v>0.00844284418539723</v>
       </c>
       <c r="C11">
         <v>0.008687458498950898</v>
       </c>
       <c r="D11">
-        <v>0.0001601555041560421</v>
+        <v>0.0001604772912864719</v>
       </c>
       <c r="E11">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F11">
-        <v>0.2659111193421716</v>
+        <v>0.2644361756264868</v>
       </c>
       <c r="G11">
         <v>0.1262697819155144</v>
@@ -785,19 +788,19 @@
         <v>19</v>
       </c>
       <c r="B12">
-        <v>0.008418017610370062</v>
+        <v>0.008443125284138316</v>
       </c>
       <c r="C12">
         <v>0.008687458498950898</v>
       </c>
       <c r="D12">
-        <v>0.0001595007627511497</v>
+        <v>0.0001601555041560421</v>
       </c>
       <c r="E12">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F12">
-        <v>0.2689121925027265</v>
+        <v>0.2659111193421716</v>
       </c>
       <c r="G12">
         <v>0.1262697819155144</v>
@@ -814,25 +817,25 @@
         <v>20</v>
       </c>
       <c r="B13">
-        <v>0.007587864829138694</v>
+        <v>0.008418017610370062</v>
       </c>
       <c r="C13">
-        <v>0.008635508151540194</v>
+        <v>0.008687458498950898</v>
       </c>
       <c r="D13">
-        <v>0.0001393500412889987</v>
+        <v>0.0001595007627511497</v>
       </c>
       <c r="E13">
-        <v>0.0001921541471413092</v>
+        <v>0.0001906209278749646</v>
       </c>
       <c r="F13">
-        <v>0.3848118923345282</v>
+        <v>0.2689121925027265</v>
       </c>
       <c r="G13">
-        <v>0.15169780312604</v>
+        <v>0.1262697819155144</v>
       </c>
       <c r="H13">
-        <v>0.2583620952127688</v>
+        <v>0.2583620952127686</v>
       </c>
       <c r="I13">
         <v>14166</v>
@@ -843,25 +846,25 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <v>0.009022455578369986</v>
+        <v>0.007587864829138694</v>
       </c>
       <c r="C14">
-        <v>0.008687458498950898</v>
+        <v>0.008635508151540194</v>
       </c>
       <c r="D14">
-        <v>0.0001738441260953471</v>
+        <v>0.0001393500412889987</v>
       </c>
       <c r="E14">
-        <v>0.0001906209278749646</v>
+        <v>0.0001921541471413092</v>
       </c>
       <c r="F14">
-        <v>0.2031679422648356</v>
+        <v>0.3848118923345282</v>
       </c>
       <c r="G14">
-        <v>0.1262697819155144</v>
+        <v>0.15169780312604</v>
       </c>
       <c r="H14">
-        <v>0.2583620952127686</v>
+        <v>0.2583620952127688</v>
       </c>
       <c r="I14">
         <v>14166</v>
@@ -872,25 +875,25 @@
         <v>22</v>
       </c>
       <c r="B15">
-        <v>0.009513742997451299</v>
+        <v>0.009022455578369986</v>
       </c>
       <c r="C15">
-        <v>0.008635508151540194</v>
+        <v>0.008687458498950898</v>
       </c>
       <c r="D15">
-        <v>0.0002127091144161235</v>
+        <v>0.0001738441260953471</v>
       </c>
       <c r="E15">
-        <v>0.0001921541471413092</v>
+        <v>0.0001906209278749646</v>
       </c>
       <c r="F15">
-        <v>0.06095386574396355</v>
+        <v>0.2031679422648356</v>
       </c>
       <c r="G15">
-        <v>0.15169780312604</v>
+        <v>0.1262697819155144</v>
       </c>
       <c r="H15">
-        <v>0.2583620952127688</v>
+        <v>0.2583620952127686</v>
       </c>
       <c r="I15">
         <v>14166</v>
@@ -901,25 +904,25 @@
         <v>23</v>
       </c>
       <c r="B16">
-        <v>0.009225854121736928</v>
+        <v>0.009513742997451299</v>
       </c>
       <c r="C16">
-        <v>0.008687458498950898</v>
+        <v>0.008635508151540194</v>
       </c>
       <c r="D16">
-        <v>0.0001822661374906326</v>
+        <v>0.0002127091144161235</v>
       </c>
       <c r="E16">
-        <v>0.0001906209278749646</v>
+        <v>0.0001921541471413092</v>
       </c>
       <c r="F16">
-        <v>0.1645648049538074</v>
+        <v>0.06095386574396355</v>
       </c>
       <c r="G16">
-        <v>0.1262697819155144</v>
+        <v>0.15169780312604</v>
       </c>
       <c r="H16">
-        <v>0.2583620952127686</v>
+        <v>0.2583620952127688</v>
       </c>
       <c r="I16">
         <v>14166</v>
@@ -930,19 +933,19 @@
         <v>24</v>
       </c>
       <c r="B17">
-        <v>0.009548220646664947</v>
+        <v>0.009225854121736928</v>
       </c>
       <c r="C17">
         <v>0.008687458498950898</v>
       </c>
       <c r="D17">
-        <v>0.0001933459958501393</v>
+        <v>0.0001822661374906326</v>
       </c>
       <c r="E17">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F17">
-        <v>0.113779158442072</v>
+        <v>0.1645648049538074</v>
       </c>
       <c r="G17">
         <v>0.1262697819155144</v>
@@ -959,19 +962,19 @@
         <v>25</v>
       </c>
       <c r="B18">
-        <v>0.01021710973531049</v>
+        <v>0.009548220646664947</v>
       </c>
       <c r="C18">
         <v>0.008687458498950898</v>
       </c>
       <c r="D18">
-        <v>0.0002201065094334888</v>
+        <v>0.0001933459958501393</v>
       </c>
       <c r="E18">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F18">
-        <v>-0.00888035030069112</v>
+        <v>0.113779158442072</v>
       </c>
       <c r="G18">
         <v>0.1262697819155144</v>
@@ -988,19 +991,19 @@
         <v>26</v>
       </c>
       <c r="B19">
-        <v>0.009873209207006982</v>
+        <v>0.01021710973531049</v>
       </c>
       <c r="C19">
         <v>0.008687458498950898</v>
       </c>
       <c r="D19">
-        <v>0.0002181271559853543</v>
+        <v>0.0002201065094334888</v>
       </c>
       <c r="E19">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F19">
-        <v>0.0001922155460098995</v>
+        <v>-0.00888035030069112</v>
       </c>
       <c r="G19">
         <v>0.1262697819155144</v>
@@ -1017,27 +1020,56 @@
         <v>27</v>
       </c>
       <c r="B20">
+        <v>0.009873209207006982</v>
+      </c>
+      <c r="C20">
+        <v>0.008687458498950898</v>
+      </c>
+      <c r="D20">
+        <v>0.0002181271559853543</v>
+      </c>
+      <c r="E20">
+        <v>0.0001906209278749646</v>
+      </c>
+      <c r="F20">
+        <v>0.0001922155460098995</v>
+      </c>
+      <c r="G20">
+        <v>0.1262697819155144</v>
+      </c>
+      <c r="H20">
+        <v>0.2583620952127686</v>
+      </c>
+      <c r="I20">
+        <v>14166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21">
         <v>0.009075753729992564</v>
       </c>
-      <c r="C20">
-        <v>0.008687458498950898</v>
-      </c>
-      <c r="D20">
+      <c r="C21">
+        <v>0.008687458498950898</v>
+      </c>
+      <c r="D21">
         <v>0.0001756371360362956</v>
       </c>
-      <c r="E20">
-        <v>0.0001906209278749646</v>
-      </c>
-      <c r="F20">
+      <c r="E21">
+        <v>0.0001906209278749646</v>
+      </c>
+      <c r="F21">
         <v>0.1949495006477631</v>
       </c>
-      <c r="G20">
-        <v>0.1262697819155144</v>
-      </c>
-      <c r="H20">
-        <v>0.2583620952127686</v>
-      </c>
-      <c r="I20">
+      <c r="G21">
+        <v>0.1262697819155144</v>
+      </c>
+      <c r="H21">
+        <v>0.2583620952127686</v>
+      </c>
+      <c r="I21">
         <v>14166</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update dense with top 15 variables
</commit_message>
<xml_diff>
--- a/results_analysis/compare_with_ibes/#compare_all.xlsx
+++ b/results_analysis/compare_with_ibes/#compare_all.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>lgbm_mae</t>
   </si>
@@ -46,6 +46,9 @@
     <t>ibes_1|fwdepsqcut|dense2｜compare large space</t>
   </si>
   <si>
+    <t>ibes_1|fwdepsqcut-sector_code|dense2｜sp500 -small space</t>
+  </si>
+  <si>
     <t>ibes_1|ni-sector_code|rnn_double｜adj_space__exclude_fwd_2</t>
   </si>
   <si>
@@ -67,10 +70,34 @@
     <t>ibes_1|fwdepsqcut|dense2｜all x 0 -fix space</t>
   </si>
   <si>
+    <t>ibes_1|fwdepsqcut|dense2｜top10_0 -small space new</t>
+  </si>
+  <si>
+    <t>ibes_1|fwdepsqcut-sector_code|dense2｜top10_0 -small space new</t>
+  </si>
+  <si>
+    <t>ibes_2|fwdepsqcut|ibes_new industry_only ws -indi space3_sp500</t>
+  </si>
+  <si>
     <t>ibes_2|fwdepsqcut|ibes_industry_all x -exclude_stock</t>
   </si>
   <si>
+    <t>ibes_1|fwdepsqcut|dense2｜new with indi code -fix space_sp500</t>
+  </si>
+  <si>
+    <t>ibes_1|fwdepsqcut-industry_code|dense2｜new with indi code -fix space_sp500</t>
+  </si>
+  <si>
+    <t>ibes_1|fwdepsqcut-sector_code|dense2｜new with indi code -fix space_sp500</t>
+  </si>
+  <si>
     <t>ibes_2|fwdepsqcut|ibes_new industry_only ws -indi space3 (compare using old)</t>
+  </si>
+  <si>
+    <t>ibes_1|fwdepsqcut|dense2｜top15 -small space</t>
+  </si>
+  <si>
+    <t>ibes_1|fwdepsqcut-sector_code|dense2｜top15 -small space</t>
   </si>
   <si>
     <t>ibes_6|fwdepsqcut|ibes_sector_only ws -indi space</t>
@@ -470,7 +497,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -539,28 +566,28 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>0.008996341110758196</v>
+        <v>0.007241847395680414</v>
       </c>
       <c r="C3">
-        <v>0.008687458498950898</v>
+        <v>0.005640138541351778</v>
       </c>
       <c r="D3">
-        <v>0.0001736821065404229</v>
+        <v>0.0001211011389144233</v>
       </c>
       <c r="E3">
-        <v>0.0001906209278749646</v>
+        <v>9.104237776586397E-05</v>
       </c>
       <c r="F3">
-        <v>0.2039105752098954</v>
+        <v>-0.01772088279750084</v>
       </c>
       <c r="G3">
-        <v>0.1262697819155144</v>
+        <v>0.2348896971370824</v>
       </c>
       <c r="H3">
-        <v>0.2583620952127686</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I3">
-        <v>14166</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -568,25 +595,25 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>0.007727376897992178</v>
+        <v>0.008996341110758196</v>
       </c>
       <c r="C4">
-        <v>0.008659154831887702</v>
+        <v>0.008687458498950898</v>
       </c>
       <c r="D4">
-        <v>0.0001456055809025543</v>
+        <v>0.0001736821065404229</v>
       </c>
       <c r="E4">
-        <v>0.0001949633210112301</v>
+        <v>0.0001906209278749646</v>
       </c>
       <c r="F4">
-        <v>0.3658146643715235</v>
+        <v>0.2039105752098954</v>
       </c>
       <c r="G4">
-        <v>0.1508369500376733</v>
+        <v>0.1262697819155144</v>
       </c>
       <c r="H4">
-        <v>0.2583620952127688</v>
+        <v>0.2583620952127686</v>
       </c>
       <c r="I4">
         <v>14166</v>
@@ -597,22 +624,22 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>0.008303107575837335</v>
+        <v>0.007727376897992178</v>
       </c>
       <c r="C5">
-        <v>0.008635508151540194</v>
+        <v>0.008659154831887702</v>
       </c>
       <c r="D5">
-        <v>0.0001612992868167532</v>
+        <v>0.0001456055809025543</v>
       </c>
       <c r="E5">
-        <v>0.0001921541471413092</v>
+        <v>0.0001949633210112301</v>
       </c>
       <c r="F5">
-        <v>0.2879126399482278</v>
+        <v>0.3658146643715235</v>
       </c>
       <c r="G5">
-        <v>0.15169780312604</v>
+        <v>0.1508369500376733</v>
       </c>
       <c r="H5">
         <v>0.2583620952127688</v>
@@ -626,25 +653,25 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>0.009050797912742738</v>
+        <v>0.008303107575837335</v>
       </c>
       <c r="C6">
-        <v>0.008687458498950898</v>
+        <v>0.008635508151540194</v>
       </c>
       <c r="D6">
-        <v>0.0001747927346526816</v>
+        <v>0.0001612992868167532</v>
       </c>
       <c r="E6">
-        <v>0.0001906209278749646</v>
+        <v>0.0001921541471413092</v>
       </c>
       <c r="F6">
-        <v>0.1988198994191919</v>
+        <v>0.2879126399482278</v>
       </c>
       <c r="G6">
-        <v>0.1262697819155144</v>
+        <v>0.15169780312604</v>
       </c>
       <c r="H6">
-        <v>0.2583620952127686</v>
+        <v>0.2583620952127688</v>
       </c>
       <c r="I6">
         <v>14166</v>
@@ -655,19 +682,19 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <v>0.009193166387152663</v>
+        <v>0.009050797912742738</v>
       </c>
       <c r="C7">
         <v>0.008687458498950898</v>
       </c>
       <c r="D7">
-        <v>0.0001790877823978381</v>
+        <v>0.0001747927346526816</v>
       </c>
       <c r="E7">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F7">
-        <v>0.1791331155760224</v>
+        <v>0.1988198994191919</v>
       </c>
       <c r="G7">
         <v>0.1262697819155144</v>
@@ -684,19 +711,19 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>0.008991444386632417</v>
+        <v>0.009193166387152663</v>
       </c>
       <c r="C8">
         <v>0.008687458498950898</v>
       </c>
       <c r="D8">
-        <v>0.0001734042650277677</v>
+        <v>0.0001790877823978381</v>
       </c>
       <c r="E8">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F8">
-        <v>0.2051840897612696</v>
+        <v>0.1791331155760224</v>
       </c>
       <c r="G8">
         <v>0.1262697819155144</v>
@@ -713,19 +740,19 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <v>0.009081839591891672</v>
+        <v>0.008991444386632417</v>
       </c>
       <c r="C9">
         <v>0.008687458498950898</v>
       </c>
       <c r="D9">
-        <v>0.000180385026887178</v>
+        <v>0.0001734042650277677</v>
       </c>
       <c r="E9">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F9">
-        <v>0.1731870648290482</v>
+        <v>0.2051840897612696</v>
       </c>
       <c r="G9">
         <v>0.1262697819155144</v>
@@ -742,25 +769,25 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <v>0.008657117254708444</v>
+        <v>0.009081839591891672</v>
       </c>
       <c r="C10">
-        <v>0.008635508151540194</v>
+        <v>0.008687458498950898</v>
       </c>
       <c r="D10">
-        <v>0.0001731025162188118</v>
+        <v>0.000180385026887178</v>
       </c>
       <c r="E10">
-        <v>0.0001921541471413092</v>
+        <v>0.0001906209278749646</v>
       </c>
       <c r="F10">
-        <v>0.2358049671192343</v>
+        <v>0.1731870648290482</v>
       </c>
       <c r="G10">
-        <v>0.15169780312604</v>
+        <v>0.1262697819155144</v>
       </c>
       <c r="H10">
-        <v>0.2583620952127688</v>
+        <v>0.2583620952127686</v>
       </c>
       <c r="I10">
         <v>14166</v>
@@ -771,28 +798,28 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <v>0.00698011858859047</v>
+        <v>0.009741377726547894</v>
       </c>
       <c r="C11">
-        <v>0.01116184410920933</v>
+        <v>0.008453919625649597</v>
       </c>
       <c r="D11">
-        <v>0.0001206003995053095</v>
+        <v>0.0001984695900641642</v>
       </c>
       <c r="E11">
-        <v>0.0002568809119206026</v>
+        <v>0.0001911183621412693</v>
       </c>
       <c r="F11">
-        <v>0.1961572221345995</v>
+        <v>0.1101416555949604</v>
       </c>
       <c r="G11">
-        <v>-0.7121988539495976</v>
+        <v>0.1431016244581829</v>
       </c>
       <c r="H11">
-        <v>-0.0971244535465241</v>
+        <v>0.4334696169476997</v>
       </c>
       <c r="I11">
-        <v>1545</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -800,28 +827,28 @@
         <v>19</v>
       </c>
       <c r="B12">
-        <v>0.008271263221934944</v>
+        <v>0.009900137342862622</v>
       </c>
       <c r="C12">
-        <v>0.008659154831887702</v>
+        <v>0.009030432768250784</v>
       </c>
       <c r="D12">
-        <v>0.000162539775585851</v>
+        <v>0.000200877532613192</v>
       </c>
       <c r="E12">
-        <v>0.0001949633210112301</v>
+        <v>0.0002181746930107264</v>
       </c>
       <c r="F12">
-        <v>0.2920577529107484</v>
+        <v>0.1862719847337182</v>
       </c>
       <c r="G12">
-        <v>0.1508369500376733</v>
+        <v>0.116203501628984</v>
       </c>
       <c r="H12">
-        <v>0.2583620952127688</v>
+        <v>0.4935486705331952</v>
       </c>
       <c r="I12">
-        <v>14166</v>
+        <v>629</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -829,28 +856,28 @@
         <v>20</v>
       </c>
       <c r="B13">
-        <v>0.008305626259430711</v>
+        <v>0.00566147729919014</v>
       </c>
       <c r="C13">
-        <v>0.008635508151540194</v>
+        <v>0.005645917892372011</v>
       </c>
       <c r="D13">
-        <v>0.0001581971829802284</v>
+        <v>8.617292926780686E-05</v>
       </c>
       <c r="E13">
-        <v>0.0001921541471413092</v>
+        <v>9.170236601052772E-05</v>
       </c>
       <c r="F13">
-        <v>0.3016074861881056</v>
+        <v>0.3048814260707366</v>
       </c>
       <c r="G13">
-        <v>0.15169780312604</v>
+        <v>0.260277926852472</v>
       </c>
       <c r="H13">
-        <v>0.2583620952127688</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I13">
-        <v>14166</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -858,25 +885,25 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <v>0.00844284418539723</v>
+        <v>0.008657117254708444</v>
       </c>
       <c r="C14">
-        <v>0.008687458498950898</v>
+        <v>0.008635508151540194</v>
       </c>
       <c r="D14">
-        <v>0.0001604772912864719</v>
+        <v>0.0001731025162188118</v>
       </c>
       <c r="E14">
-        <v>0.0001906209278749646</v>
+        <v>0.0001921541471413092</v>
       </c>
       <c r="F14">
-        <v>0.2644361756264868</v>
+        <v>0.2358049671192343</v>
       </c>
       <c r="G14">
-        <v>0.1262697819155144</v>
+        <v>0.15169780312604</v>
       </c>
       <c r="H14">
-        <v>0.2583620952127686</v>
+        <v>0.2583620952127688</v>
       </c>
       <c r="I14">
         <v>14166</v>
@@ -887,28 +914,28 @@
         <v>22</v>
       </c>
       <c r="B15">
-        <v>0.008443125284138316</v>
+        <v>0.006498537234416675</v>
       </c>
       <c r="C15">
-        <v>0.008687458498950898</v>
+        <v>0.005640138541351778</v>
       </c>
       <c r="D15">
-        <v>0.0001601555041560421</v>
+        <v>0.0001029319227940973</v>
       </c>
       <c r="E15">
-        <v>0.0001906209278749646</v>
+        <v>9.104237776586397E-05</v>
       </c>
       <c r="F15">
-        <v>0.2659111193421716</v>
+        <v>0.1349712457446069</v>
       </c>
       <c r="G15">
-        <v>0.1262697819155144</v>
+        <v>0.2348896971370824</v>
       </c>
       <c r="H15">
-        <v>0.2583620952127686</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I15">
-        <v>14166</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -916,28 +943,28 @@
         <v>23</v>
       </c>
       <c r="B16">
-        <v>0.008418017610370062</v>
+        <v>0.006748081351245411</v>
       </c>
       <c r="C16">
-        <v>0.008687458498950898</v>
+        <v>0.005640138541351778</v>
       </c>
       <c r="D16">
-        <v>0.0001595007627511497</v>
+        <v>0.0001082335137856306</v>
       </c>
       <c r="E16">
-        <v>0.0001906209278749646</v>
+        <v>9.104237776586397E-05</v>
       </c>
       <c r="F16">
-        <v>0.2689121925027265</v>
+        <v>0.09041724804895079</v>
       </c>
       <c r="G16">
-        <v>0.1262697819155144</v>
+        <v>0.2348896971370824</v>
       </c>
       <c r="H16">
-        <v>0.2583620952127686</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I16">
-        <v>14166</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -945,28 +972,28 @@
         <v>24</v>
       </c>
       <c r="B17">
-        <v>0.007587864829138694</v>
+        <v>0.007232949133456665</v>
       </c>
       <c r="C17">
-        <v>0.008635508151540194</v>
+        <v>0.005640138541351778</v>
       </c>
       <c r="D17">
-        <v>0.0001393500412889987</v>
+        <v>0.0001213274276709267</v>
       </c>
       <c r="E17">
-        <v>0.0001921541471413092</v>
+        <v>9.104237776586397E-05</v>
       </c>
       <c r="F17">
-        <v>0.3848118923345282</v>
+        <v>-0.01962258904981384</v>
       </c>
       <c r="G17">
-        <v>0.15169780312604</v>
+        <v>0.2348896971370824</v>
       </c>
       <c r="H17">
-        <v>0.2583620952127688</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I17">
-        <v>14166</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -974,28 +1001,28 @@
         <v>25</v>
       </c>
       <c r="B18">
-        <v>0.009022455578369986</v>
+        <v>0.00698011858859047</v>
       </c>
       <c r="C18">
-        <v>0.008687458498950898</v>
+        <v>0.01116184410920933</v>
       </c>
       <c r="D18">
-        <v>0.0001738441260953471</v>
+        <v>0.0001206003995053095</v>
       </c>
       <c r="E18">
-        <v>0.0001906209278749646</v>
+        <v>0.0002568809119206026</v>
       </c>
       <c r="F18">
-        <v>0.2031679422648356</v>
+        <v>0.1961572221345995</v>
       </c>
       <c r="G18">
-        <v>0.1262697819155144</v>
+        <v>-0.7121988539495976</v>
       </c>
       <c r="H18">
-        <v>0.2583620952127686</v>
+        <v>-0.0971244535465241</v>
       </c>
       <c r="I18">
-        <v>14166</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1003,28 +1030,28 @@
         <v>26</v>
       </c>
       <c r="B19">
-        <v>0.009513742997451299</v>
+        <v>0.009500780046706191</v>
       </c>
       <c r="C19">
-        <v>0.008635508151540194</v>
+        <v>0.008679017950585495</v>
       </c>
       <c r="D19">
-        <v>0.0002127091144161235</v>
+        <v>0.0001906222323622052</v>
       </c>
       <c r="E19">
-        <v>0.0001921541471413092</v>
+        <v>0.0001903704215854449</v>
       </c>
       <c r="F19">
-        <v>0.06095386574396355</v>
+        <v>0.1254597737230357</v>
       </c>
       <c r="G19">
-        <v>0.15169780312604</v>
+        <v>0.1266150358923953</v>
       </c>
       <c r="H19">
-        <v>0.2583620952127688</v>
+        <v>0.258876568546933</v>
       </c>
       <c r="I19">
-        <v>14166</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1032,28 +1059,28 @@
         <v>27</v>
       </c>
       <c r="B20">
-        <v>0.005697104856796651</v>
+        <v>0.009511178178242779</v>
       </c>
       <c r="C20">
-        <v>0.005645917892372011</v>
+        <v>0.008679017950585495</v>
       </c>
       <c r="D20">
-        <v>8.879743897162471E-05</v>
+        <v>0.0001908835104177435</v>
       </c>
       <c r="E20">
-        <v>9.170236601052772E-05</v>
+        <v>0.0001903704215854449</v>
       </c>
       <c r="F20">
-        <v>0.283710677227887</v>
+        <v>0.1242610773958542</v>
       </c>
       <c r="G20">
-        <v>0.260277926852472</v>
+        <v>0.1266150358923953</v>
       </c>
       <c r="H20">
-        <v>0.4208397194991282</v>
+        <v>0.258876568546933</v>
       </c>
       <c r="I20">
-        <v>6771</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1061,25 +1088,25 @@
         <v>28</v>
       </c>
       <c r="B21">
-        <v>0.009225854121736928</v>
+        <v>0.008271263221934944</v>
       </c>
       <c r="C21">
-        <v>0.008687458498950898</v>
+        <v>0.008659154831887702</v>
       </c>
       <c r="D21">
-        <v>0.0001822661374906326</v>
+        <v>0.000162539775585851</v>
       </c>
       <c r="E21">
-        <v>0.0001906209278749646</v>
+        <v>0.0001949633210112301</v>
       </c>
       <c r="F21">
-        <v>0.1645648049538074</v>
+        <v>0.2920577529107484</v>
       </c>
       <c r="G21">
-        <v>0.1262697819155144</v>
+        <v>0.1508369500376733</v>
       </c>
       <c r="H21">
-        <v>0.2583620952127686</v>
+        <v>0.2583620952127688</v>
       </c>
       <c r="I21">
         <v>14166</v>
@@ -1090,25 +1117,25 @@
         <v>29</v>
       </c>
       <c r="B22">
-        <v>0.009548220646664947</v>
+        <v>0.008305626259430711</v>
       </c>
       <c r="C22">
-        <v>0.008687458498950898</v>
+        <v>0.008635508151540194</v>
       </c>
       <c r="D22">
-        <v>0.0001933459958501393</v>
+        <v>0.0001581971829802284</v>
       </c>
       <c r="E22">
-        <v>0.0001906209278749646</v>
+        <v>0.0001921541471413092</v>
       </c>
       <c r="F22">
-        <v>0.113779158442072</v>
+        <v>0.3016074861881056</v>
       </c>
       <c r="G22">
-        <v>0.1262697819155144</v>
+        <v>0.15169780312604</v>
       </c>
       <c r="H22">
-        <v>0.2583620952127686</v>
+        <v>0.2583620952127688</v>
       </c>
       <c r="I22">
         <v>14166</v>
@@ -1119,19 +1146,19 @@
         <v>30</v>
       </c>
       <c r="B23">
-        <v>0.01021710973531049</v>
+        <v>0.00844284418539723</v>
       </c>
       <c r="C23">
         <v>0.008687458498950898</v>
       </c>
       <c r="D23">
-        <v>0.0002201065094334888</v>
+        <v>0.0001604772912864719</v>
       </c>
       <c r="E23">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F23">
-        <v>-0.00888035030069112</v>
+        <v>0.2644361756264868</v>
       </c>
       <c r="G23">
         <v>0.1262697819155144</v>
@@ -1148,19 +1175,19 @@
         <v>31</v>
       </c>
       <c r="B24">
-        <v>0.009873209207006982</v>
+        <v>0.008443125284138316</v>
       </c>
       <c r="C24">
         <v>0.008687458498950898</v>
       </c>
       <c r="D24">
-        <v>0.0002181271559853543</v>
+        <v>0.0001601555041560421</v>
       </c>
       <c r="E24">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F24">
-        <v>0.0001922155460098995</v>
+        <v>0.2659111193421716</v>
       </c>
       <c r="G24">
         <v>0.1262697819155144</v>
@@ -1177,19 +1204,19 @@
         <v>32</v>
       </c>
       <c r="B25">
-        <v>0.009075753729992564</v>
+        <v>0.008418017610370062</v>
       </c>
       <c r="C25">
         <v>0.008687458498950898</v>
       </c>
       <c r="D25">
-        <v>0.0001756371360362956</v>
+        <v>0.0001595007627511497</v>
       </c>
       <c r="E25">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F25">
-        <v>0.1949495006477631</v>
+        <v>0.2689121925027265</v>
       </c>
       <c r="G25">
         <v>0.1262697819155144</v>
@@ -1198,6 +1225,267 @@
         <v>0.2583620952127686</v>
       </c>
       <c r="I25">
+        <v>14166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>0.007587864829138694</v>
+      </c>
+      <c r="C26">
+        <v>0.008635508151540194</v>
+      </c>
+      <c r="D26">
+        <v>0.0001393500412889987</v>
+      </c>
+      <c r="E26">
+        <v>0.0001921541471413092</v>
+      </c>
+      <c r="F26">
+        <v>0.3848118923345282</v>
+      </c>
+      <c r="G26">
+        <v>0.15169780312604</v>
+      </c>
+      <c r="H26">
+        <v>0.2583620952127688</v>
+      </c>
+      <c r="I26">
+        <v>14166</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27">
+        <v>0.009022455578369986</v>
+      </c>
+      <c r="C27">
+        <v>0.008687458498950898</v>
+      </c>
+      <c r="D27">
+        <v>0.0001738441260953471</v>
+      </c>
+      <c r="E27">
+        <v>0.0001906209278749646</v>
+      </c>
+      <c r="F27">
+        <v>0.2031679422648356</v>
+      </c>
+      <c r="G27">
+        <v>0.1262697819155144</v>
+      </c>
+      <c r="H27">
+        <v>0.2583620952127686</v>
+      </c>
+      <c r="I27">
+        <v>14166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <v>0.009513742997451299</v>
+      </c>
+      <c r="C28">
+        <v>0.008635508151540194</v>
+      </c>
+      <c r="D28">
+        <v>0.0002127091144161235</v>
+      </c>
+      <c r="E28">
+        <v>0.0001921541471413092</v>
+      </c>
+      <c r="F28">
+        <v>0.06095386574396355</v>
+      </c>
+      <c r="G28">
+        <v>0.15169780312604</v>
+      </c>
+      <c r="H28">
+        <v>0.2583620952127688</v>
+      </c>
+      <c r="I28">
+        <v>14166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29">
+        <v>0.005697104856796651</v>
+      </c>
+      <c r="C29">
+        <v>0.005645917892372011</v>
+      </c>
+      <c r="D29">
+        <v>8.879743897162471E-05</v>
+      </c>
+      <c r="E29">
+        <v>9.170236601052772E-05</v>
+      </c>
+      <c r="F29">
+        <v>0.283710677227887</v>
+      </c>
+      <c r="G29">
+        <v>0.260277926852472</v>
+      </c>
+      <c r="H29">
+        <v>0.4208397194991282</v>
+      </c>
+      <c r="I29">
+        <v>6771</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30">
+        <v>0.009225854121736928</v>
+      </c>
+      <c r="C30">
+        <v>0.008687458498950898</v>
+      </c>
+      <c r="D30">
+        <v>0.0001822661374906326</v>
+      </c>
+      <c r="E30">
+        <v>0.0001906209278749646</v>
+      </c>
+      <c r="F30">
+        <v>0.1645648049538074</v>
+      </c>
+      <c r="G30">
+        <v>0.1262697819155144</v>
+      </c>
+      <c r="H30">
+        <v>0.2583620952127686</v>
+      </c>
+      <c r="I30">
+        <v>14166</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31">
+        <v>0.009548220646664947</v>
+      </c>
+      <c r="C31">
+        <v>0.008687458498950898</v>
+      </c>
+      <c r="D31">
+        <v>0.0001933459958501393</v>
+      </c>
+      <c r="E31">
+        <v>0.0001906209278749646</v>
+      </c>
+      <c r="F31">
+        <v>0.113779158442072</v>
+      </c>
+      <c r="G31">
+        <v>0.1262697819155144</v>
+      </c>
+      <c r="H31">
+        <v>0.2583620952127686</v>
+      </c>
+      <c r="I31">
+        <v>14166</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32">
+        <v>0.01021710973531049</v>
+      </c>
+      <c r="C32">
+        <v>0.008687458498950898</v>
+      </c>
+      <c r="D32">
+        <v>0.0002201065094334888</v>
+      </c>
+      <c r="E32">
+        <v>0.0001906209278749646</v>
+      </c>
+      <c r="F32">
+        <v>-0.00888035030069112</v>
+      </c>
+      <c r="G32">
+        <v>0.1262697819155144</v>
+      </c>
+      <c r="H32">
+        <v>0.2583620952127686</v>
+      </c>
+      <c r="I32">
+        <v>14166</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>0.009873209207006982</v>
+      </c>
+      <c r="C33">
+        <v>0.008687458498950898</v>
+      </c>
+      <c r="D33">
+        <v>0.0002181271559853543</v>
+      </c>
+      <c r="E33">
+        <v>0.0001906209278749646</v>
+      </c>
+      <c r="F33">
+        <v>0.0001922155460098995</v>
+      </c>
+      <c r="G33">
+        <v>0.1262697819155144</v>
+      </c>
+      <c r="H33">
+        <v>0.2583620952127686</v>
+      </c>
+      <c r="I33">
+        <v>14166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>0.009075753729992564</v>
+      </c>
+      <c r="C34">
+        <v>0.008687458498950898</v>
+      </c>
+      <c r="D34">
+        <v>0.0001756371360362956</v>
+      </c>
+      <c r="E34">
+        <v>0.0001906209278749646</v>
+      </c>
+      <c r="F34">
+        <v>0.1949495006477631</v>
+      </c>
+      <c r="G34">
+        <v>0.1262697819155144</v>
+      </c>
+      <c r="H34">
+        <v>0.2583620952127686</v>
+      </c>
+      <c r="I34">
         <v>14166</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update dense top features
</commit_message>
<xml_diff>
--- a/results_analysis/compare_with_ibes/#compare_all.xlsx
+++ b/results_analysis/compare_with_ibes/#compare_all.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>lgbm_mae</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>ibes_1|fwdepsqcut|dense2｜all x 0 -fix space</t>
+  </si>
+  <si>
+    <t>ibes_1|fwdepsqcut|dense2｜small_space -best_col 10 -code 0</t>
   </si>
   <si>
     <t>ibes_2|fwdepsqcut|ibes_new industry_only ws -indi space3_sp500</t>
@@ -497,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -798,28 +801,28 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <v>0.00566147729919014</v>
+        <v>0.009796859060637545</v>
       </c>
       <c r="C11">
-        <v>0.005645917892372011</v>
+        <v>0.00916128901404265</v>
       </c>
       <c r="D11">
-        <v>8.617292926780686E-05</v>
+        <v>0.0001979826847859096</v>
       </c>
       <c r="E11">
-        <v>9.170236601052772E-05</v>
+        <v>0.0002092462997132058</v>
       </c>
       <c r="F11">
-        <v>0.3048814260707366</v>
+        <v>0.07836738039900737</v>
       </c>
       <c r="G11">
-        <v>0.260277926852472</v>
+        <v>0.02593393177269743</v>
       </c>
       <c r="H11">
-        <v>0.4208397194991282</v>
+        <v>0.1106454438525972</v>
       </c>
       <c r="I11">
-        <v>6771</v>
+        <v>4659</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -827,28 +830,28 @@
         <v>19</v>
       </c>
       <c r="B12">
-        <v>0.008657117254708444</v>
+        <v>0.00566147729919014</v>
       </c>
       <c r="C12">
-        <v>0.008635508151540194</v>
+        <v>0.005645917892372011</v>
       </c>
       <c r="D12">
-        <v>0.0001731025162188118</v>
+        <v>8.617292926780686E-05</v>
       </c>
       <c r="E12">
-        <v>0.0001921541471413092</v>
+        <v>9.170236601052772E-05</v>
       </c>
       <c r="F12">
-        <v>0.2358049671192343</v>
+        <v>0.3048814260707366</v>
       </c>
       <c r="G12">
-        <v>0.15169780312604</v>
+        <v>0.260277926852472</v>
       </c>
       <c r="H12">
-        <v>0.2583620952127688</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I12">
-        <v>14166</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -856,28 +859,28 @@
         <v>20</v>
       </c>
       <c r="B13">
-        <v>0.009187624256106797</v>
+        <v>0.008657117254708444</v>
       </c>
       <c r="C13">
-        <v>0.007760626981832584</v>
+        <v>0.008635508151540194</v>
       </c>
       <c r="D13">
-        <v>0.000170123123921569</v>
+        <v>0.0001731025162188118</v>
       </c>
       <c r="E13">
-        <v>0.0001663066979293028</v>
+        <v>0.0001921541471413092</v>
       </c>
       <c r="F13">
-        <v>0.1811552644422214</v>
+        <v>0.2358049671192343</v>
       </c>
       <c r="G13">
-        <v>0.1995246680857482</v>
+        <v>0.15169780312604</v>
       </c>
       <c r="H13">
-        <v>0.24728778214858</v>
+        <v>0.2583620952127688</v>
       </c>
       <c r="I13">
-        <v>140</v>
+        <v>14166</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -885,28 +888,28 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <v>0.006498537234416675</v>
+        <v>0.009187624256106797</v>
       </c>
       <c r="C14">
-        <v>0.005640138541351778</v>
+        <v>0.007760626981832584</v>
       </c>
       <c r="D14">
-        <v>0.0001029319227940973</v>
+        <v>0.000170123123921569</v>
       </c>
       <c r="E14">
-        <v>9.104237776586397E-05</v>
+        <v>0.0001663066979293028</v>
       </c>
       <c r="F14">
-        <v>0.1349712457446069</v>
+        <v>0.1811552644422214</v>
       </c>
       <c r="G14">
-        <v>0.2348896971370824</v>
+        <v>0.1995246680857482</v>
       </c>
       <c r="H14">
-        <v>0.4208397194991282</v>
+        <v>0.24728778214858</v>
       </c>
       <c r="I14">
-        <v>6771</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -914,19 +917,19 @@
         <v>22</v>
       </c>
       <c r="B15">
-        <v>0.006748081351245411</v>
+        <v>0.006498537234416675</v>
       </c>
       <c r="C15">
         <v>0.005640138541351778</v>
       </c>
       <c r="D15">
-        <v>0.0001082335137856306</v>
+        <v>0.0001029319227940973</v>
       </c>
       <c r="E15">
         <v>9.104237776586397E-05</v>
       </c>
       <c r="F15">
-        <v>0.09041724804895079</v>
+        <v>0.1349712457446069</v>
       </c>
       <c r="G15">
         <v>0.2348896971370824</v>
@@ -943,19 +946,19 @@
         <v>23</v>
       </c>
       <c r="B16">
-        <v>0.007232949133456665</v>
+        <v>0.006748081351245411</v>
       </c>
       <c r="C16">
         <v>0.005640138541351778</v>
       </c>
       <c r="D16">
-        <v>0.0001213274276709267</v>
+        <v>0.0001082335137856306</v>
       </c>
       <c r="E16">
         <v>9.104237776586397E-05</v>
       </c>
       <c r="F16">
-        <v>-0.01962258904981384</v>
+        <v>0.09041724804895079</v>
       </c>
       <c r="G16">
         <v>0.2348896971370824</v>
@@ -972,28 +975,28 @@
         <v>24</v>
       </c>
       <c r="B17">
-        <v>0.00698011858859047</v>
+        <v>0.007232949133456665</v>
       </c>
       <c r="C17">
-        <v>0.01116184410920933</v>
+        <v>0.005640138541351778</v>
       </c>
       <c r="D17">
-        <v>0.0001206003995053095</v>
+        <v>0.0001213274276709267</v>
       </c>
       <c r="E17">
-        <v>0.0002568809119206026</v>
+        <v>9.104237776586397E-05</v>
       </c>
       <c r="F17">
-        <v>0.1961572221345995</v>
+        <v>-0.01962258904981384</v>
       </c>
       <c r="G17">
-        <v>-0.7121988539495976</v>
+        <v>0.2348896971370824</v>
       </c>
       <c r="H17">
-        <v>-0.0971244535465241</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I17">
-        <v>1545</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1001,28 +1004,28 @@
         <v>25</v>
       </c>
       <c r="B18">
-        <v>0.009500780046706191</v>
+        <v>0.00698011858859047</v>
       </c>
       <c r="C18">
-        <v>0.008679017950585495</v>
+        <v>0.01116184410920933</v>
       </c>
       <c r="D18">
-        <v>0.0001906222323622052</v>
+        <v>0.0001206003995053095</v>
       </c>
       <c r="E18">
-        <v>0.0001903704215854449</v>
+        <v>0.0002568809119206026</v>
       </c>
       <c r="F18">
-        <v>0.1254597737230357</v>
+        <v>0.1961572221345995</v>
       </c>
       <c r="G18">
-        <v>0.1266150358923953</v>
+        <v>-0.7121988539495976</v>
       </c>
       <c r="H18">
-        <v>0.258876568546933</v>
+        <v>-0.0971244535465241</v>
       </c>
       <c r="I18">
-        <v>14156</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1030,19 +1033,19 @@
         <v>26</v>
       </c>
       <c r="B19">
-        <v>0.009511178178242779</v>
+        <v>0.009500780046706191</v>
       </c>
       <c r="C19">
         <v>0.008679017950585495</v>
       </c>
       <c r="D19">
-        <v>0.0001908835104177435</v>
+        <v>0.0001906222323622052</v>
       </c>
       <c r="E19">
         <v>0.0001903704215854449</v>
       </c>
       <c r="F19">
-        <v>0.1242610773958542</v>
+        <v>0.1254597737230357</v>
       </c>
       <c r="G19">
         <v>0.1266150358923953</v>
@@ -1059,28 +1062,28 @@
         <v>27</v>
       </c>
       <c r="B20">
-        <v>0.009537818792305376</v>
+        <v>0.009511178178242779</v>
       </c>
       <c r="C20">
-        <v>0.008331870765561454</v>
+        <v>0.008679017950585495</v>
       </c>
       <c r="D20">
-        <v>0.0001882493670466495</v>
+        <v>0.0001908835104177435</v>
       </c>
       <c r="E20">
-        <v>0.0001864150531956526</v>
+        <v>0.0001903704215854449</v>
       </c>
       <c r="F20">
-        <v>0.1478472391608965</v>
+        <v>0.1242610773958542</v>
       </c>
       <c r="G20">
-        <v>0.1561506700669093</v>
+        <v>0.1266150358923953</v>
       </c>
       <c r="H20">
-        <v>0.4578656362182956</v>
+        <v>0.258876568546933</v>
       </c>
       <c r="I20">
-        <v>2594</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1088,28 +1091,28 @@
         <v>28</v>
       </c>
       <c r="B21">
-        <v>0.008271263221934944</v>
+        <v>0.009537818792305376</v>
       </c>
       <c r="C21">
-        <v>0.008659154831887702</v>
+        <v>0.008331870765561454</v>
       </c>
       <c r="D21">
-        <v>0.000162539775585851</v>
+        <v>0.0001882493670466495</v>
       </c>
       <c r="E21">
-        <v>0.0001949633210112301</v>
+        <v>0.0001864150531956526</v>
       </c>
       <c r="F21">
-        <v>0.2920577529107484</v>
+        <v>0.1478472391608965</v>
       </c>
       <c r="G21">
-        <v>0.1508369500376733</v>
+        <v>0.1561506700669093</v>
       </c>
       <c r="H21">
-        <v>0.2583620952127688</v>
+        <v>0.4578656362182956</v>
       </c>
       <c r="I21">
-        <v>14166</v>
+        <v>2594</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1117,22 +1120,22 @@
         <v>29</v>
       </c>
       <c r="B22">
-        <v>0.008305626259430711</v>
+        <v>0.008271263221934944</v>
       </c>
       <c r="C22">
-        <v>0.008635508151540194</v>
+        <v>0.008659154831887702</v>
       </c>
       <c r="D22">
-        <v>0.0001581971829802284</v>
+        <v>0.000162539775585851</v>
       </c>
       <c r="E22">
-        <v>0.0001921541471413092</v>
+        <v>0.0001949633210112301</v>
       </c>
       <c r="F22">
-        <v>0.3016074861881056</v>
+        <v>0.2920577529107484</v>
       </c>
       <c r="G22">
-        <v>0.15169780312604</v>
+        <v>0.1508369500376733</v>
       </c>
       <c r="H22">
         <v>0.2583620952127688</v>
@@ -1146,25 +1149,25 @@
         <v>30</v>
       </c>
       <c r="B23">
-        <v>0.00844284418539723</v>
+        <v>0.008305626259430711</v>
       </c>
       <c r="C23">
-        <v>0.008687458498950898</v>
+        <v>0.008635508151540194</v>
       </c>
       <c r="D23">
-        <v>0.0001604772912864719</v>
+        <v>0.0001581971829802284</v>
       </c>
       <c r="E23">
-        <v>0.0001906209278749646</v>
+        <v>0.0001921541471413092</v>
       </c>
       <c r="F23">
-        <v>0.2644361756264868</v>
+        <v>0.3016074861881056</v>
       </c>
       <c r="G23">
-        <v>0.1262697819155144</v>
+        <v>0.15169780312604</v>
       </c>
       <c r="H23">
-        <v>0.2583620952127686</v>
+        <v>0.2583620952127688</v>
       </c>
       <c r="I23">
         <v>14166</v>
@@ -1175,19 +1178,19 @@
         <v>31</v>
       </c>
       <c r="B24">
-        <v>0.008443125284138316</v>
+        <v>0.00844284418539723</v>
       </c>
       <c r="C24">
         <v>0.008687458498950898</v>
       </c>
       <c r="D24">
-        <v>0.0001601555041560421</v>
+        <v>0.0001604772912864719</v>
       </c>
       <c r="E24">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F24">
-        <v>0.2659111193421716</v>
+        <v>0.2644361756264868</v>
       </c>
       <c r="G24">
         <v>0.1262697819155144</v>
@@ -1204,19 +1207,19 @@
         <v>32</v>
       </c>
       <c r="B25">
-        <v>0.008418017610370062</v>
+        <v>0.008443125284138316</v>
       </c>
       <c r="C25">
         <v>0.008687458498950898</v>
       </c>
       <c r="D25">
-        <v>0.0001595007627511497</v>
+        <v>0.0001601555041560421</v>
       </c>
       <c r="E25">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F25">
-        <v>0.2689121925027265</v>
+        <v>0.2659111193421716</v>
       </c>
       <c r="G25">
         <v>0.1262697819155144</v>
@@ -1233,25 +1236,25 @@
         <v>33</v>
       </c>
       <c r="B26">
-        <v>0.007587864829138694</v>
+        <v>0.008418017610370062</v>
       </c>
       <c r="C26">
-        <v>0.008635508151540194</v>
+        <v>0.008687458498950898</v>
       </c>
       <c r="D26">
-        <v>0.0001393500412889987</v>
+        <v>0.0001595007627511497</v>
       </c>
       <c r="E26">
-        <v>0.0001921541471413092</v>
+        <v>0.0001906209278749646</v>
       </c>
       <c r="F26">
-        <v>0.3848118923345282</v>
+        <v>0.2689121925027265</v>
       </c>
       <c r="G26">
-        <v>0.15169780312604</v>
+        <v>0.1262697819155144</v>
       </c>
       <c r="H26">
-        <v>0.2583620952127688</v>
+        <v>0.2583620952127686</v>
       </c>
       <c r="I26">
         <v>14166</v>
@@ -1262,25 +1265,25 @@
         <v>34</v>
       </c>
       <c r="B27">
-        <v>0.009022455578369986</v>
+        <v>0.007587864829138694</v>
       </c>
       <c r="C27">
-        <v>0.008687458498950898</v>
+        <v>0.008635508151540194</v>
       </c>
       <c r="D27">
-        <v>0.0001738441260953471</v>
+        <v>0.0001393500412889987</v>
       </c>
       <c r="E27">
-        <v>0.0001906209278749646</v>
+        <v>0.0001921541471413092</v>
       </c>
       <c r="F27">
-        <v>0.2031679422648356</v>
+        <v>0.3848118923345282</v>
       </c>
       <c r="G27">
-        <v>0.1262697819155144</v>
+        <v>0.15169780312604</v>
       </c>
       <c r="H27">
-        <v>0.2583620952127686</v>
+        <v>0.2583620952127688</v>
       </c>
       <c r="I27">
         <v>14166</v>
@@ -1291,25 +1294,25 @@
         <v>35</v>
       </c>
       <c r="B28">
-        <v>0.009513742997451299</v>
+        <v>0.009022455578369986</v>
       </c>
       <c r="C28">
-        <v>0.008635508151540194</v>
+        <v>0.008687458498950898</v>
       </c>
       <c r="D28">
-        <v>0.0002127091144161235</v>
+        <v>0.0001738441260953471</v>
       </c>
       <c r="E28">
-        <v>0.0001921541471413092</v>
+        <v>0.0001906209278749646</v>
       </c>
       <c r="F28">
-        <v>0.06095386574396355</v>
+        <v>0.2031679422648356</v>
       </c>
       <c r="G28">
-        <v>0.15169780312604</v>
+        <v>0.1262697819155144</v>
       </c>
       <c r="H28">
-        <v>0.2583620952127688</v>
+        <v>0.2583620952127686</v>
       </c>
       <c r="I28">
         <v>14166</v>
@@ -1320,28 +1323,28 @@
         <v>36</v>
       </c>
       <c r="B29">
-        <v>0.005697104856796651</v>
+        <v>0.009513742997451299</v>
       </c>
       <c r="C29">
-        <v>0.005645917892372011</v>
+        <v>0.008635508151540194</v>
       </c>
       <c r="D29">
-        <v>8.879743897162471E-05</v>
+        <v>0.0002127091144161235</v>
       </c>
       <c r="E29">
-        <v>9.170236601052772E-05</v>
+        <v>0.0001921541471413092</v>
       </c>
       <c r="F29">
-        <v>0.283710677227887</v>
+        <v>0.06095386574396355</v>
       </c>
       <c r="G29">
-        <v>0.260277926852472</v>
+        <v>0.15169780312604</v>
       </c>
       <c r="H29">
-        <v>0.4208397194991282</v>
+        <v>0.2583620952127688</v>
       </c>
       <c r="I29">
-        <v>6771</v>
+        <v>14166</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1349,28 +1352,28 @@
         <v>37</v>
       </c>
       <c r="B30">
-        <v>0.009225854121736928</v>
+        <v>0.005697104856796651</v>
       </c>
       <c r="C30">
-        <v>0.008687458498950898</v>
+        <v>0.005645917892372011</v>
       </c>
       <c r="D30">
-        <v>0.0001822661374906326</v>
+        <v>8.879743897162471E-05</v>
       </c>
       <c r="E30">
-        <v>0.0001906209278749646</v>
+        <v>9.170236601052772E-05</v>
       </c>
       <c r="F30">
-        <v>0.1645648049538074</v>
+        <v>0.283710677227887</v>
       </c>
       <c r="G30">
-        <v>0.1262697819155144</v>
+        <v>0.260277926852472</v>
       </c>
       <c r="H30">
-        <v>0.2583620952127686</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I30">
-        <v>14166</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1378,19 +1381,19 @@
         <v>38</v>
       </c>
       <c r="B31">
-        <v>0.009548220646664947</v>
+        <v>0.009225854121736928</v>
       </c>
       <c r="C31">
         <v>0.008687458498950898</v>
       </c>
       <c r="D31">
-        <v>0.0001933459958501393</v>
+        <v>0.0001822661374906326</v>
       </c>
       <c r="E31">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F31">
-        <v>0.113779158442072</v>
+        <v>0.1645648049538074</v>
       </c>
       <c r="G31">
         <v>0.1262697819155144</v>
@@ -1407,19 +1410,19 @@
         <v>39</v>
       </c>
       <c r="B32">
-        <v>0.01021710973531049</v>
+        <v>0.009548220646664947</v>
       </c>
       <c r="C32">
         <v>0.008687458498950898</v>
       </c>
       <c r="D32">
-        <v>0.0002201065094334888</v>
+        <v>0.0001933459958501393</v>
       </c>
       <c r="E32">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F32">
-        <v>-0.00888035030069112</v>
+        <v>0.113779158442072</v>
       </c>
       <c r="G32">
         <v>0.1262697819155144</v>
@@ -1436,19 +1439,19 @@
         <v>40</v>
       </c>
       <c r="B33">
-        <v>0.009873209207006982</v>
+        <v>0.01021710973531049</v>
       </c>
       <c r="C33">
         <v>0.008687458498950898</v>
       </c>
       <c r="D33">
-        <v>0.0002181271559853543</v>
+        <v>0.0002201065094334888</v>
       </c>
       <c r="E33">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F33">
-        <v>0.0001922155460098995</v>
+        <v>-0.00888035030069112</v>
       </c>
       <c r="G33">
         <v>0.1262697819155144</v>
@@ -1465,19 +1468,19 @@
         <v>41</v>
       </c>
       <c r="B34">
-        <v>0.009075753729992564</v>
+        <v>0.009873209207006982</v>
       </c>
       <c r="C34">
         <v>0.008687458498950898</v>
       </c>
       <c r="D34">
-        <v>0.0001756371360362956</v>
+        <v>0.0002181271559853543</v>
       </c>
       <c r="E34">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F34">
-        <v>0.1949495006477631</v>
+        <v>0.0001922155460098995</v>
       </c>
       <c r="G34">
         <v>0.1262697819155144</v>
@@ -1486,6 +1489,35 @@
         <v>0.2583620952127686</v>
       </c>
       <c r="I34">
+        <v>14166</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>0.009075753729992564</v>
+      </c>
+      <c r="C35">
+        <v>0.008687458498950898</v>
+      </c>
+      <c r="D35">
+        <v>0.0001756371360362956</v>
+      </c>
+      <c r="E35">
+        <v>0.0001906209278749646</v>
+      </c>
+      <c r="F35">
+        <v>0.1949495006477631</v>
+      </c>
+      <c r="G35">
+        <v>0.1262697819155144</v>
+      </c>
+      <c r="H35">
+        <v>0.2583620952127686</v>
+      </c>
+      <c r="I35">
         <v>14166</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update lgbm/dense hyperopt compare
</commit_message>
<xml_diff>
--- a/results_analysis/compare_with_ibes/#compare_all.xlsx
+++ b/results_analysis/compare_with_ibes/#compare_all.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>lgbm_mae</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>ibes_1|fwdepsqcut-15|dense2｜mini_tune15 -code 0 -exclude_fwd True</t>
+  </si>
+  <si>
+    <t>ibes_1|fwdepsqcut|cnn_rnn｜industry_exclude</t>
   </si>
   <si>
     <t>ibes_1|fwdepsqcut|rnn_eps｜all</t>
@@ -581,7 +584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2303,28 +2306,28 @@
         <v>67</v>
       </c>
       <c r="B60">
-        <v>0.009873209207006982</v>
+        <v>0.008143992441724007</v>
       </c>
       <c r="C60">
-        <v>0.008687458498950898</v>
+        <v>0.007878813965581622</v>
       </c>
       <c r="D60">
-        <v>0.0002181271559853543</v>
+        <v>0.0001471335863405383</v>
       </c>
       <c r="E60">
-        <v>0.0001906209278749646</v>
+        <v>0.0001597126811451271</v>
       </c>
       <c r="F60">
-        <v>0.0001922155460098995</v>
+        <v>0.2028347328879045</v>
       </c>
       <c r="G60">
-        <v>0.1262697819155144</v>
+        <v>0.1346815822760543</v>
       </c>
       <c r="H60">
-        <v>0.2583620952127686</v>
+        <v>0.3174117902090396</v>
       </c>
       <c r="I60">
-        <v>14166</v>
+        <v>6106</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2332,19 +2335,19 @@
         <v>68</v>
       </c>
       <c r="B61">
-        <v>0.009075753729992564</v>
+        <v>0.009873209207006982</v>
       </c>
       <c r="C61">
         <v>0.008687458498950898</v>
       </c>
       <c r="D61">
-        <v>0.0001756371360362956</v>
+        <v>0.0002181271559853543</v>
       </c>
       <c r="E61">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F61">
-        <v>0.1949495006477631</v>
+        <v>0.0001922155460098995</v>
       </c>
       <c r="G61">
         <v>0.1262697819155144</v>
@@ -2361,27 +2364,56 @@
         <v>69</v>
       </c>
       <c r="B62">
+        <v>0.009075753729992564</v>
+      </c>
+      <c r="C62">
+        <v>0.008687458498950898</v>
+      </c>
+      <c r="D62">
+        <v>0.0001756371360362956</v>
+      </c>
+      <c r="E62">
+        <v>0.0001906209278749646</v>
+      </c>
+      <c r="F62">
+        <v>0.1949495006477631</v>
+      </c>
+      <c r="G62">
+        <v>0.1262697819155144</v>
+      </c>
+      <c r="H62">
+        <v>0.2583620952127686</v>
+      </c>
+      <c r="I62">
+        <v>14166</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B63">
         <v>0.007268678906681078</v>
       </c>
-      <c r="C62">
+      <c r="C63">
         <v>0.006046426867297824</v>
       </c>
-      <c r="D62">
+      <c r="D63">
         <v>0.0001164217038619287</v>
       </c>
-      <c r="E62">
+      <c r="E63">
         <v>9.355464689912527E-05</v>
       </c>
-      <c r="F62">
+      <c r="F63">
         <v>0.2283759127095218</v>
       </c>
-      <c r="G62">
+      <c r="G63">
         <v>0.3799350410561445</v>
       </c>
-      <c r="H62">
+      <c r="H63">
         <v>0.545155985157215</v>
       </c>
-      <c r="I62">
+      <c r="I63">
         <v>132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update lgbm for qoq
</commit_message>
<xml_diff>
--- a/results_analysis/compare_with_ibes/#compare_all.xlsx
+++ b/results_analysis/compare_with_ibes/#compare_all.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>lgbm_mae</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>ibes_1|fwdepsqcut|rnn_eps｜all</t>
+  </si>
+  <si>
+    <t>ibes_1|fwdepsqcut-46|dense2｜compare_hyperopt -code 0 -exclude_fwd True</t>
   </si>
   <si>
     <t>ibes_1|ni|rnn_double｜all</t>
@@ -587,7 +590,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2396,28 +2399,28 @@
         <v>70</v>
       </c>
       <c r="B63">
-        <v>0.009075753729992564</v>
+        <v>0.009425532281481011</v>
       </c>
       <c r="C63">
-        <v>0.008687458498950898</v>
+        <v>0.008679017950585495</v>
       </c>
       <c r="D63">
-        <v>0.0001756371360362956</v>
+        <v>0.0001866655144276845</v>
       </c>
       <c r="E63">
-        <v>0.0001906209278749646</v>
+        <v>0.0001903704215854449</v>
       </c>
       <c r="F63">
-        <v>0.1949495006477631</v>
+        <v>0.1436124779217507</v>
       </c>
       <c r="G63">
-        <v>0.1262697819155144</v>
+        <v>0.1266150358923953</v>
       </c>
       <c r="H63">
-        <v>0.2583620952127686</v>
+        <v>0.258876568546933</v>
       </c>
       <c r="I63">
-        <v>14166</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2425,27 +2428,56 @@
         <v>71</v>
       </c>
       <c r="B64">
+        <v>0.009075753729992564</v>
+      </c>
+      <c r="C64">
+        <v>0.008687458498950898</v>
+      </c>
+      <c r="D64">
+        <v>0.0001756371360362956</v>
+      </c>
+      <c r="E64">
+        <v>0.0001906209278749646</v>
+      </c>
+      <c r="F64">
+        <v>0.1949495006477631</v>
+      </c>
+      <c r="G64">
+        <v>0.1262697819155144</v>
+      </c>
+      <c r="H64">
+        <v>0.2583620952127686</v>
+      </c>
+      <c r="I64">
+        <v>14166</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65">
         <v>0.007268678906681078</v>
       </c>
-      <c r="C64">
+      <c r="C65">
         <v>0.006046426867297824</v>
       </c>
-      <c r="D64">
+      <c r="D65">
         <v>0.0001164217038619287</v>
       </c>
-      <c r="E64">
+      <c r="E65">
         <v>9.355464689912527E-05</v>
       </c>
-      <c r="F64">
+      <c r="F65">
         <v>0.2283759127095218</v>
       </c>
-      <c r="G64">
+      <c r="G65">
         <v>0.3799350410561445</v>
       </c>
-      <c r="H64">
+      <c r="H65">
         <v>0.545155985157215</v>
       </c>
-      <c r="I64">
+      <c r="I65">
         <v>132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update ibes qoq for lgbm
</commit_message>
<xml_diff>
--- a/results_analysis/compare_with_ibes/#compare_all.xlsx
+++ b/results_analysis/compare_with_ibes/#compare_all.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>lgbm_mae</t>
   </si>
@@ -40,27 +40,27 @@
     <t>len</t>
   </si>
   <si>
+    <t>lgbm_mae_org</t>
+  </si>
+  <si>
+    <t>consensus_medae_org</t>
+  </si>
+  <si>
+    <t>lgbm_medae_org</t>
+  </si>
+  <si>
+    <t>consensus_mae_org</t>
+  </si>
+  <si>
+    <t>consensus_mse_org</t>
+  </si>
+  <si>
     <t>lgbm_mse_org</t>
   </si>
   <si>
     <t>lgbm_r2_org</t>
   </si>
   <si>
-    <t>consensus_mae_org</t>
-  </si>
-  <si>
-    <t>consensus_mse_org</t>
-  </si>
-  <si>
-    <t>lgbm_medae_org</t>
-  </si>
-  <si>
-    <t>consensus_medae_org</t>
-  </si>
-  <si>
-    <t>lgbm_mae_org</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>ibes_1|fwdepsqcut|dense2｜small_space -best_col 20 -code 0 -exclude_fwd True</t>
+  </si>
+  <si>
+    <t>ibes_qoq_1|fwdepsqcut|q_1｜ibes_qoqcut8_entire</t>
   </si>
   <si>
     <t>ibes_1|fwdepsqcut-30|dense2｜try_old_fix_space -code 0 -exclude_fwd True</t>
@@ -635,7 +638,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P73"/>
+  <dimension ref="A1:P74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -894,25 +897,25 @@
         <v>14156</v>
       </c>
       <c r="J8">
+        <v>0.008951069054337348</v>
+      </c>
+      <c r="K8">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="L8">
+        <v>0.004259924319068574</v>
+      </c>
+      <c r="M8">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="N8">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="O8">
         <v>0.0003414374258527852</v>
       </c>
-      <c r="K8">
+      <c r="P8">
         <v>0.2516268396831602</v>
-      </c>
-      <c r="L8">
-        <v>0.009674189396799987</v>
-      </c>
-      <c r="M8">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N8">
-        <v>0.004259924319068574</v>
-      </c>
-      <c r="O8">
-        <v>0.004818030126325817</v>
-      </c>
-      <c r="P8">
-        <v>0.008951069054337348</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1060,25 +1063,25 @@
         <v>14156</v>
       </c>
       <c r="J13">
+        <v>0.00941140169945745</v>
+      </c>
+      <c r="K13">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="L13">
+        <v>0.004590555422836876</v>
+      </c>
+      <c r="M13">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="N13">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="O13">
         <v>0.0003713407546776094</v>
       </c>
-      <c r="K13">
+      <c r="P13">
         <v>0.1860837943045432</v>
-      </c>
-      <c r="L13">
-        <v>0.009674189396799985</v>
-      </c>
-      <c r="M13">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N13">
-        <v>0.004590555422836876</v>
-      </c>
-      <c r="O13">
-        <v>0.004818030126325817</v>
-      </c>
-      <c r="P13">
-        <v>0.00941140169945745</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1110,25 +1113,25 @@
         <v>14156</v>
       </c>
       <c r="J14">
+        <v>0.009901025034115019</v>
+      </c>
+      <c r="K14">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="L14">
+        <v>0.005167135423672592</v>
+      </c>
+      <c r="M14">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="N14">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="O14">
         <v>0.0003847976244374441</v>
       </c>
-      <c r="K14">
+      <c r="P14">
         <v>0.1565886089862186</v>
-      </c>
-      <c r="L14">
-        <v>0.009674189396799985</v>
-      </c>
-      <c r="M14">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N14">
-        <v>0.005167135423672592</v>
-      </c>
-      <c r="O14">
-        <v>0.004818030126325817</v>
-      </c>
-      <c r="P14">
-        <v>0.009901025034115019</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1281,49 +1284,49 @@
         <v>34</v>
       </c>
       <c r="B20">
-        <v>0.002812384873893973</v>
+        <v>0.003208711377129972</v>
       </c>
       <c r="C20">
-        <v>0.002283724402157329</v>
+        <v>0.002538761048289119</v>
       </c>
       <c r="D20">
-        <v>1.516508609570697E-05</v>
+        <v>2.210896317387241E-05</v>
       </c>
       <c r="E20">
-        <v>1.523207734796392E-05</v>
+        <v>2.103311528121684E-05</v>
       </c>
       <c r="F20">
-        <v>-0.05766541073617004</v>
+        <v>-0.05017806464506647</v>
       </c>
       <c r="G20">
-        <v>-0.06233761173040864</v>
+        <v>0.0009248228524665336</v>
       </c>
       <c r="H20">
-        <v>0.2312337712453068</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I20">
-        <v>1459</v>
+        <v>11611</v>
       </c>
       <c r="J20">
-        <v>0.0001562888432910191</v>
+        <v>0.005213165544267774</v>
       </c>
       <c r="K20">
-        <v>-0.007754190208037803</v>
+        <v>0.001592932311570713</v>
       </c>
       <c r="L20">
-        <v>0.004271078110726871</v>
+        <v>0.00173711317318318</v>
       </c>
       <c r="M20">
-        <v>0.0001192250906230086</v>
+        <v>0.004580501696160511</v>
       </c>
       <c r="N20">
-        <v>0.001561632046979175</v>
+        <v>0.0001631540263502446</v>
       </c>
       <c r="O20">
-        <v>0.00157889310668356</v>
+        <v>0.0002098592232396584</v>
       </c>
       <c r="P20">
-        <v>0.005138249283900753</v>
+        <v>-0.01180186309853548</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1355,25 +1358,25 @@
         <v>49</v>
       </c>
       <c r="J21">
+        <v>0.007217175147339313</v>
+      </c>
+      <c r="K21">
+        <v>0.00129198945232948</v>
+      </c>
+      <c r="L21">
+        <v>0.002972419699024923</v>
+      </c>
+      <c r="M21">
+        <v>0.004529835290885987</v>
+      </c>
+      <c r="N21">
+        <v>0.0001158352549329261</v>
+      </c>
+      <c r="O21">
         <v>0.0003123469992588732</v>
       </c>
-      <c r="K21">
+      <c r="P21">
         <v>-0.01652918306199047</v>
-      </c>
-      <c r="L21">
-        <v>0.004529835290885987</v>
-      </c>
-      <c r="M21">
-        <v>0.0001158352549329261</v>
-      </c>
-      <c r="N21">
-        <v>0.002972419699024923</v>
-      </c>
-      <c r="O21">
-        <v>0.00129198945232948</v>
-      </c>
-      <c r="P21">
-        <v>0.007217175147339313</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1700,19 +1703,19 @@
         <v>47</v>
       </c>
       <c r="B33">
-        <v>0.003046448578040632</v>
+        <v>0.00304699828992123</v>
       </c>
       <c r="C33">
         <v>0.002499571894821071</v>
       </c>
       <c r="D33">
-        <v>1.903387050494043E-05</v>
+        <v>1.903121423403654E-05</v>
       </c>
       <c r="E33">
         <v>1.967007435869721E-05</v>
       </c>
       <c r="F33">
-        <v>-0.008721084963113857</v>
+        <v>-0.008580312939503454</v>
       </c>
       <c r="G33">
         <v>-0.04243741404356438</v>
@@ -1724,25 +1727,25 @@
         <v>11611</v>
       </c>
       <c r="J33">
-        <v>0.0002079441691750461</v>
+        <v>0.005107549406927882</v>
       </c>
       <c r="K33">
-        <v>-0.002568743674014051</v>
+        <v>0.001592932311570713</v>
       </c>
       <c r="L33">
+        <v>0.001554596452837835</v>
+      </c>
+      <c r="M33">
         <v>0.004580501696160511</v>
       </c>
-      <c r="M33">
+      <c r="N33">
         <v>0.0001631540263502446</v>
       </c>
-      <c r="N33">
-        <v>0.00157181670829126</v>
-      </c>
       <c r="O33">
-        <v>0.001592932311570713</v>
+        <v>0.000207986162951978</v>
       </c>
       <c r="P33">
-        <v>0.005106354780984327</v>
+        <v>-0.002771209789547591</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -2069,28 +2072,49 @@
         <v>59</v>
       </c>
       <c r="B45">
-        <v>0.009431375487177065</v>
+        <v>0.003030458698074221</v>
       </c>
       <c r="C45">
-        <v>0.008331870765561454</v>
+        <v>0.002499571894821071</v>
       </c>
       <c r="D45">
-        <v>0.0001851619411854762</v>
+        <v>1.91281128971015E-05</v>
       </c>
       <c r="E45">
-        <v>0.0001864150531956526</v>
+        <v>1.967007435869721E-05</v>
       </c>
       <c r="F45">
-        <v>0.1618231611666948</v>
+        <v>-0.01371556509502225</v>
       </c>
       <c r="G45">
-        <v>0.1561506700669093</v>
+        <v>-0.04243741404356438</v>
       </c>
       <c r="H45">
-        <v>0.4578656362182956</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I45">
-        <v>2594</v>
+        <v>11611</v>
+      </c>
+      <c r="J45">
+        <v>0.005089488294347637</v>
+      </c>
+      <c r="K45">
+        <v>0.001592932311570713</v>
+      </c>
+      <c r="L45">
+        <v>0.001547174514616301</v>
+      </c>
+      <c r="M45">
+        <v>0.004580501696160511</v>
+      </c>
+      <c r="N45">
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="O45">
+        <v>0.0002081444394071696</v>
+      </c>
+      <c r="P45">
+        <v>-0.00353431378743374</v>
       </c>
     </row>
     <row r="46" spans="1:16">
@@ -2098,19 +2122,19 @@
         <v>60</v>
       </c>
       <c r="B46">
-        <v>0.009213138281419604</v>
+        <v>0.009431375487177065</v>
       </c>
       <c r="C46">
         <v>0.008331870765561454</v>
       </c>
       <c r="D46">
-        <v>0.0001786321245598429</v>
+        <v>0.0001851619411854762</v>
       </c>
       <c r="E46">
         <v>0.0001864150531956526</v>
       </c>
       <c r="F46">
-        <v>0.1913818330103436</v>
+        <v>0.1618231611666948</v>
       </c>
       <c r="G46">
         <v>0.1561506700669093</v>
@@ -2127,28 +2151,28 @@
         <v>61</v>
       </c>
       <c r="B47">
-        <v>0.009521740671266687</v>
+        <v>0.009213138281419604</v>
       </c>
       <c r="C47">
-        <v>0.008473401446470291</v>
+        <v>0.008331870765561454</v>
       </c>
       <c r="D47">
-        <v>0.0001891421517246861</v>
+        <v>0.0001786321245598429</v>
       </c>
       <c r="E47">
-        <v>0.0001919309980664785</v>
+        <v>0.0001864150531956526</v>
       </c>
       <c r="F47">
-        <v>0.1616607241628776</v>
+        <v>0.1913818330103436</v>
       </c>
       <c r="G47">
-        <v>0.1492996539240107</v>
+        <v>0.1561506700669093</v>
       </c>
       <c r="H47">
-        <v>0.4756280385081123</v>
+        <v>0.4578656362182956</v>
       </c>
       <c r="I47">
-        <v>1913</v>
+        <v>2594</v>
       </c>
     </row>
     <row r="48" spans="1:16">
@@ -2156,28 +2180,28 @@
         <v>62</v>
       </c>
       <c r="B48">
-        <v>0.008305626259430711</v>
+        <v>0.009521740671266687</v>
       </c>
       <c r="C48">
-        <v>0.008635508151540194</v>
+        <v>0.008473401446470291</v>
       </c>
       <c r="D48">
-        <v>0.0001581971829802284</v>
+        <v>0.0001891421517246861</v>
       </c>
       <c r="E48">
-        <v>0.0001921541471413092</v>
+        <v>0.0001919309980664785</v>
       </c>
       <c r="F48">
-        <v>0.3016074861881056</v>
+        <v>0.1616607241628776</v>
       </c>
       <c r="G48">
-        <v>0.15169780312604</v>
+        <v>0.1492996539240107</v>
       </c>
       <c r="H48">
-        <v>0.2583620952127688</v>
+        <v>0.4756280385081123</v>
       </c>
       <c r="I48">
-        <v>14166</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -2185,28 +2209,28 @@
         <v>63</v>
       </c>
       <c r="B49">
-        <v>0.008566233899661557</v>
+        <v>0.008305626259430711</v>
       </c>
       <c r="C49">
-        <v>0.008733878054388279</v>
+        <v>0.008635508151540194</v>
       </c>
       <c r="D49">
-        <v>0.0001667117782159728</v>
+        <v>0.0001581971829802284</v>
       </c>
       <c r="E49">
-        <v>0.0001961492659581503</v>
+        <v>0.0001921541471413092</v>
       </c>
       <c r="F49">
-        <v>0.2589089573160904</v>
+        <v>0.3016074861881056</v>
       </c>
       <c r="G49">
-        <v>0.1280492261183163</v>
+        <v>0.15169780312604</v>
       </c>
       <c r="H49">
-        <v>0.2582640092197721</v>
+        <v>0.2583620952127688</v>
       </c>
       <c r="I49">
-        <v>14156</v>
+        <v>14166</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -2214,28 +2238,28 @@
         <v>64</v>
       </c>
       <c r="B50">
-        <v>0.00844284418539723</v>
+        <v>0.008566233899661557</v>
       </c>
       <c r="C50">
-        <v>0.008687458498950898</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D50">
-        <v>0.0001604772912864719</v>
+        <v>0.0001667117782159728</v>
       </c>
       <c r="E50">
-        <v>0.0001906209278749646</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F50">
-        <v>0.2644361756264868</v>
+        <v>0.2589089573160904</v>
       </c>
       <c r="G50">
-        <v>0.1262697819155144</v>
+        <v>0.1280492261183163</v>
       </c>
       <c r="H50">
-        <v>0.2583620952127686</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I50">
-        <v>14166</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -2243,19 +2267,19 @@
         <v>65</v>
       </c>
       <c r="B51">
-        <v>0.008443125284138316</v>
+        <v>0.00844284418539723</v>
       </c>
       <c r="C51">
         <v>0.008687458498950898</v>
       </c>
       <c r="D51">
-        <v>0.0001601555041560421</v>
+        <v>0.0001604772912864719</v>
       </c>
       <c r="E51">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F51">
-        <v>0.2659111193421716</v>
+        <v>0.2644361756264868</v>
       </c>
       <c r="G51">
         <v>0.1262697819155144</v>
@@ -2272,19 +2296,19 @@
         <v>66</v>
       </c>
       <c r="B52">
-        <v>0.008418017610370062</v>
+        <v>0.008443125284138316</v>
       </c>
       <c r="C52">
         <v>0.008687458498950898</v>
       </c>
       <c r="D52">
-        <v>0.0001595007627511497</v>
+        <v>0.0001601555041560421</v>
       </c>
       <c r="E52">
         <v>0.0001906209278749646</v>
       </c>
       <c r="F52">
-        <v>0.2689121925027265</v>
+        <v>0.2659111193421716</v>
       </c>
       <c r="G52">
         <v>0.1262697819155144</v>
@@ -2301,28 +2325,28 @@
         <v>67</v>
       </c>
       <c r="B53">
-        <v>0.006737431007939466</v>
+        <v>0.008418017610370062</v>
       </c>
       <c r="C53">
-        <v>0.005640138541351778</v>
+        <v>0.008687458498950898</v>
       </c>
       <c r="D53">
-        <v>0.0001099373919831</v>
+        <v>0.0001595007627511497</v>
       </c>
       <c r="E53">
-        <v>9.104237776586397E-05</v>
+        <v>0.0001906209278749646</v>
       </c>
       <c r="F53">
-        <v>0.07609803983297014</v>
+        <v>0.2689121925027265</v>
       </c>
       <c r="G53">
-        <v>0.2348896971370824</v>
+        <v>0.1262697819155144</v>
       </c>
       <c r="H53">
-        <v>0.4208397194991282</v>
+        <v>0.2583620952127686</v>
       </c>
       <c r="I53">
-        <v>6771</v>
+        <v>14166</v>
       </c>
     </row>
     <row r="54" spans="1:16">
@@ -2330,28 +2354,28 @@
         <v>68</v>
       </c>
       <c r="B54">
-        <v>0.008568525319576314</v>
+        <v>0.006737431007939466</v>
       </c>
       <c r="C54">
-        <v>0.008679017950585495</v>
+        <v>0.005640138541351778</v>
       </c>
       <c r="D54">
-        <v>0.0001555938584338752</v>
+        <v>0.0001099373919831</v>
       </c>
       <c r="E54">
-        <v>0.0001903704215854449</v>
+        <v>9.104237776586397E-05</v>
       </c>
       <c r="F54">
-        <v>0.2861635997237094</v>
+        <v>0.07609803983297014</v>
       </c>
       <c r="G54">
-        <v>0.1266150358923953</v>
+        <v>0.2348896971370824</v>
       </c>
       <c r="H54">
-        <v>0.258876568546933</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I54">
-        <v>14156</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="55" spans="1:16">
@@ -2359,19 +2383,19 @@
         <v>69</v>
       </c>
       <c r="B55">
-        <v>0.008568301756599091</v>
+        <v>0.008568525319576314</v>
       </c>
       <c r="C55">
         <v>0.008679017950585495</v>
       </c>
       <c r="D55">
-        <v>0.0001558200457817436</v>
+        <v>0.0001555938584338752</v>
       </c>
       <c r="E55">
         <v>0.0001903704215854449</v>
       </c>
       <c r="F55">
-        <v>0.2851258931984286</v>
+        <v>0.2861635997237094</v>
       </c>
       <c r="G55">
         <v>0.1266150358923953</v>
@@ -2388,49 +2412,28 @@
         <v>70</v>
       </c>
       <c r="B56">
-        <v>0.008450726600709063</v>
+        <v>0.008568301756599091</v>
       </c>
       <c r="C56">
-        <v>0.008433226871355401</v>
+        <v>0.008679017950585495</v>
       </c>
       <c r="D56">
-        <v>0.0001549249612650655</v>
+        <v>0.0001558200457817436</v>
       </c>
       <c r="E56">
-        <v>0.0001840954346652929</v>
+        <v>0.0001903704215854449</v>
       </c>
       <c r="F56">
-        <v>0.2658406287925501</v>
+        <v>0.2851258931984286</v>
       </c>
       <c r="G56">
-        <v>0.1276074077901983</v>
+        <v>0.1266150358923953</v>
       </c>
       <c r="H56">
-        <v>0.2996835042774059</v>
+        <v>0.258876568546933</v>
       </c>
       <c r="I56">
-        <v>10862</v>
-      </c>
-      <c r="J56">
-        <v>0.0003600819593885352</v>
-      </c>
-      <c r="K56">
-        <v>0.19021395116394</v>
-      </c>
-      <c r="L56">
-        <v>0.009263287100042681</v>
-      </c>
-      <c r="M56">
-        <v>0.0003114048906305079</v>
-      </c>
-      <c r="N56">
-        <v>0.005164425551457941</v>
-      </c>
-      <c r="O56">
-        <v>0.004749269227434182</v>
-      </c>
-      <c r="P56">
-        <v>0.009425485247894754</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="57" spans="1:16">
@@ -2438,28 +2441,49 @@
         <v>71</v>
       </c>
       <c r="B57">
-        <v>0.008663322838252873</v>
+        <v>0.008450726600709063</v>
       </c>
       <c r="C57">
-        <v>0.008331870765561454</v>
+        <v>0.008433226871355401</v>
       </c>
       <c r="D57">
-        <v>0.0001555658409623722</v>
+        <v>0.0001549249612650655</v>
       </c>
       <c r="E57">
-        <v>0.0001864150531956526</v>
+        <v>0.0001840954346652929</v>
       </c>
       <c r="F57">
-        <v>0.2957965121046511</v>
+        <v>0.2658406287925501</v>
       </c>
       <c r="G57">
-        <v>0.1561506700669093</v>
+        <v>0.1276074077901983</v>
       </c>
       <c r="H57">
-        <v>0.4578656362182956</v>
+        <v>0.2996835042774059</v>
       </c>
       <c r="I57">
-        <v>2594</v>
+        <v>10862</v>
+      </c>
+      <c r="J57">
+        <v>0.009425485247894754</v>
+      </c>
+      <c r="K57">
+        <v>0.004749269227434182</v>
+      </c>
+      <c r="L57">
+        <v>0.005164425551457941</v>
+      </c>
+      <c r="M57">
+        <v>0.009263287100042681</v>
+      </c>
+      <c r="N57">
+        <v>0.0003114048906305079</v>
+      </c>
+      <c r="O57">
+        <v>0.0003600819593885352</v>
+      </c>
+      <c r="P57">
+        <v>0.19021395116394</v>
       </c>
     </row>
     <row r="58" spans="1:16">
@@ -2467,49 +2491,28 @@
         <v>72</v>
       </c>
       <c r="B58">
-        <v>0.007042340695254111</v>
+        <v>0.008663322838252873</v>
       </c>
       <c r="C58">
-        <v>0.008074502417539058</v>
+        <v>0.008331870765561454</v>
       </c>
       <c r="D58">
-        <v>0.0001164246615512812</v>
+        <v>0.0001555658409623722</v>
       </c>
       <c r="E58">
-        <v>0.0001634338822360271</v>
+        <v>0.0001864150531956526</v>
       </c>
       <c r="F58">
-        <v>0.3809904691868308</v>
+        <v>0.2957965121046511</v>
       </c>
       <c r="G58">
-        <v>0.1310506776320999</v>
+        <v>0.1561506700669093</v>
       </c>
       <c r="H58">
-        <v>0.2582640092197721</v>
+        <v>0.4578656362182956</v>
       </c>
       <c r="I58">
-        <v>14156</v>
-      </c>
-      <c r="J58">
-        <v>0.0003344607981243851</v>
-      </c>
-      <c r="K58">
-        <v>0.2669184291403396</v>
-      </c>
-      <c r="L58">
-        <v>0.009674189396799985</v>
-      </c>
-      <c r="M58">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N58">
-        <v>0.004128330862335852</v>
-      </c>
-      <c r="O58">
-        <v>0.004818030126325817</v>
-      </c>
-      <c r="P58">
-        <v>0.00867861064019221</v>
+        <v>2594</v>
       </c>
     </row>
     <row r="59" spans="1:16">
@@ -2517,28 +2520,49 @@
         <v>73</v>
       </c>
       <c r="B59">
-        <v>0.009515496626389803</v>
+        <v>0.007042340695254111</v>
       </c>
       <c r="C59">
-        <v>0.008308090246589133</v>
+        <v>0.008074502417539058</v>
       </c>
       <c r="D59">
-        <v>0.0001993153466151802</v>
+        <v>0.0001164246615512812</v>
       </c>
       <c r="E59">
-        <v>0.00017724771883908</v>
+        <v>0.0001634338822360271</v>
       </c>
       <c r="F59">
-        <v>0.1010295363033313</v>
+        <v>0.3809904691868308</v>
       </c>
       <c r="G59">
-        <v>0.2005609868988942</v>
+        <v>0.1310506776320999</v>
       </c>
       <c r="H59">
-        <v>0.2957094929413533</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I59">
-        <v>2745</v>
+        <v>14156</v>
+      </c>
+      <c r="J59">
+        <v>0.00867861064019221</v>
+      </c>
+      <c r="K59">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="L59">
+        <v>0.004128330862335852</v>
+      </c>
+      <c r="M59">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="N59">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="O59">
+        <v>0.0003344607981243851</v>
+      </c>
+      <c r="P59">
+        <v>0.2669184291403396</v>
       </c>
     </row>
     <row r="60" spans="1:16">
@@ -2546,28 +2570,28 @@
         <v>74</v>
       </c>
       <c r="B60">
-        <v>0.009022455578369986</v>
+        <v>0.009515496626389803</v>
       </c>
       <c r="C60">
-        <v>0.008687458498950898</v>
+        <v>0.008308090246589133</v>
       </c>
       <c r="D60">
-        <v>0.0001738441260953471</v>
+        <v>0.0001993153466151802</v>
       </c>
       <c r="E60">
-        <v>0.0001906209278749646</v>
+        <v>0.00017724771883908</v>
       </c>
       <c r="F60">
-        <v>0.2031679422648356</v>
+        <v>0.1010295363033313</v>
       </c>
       <c r="G60">
-        <v>0.1262697819155144</v>
+        <v>0.2005609868988942</v>
       </c>
       <c r="H60">
-        <v>0.2583620952127686</v>
+        <v>0.2957094929413533</v>
       </c>
       <c r="I60">
-        <v>14166</v>
+        <v>2745</v>
       </c>
     </row>
     <row r="61" spans="1:16">
@@ -2575,25 +2599,25 @@
         <v>75</v>
       </c>
       <c r="B61">
-        <v>0.009513742997451299</v>
+        <v>0.009022455578369986</v>
       </c>
       <c r="C61">
-        <v>0.008635508151540194</v>
+        <v>0.008687458498950898</v>
       </c>
       <c r="D61">
-        <v>0.0002127091144161235</v>
+        <v>0.0001738441260953471</v>
       </c>
       <c r="E61">
-        <v>0.0001921541471413092</v>
+        <v>0.0001906209278749646</v>
       </c>
       <c r="F61">
-        <v>0.06095386574396355</v>
+        <v>0.2031679422648356</v>
       </c>
       <c r="G61">
-        <v>0.15169780312604</v>
+        <v>0.1262697819155144</v>
       </c>
       <c r="H61">
-        <v>0.2583620952127688</v>
+        <v>0.2583620952127686</v>
       </c>
       <c r="I61">
         <v>14166</v>
@@ -2604,28 +2628,28 @@
         <v>76</v>
       </c>
       <c r="B62">
-        <v>0.005697104856796651</v>
+        <v>0.009513742997451299</v>
       </c>
       <c r="C62">
-        <v>0.005645917892372011</v>
+        <v>0.008635508151540194</v>
       </c>
       <c r="D62">
-        <v>8.879743897162471E-05</v>
+        <v>0.0002127091144161235</v>
       </c>
       <c r="E62">
-        <v>9.170236601052772E-05</v>
+        <v>0.0001921541471413092</v>
       </c>
       <c r="F62">
-        <v>0.283710677227887</v>
+        <v>0.06095386574396355</v>
       </c>
       <c r="G62">
-        <v>0.260277926852472</v>
+        <v>0.15169780312604</v>
       </c>
       <c r="H62">
-        <v>0.4208397194991282</v>
+        <v>0.2583620952127688</v>
       </c>
       <c r="I62">
-        <v>6771</v>
+        <v>14166</v>
       </c>
     </row>
     <row r="63" spans="1:16">
@@ -2633,28 +2657,28 @@
         <v>77</v>
       </c>
       <c r="B63">
-        <v>0.009562492443911191</v>
+        <v>0.005697104856796651</v>
       </c>
       <c r="C63">
-        <v>0.008308090246589133</v>
+        <v>0.005645917892372011</v>
       </c>
       <c r="D63">
-        <v>0.000199661525996111</v>
+        <v>8.879743897162471E-05</v>
       </c>
       <c r="E63">
-        <v>0.00017724771883908</v>
+        <v>9.170236601052772E-05</v>
       </c>
       <c r="F63">
-        <v>0.09946816612345044</v>
+        <v>0.283710677227887</v>
       </c>
       <c r="G63">
-        <v>0.2005609868988942</v>
+        <v>0.260277926852472</v>
       </c>
       <c r="H63">
-        <v>0.2957094929413533</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I63">
-        <v>2745</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="64" spans="1:16">
@@ -2662,28 +2686,28 @@
         <v>78</v>
       </c>
       <c r="B64">
-        <v>0.00922109220409561</v>
+        <v>0.009562492443911191</v>
       </c>
       <c r="C64">
-        <v>0.008679017950585495</v>
+        <v>0.008308090246589133</v>
       </c>
       <c r="D64">
-        <v>0.0001821404655544099</v>
+        <v>0.000199661525996111</v>
       </c>
       <c r="E64">
-        <v>0.0001903704215854449</v>
+        <v>0.00017724771883908</v>
       </c>
       <c r="F64">
-        <v>0.1643725813813959</v>
+        <v>0.09946816612345044</v>
       </c>
       <c r="G64">
-        <v>0.1266150358923953</v>
+        <v>0.2005609868988942</v>
       </c>
       <c r="H64">
-        <v>0.258876568546933</v>
+        <v>0.2957094929413533</v>
       </c>
       <c r="I64">
-        <v>14156</v>
+        <v>2745</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -2691,19 +2715,19 @@
         <v>79</v>
       </c>
       <c r="B65">
-        <v>0.009543193605630669</v>
+        <v>0.00922109220409561</v>
       </c>
       <c r="C65">
         <v>0.008679017950585495</v>
       </c>
       <c r="D65">
-        <v>0.0001932073203207784</v>
+        <v>0.0001821404655544099</v>
       </c>
       <c r="E65">
         <v>0.0001903704215854449</v>
       </c>
       <c r="F65">
-        <v>0.1135998590623956</v>
+        <v>0.1643725813813959</v>
       </c>
       <c r="G65">
         <v>0.1266150358923953</v>
@@ -2720,19 +2744,19 @@
         <v>80</v>
       </c>
       <c r="B66">
-        <v>0.01021070502741315</v>
+        <v>0.009543193605630669</v>
       </c>
       <c r="C66">
         <v>0.008679017950585495</v>
       </c>
       <c r="D66">
-        <v>0.0002199208428079721</v>
+        <v>0.0001932073203207784</v>
       </c>
       <c r="E66">
         <v>0.0001903704215854449</v>
       </c>
       <c r="F66">
-        <v>-0.008956936706391971</v>
+        <v>0.1135998590623956</v>
       </c>
       <c r="G66">
         <v>0.1266150358923953</v>
@@ -2749,19 +2773,19 @@
         <v>81</v>
       </c>
       <c r="B67">
-        <v>0.009313491338202078</v>
+        <v>0.01021070502741315</v>
       </c>
       <c r="C67">
         <v>0.008679017950585495</v>
       </c>
       <c r="D67">
-        <v>0.0001903405980438034</v>
+        <v>0.0002199208428079721</v>
       </c>
       <c r="E67">
         <v>0.0001903704215854449</v>
       </c>
       <c r="F67">
-        <v>0.1267518608919368</v>
+        <v>-0.008956936706391971</v>
       </c>
       <c r="G67">
         <v>0.1266150358923953</v>
@@ -2778,28 +2802,28 @@
         <v>82</v>
       </c>
       <c r="B68">
-        <v>0.008143992441724007</v>
+        <v>0.009313491338202078</v>
       </c>
       <c r="C68">
-        <v>0.007878813965581622</v>
+        <v>0.008679017950585495</v>
       </c>
       <c r="D68">
-        <v>0.0001471335863405383</v>
+        <v>0.0001903405980438034</v>
       </c>
       <c r="E68">
-        <v>0.0001597126811451271</v>
+        <v>0.0001903704215854449</v>
       </c>
       <c r="F68">
-        <v>0.2028347328879045</v>
+        <v>0.1267518608919368</v>
       </c>
       <c r="G68">
-        <v>0.1346815822760543</v>
+        <v>0.1266150358923953</v>
       </c>
       <c r="H68">
-        <v>0.3174117902090396</v>
+        <v>0.258876568546933</v>
       </c>
       <c r="I68">
-        <v>6106</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -2807,28 +2831,28 @@
         <v>83</v>
       </c>
       <c r="B69">
-        <v>0.009873209207006982</v>
+        <v>0.008143992441724007</v>
       </c>
       <c r="C69">
-        <v>0.008687458498950898</v>
+        <v>0.007878813965581622</v>
       </c>
       <c r="D69">
-        <v>0.0002181271559853543</v>
+        <v>0.0001471335863405383</v>
       </c>
       <c r="E69">
-        <v>0.0001906209278749646</v>
+        <v>0.0001597126811451271</v>
       </c>
       <c r="F69">
-        <v>0.0001922155460098995</v>
+        <v>0.2028347328879045</v>
       </c>
       <c r="G69">
-        <v>0.1262697819155144</v>
+        <v>0.1346815822760543</v>
       </c>
       <c r="H69">
-        <v>0.2583620952127686</v>
+        <v>0.3174117902090396</v>
       </c>
       <c r="I69">
-        <v>14166</v>
+        <v>6106</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -2836,28 +2860,28 @@
         <v>84</v>
       </c>
       <c r="B70">
-        <v>0.009425532281481011</v>
+        <v>0.009873209207006982</v>
       </c>
       <c r="C70">
-        <v>0.008679017950585495</v>
+        <v>0.008687458498950898</v>
       </c>
       <c r="D70">
-        <v>0.0001866655144276845</v>
+        <v>0.0002181271559853543</v>
       </c>
       <c r="E70">
-        <v>0.0001903704215854449</v>
+        <v>0.0001906209278749646</v>
       </c>
       <c r="F70">
-        <v>0.1436124779217507</v>
+        <v>0.0001922155460098995</v>
       </c>
       <c r="G70">
-        <v>0.1266150358923953</v>
+        <v>0.1262697819155144</v>
       </c>
       <c r="H70">
-        <v>0.258876568546933</v>
+        <v>0.2583620952127686</v>
       </c>
       <c r="I70">
-        <v>14156</v>
+        <v>14166</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -2865,28 +2889,28 @@
         <v>85</v>
       </c>
       <c r="B71">
-        <v>0.009075753729992564</v>
+        <v>0.009425532281481011</v>
       </c>
       <c r="C71">
-        <v>0.008687458498950898</v>
+        <v>0.008679017950585495</v>
       </c>
       <c r="D71">
-        <v>0.0001756371360362956</v>
+        <v>0.0001866655144276845</v>
       </c>
       <c r="E71">
-        <v>0.0001906209278749646</v>
+        <v>0.0001903704215854449</v>
       </c>
       <c r="F71">
-        <v>0.1949495006477631</v>
+        <v>0.1436124779217507</v>
       </c>
       <c r="G71">
-        <v>0.1262697819155144</v>
+        <v>0.1266150358923953</v>
       </c>
       <c r="H71">
-        <v>0.2583620952127686</v>
+        <v>0.258876568546933</v>
       </c>
       <c r="I71">
-        <v>14166</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -2894,28 +2918,28 @@
         <v>86</v>
       </c>
       <c r="B72">
-        <v>0.007268678906681078</v>
+        <v>0.009075753729992564</v>
       </c>
       <c r="C72">
-        <v>0.006046426867297824</v>
+        <v>0.008687458498950898</v>
       </c>
       <c r="D72">
-        <v>0.0001164217038619287</v>
+        <v>0.0001756371360362956</v>
       </c>
       <c r="E72">
-        <v>9.355464689912527E-05</v>
+        <v>0.0001906209278749646</v>
       </c>
       <c r="F72">
-        <v>0.2283759127095218</v>
+        <v>0.1949495006477631</v>
       </c>
       <c r="G72">
-        <v>0.3799350410561445</v>
+        <v>0.1262697819155144</v>
       </c>
       <c r="H72">
-        <v>0.545155985157215</v>
+        <v>0.2583620952127686</v>
       </c>
       <c r="I72">
-        <v>132</v>
+        <v>14166</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -2923,27 +2947,56 @@
         <v>87</v>
       </c>
       <c r="B73">
+        <v>0.007268678906681078</v>
+      </c>
+      <c r="C73">
+        <v>0.006046426867297824</v>
+      </c>
+      <c r="D73">
+        <v>0.0001164217038619287</v>
+      </c>
+      <c r="E73">
+        <v>9.355464689912527E-05</v>
+      </c>
+      <c r="F73">
+        <v>0.2283759127095218</v>
+      </c>
+      <c r="G73">
+        <v>0.3799350410561445</v>
+      </c>
+      <c r="H73">
+        <v>0.545155985157215</v>
+      </c>
+      <c r="I73">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B74">
         <v>0.00762709903395546</v>
       </c>
-      <c r="C73">
+      <c r="C74">
         <v>0.008679017950585495</v>
       </c>
-      <c r="D73">
+      <c r="D74">
         <v>0.0001379308745364617</v>
       </c>
-      <c r="E73">
+      <c r="E74">
         <v>0.0001903704215854449</v>
       </c>
-      <c r="F73">
+      <c r="F74">
         <v>0.3671981660644249</v>
       </c>
-      <c r="G73">
+      <c r="G74">
         <v>0.1266150358923953</v>
       </c>
-      <c r="H73">
+      <c r="H74">
         <v>0.258876568546933</v>
       </c>
-      <c r="I73">
+      <c r="I74">
         <v>14156</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update lgbm qoq hyperspace
</commit_message>
<xml_diff>
--- a/results_analysis/compare_with_ibes/#compare_all.xlsx
+++ b/results_analysis/compare_with_ibes/#compare_all.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>lgbm_mae</t>
   </si>
@@ -40,27 +40,27 @@
     <t>len</t>
   </si>
   <si>
+    <t>consensus_mse_org</t>
+  </si>
+  <si>
+    <t>consensus_medae_org</t>
+  </si>
+  <si>
+    <t>consensus_mae_org</t>
+  </si>
+  <si>
+    <t>lgbm_mae_org</t>
+  </si>
+  <si>
     <t>lgbm_medae_org</t>
   </si>
   <si>
-    <t>consensus_mae_org</t>
-  </si>
-  <si>
-    <t>lgbm_mae_org</t>
-  </si>
-  <si>
     <t>lgbm_r2_org</t>
   </si>
   <si>
     <t>lgbm_mse_org</t>
   </si>
   <si>
-    <t>consensus_medae_org</t>
-  </si>
-  <si>
-    <t>consensus_mse_org</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>ibes_qoq_1|fwdepsqcut|q_1｜ibes_qoq_tune10</t>
+  </si>
+  <si>
+    <t>ibes_qoq_2|fwdepsqcut|q_2｜ibes_qoq_tune10_ind</t>
   </si>
   <si>
     <t>ibes_qoq_1|fwdepsqcut|q_1｜ibes_qoq</t>
@@ -506,7 +509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -591,25 +594,25 @@
         <v>14156</v>
       </c>
       <c r="J2">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="K2">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="L2">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="M2">
+        <v>0.01071193221870467</v>
+      </c>
+      <c r="N2">
         <v>0.005638666708596741</v>
       </c>
-      <c r="K2">
-        <v>0.009674189396799987</v>
-      </c>
-      <c r="L2">
-        <v>0.01071193221870467</v>
-      </c>
-      <c r="M2">
+      <c r="O2">
         <v>0.06836645151013176</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>0.0004250480609163007</v>
-      </c>
-      <c r="O2">
-        <v>0.004818030126325817</v>
-      </c>
-      <c r="P2">
-        <v>0.0003384092866814527</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -641,25 +644,25 @@
         <v>6771</v>
       </c>
       <c r="J3">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="K3">
+        <v>0.003193202088483064</v>
+      </c>
+      <c r="L3">
+        <v>0.005813234561065725</v>
+      </c>
+      <c r="M3">
+        <v>0.005632685300523813</v>
+      </c>
+      <c r="N3">
         <v>0.003171635367762127</v>
       </c>
-      <c r="K3">
-        <v>0.005813234561065725</v>
-      </c>
-      <c r="L3">
-        <v>0.005632685300523813</v>
-      </c>
-      <c r="M3">
+      <c r="O3">
         <v>0.3564407544954944</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>0.0001152638129503358</v>
-      </c>
-      <c r="O3">
-        <v>0.003193202088483064</v>
-      </c>
-      <c r="P3">
-        <v>0.0001037297229528328</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -691,25 +694,25 @@
         <v>42468</v>
       </c>
       <c r="J4">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="K4">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="L4">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="M4">
+        <v>0.009106885821888167</v>
+      </c>
+      <c r="N4">
         <v>0.004616722796530505</v>
       </c>
-      <c r="K4">
-        <v>0.009674189396799987</v>
-      </c>
-      <c r="L4">
-        <v>0.009106885821888167</v>
-      </c>
-      <c r="M4">
+      <c r="O4">
         <v>0.269966598412229</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>0.000333070102780211</v>
-      </c>
-      <c r="O4">
-        <v>0.004818030126325817</v>
-      </c>
-      <c r="P4">
-        <v>0.0003384092866814527</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -741,25 +744,25 @@
         <v>14156</v>
       </c>
       <c r="J5">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="K5">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="L5">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="M5">
+        <v>0.008950010380536522</v>
+      </c>
+      <c r="N5">
         <v>0.004615286290830784</v>
       </c>
-      <c r="K5">
-        <v>0.009674189396799985</v>
-      </c>
-      <c r="L5">
-        <v>0.008950010380536522</v>
-      </c>
-      <c r="M5">
+      <c r="O5">
         <v>0.2798459788092014</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>0.0003285627388197843</v>
-      </c>
-      <c r="O5">
-        <v>0.004818030126325817</v>
-      </c>
-      <c r="P5">
-        <v>0.0003384092866814527</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -791,25 +794,25 @@
         <v>14156</v>
       </c>
       <c r="J6">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="K6">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="L6">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="M6">
+        <v>0.00941140169945745</v>
+      </c>
+      <c r="N6">
         <v>0.004590555422836876</v>
       </c>
-      <c r="K6">
-        <v>0.009674189396799985</v>
-      </c>
-      <c r="L6">
-        <v>0.00941140169945745</v>
-      </c>
-      <c r="M6">
+      <c r="O6">
         <v>0.1860837943045432</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>0.0003713407546776094</v>
-      </c>
-      <c r="O6">
-        <v>0.004818030126325817</v>
-      </c>
-      <c r="P6">
-        <v>0.0003384092866814527</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -841,25 +844,25 @@
         <v>24768</v>
       </c>
       <c r="J7">
+        <v>0.0001796235360933539</v>
+      </c>
+      <c r="K7">
+        <v>0.003559726400188349</v>
+      </c>
+      <c r="L7">
+        <v>0.006875190708555331</v>
+      </c>
+      <c r="M7">
+        <v>0.008363098231375462</v>
+      </c>
+      <c r="N7">
         <v>0.004275415213561056</v>
       </c>
-      <c r="K7">
-        <v>0.006875190708555331</v>
-      </c>
-      <c r="L7">
-        <v>0.008363098231375462</v>
-      </c>
-      <c r="M7">
+      <c r="O7">
         <v>-0.00724317687482956</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>0.0002632414236722758</v>
-      </c>
-      <c r="O7">
-        <v>0.003559726400188349</v>
-      </c>
-      <c r="P7">
-        <v>0.0001796235360933539</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -891,25 +894,25 @@
         <v>14156</v>
       </c>
       <c r="J8">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="K8">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="L8">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="M8">
+        <v>0.009901025034115019</v>
+      </c>
+      <c r="N8">
         <v>0.005167135423672592</v>
       </c>
-      <c r="K8">
-        <v>0.009674189396799985</v>
-      </c>
-      <c r="L8">
-        <v>0.009901025034115019</v>
-      </c>
-      <c r="M8">
+      <c r="O8">
         <v>0.1565886089862186</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>0.0003847976244374441</v>
-      </c>
-      <c r="O8">
-        <v>0.004818030126325817</v>
-      </c>
-      <c r="P8">
-        <v>0.0003384092866814527</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -941,25 +944,25 @@
         <v>11611</v>
       </c>
       <c r="J9">
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="K9">
+        <v>0.001592932311570713</v>
+      </c>
+      <c r="L9">
+        <v>0.004580501696160511</v>
+      </c>
+      <c r="M9">
+        <v>0.005213165544267774</v>
+      </c>
+      <c r="N9">
         <v>0.00173711317318318</v>
       </c>
-      <c r="K9">
-        <v>0.004580501696160511</v>
-      </c>
-      <c r="L9">
-        <v>0.005213165544267774</v>
-      </c>
-      <c r="M9">
+      <c r="O9">
         <v>-0.01180186309853548</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>0.0002098592232396584</v>
-      </c>
-      <c r="O9">
-        <v>0.001592932311570713</v>
-      </c>
-      <c r="P9">
-        <v>0.0001631540263502446</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -991,25 +994,25 @@
         <v>49</v>
       </c>
       <c r="J10">
+        <v>0.0001158352549329261</v>
+      </c>
+      <c r="K10">
+        <v>0.00129198945232948</v>
+      </c>
+      <c r="L10">
+        <v>0.004529835290885987</v>
+      </c>
+      <c r="M10">
+        <v>0.007217175147339313</v>
+      </c>
+      <c r="N10">
         <v>0.002972419699024923</v>
       </c>
-      <c r="K10">
-        <v>0.004529835290885987</v>
-      </c>
-      <c r="L10">
-        <v>0.007217175147339313</v>
-      </c>
-      <c r="M10">
+      <c r="O10">
         <v>-0.01652918306199047</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>0.0003123469992588732</v>
-      </c>
-      <c r="O10">
-        <v>0.00129198945232948</v>
-      </c>
-      <c r="P10">
-        <v>0.0001158352549329261</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1041,25 +1044,25 @@
         <v>14156</v>
       </c>
       <c r="J11">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="K11">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="L11">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="M11">
+        <v>0.0102119158074488</v>
+      </c>
+      <c r="N11">
         <v>0.005239736253559311</v>
       </c>
-      <c r="K11">
-        <v>0.009674189396799987</v>
-      </c>
-      <c r="L11">
-        <v>0.0102119158074488</v>
-      </c>
-      <c r="M11">
+      <c r="O11">
         <v>0.1218694481841025</v>
       </c>
-      <c r="N11">
+      <c r="P11">
         <v>0.0004006378783650764</v>
-      </c>
-      <c r="O11">
-        <v>0.004818030126325817</v>
-      </c>
-      <c r="P11">
-        <v>0.0003384092866814527</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1091,25 +1094,25 @@
         <v>6771</v>
       </c>
       <c r="J12">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="K12">
+        <v>0.003193202088483064</v>
+      </c>
+      <c r="L12">
+        <v>0.005813234561065725</v>
+      </c>
+      <c r="M12">
+        <v>0.00595976388177965</v>
+      </c>
+      <c r="N12">
         <v>0.002972129451884979</v>
       </c>
-      <c r="K12">
-        <v>0.005813234561065725</v>
-      </c>
-      <c r="L12">
-        <v>0.00595976388177965</v>
-      </c>
-      <c r="M12">
+      <c r="O12">
         <v>0.2046421514566161</v>
       </c>
-      <c r="N12">
+      <c r="P12">
         <v>0.0001424514975481683</v>
-      </c>
-      <c r="O12">
-        <v>0.003193202088483064</v>
-      </c>
-      <c r="P12">
-        <v>0.0001037297229528328</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1141,25 +1144,25 @@
         <v>6771</v>
       </c>
       <c r="J13">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="K13">
+        <v>0.003193202088483064</v>
+      </c>
+      <c r="L13">
+        <v>0.005813234561065725</v>
+      </c>
+      <c r="M13">
+        <v>0.00592641693601841</v>
+      </c>
+      <c r="N13">
         <v>0.003005755874836842</v>
       </c>
-      <c r="K13">
-        <v>0.005813234561065725</v>
-      </c>
-      <c r="L13">
-        <v>0.00592641693601841</v>
-      </c>
-      <c r="M13">
+      <c r="O13">
         <v>0.2264121702660996</v>
       </c>
-      <c r="N13">
+      <c r="P13">
         <v>0.00013855240761432</v>
-      </c>
-      <c r="O13">
-        <v>0.003193202088483064</v>
-      </c>
-      <c r="P13">
-        <v>0.0001037297229528328</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1191,25 +1194,25 @@
         <v>14156</v>
       </c>
       <c r="J14">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="K14">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="L14">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="M14">
+        <v>0.008942022948316988</v>
+      </c>
+      <c r="N14">
         <v>0.004617426367895965</v>
       </c>
-      <c r="K14">
-        <v>0.009674189396799985</v>
-      </c>
-      <c r="L14">
-        <v>0.008942022948316988</v>
-      </c>
-      <c r="M14">
+      <c r="O14">
         <v>0.2810892232598902</v>
       </c>
-      <c r="N14">
+      <c r="P14">
         <v>0.0003279955215444224</v>
-      </c>
-      <c r="O14">
-        <v>0.004818030126325817</v>
-      </c>
-      <c r="P14">
-        <v>0.0003384092866814527</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1241,25 +1244,25 @@
         <v>11611</v>
       </c>
       <c r="J15">
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="K15">
+        <v>0.001592932311570713</v>
+      </c>
+      <c r="L15">
+        <v>0.004580501696160511</v>
+      </c>
+      <c r="M15">
+        <v>0.005089153979501482</v>
+      </c>
+      <c r="N15">
         <v>0.001554417436991534</v>
       </c>
-      <c r="K15">
-        <v>0.004580501696160511</v>
-      </c>
-      <c r="L15">
-        <v>0.005089153979501482</v>
-      </c>
-      <c r="M15">
+      <c r="O15">
         <v>-0.004454544482717981</v>
       </c>
-      <c r="N15">
+      <c r="P15">
         <v>0.0002083353057278959</v>
-      </c>
-      <c r="O15">
-        <v>0.001592932311570713</v>
-      </c>
-      <c r="P15">
-        <v>0.0001631540263502446</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1267,49 +1270,49 @@
         <v>30</v>
       </c>
       <c r="B16">
-        <v>0.00304699828992123</v>
+        <v>0.003103990424644728</v>
       </c>
       <c r="C16">
-        <v>0.002499571894821071</v>
+        <v>0.00254141838673398</v>
       </c>
       <c r="D16">
-        <v>1.903121423403654E-05</v>
+        <v>2.156002471405648E-05</v>
       </c>
       <c r="E16">
-        <v>1.967007435869721E-05</v>
+        <v>2.106152912726658E-05</v>
       </c>
       <c r="F16">
-        <v>-0.008580312939503454</v>
+        <v>-0.02262657763782516</v>
       </c>
       <c r="G16">
-        <v>-0.04243741404356438</v>
+        <v>0.001017868166272584</v>
       </c>
       <c r="H16">
-        <v>0.2133795918767654</v>
+        <v>0.212555477012045</v>
       </c>
       <c r="I16">
-        <v>11611</v>
+        <v>11542</v>
       </c>
       <c r="J16">
-        <v>0.001554596452837835</v>
+        <v>0.000163888349337522</v>
       </c>
       <c r="K16">
-        <v>0.004580501696160511</v>
+        <v>0.001597174444307401</v>
       </c>
       <c r="L16">
-        <v>0.005107549406927882</v>
+        <v>0.004589584286176587</v>
       </c>
       <c r="M16">
-        <v>-0.002771209789547591</v>
+        <v>0.00510134746390362</v>
       </c>
       <c r="N16">
-        <v>0.000207986162951978</v>
+        <v>0.001583264354559398</v>
       </c>
       <c r="O16">
-        <v>0.001592932311570713</v>
+        <v>-0.005012774390606101</v>
       </c>
       <c r="P16">
-        <v>0.0001631540263502446</v>
+        <v>0.0002091701444985722</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1317,49 +1320,49 @@
         <v>31</v>
       </c>
       <c r="B17">
-        <v>0.006549373422714545</v>
+        <v>0.00304699828992123</v>
       </c>
       <c r="C17">
-        <v>0.005670204101840715</v>
+        <v>0.002499571894821071</v>
       </c>
       <c r="D17">
-        <v>0.0001064697656049724</v>
+        <v>1.903121423403654E-05</v>
       </c>
       <c r="E17">
-        <v>9.344840654260834E-05</v>
+        <v>1.967007435869721E-05</v>
       </c>
       <c r="F17">
-        <v>0.1346849985258249</v>
+        <v>-0.008580312939503454</v>
       </c>
       <c r="G17">
-        <v>0.2405138906269937</v>
+        <v>-0.04243741404356438</v>
       </c>
       <c r="H17">
-        <v>0.4208397194991282</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I17">
-        <v>6771</v>
+        <v>11611</v>
       </c>
       <c r="J17">
-        <v>0.003715325925925931</v>
+        <v>0.0001631540263502446</v>
       </c>
       <c r="K17">
-        <v>0.005813234561065723</v>
+        <v>0.001592932311570713</v>
       </c>
       <c r="L17">
-        <v>0.006776662396495037</v>
+        <v>0.004580501696160511</v>
       </c>
       <c r="M17">
-        <v>0.1058242633905934</v>
+        <v>0.005107549406927882</v>
       </c>
       <c r="N17">
-        <v>0.000160150142460433</v>
+        <v>0.001554596452837835</v>
       </c>
       <c r="O17">
-        <v>0.003193202088483064</v>
+        <v>-0.002771209789547591</v>
       </c>
       <c r="P17">
-        <v>0.0001037297229528328</v>
+        <v>0.000207986162951978</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -1367,49 +1370,49 @@
         <v>32</v>
       </c>
       <c r="B18">
-        <v>0.002783525716284511</v>
+        <v>0.006549373422714545</v>
       </c>
       <c r="C18">
-        <v>0.002457544020376962</v>
+        <v>0.005670204101840715</v>
       </c>
       <c r="D18">
-        <v>1.713865210259099E-05</v>
+        <v>0.0001064697656049724</v>
       </c>
       <c r="E18">
-        <v>1.89022549270271E-05</v>
+        <v>9.344840654260834E-05</v>
       </c>
       <c r="F18">
-        <v>-0.05370835704473098</v>
+        <v>0.1346849985258249</v>
       </c>
       <c r="G18">
-        <v>-0.1621371309933592</v>
+        <v>0.2405138906269937</v>
       </c>
       <c r="H18">
-        <v>0.3649062991209757</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I18">
-        <v>4010</v>
+        <v>6771</v>
       </c>
       <c r="J18">
-        <v>0.001362431751651251</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="K18">
-        <v>0.004349183403839366</v>
+        <v>0.003193202088483064</v>
       </c>
       <c r="L18">
-        <v>0.004501420066184821</v>
+        <v>0.005813234561065723</v>
       </c>
       <c r="M18">
-        <v>-0.006214540120261569</v>
+        <v>0.006776662396495037</v>
       </c>
       <c r="N18">
-        <v>0.0002742305932959652</v>
+        <v>0.003715325925925931</v>
       </c>
       <c r="O18">
-        <v>0.001438312583710056</v>
+        <v>0.1058242633905934</v>
       </c>
       <c r="P18">
-        <v>0.0001730864695810989</v>
+        <v>0.000160150142460433</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -1417,49 +1420,49 @@
         <v>33</v>
       </c>
       <c r="B19">
-        <v>0.00929322862430519</v>
+        <v>0.002783525716284511</v>
       </c>
       <c r="C19">
-        <v>0.008733878054388279</v>
+        <v>0.002457544020376962</v>
       </c>
       <c r="D19">
-        <v>0.000192984991667648</v>
+        <v>1.713865210259099E-05</v>
       </c>
       <c r="E19">
-        <v>0.0001961492659581503</v>
+        <v>1.89022549270271E-05</v>
       </c>
       <c r="F19">
-        <v>0.1421155108066621</v>
+        <v>-0.05370835704473098</v>
       </c>
       <c r="G19">
-        <v>0.1280492261183164</v>
+        <v>-0.1621371309933592</v>
       </c>
       <c r="H19">
-        <v>0.2582640092197721</v>
+        <v>0.3649062991209757</v>
       </c>
       <c r="I19">
-        <v>14156</v>
+        <v>4010</v>
       </c>
       <c r="J19">
-        <v>0.005409147625572685</v>
+        <v>0.0001730864695810989</v>
       </c>
       <c r="K19">
-        <v>0.009674189396799987</v>
+        <v>0.001438312583710056</v>
       </c>
       <c r="L19">
-        <v>0.01035431191953904</v>
+        <v>0.004349183403839366</v>
       </c>
       <c r="M19">
-        <v>0.1230344532976788</v>
+        <v>0.004501420066184821</v>
       </c>
       <c r="N19">
-        <v>0.0004001063569688302</v>
+        <v>0.001362431751651251</v>
       </c>
       <c r="O19">
-        <v>0.004818030126325817</v>
+        <v>-0.006214540120261569</v>
       </c>
       <c r="P19">
-        <v>0.0003384092866814527</v>
+        <v>0.0002742305932959652</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1467,49 +1470,49 @@
         <v>34</v>
       </c>
       <c r="B20">
-        <v>0.003030458698074221</v>
+        <v>0.00929322862430519</v>
       </c>
       <c r="C20">
-        <v>0.002499571894821071</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D20">
-        <v>1.91281128971015E-05</v>
+        <v>0.000192984991667648</v>
       </c>
       <c r="E20">
-        <v>1.967007435869721E-05</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F20">
-        <v>-0.01371556509502225</v>
+        <v>0.1421155108066621</v>
       </c>
       <c r="G20">
-        <v>-0.04243741404356438</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H20">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I20">
-        <v>11611</v>
+        <v>14156</v>
       </c>
       <c r="J20">
-        <v>0.001547174514616301</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="K20">
-        <v>0.004580501696160511</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="L20">
-        <v>0.005089488294347637</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="M20">
-        <v>-0.00353431378743374</v>
+        <v>0.01035431191953904</v>
       </c>
       <c r="N20">
-        <v>0.0002081444394071696</v>
+        <v>0.005409147625572685</v>
       </c>
       <c r="O20">
-        <v>0.001592932311570713</v>
+        <v>0.1230344532976788</v>
       </c>
       <c r="P20">
-        <v>0.0001631540263502446</v>
+        <v>0.0004001063569688302</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1517,49 +1520,49 @@
         <v>35</v>
       </c>
       <c r="B21">
-        <v>0.008532806478705164</v>
+        <v>0.003030458698074221</v>
       </c>
       <c r="C21">
-        <v>0.008733878054388279</v>
+        <v>0.002499571894821071</v>
       </c>
       <c r="D21">
-        <v>0.0001656454412935777</v>
+        <v>1.91281128971015E-05</v>
       </c>
       <c r="E21">
-        <v>0.0001961492659581503</v>
+        <v>1.967007435869721E-05</v>
       </c>
       <c r="F21">
-        <v>0.2636491907304709</v>
+        <v>-0.01371556509502225</v>
       </c>
       <c r="G21">
-        <v>0.1280492261183164</v>
+        <v>-0.04243741404356438</v>
       </c>
       <c r="H21">
-        <v>0.2582640092197721</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I21">
-        <v>14156</v>
+        <v>11611</v>
       </c>
       <c r="J21">
-        <v>0.004730871750625608</v>
+        <v>0.0001631540263502446</v>
       </c>
       <c r="K21">
-        <v>0.009674189396799987</v>
+        <v>0.001592932311570713</v>
       </c>
       <c r="L21">
-        <v>0.009554445336689437</v>
+        <v>0.004580501696160511</v>
       </c>
       <c r="M21">
-        <v>0.179378395374721</v>
+        <v>0.005089488294347637</v>
       </c>
       <c r="N21">
-        <v>0.0003744000227958637</v>
+        <v>0.001547174514616301</v>
       </c>
       <c r="O21">
-        <v>0.004818030126325817</v>
+        <v>-0.00353431378743374</v>
       </c>
       <c r="P21">
-        <v>0.0003384092866814527</v>
+        <v>0.0002081444394071696</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1567,19 +1570,19 @@
         <v>36</v>
       </c>
       <c r="B22">
-        <v>0.008529233938818522</v>
+        <v>0.008532806478705164</v>
       </c>
       <c r="C22">
         <v>0.008733878054388279</v>
       </c>
       <c r="D22">
-        <v>0.0001653251466070655</v>
+        <v>0.0001656454412935777</v>
       </c>
       <c r="E22">
         <v>0.0001961492659581503</v>
       </c>
       <c r="F22">
-        <v>0.2650730104853413</v>
+        <v>0.2636491907304709</v>
       </c>
       <c r="G22">
         <v>0.1280492261183164</v>
@@ -1591,25 +1594,25 @@
         <v>14156</v>
       </c>
       <c r="J22">
-        <v>0.004764640177213803</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="K22">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="L22">
         <v>0.009674189396799987</v>
       </c>
-      <c r="L22">
-        <v>0.009555217528480035</v>
-      </c>
       <c r="M22">
-        <v>0.1788608663781261</v>
+        <v>0.009554445336689437</v>
       </c>
       <c r="N22">
-        <v>0.0003746361399868205</v>
+        <v>0.004730871750625608</v>
       </c>
       <c r="O22">
-        <v>0.004818030126325817</v>
+        <v>0.179378395374721</v>
       </c>
       <c r="P22">
-        <v>0.0003384092866814527</v>
+        <v>0.0003744000227958637</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1617,19 +1620,19 @@
         <v>37</v>
       </c>
       <c r="B23">
-        <v>0.008505250051591662</v>
+        <v>0.008529233938818522</v>
       </c>
       <c r="C23">
         <v>0.008733878054388279</v>
       </c>
       <c r="D23">
-        <v>0.0001646168902522808</v>
+        <v>0.0001653251466070655</v>
       </c>
       <c r="E23">
         <v>0.0001961492659581503</v>
       </c>
       <c r="F23">
-        <v>0.268221452941368</v>
+        <v>0.2650730104853413</v>
       </c>
       <c r="G23">
         <v>0.1280492261183164</v>
@@ -1641,25 +1644,25 @@
         <v>14156</v>
       </c>
       <c r="J23">
-        <v>0.004756476812602748</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="K23">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="L23">
         <v>0.009674189396799987</v>
       </c>
-      <c r="L23">
-        <v>0.009526287265811475</v>
-      </c>
       <c r="M23">
-        <v>0.1810824657398455</v>
+        <v>0.009555217528480035</v>
       </c>
       <c r="N23">
-        <v>0.0003736225585176234</v>
+        <v>0.004764640177213803</v>
       </c>
       <c r="O23">
-        <v>0.004818030126325817</v>
+        <v>0.1788608663781261</v>
       </c>
       <c r="P23">
-        <v>0.0003384092866814527</v>
+        <v>0.0003746361399868205</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -1667,49 +1670,49 @@
         <v>38</v>
       </c>
       <c r="B24">
-        <v>0.006299187529923155</v>
+        <v>0.008505250051591662</v>
       </c>
       <c r="C24">
-        <v>0.00553167406053466</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D24">
-        <v>9.00395869891457E-05</v>
+        <v>0.0001646168902522808</v>
       </c>
       <c r="E24">
-        <v>8.170381435551846E-05</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F24">
-        <v>0.1391419988807219</v>
+        <v>0.268221452941368</v>
       </c>
       <c r="G24">
-        <v>0.2188393498696173</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H24">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I24">
-        <v>6771</v>
+        <v>14156</v>
       </c>
       <c r="J24">
-        <v>0.003667719421830667</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="K24">
-        <v>0.005813234561065723</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="L24">
-        <v>0.00674135934653288</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="M24">
-        <v>0.1045681259196538</v>
+        <v>0.009526287265811475</v>
       </c>
       <c r="N24">
-        <v>0.0001603751212724098</v>
+        <v>0.004756476812602748</v>
       </c>
       <c r="O24">
-        <v>0.003193202088483064</v>
+        <v>0.1810824657398455</v>
       </c>
       <c r="P24">
-        <v>0.0001037297229528328</v>
+        <v>0.0003736225585176234</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -1717,49 +1720,49 @@
         <v>39</v>
       </c>
       <c r="B25">
-        <v>0.00869522801124366</v>
+        <v>0.006299187529923155</v>
       </c>
       <c r="C25">
-        <v>0.008722720041403264</v>
+        <v>0.00553167406053466</v>
       </c>
       <c r="D25">
-        <v>0.0001671499749450426</v>
+        <v>9.00395869891457E-05</v>
       </c>
       <c r="E25">
-        <v>0.0001985649052123504</v>
+        <v>8.170381435551846E-05</v>
       </c>
       <c r="F25">
-        <v>0.2822259777859754</v>
+        <v>0.1391419988807219</v>
       </c>
       <c r="G25">
-        <v>0.147324247391146</v>
+        <v>0.2188393498696173</v>
       </c>
       <c r="H25">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I25">
-        <v>14156</v>
+        <v>6771</v>
       </c>
       <c r="J25">
-        <v>0.005173194757001598</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="K25">
-        <v>0.009674189396799985</v>
+        <v>0.003193202088483064</v>
       </c>
       <c r="L25">
-        <v>0.009719161233546112</v>
+        <v>0.005813234561065723</v>
       </c>
       <c r="M25">
-        <v>0.2030564380000814</v>
+        <v>0.00674135934653288</v>
       </c>
       <c r="N25">
-        <v>0.0003635971635380399</v>
+        <v>0.003667719421830667</v>
       </c>
       <c r="O25">
-        <v>0.004818030126325817</v>
+        <v>0.1045681259196538</v>
       </c>
       <c r="P25">
-        <v>0.0003384092866814527</v>
+        <v>0.0001603751212724098</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -1767,19 +1770,19 @@
         <v>40</v>
       </c>
       <c r="B26">
-        <v>0.007668256776450208</v>
+        <v>0.00869522801124366</v>
       </c>
       <c r="C26">
         <v>0.008722720041403264</v>
       </c>
       <c r="D26">
-        <v>0.0001436777206558706</v>
+        <v>0.0001671499749450426</v>
       </c>
       <c r="E26">
         <v>0.0001985649052123504</v>
       </c>
       <c r="F26">
-        <v>0.3830203355303232</v>
+        <v>0.2822259777859754</v>
       </c>
       <c r="G26">
         <v>0.147324247391146</v>
@@ -1791,25 +1794,25 @@
         <v>14156</v>
       </c>
       <c r="J26">
-        <v>0.004128330862335852</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="K26">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="L26">
         <v>0.009674189396799985</v>
       </c>
-      <c r="L26">
-        <v>0.00867861064019221</v>
-      </c>
       <c r="M26">
-        <v>0.2669184291403396</v>
+        <v>0.009719161233546112</v>
       </c>
       <c r="N26">
-        <v>0.0003344607981243851</v>
+        <v>0.005173194757001598</v>
       </c>
       <c r="O26">
-        <v>0.004818030126325817</v>
+        <v>0.2030564380000814</v>
       </c>
       <c r="P26">
-        <v>0.0003384092866814527</v>
+        <v>0.0003635971635380399</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -1817,19 +1820,19 @@
         <v>41</v>
       </c>
       <c r="B27">
-        <v>0.00958912348219286</v>
+        <v>0.007668256776450208</v>
       </c>
       <c r="C27">
         <v>0.008722720041403264</v>
       </c>
       <c r="D27">
-        <v>0.00021842684931279</v>
+        <v>0.0001436777206558706</v>
       </c>
       <c r="E27">
         <v>0.0001985649052123504</v>
       </c>
       <c r="F27">
-        <v>0.06203325341612431</v>
+        <v>0.3830203355303232</v>
       </c>
       <c r="G27">
         <v>0.147324247391146</v>
@@ -1841,25 +1844,25 @@
         <v>14156</v>
       </c>
       <c r="J27">
-        <v>0.005560650653515711</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="K27">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="L27">
         <v>0.009674189396799985</v>
       </c>
-      <c r="L27">
-        <v>0.01064772150300563</v>
-      </c>
       <c r="M27">
-        <v>0.05448840836791147</v>
+        <v>0.00867861064019221</v>
       </c>
       <c r="N27">
-        <v>0.0004313797729252501</v>
+        <v>0.004128330862335852</v>
       </c>
       <c r="O27">
-        <v>0.004818030126325817</v>
+        <v>0.2669184291403396</v>
       </c>
       <c r="P27">
-        <v>0.0003384092866814527</v>
+        <v>0.0003344607981243851</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -1867,49 +1870,49 @@
         <v>42</v>
       </c>
       <c r="B28">
-        <v>0.005743153097997238</v>
+        <v>0.00958912348219286</v>
       </c>
       <c r="C28">
-        <v>0.005699109365498782</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D28">
-        <v>9.179016309205035E-05</v>
+        <v>0.00021842684931279</v>
       </c>
       <c r="E28">
-        <v>9.470932808225897E-05</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F28">
-        <v>0.2786526717712858</v>
+        <v>0.06203325341612431</v>
       </c>
       <c r="G28">
-        <v>0.2557119579146814</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H28">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I28">
-        <v>6771</v>
+        <v>14156</v>
       </c>
       <c r="J28">
-        <v>0.002972129451884979</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="K28">
-        <v>0.005813234561065725</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="L28">
-        <v>0.00595976388177965</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="M28">
-        <v>0.2046421514566161</v>
+        <v>0.01064772150300563</v>
       </c>
       <c r="N28">
-        <v>0.0001424514975481683</v>
+        <v>0.005560650653515711</v>
       </c>
       <c r="O28">
-        <v>0.003193202088483064</v>
+        <v>0.05448840836791147</v>
       </c>
       <c r="P28">
-        <v>0.0001037297229528328</v>
+        <v>0.0004313797729252501</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -1917,49 +1920,49 @@
         <v>43</v>
       </c>
       <c r="B29">
-        <v>0.009301347310769852</v>
+        <v>0.005743153097997238</v>
       </c>
       <c r="C29">
-        <v>0.008733878054388279</v>
+        <v>0.005699109365498782</v>
       </c>
       <c r="D29">
-        <v>0.0001883109214593075</v>
+        <v>9.179016309205035E-05</v>
       </c>
       <c r="E29">
-        <v>0.0001961492659581503</v>
+        <v>9.470932808225897E-05</v>
       </c>
       <c r="F29">
-        <v>0.1628933562675233</v>
+        <v>0.2786526717712858</v>
       </c>
       <c r="G29">
-        <v>0.1280492261183164</v>
+        <v>0.2557119579146814</v>
       </c>
       <c r="H29">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I29">
-        <v>14156</v>
+        <v>6771</v>
       </c>
       <c r="J29">
-        <v>0.005399385735558927</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="K29">
-        <v>0.009674189396799987</v>
+        <v>0.003193202088483064</v>
       </c>
       <c r="L29">
-        <v>0.01035467890006862</v>
+        <v>0.005813234561065725</v>
       </c>
       <c r="M29">
-        <v>0.1175458874123242</v>
+        <v>0.00595976388177965</v>
       </c>
       <c r="N29">
-        <v>0.0004026104577395279</v>
+        <v>0.002972129451884979</v>
       </c>
       <c r="O29">
-        <v>0.004818030126325817</v>
+        <v>0.2046421514566161</v>
       </c>
       <c r="P29">
-        <v>0.0003384092866814527</v>
+        <v>0.0001424514975481683</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -1967,49 +1970,99 @@
         <v>44</v>
       </c>
       <c r="B30">
+        <v>0.009301347310769852</v>
+      </c>
+      <c r="C30">
+        <v>0.008733878054388279</v>
+      </c>
+      <c r="D30">
+        <v>0.0001883109214593075</v>
+      </c>
+      <c r="E30">
+        <v>0.0001961492659581503</v>
+      </c>
+      <c r="F30">
+        <v>0.1628933562675233</v>
+      </c>
+      <c r="G30">
+        <v>0.1280492261183164</v>
+      </c>
+      <c r="H30">
+        <v>0.2582640092197721</v>
+      </c>
+      <c r="I30">
+        <v>14156</v>
+      </c>
+      <c r="J30">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="K30">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="L30">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="M30">
+        <v>0.01035467890006862</v>
+      </c>
+      <c r="N30">
+        <v>0.005399385735558927</v>
+      </c>
+      <c r="O30">
+        <v>0.1175458874123242</v>
+      </c>
+      <c r="P30">
+        <v>0.0004026104577395279</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31">
         <v>0.00303210497017975</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <v>0.002499571894821071</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <v>1.909735738640315E-05</v>
       </c>
-      <c r="E30">
+      <c r="E31">
         <v>1.967007435869721E-05</v>
       </c>
-      <c r="F30">
+      <c r="F31">
         <v>-0.0120856426831728</v>
       </c>
-      <c r="G30">
+      <c r="G31">
         <v>-0.04243741404356438</v>
       </c>
-      <c r="H30">
+      <c r="H31">
         <v>0.2133795918767654</v>
       </c>
-      <c r="I30">
+      <c r="I31">
         <v>11611</v>
       </c>
-      <c r="J30">
+      <c r="J31">
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="K31">
+        <v>0.001592932311570713</v>
+      </c>
+      <c r="L31">
+        <v>0.004580501696160511</v>
+      </c>
+      <c r="M31">
+        <v>0.005090949099942899</v>
+      </c>
+      <c r="N31">
         <v>0.001550051802718652</v>
       </c>
-      <c r="K30">
-        <v>0.004580501696160511</v>
-      </c>
-      <c r="L30">
-        <v>0.005090949099942899</v>
-      </c>
-      <c r="M30">
+      <c r="O31">
         <v>-0.002911711704464803</v>
       </c>
-      <c r="N30">
+      <c r="P31">
         <v>0.0002080153046483946</v>
-      </c>
-      <c r="O30">
-        <v>0.001592932311570713</v>
-      </c>
-      <c r="P30">
-        <v>0.0001631540263502446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. rename preprocess .py 2. update load_data_lgbm.py for ibes_qoq x
</commit_message>
<xml_diff>
--- a/results_analysis/compare_with_ibes/#compare_all.xlsx
+++ b/results_analysis/compare_with_ibes/#compare_all.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>lgbm_mae</t>
   </si>
@@ -40,27 +40,27 @@
     <t>len</t>
   </si>
   <si>
+    <t>lgbm_mae_org</t>
+  </si>
+  <si>
+    <t>lgbm_medae_org</t>
+  </si>
+  <si>
     <t>consensus_mse_org</t>
   </si>
   <si>
+    <t>consensus_mae_org</t>
+  </si>
+  <si>
+    <t>consensus_medae_org</t>
+  </si>
+  <si>
+    <t>lgbm_mse_org</t>
+  </si>
+  <si>
     <t>lgbm_r2_org</t>
   </si>
   <si>
-    <t>consensus_medae_org</t>
-  </si>
-  <si>
-    <t>consensus_mae_org</t>
-  </si>
-  <si>
-    <t>lgbm_mse_org</t>
-  </si>
-  <si>
-    <t>lgbm_mae_org</t>
-  </si>
-  <si>
-    <t>lgbm_medae_org</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>ibes_qoq_1|fwdepsqcut|q_1｜ibes_qoq_tune10</t>
+  </si>
+  <si>
+    <t>ibes_2|ni_depthwise|xgb ind4 -sample_type industry -x_type ni</t>
   </si>
   <si>
     <t>ibes_qoq_2|fwdepsqcut|q_2｜ibes_qoq_tune10_ind</t>
@@ -515,7 +518,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -600,25 +603,25 @@
         <v>14156</v>
       </c>
       <c r="J2">
+        <v>0.01071193221870467</v>
+      </c>
+      <c r="K2">
+        <v>0.005638666708596741</v>
+      </c>
+      <c r="L2">
         <v>0.0003384092866814527</v>
-      </c>
-      <c r="K2">
-        <v>0.06836645151013176</v>
-      </c>
-      <c r="L2">
-        <v>0.004818030126325817</v>
       </c>
       <c r="M2">
         <v>0.009674189396799987</v>
       </c>
       <c r="N2">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="O2">
         <v>0.0004250480609163007</v>
       </c>
-      <c r="O2">
-        <v>0.01071193221870467</v>
-      </c>
       <c r="P2">
-        <v>0.005638666708596741</v>
+        <v>0.06836645151013176</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -650,25 +653,25 @@
         <v>6771</v>
       </c>
       <c r="J3">
+        <v>0.005632685300523813</v>
+      </c>
+      <c r="K3">
+        <v>0.003171635367762127</v>
+      </c>
+      <c r="L3">
         <v>0.0001037297229528328</v>
-      </c>
-      <c r="K3">
-        <v>0.3564407544954944</v>
-      </c>
-      <c r="L3">
-        <v>0.003193202088483064</v>
       </c>
       <c r="M3">
         <v>0.005813234561065725</v>
       </c>
       <c r="N3">
+        <v>0.003193202088483064</v>
+      </c>
+      <c r="O3">
         <v>0.0001152638129503358</v>
       </c>
-      <c r="O3">
-        <v>0.005632685300523813</v>
-      </c>
       <c r="P3">
-        <v>0.003171635367762127</v>
+        <v>0.3564407544954944</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -700,25 +703,25 @@
         <v>42468</v>
       </c>
       <c r="J4">
+        <v>0.009106885821888167</v>
+      </c>
+      <c r="K4">
+        <v>0.004616722796530505</v>
+      </c>
+      <c r="L4">
         <v>0.0003384092866814527</v>
-      </c>
-      <c r="K4">
-        <v>0.269966598412229</v>
-      </c>
-      <c r="L4">
-        <v>0.004818030126325817</v>
       </c>
       <c r="M4">
         <v>0.009674189396799987</v>
       </c>
       <c r="N4">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="O4">
         <v>0.000333070102780211</v>
       </c>
-      <c r="O4">
-        <v>0.009106885821888167</v>
-      </c>
       <c r="P4">
-        <v>0.004616722796530505</v>
+        <v>0.269966598412229</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -750,25 +753,25 @@
         <v>14156</v>
       </c>
       <c r="J5">
+        <v>0.008950010380536522</v>
+      </c>
+      <c r="K5">
+        <v>0.004615286290830784</v>
+      </c>
+      <c r="L5">
         <v>0.0003384092866814527</v>
-      </c>
-      <c r="K5">
-        <v>0.2798459788092014</v>
-      </c>
-      <c r="L5">
-        <v>0.004818030126325817</v>
       </c>
       <c r="M5">
         <v>0.009674189396799985</v>
       </c>
       <c r="N5">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="O5">
         <v>0.0003285627388197843</v>
       </c>
-      <c r="O5">
-        <v>0.008950010380536522</v>
-      </c>
       <c r="P5">
-        <v>0.004615286290830784</v>
+        <v>0.2798459788092014</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -800,25 +803,25 @@
         <v>14156</v>
       </c>
       <c r="J6">
+        <v>0.00941140169945745</v>
+      </c>
+      <c r="K6">
+        <v>0.004590555422836876</v>
+      </c>
+      <c r="L6">
         <v>0.0003384092866814527</v>
-      </c>
-      <c r="K6">
-        <v>0.1860837943045432</v>
-      </c>
-      <c r="L6">
-        <v>0.004818030126325817</v>
       </c>
       <c r="M6">
         <v>0.009674189396799985</v>
       </c>
       <c r="N6">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="O6">
         <v>0.0003713407546776094</v>
       </c>
-      <c r="O6">
-        <v>0.00941140169945745</v>
-      </c>
       <c r="P6">
-        <v>0.004590555422836876</v>
+        <v>0.1860837943045432</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -850,25 +853,25 @@
         <v>24768</v>
       </c>
       <c r="J7">
+        <v>0.008363098231375462</v>
+      </c>
+      <c r="K7">
+        <v>0.004275415213561056</v>
+      </c>
+      <c r="L7">
         <v>0.0001796235360933539</v>
-      </c>
-      <c r="K7">
-        <v>-0.00724317687482956</v>
-      </c>
-      <c r="L7">
-        <v>0.003559726400188349</v>
       </c>
       <c r="M7">
         <v>0.006875190708555331</v>
       </c>
       <c r="N7">
+        <v>0.003559726400188349</v>
+      </c>
+      <c r="O7">
         <v>0.0002632414236722758</v>
       </c>
-      <c r="O7">
-        <v>0.008363098231375462</v>
-      </c>
       <c r="P7">
-        <v>0.004275415213561056</v>
+        <v>-0.00724317687482956</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -900,25 +903,25 @@
         <v>14156</v>
       </c>
       <c r="J8">
+        <v>0.009901025034115019</v>
+      </c>
+      <c r="K8">
+        <v>0.005167135423672592</v>
+      </c>
+      <c r="L8">
         <v>0.0003384092866814527</v>
-      </c>
-      <c r="K8">
-        <v>0.1565886089862186</v>
-      </c>
-      <c r="L8">
-        <v>0.004818030126325817</v>
       </c>
       <c r="M8">
         <v>0.009674189396799985</v>
       </c>
       <c r="N8">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="O8">
         <v>0.0003847976244374441</v>
       </c>
-      <c r="O8">
-        <v>0.009901025034115019</v>
-      </c>
       <c r="P8">
-        <v>0.005167135423672592</v>
+        <v>0.1565886089862186</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -950,25 +953,25 @@
         <v>11542</v>
       </c>
       <c r="J9">
+        <v>0.00512210974064752</v>
+      </c>
+      <c r="K9">
+        <v>0.001602037466360856</v>
+      </c>
+      <c r="L9">
         <v>0.000163888349337522</v>
-      </c>
-      <c r="K9">
-        <v>-0.005102592401121431</v>
-      </c>
-      <c r="L9">
-        <v>0.001597174444307401</v>
       </c>
       <c r="M9">
         <v>0.004589584286176587</v>
       </c>
       <c r="N9">
+        <v>0.001597174444307401</v>
+      </c>
+      <c r="O9">
         <v>0.000209188838038313</v>
       </c>
-      <c r="O9">
-        <v>0.00512210974064752</v>
-      </c>
       <c r="P9">
-        <v>0.001602037466360856</v>
+        <v>-0.005102592401121431</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1000,25 +1003,25 @@
         <v>11611</v>
       </c>
       <c r="J10">
+        <v>0.005213165544267774</v>
+      </c>
+      <c r="K10">
+        <v>0.00173711317318318</v>
+      </c>
+      <c r="L10">
         <v>0.0001631540263502446</v>
-      </c>
-      <c r="K10">
-        <v>-0.01180186309853548</v>
-      </c>
-      <c r="L10">
-        <v>0.001592932311570713</v>
       </c>
       <c r="M10">
         <v>0.004580501696160511</v>
       </c>
       <c r="N10">
+        <v>0.001592932311570713</v>
+      </c>
+      <c r="O10">
         <v>0.0002098592232396584</v>
       </c>
-      <c r="O10">
-        <v>0.005213165544267774</v>
-      </c>
       <c r="P10">
-        <v>0.00173711317318318</v>
+        <v>-0.01180186309853548</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1050,25 +1053,25 @@
         <v>49</v>
       </c>
       <c r="J11">
+        <v>0.007217175147339313</v>
+      </c>
+      <c r="K11">
+        <v>0.002972419699024923</v>
+      </c>
+      <c r="L11">
         <v>0.0001158352549329261</v>
-      </c>
-      <c r="K11">
-        <v>-0.01652918306199047</v>
-      </c>
-      <c r="L11">
-        <v>0.00129198945232948</v>
       </c>
       <c r="M11">
         <v>0.004529835290885987</v>
       </c>
       <c r="N11">
+        <v>0.00129198945232948</v>
+      </c>
+      <c r="O11">
         <v>0.0003123469992588732</v>
       </c>
-      <c r="O11">
-        <v>0.007217175147339313</v>
-      </c>
       <c r="P11">
-        <v>0.002972419699024923</v>
+        <v>-0.01652918306199047</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1100,25 +1103,25 @@
         <v>14156</v>
       </c>
       <c r="J12">
+        <v>0.0102119158074488</v>
+      </c>
+      <c r="K12">
+        <v>0.005239736253559311</v>
+      </c>
+      <c r="L12">
         <v>0.0003384092866814527</v>
-      </c>
-      <c r="K12">
-        <v>0.1218694481841025</v>
-      </c>
-      <c r="L12">
-        <v>0.004818030126325817</v>
       </c>
       <c r="M12">
         <v>0.009674189396799987</v>
       </c>
       <c r="N12">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="O12">
         <v>0.0004006378783650764</v>
       </c>
-      <c r="O12">
-        <v>0.0102119158074488</v>
-      </c>
       <c r="P12">
-        <v>0.005239736253559311</v>
+        <v>0.1218694481841025</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1150,25 +1153,25 @@
         <v>6771</v>
       </c>
       <c r="J13">
+        <v>0.00595976388177965</v>
+      </c>
+      <c r="K13">
+        <v>0.002972129451884979</v>
+      </c>
+      <c r="L13">
         <v>0.0001037297229528328</v>
-      </c>
-      <c r="K13">
-        <v>0.2046421514566161</v>
-      </c>
-      <c r="L13">
-        <v>0.003193202088483064</v>
       </c>
       <c r="M13">
         <v>0.005813234561065725</v>
       </c>
       <c r="N13">
+        <v>0.003193202088483064</v>
+      </c>
+      <c r="O13">
         <v>0.0001424514975481683</v>
       </c>
-      <c r="O13">
-        <v>0.00595976388177965</v>
-      </c>
       <c r="P13">
-        <v>0.002972129451884979</v>
+        <v>0.2046421514566161</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1200,25 +1203,25 @@
         <v>6771</v>
       </c>
       <c r="J14">
+        <v>0.00592641693601841</v>
+      </c>
+      <c r="K14">
+        <v>0.003005755874836842</v>
+      </c>
+      <c r="L14">
         <v>0.0001037297229528328</v>
-      </c>
-      <c r="K14">
-        <v>0.2264121702660996</v>
-      </c>
-      <c r="L14">
-        <v>0.003193202088483064</v>
       </c>
       <c r="M14">
         <v>0.005813234561065725</v>
       </c>
       <c r="N14">
+        <v>0.003193202088483064</v>
+      </c>
+      <c r="O14">
         <v>0.00013855240761432</v>
       </c>
-      <c r="O14">
-        <v>0.00592641693601841</v>
-      </c>
       <c r="P14">
-        <v>0.003005755874836842</v>
+        <v>0.2264121702660996</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1250,25 +1253,25 @@
         <v>14156</v>
       </c>
       <c r="J15">
+        <v>0.008942022948316988</v>
+      </c>
+      <c r="K15">
+        <v>0.004617426367895965</v>
+      </c>
+      <c r="L15">
         <v>0.0003384092866814527</v>
-      </c>
-      <c r="K15">
-        <v>0.2810892232598902</v>
-      </c>
-      <c r="L15">
-        <v>0.004818030126325817</v>
       </c>
       <c r="M15">
         <v>0.009674189396799985</v>
       </c>
       <c r="N15">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="O15">
         <v>0.0003279955215444224</v>
       </c>
-      <c r="O15">
-        <v>0.008942022948316988</v>
-      </c>
       <c r="P15">
-        <v>0.004617426367895965</v>
+        <v>0.2810892232598902</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1300,25 +1303,25 @@
         <v>11611</v>
       </c>
       <c r="J16">
+        <v>0.005089153979501482</v>
+      </c>
+      <c r="K16">
+        <v>0.001554417436991534</v>
+      </c>
+      <c r="L16">
         <v>0.0001631540263502446</v>
-      </c>
-      <c r="K16">
-        <v>-0.004454544482717981</v>
-      </c>
-      <c r="L16">
-        <v>0.001592932311570713</v>
       </c>
       <c r="M16">
         <v>0.004580501696160511</v>
       </c>
       <c r="N16">
+        <v>0.001592932311570713</v>
+      </c>
+      <c r="O16">
         <v>0.0002083353057278959</v>
       </c>
-      <c r="O16">
-        <v>0.005089153979501482</v>
-      </c>
       <c r="P16">
-        <v>0.001554417436991534</v>
+        <v>-0.004454544482717981</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1326,49 +1329,49 @@
         <v>31</v>
       </c>
       <c r="B17">
-        <v>0.003103990424644728</v>
+        <v>0.007781992577683896</v>
       </c>
       <c r="C17">
-        <v>0.00254141838673398</v>
+        <v>0.00859065864792076</v>
       </c>
       <c r="D17">
-        <v>2.156002471405648E-05</v>
+        <v>0.0001409300345186765</v>
       </c>
       <c r="E17">
-        <v>2.106152912726658E-05</v>
+        <v>0.0001927871917829494</v>
       </c>
       <c r="F17">
-        <v>-0.02262657763782516</v>
+        <v>0.3590392616833861</v>
       </c>
       <c r="G17">
-        <v>0.001017868166272584</v>
+        <v>0.1231888844332176</v>
       </c>
       <c r="H17">
-        <v>0.212555477012045</v>
+        <v>0.1607683912702015</v>
       </c>
       <c r="I17">
-        <v>11542</v>
+        <v>12165</v>
       </c>
       <c r="J17">
-        <v>0.000163888349337522</v>
+        <v>0.008612572238732815</v>
       </c>
       <c r="K17">
-        <v>-0.005012774390606101</v>
+        <v>0.004522763064395587</v>
       </c>
       <c r="L17">
-        <v>0.001597174444307401</v>
+        <v>0.0002898025533356035</v>
       </c>
       <c r="M17">
-        <v>0.004589584286176587</v>
+        <v>0.009443827890009157</v>
       </c>
       <c r="N17">
-        <v>0.0002091701444985722</v>
+        <v>0.004755169990739034</v>
       </c>
       <c r="O17">
-        <v>0.00510134746390362</v>
+        <v>0.000242169264872158</v>
       </c>
       <c r="P17">
-        <v>0.001583264354559398</v>
+        <v>0.2987083812604719</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -1376,49 +1379,49 @@
         <v>32</v>
       </c>
       <c r="B18">
-        <v>0.00304699828992123</v>
+        <v>0.003103990424644728</v>
       </c>
       <c r="C18">
-        <v>0.002499571894821071</v>
+        <v>0.00254141838673398</v>
       </c>
       <c r="D18">
-        <v>1.903121423403654E-05</v>
+        <v>2.156002471405648E-05</v>
       </c>
       <c r="E18">
-        <v>1.967007435869721E-05</v>
+        <v>2.106152912726658E-05</v>
       </c>
       <c r="F18">
-        <v>-0.008580312939503454</v>
+        <v>-0.02262657763782516</v>
       </c>
       <c r="G18">
-        <v>-0.04243741404356438</v>
+        <v>0.001017868166272584</v>
       </c>
       <c r="H18">
-        <v>0.2133795918767654</v>
+        <v>0.212555477012045</v>
       </c>
       <c r="I18">
-        <v>11611</v>
+        <v>11542</v>
       </c>
       <c r="J18">
-        <v>0.0001631540263502446</v>
+        <v>0.00510134746390362</v>
       </c>
       <c r="K18">
-        <v>-0.002771209789547591</v>
+        <v>0.001583264354559398</v>
       </c>
       <c r="L18">
-        <v>0.001592932311570713</v>
+        <v>0.000163888349337522</v>
       </c>
       <c r="M18">
-        <v>0.004580501696160511</v>
+        <v>0.004589584286176587</v>
       </c>
       <c r="N18">
-        <v>0.000207986162951978</v>
+        <v>0.001597174444307401</v>
       </c>
       <c r="O18">
-        <v>0.005107549406927882</v>
+        <v>0.0002091701444985722</v>
       </c>
       <c r="P18">
-        <v>0.001554596452837835</v>
+        <v>-0.005012774390606101</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -1426,49 +1429,49 @@
         <v>33</v>
       </c>
       <c r="B19">
-        <v>0.006549373422714545</v>
+        <v>0.00304699828992123</v>
       </c>
       <c r="C19">
-        <v>0.005670204101840715</v>
+        <v>0.002499571894821071</v>
       </c>
       <c r="D19">
-        <v>0.0001064697656049724</v>
+        <v>1.903121423403654E-05</v>
       </c>
       <c r="E19">
-        <v>9.344840654260834E-05</v>
+        <v>1.967007435869721E-05</v>
       </c>
       <c r="F19">
-        <v>0.1346849985258249</v>
+        <v>-0.008580312939503454</v>
       </c>
       <c r="G19">
-        <v>0.2405138906269937</v>
+        <v>-0.04243741404356438</v>
       </c>
       <c r="H19">
-        <v>0.4208397194991282</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I19">
-        <v>6771</v>
+        <v>11611</v>
       </c>
       <c r="J19">
-        <v>0.0001037297229528328</v>
+        <v>0.005107549406927882</v>
       </c>
       <c r="K19">
-        <v>0.1058242633905934</v>
+        <v>0.001554596452837835</v>
       </c>
       <c r="L19">
-        <v>0.003193202088483064</v>
+        <v>0.0001631540263502446</v>
       </c>
       <c r="M19">
-        <v>0.005813234561065723</v>
+        <v>0.004580501696160511</v>
       </c>
       <c r="N19">
-        <v>0.000160150142460433</v>
+        <v>0.001592932311570713</v>
       </c>
       <c r="O19">
-        <v>0.006776662396495037</v>
+        <v>0.000207986162951978</v>
       </c>
       <c r="P19">
-        <v>0.003715325925925931</v>
+        <v>-0.002771209789547591</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1476,49 +1479,49 @@
         <v>34</v>
       </c>
       <c r="B20">
-        <v>0.002783525716284511</v>
+        <v>0.006549373422714545</v>
       </c>
       <c r="C20">
-        <v>0.002457544020376962</v>
+        <v>0.005670204101840715</v>
       </c>
       <c r="D20">
-        <v>1.713865210259099E-05</v>
+        <v>0.0001064697656049724</v>
       </c>
       <c r="E20">
-        <v>1.89022549270271E-05</v>
+        <v>9.344840654260834E-05</v>
       </c>
       <c r="F20">
-        <v>-0.05370835704473098</v>
+        <v>0.1346849985258249</v>
       </c>
       <c r="G20">
-        <v>-0.1621371309933592</v>
+        <v>0.2405138906269937</v>
       </c>
       <c r="H20">
-        <v>0.3649062991209757</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I20">
-        <v>4010</v>
+        <v>6771</v>
       </c>
       <c r="J20">
-        <v>0.0001730864695810989</v>
+        <v>0.006776662396495037</v>
       </c>
       <c r="K20">
-        <v>-0.006214540120261569</v>
+        <v>0.003715325925925931</v>
       </c>
       <c r="L20">
-        <v>0.001438312583710056</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="M20">
-        <v>0.004349183403839366</v>
+        <v>0.005813234561065723</v>
       </c>
       <c r="N20">
-        <v>0.0002742305932959652</v>
+        <v>0.003193202088483064</v>
       </c>
       <c r="O20">
-        <v>0.004501420066184821</v>
+        <v>0.000160150142460433</v>
       </c>
       <c r="P20">
-        <v>0.001362431751651251</v>
+        <v>0.1058242633905934</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1526,49 +1529,49 @@
         <v>35</v>
       </c>
       <c r="B21">
-        <v>0.00929322862430519</v>
+        <v>0.002783525716284511</v>
       </c>
       <c r="C21">
-        <v>0.008733878054388279</v>
+        <v>0.002457544020376962</v>
       </c>
       <c r="D21">
-        <v>0.000192984991667648</v>
+        <v>1.713865210259099E-05</v>
       </c>
       <c r="E21">
-        <v>0.0001961492659581503</v>
+        <v>1.89022549270271E-05</v>
       </c>
       <c r="F21">
-        <v>0.1421155108066621</v>
+        <v>-0.05370835704473098</v>
       </c>
       <c r="G21">
-        <v>0.1280492261183164</v>
+        <v>-0.1621371309933592</v>
       </c>
       <c r="H21">
-        <v>0.2582640092197721</v>
+        <v>0.3649062991209757</v>
       </c>
       <c r="I21">
-        <v>14156</v>
+        <v>4010</v>
       </c>
       <c r="J21">
-        <v>0.0003384092866814527</v>
+        <v>0.004501420066184821</v>
       </c>
       <c r="K21">
-        <v>0.1230344532976788</v>
+        <v>0.001362431751651251</v>
       </c>
       <c r="L21">
-        <v>0.004818030126325817</v>
+        <v>0.0001730864695810989</v>
       </c>
       <c r="M21">
-        <v>0.009674189396799987</v>
+        <v>0.004349183403839366</v>
       </c>
       <c r="N21">
-        <v>0.0004001063569688302</v>
+        <v>0.001438312583710056</v>
       </c>
       <c r="O21">
-        <v>0.01035431191953904</v>
+        <v>0.0002742305932959652</v>
       </c>
       <c r="P21">
-        <v>0.005409147625572685</v>
+        <v>-0.006214540120261569</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1576,49 +1579,49 @@
         <v>36</v>
       </c>
       <c r="B22">
-        <v>0.003030458698074221</v>
+        <v>0.00929322862430519</v>
       </c>
       <c r="C22">
-        <v>0.002499571894821071</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D22">
-        <v>1.91281128971015E-05</v>
+        <v>0.000192984991667648</v>
       </c>
       <c r="E22">
-        <v>1.967007435869721E-05</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F22">
-        <v>-0.01371556509502225</v>
+        <v>0.1421155108066621</v>
       </c>
       <c r="G22">
-        <v>-0.04243741404356438</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H22">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I22">
-        <v>11611</v>
+        <v>14156</v>
       </c>
       <c r="J22">
-        <v>0.0001631540263502446</v>
+        <v>0.01035431191953904</v>
       </c>
       <c r="K22">
-        <v>-0.00353431378743374</v>
+        <v>0.005409147625572685</v>
       </c>
       <c r="L22">
-        <v>0.001592932311570713</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="M22">
-        <v>0.004580501696160511</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="N22">
-        <v>0.0002081444394071696</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="O22">
-        <v>0.005089488294347637</v>
+        <v>0.0004001063569688302</v>
       </c>
       <c r="P22">
-        <v>0.001547174514616301</v>
+        <v>0.1230344532976788</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1626,49 +1629,49 @@
         <v>37</v>
       </c>
       <c r="B23">
-        <v>0.008532806478705164</v>
+        <v>0.003030458698074221</v>
       </c>
       <c r="C23">
-        <v>0.008733878054388279</v>
+        <v>0.002499571894821071</v>
       </c>
       <c r="D23">
-        <v>0.0001656454412935777</v>
+        <v>1.91281128971015E-05</v>
       </c>
       <c r="E23">
-        <v>0.0001961492659581503</v>
+        <v>1.967007435869721E-05</v>
       </c>
       <c r="F23">
-        <v>0.2636491907304709</v>
+        <v>-0.01371556509502225</v>
       </c>
       <c r="G23">
-        <v>0.1280492261183164</v>
+        <v>-0.04243741404356438</v>
       </c>
       <c r="H23">
-        <v>0.2582640092197721</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I23">
-        <v>14156</v>
+        <v>11611</v>
       </c>
       <c r="J23">
-        <v>0.0003384092866814527</v>
+        <v>0.005089488294347637</v>
       </c>
       <c r="K23">
-        <v>0.179378395374721</v>
+        <v>0.001547174514616301</v>
       </c>
       <c r="L23">
-        <v>0.004818030126325817</v>
+        <v>0.0001631540263502446</v>
       </c>
       <c r="M23">
-        <v>0.009674189396799987</v>
+        <v>0.004580501696160511</v>
       </c>
       <c r="N23">
-        <v>0.0003744000227958637</v>
+        <v>0.001592932311570713</v>
       </c>
       <c r="O23">
-        <v>0.009554445336689437</v>
+        <v>0.0002081444394071696</v>
       </c>
       <c r="P23">
-        <v>0.004730871750625608</v>
+        <v>-0.00353431378743374</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -1676,19 +1679,19 @@
         <v>38</v>
       </c>
       <c r="B24">
-        <v>0.008529233938818522</v>
+        <v>0.008532806478705164</v>
       </c>
       <c r="C24">
         <v>0.008733878054388279</v>
       </c>
       <c r="D24">
-        <v>0.0001653251466070655</v>
+        <v>0.0001656454412935777</v>
       </c>
       <c r="E24">
         <v>0.0001961492659581503</v>
       </c>
       <c r="F24">
-        <v>0.2650730104853413</v>
+        <v>0.2636491907304709</v>
       </c>
       <c r="G24">
         <v>0.1280492261183164</v>
@@ -1700,25 +1703,25 @@
         <v>14156</v>
       </c>
       <c r="J24">
+        <v>0.009554445336689437</v>
+      </c>
+      <c r="K24">
+        <v>0.004730871750625608</v>
+      </c>
+      <c r="L24">
         <v>0.0003384092866814527</v>
-      </c>
-      <c r="K24">
-        <v>0.1788608663781261</v>
-      </c>
-      <c r="L24">
-        <v>0.004818030126325817</v>
       </c>
       <c r="M24">
         <v>0.009674189396799987</v>
       </c>
       <c r="N24">
-        <v>0.0003746361399868205</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="O24">
-        <v>0.009555217528480035</v>
+        <v>0.0003744000227958637</v>
       </c>
       <c r="P24">
-        <v>0.004764640177213803</v>
+        <v>0.179378395374721</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -1726,19 +1729,19 @@
         <v>39</v>
       </c>
       <c r="B25">
-        <v>0.008505250051591662</v>
+        <v>0.008529233938818522</v>
       </c>
       <c r="C25">
         <v>0.008733878054388279</v>
       </c>
       <c r="D25">
-        <v>0.0001646168902522808</v>
+        <v>0.0001653251466070655</v>
       </c>
       <c r="E25">
         <v>0.0001961492659581503</v>
       </c>
       <c r="F25">
-        <v>0.268221452941368</v>
+        <v>0.2650730104853413</v>
       </c>
       <c r="G25">
         <v>0.1280492261183164</v>
@@ -1750,25 +1753,25 @@
         <v>14156</v>
       </c>
       <c r="J25">
+        <v>0.009555217528480035</v>
+      </c>
+      <c r="K25">
+        <v>0.004764640177213803</v>
+      </c>
+      <c r="L25">
         <v>0.0003384092866814527</v>
-      </c>
-      <c r="K25">
-        <v>0.1810824657398455</v>
-      </c>
-      <c r="L25">
-        <v>0.004818030126325817</v>
       </c>
       <c r="M25">
         <v>0.009674189396799987</v>
       </c>
       <c r="N25">
-        <v>0.0003736225585176234</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="O25">
-        <v>0.009526287265811475</v>
+        <v>0.0003746361399868205</v>
       </c>
       <c r="P25">
-        <v>0.004756476812602748</v>
+        <v>0.1788608663781261</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -1776,49 +1779,49 @@
         <v>40</v>
       </c>
       <c r="B26">
-        <v>0.006299187529923155</v>
+        <v>0.008505250051591662</v>
       </c>
       <c r="C26">
-        <v>0.00553167406053466</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D26">
-        <v>9.00395869891457E-05</v>
+        <v>0.0001646168902522808</v>
       </c>
       <c r="E26">
-        <v>8.170381435551846E-05</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F26">
-        <v>0.1391419988807219</v>
+        <v>0.268221452941368</v>
       </c>
       <c r="G26">
-        <v>0.2188393498696173</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H26">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I26">
-        <v>6771</v>
+        <v>14156</v>
       </c>
       <c r="J26">
-        <v>0.0001037297229528328</v>
+        <v>0.009526287265811475</v>
       </c>
       <c r="K26">
-        <v>0.1045681259196538</v>
+        <v>0.004756476812602748</v>
       </c>
       <c r="L26">
-        <v>0.003193202088483064</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="M26">
-        <v>0.005813234561065723</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="N26">
-        <v>0.0001603751212724098</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="O26">
-        <v>0.00674135934653288</v>
+        <v>0.0003736225585176234</v>
       </c>
       <c r="P26">
-        <v>0.003667719421830667</v>
+        <v>0.1810824657398455</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -1826,49 +1829,49 @@
         <v>41</v>
       </c>
       <c r="B27">
-        <v>0.00869522801124366</v>
+        <v>0.006299187529923155</v>
       </c>
       <c r="C27">
-        <v>0.008722720041403264</v>
+        <v>0.00553167406053466</v>
       </c>
       <c r="D27">
-        <v>0.0001671499749450426</v>
+        <v>9.00395869891457E-05</v>
       </c>
       <c r="E27">
-        <v>0.0001985649052123504</v>
+        <v>8.170381435551846E-05</v>
       </c>
       <c r="F27">
-        <v>0.2822259777859754</v>
+        <v>0.1391419988807219</v>
       </c>
       <c r="G27">
-        <v>0.147324247391146</v>
+        <v>0.2188393498696173</v>
       </c>
       <c r="H27">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I27">
-        <v>14156</v>
+        <v>6771</v>
       </c>
       <c r="J27">
-        <v>0.0003384092866814527</v>
+        <v>0.00674135934653288</v>
       </c>
       <c r="K27">
-        <v>0.2030564380000814</v>
+        <v>0.003667719421830667</v>
       </c>
       <c r="L27">
-        <v>0.004818030126325817</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="M27">
-        <v>0.009674189396799985</v>
+        <v>0.005813234561065723</v>
       </c>
       <c r="N27">
-        <v>0.0003635971635380399</v>
+        <v>0.003193202088483064</v>
       </c>
       <c r="O27">
-        <v>0.009719161233546112</v>
+        <v>0.0001603751212724098</v>
       </c>
       <c r="P27">
-        <v>0.005173194757001598</v>
+        <v>0.1045681259196538</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -1876,19 +1879,19 @@
         <v>42</v>
       </c>
       <c r="B28">
-        <v>0.007668256776450208</v>
+        <v>0.00869522801124366</v>
       </c>
       <c r="C28">
         <v>0.008722720041403264</v>
       </c>
       <c r="D28">
-        <v>0.0001436777206558706</v>
+        <v>0.0001671499749450426</v>
       </c>
       <c r="E28">
         <v>0.0001985649052123504</v>
       </c>
       <c r="F28">
-        <v>0.3830203355303232</v>
+        <v>0.2822259777859754</v>
       </c>
       <c r="G28">
         <v>0.147324247391146</v>
@@ -1900,25 +1903,25 @@
         <v>14156</v>
       </c>
       <c r="J28">
+        <v>0.009719161233546112</v>
+      </c>
+      <c r="K28">
+        <v>0.005173194757001598</v>
+      </c>
+      <c r="L28">
         <v>0.0003384092866814527</v>
-      </c>
-      <c r="K28">
-        <v>0.2669184291403396</v>
-      </c>
-      <c r="L28">
-        <v>0.004818030126325817</v>
       </c>
       <c r="M28">
         <v>0.009674189396799985</v>
       </c>
       <c r="N28">
-        <v>0.0003344607981243851</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="O28">
-        <v>0.00867861064019221</v>
+        <v>0.0003635971635380399</v>
       </c>
       <c r="P28">
-        <v>0.004128330862335852</v>
+        <v>0.2030564380000814</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -1926,19 +1929,19 @@
         <v>43</v>
       </c>
       <c r="B29">
-        <v>0.00958912348219286</v>
+        <v>0.007668256776450208</v>
       </c>
       <c r="C29">
         <v>0.008722720041403264</v>
       </c>
       <c r="D29">
-        <v>0.00021842684931279</v>
+        <v>0.0001436777206558706</v>
       </c>
       <c r="E29">
         <v>0.0001985649052123504</v>
       </c>
       <c r="F29">
-        <v>0.06203325341612431</v>
+        <v>0.3830203355303232</v>
       </c>
       <c r="G29">
         <v>0.147324247391146</v>
@@ -1950,25 +1953,25 @@
         <v>14156</v>
       </c>
       <c r="J29">
+        <v>0.00867861064019221</v>
+      </c>
+      <c r="K29">
+        <v>0.004128330862335852</v>
+      </c>
+      <c r="L29">
         <v>0.0003384092866814527</v>
-      </c>
-      <c r="K29">
-        <v>0.05448840836791147</v>
-      </c>
-      <c r="L29">
-        <v>0.004818030126325817</v>
       </c>
       <c r="M29">
         <v>0.009674189396799985</v>
       </c>
       <c r="N29">
-        <v>0.0004313797729252501</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="O29">
-        <v>0.01064772150300563</v>
+        <v>0.0003344607981243851</v>
       </c>
       <c r="P29">
-        <v>0.005560650653515711</v>
+        <v>0.2669184291403396</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -1976,49 +1979,49 @@
         <v>44</v>
       </c>
       <c r="B30">
-        <v>0.005743153097997238</v>
+        <v>0.00958912348219286</v>
       </c>
       <c r="C30">
-        <v>0.005699109365498782</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D30">
-        <v>9.179016309205035E-05</v>
+        <v>0.00021842684931279</v>
       </c>
       <c r="E30">
-        <v>9.470932808225897E-05</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F30">
-        <v>0.2786526717712858</v>
+        <v>0.06203325341612431</v>
       </c>
       <c r="G30">
-        <v>0.2557119579146814</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H30">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I30">
-        <v>6771</v>
+        <v>14156</v>
       </c>
       <c r="J30">
-        <v>0.0001037297229528328</v>
+        <v>0.01064772150300563</v>
       </c>
       <c r="K30">
-        <v>0.2046421514566161</v>
+        <v>0.005560650653515711</v>
       </c>
       <c r="L30">
-        <v>0.003193202088483064</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="M30">
-        <v>0.005813234561065725</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="N30">
-        <v>0.0001424514975481683</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="O30">
-        <v>0.00595976388177965</v>
+        <v>0.0004313797729252501</v>
       </c>
       <c r="P30">
-        <v>0.002972129451884979</v>
+        <v>0.05448840836791147</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -2026,49 +2029,49 @@
         <v>45</v>
       </c>
       <c r="B31">
-        <v>0.009301347310769852</v>
+        <v>0.005743153097997238</v>
       </c>
       <c r="C31">
-        <v>0.008733878054388279</v>
+        <v>0.005699109365498782</v>
       </c>
       <c r="D31">
-        <v>0.0001883109214593075</v>
+        <v>9.179016309205035E-05</v>
       </c>
       <c r="E31">
-        <v>0.0001961492659581503</v>
+        <v>9.470932808225897E-05</v>
       </c>
       <c r="F31">
-        <v>0.1628933562675233</v>
+        <v>0.2786526717712858</v>
       </c>
       <c r="G31">
-        <v>0.1280492261183164</v>
+        <v>0.2557119579146814</v>
       </c>
       <c r="H31">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I31">
-        <v>14156</v>
+        <v>6771</v>
       </c>
       <c r="J31">
-        <v>0.0003384092866814527</v>
+        <v>0.00595976388177965</v>
       </c>
       <c r="K31">
-        <v>0.1175458874123242</v>
+        <v>0.002972129451884979</v>
       </c>
       <c r="L31">
-        <v>0.004818030126325817</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="M31">
-        <v>0.009674189396799987</v>
+        <v>0.005813234561065725</v>
       </c>
       <c r="N31">
-        <v>0.0004026104577395279</v>
+        <v>0.003193202088483064</v>
       </c>
       <c r="O31">
-        <v>0.01035467890006862</v>
+        <v>0.0001424514975481683</v>
       </c>
       <c r="P31">
-        <v>0.005399385735558927</v>
+        <v>0.2046421514566161</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -2076,49 +2079,49 @@
         <v>46</v>
       </c>
       <c r="B32">
-        <v>0.00303210497017975</v>
+        <v>0.009301347310769852</v>
       </c>
       <c r="C32">
-        <v>0.002499571894821071</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D32">
-        <v>1.909735738640315E-05</v>
+        <v>0.0001883109214593075</v>
       </c>
       <c r="E32">
-        <v>1.967007435869721E-05</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F32">
-        <v>-0.0120856426831728</v>
+        <v>0.1628933562675233</v>
       </c>
       <c r="G32">
-        <v>-0.04243741404356438</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H32">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I32">
-        <v>11611</v>
+        <v>14156</v>
       </c>
       <c r="J32">
-        <v>0.0001631540263502446</v>
+        <v>0.01035467890006862</v>
       </c>
       <c r="K32">
-        <v>-0.002911711704464803</v>
+        <v>0.005399385735558927</v>
       </c>
       <c r="L32">
-        <v>0.001592932311570713</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="M32">
-        <v>0.004580501696160511</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="N32">
-        <v>0.0002080153046483946</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="O32">
-        <v>0.005090949099942899</v>
+        <v>0.0004026104577395279</v>
       </c>
       <c r="P32">
-        <v>0.001550051802718652</v>
+        <v>0.1175458874123242</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -2126,49 +2129,99 @@
         <v>47</v>
       </c>
       <c r="B33">
+        <v>0.00303210497017975</v>
+      </c>
+      <c r="C33">
+        <v>0.002499571894821071</v>
+      </c>
+      <c r="D33">
+        <v>1.909735738640315E-05</v>
+      </c>
+      <c r="E33">
+        <v>1.967007435869721E-05</v>
+      </c>
+      <c r="F33">
+        <v>-0.0120856426831728</v>
+      </c>
+      <c r="G33">
+        <v>-0.04243741404356438</v>
+      </c>
+      <c r="H33">
+        <v>0.2133795918767654</v>
+      </c>
+      <c r="I33">
+        <v>11611</v>
+      </c>
+      <c r="J33">
+        <v>0.005090949099942899</v>
+      </c>
+      <c r="K33">
+        <v>0.001550051802718652</v>
+      </c>
+      <c r="L33">
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="M33">
+        <v>0.004580501696160511</v>
+      </c>
+      <c r="N33">
+        <v>0.001592932311570713</v>
+      </c>
+      <c r="O33">
+        <v>0.0002080153046483946</v>
+      </c>
+      <c r="P33">
+        <v>-0.002911711704464803</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34">
         <v>0.008142928261746932</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <v>0.008733878054388279</v>
       </c>
-      <c r="D33">
+      <c r="D34">
         <v>0.0001648112327367591</v>
       </c>
-      <c r="E33">
+      <c r="E34">
         <v>0.0001961492659581503</v>
       </c>
-      <c r="F33">
+      <c r="F34">
         <v>0.2673575339309593</v>
       </c>
-      <c r="G33">
+      <c r="G34">
         <v>0.1280492261183164</v>
       </c>
-      <c r="H33">
+      <c r="H34">
         <v>0.2582640092197721</v>
       </c>
-      <c r="I33">
+      <c r="I34">
         <v>14156</v>
       </c>
-      <c r="J33">
+      <c r="J34">
+        <v>0.009263751492683912</v>
+      </c>
+      <c r="K34">
+        <v>0.004666820467017538</v>
+      </c>
+      <c r="L34">
         <v>0.0003384092866814527</v>
       </c>
-      <c r="K33">
+      <c r="M34">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="N34">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="O34">
+        <v>0.0003438074749231005</v>
+      </c>
+      <c r="P34">
         <v>0.2464320924804251</v>
-      </c>
-      <c r="L33">
-        <v>0.004818030126325817</v>
-      </c>
-      <c r="M33">
-        <v>0.009674189396799987</v>
-      </c>
-      <c r="N33">
-        <v>0.0003438074749231005</v>
-      </c>
-      <c r="O33">
-        <v>0.009263751492683912</v>
-      </c>
-      <c r="P33">
-        <v>0.004666820467017538</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update ibes_qoq for lgbm
</commit_message>
<xml_diff>
--- a/results_analysis/compare_with_ibes/#compare_all.xlsx
+++ b/results_analysis/compare_with_ibes/#compare_all.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>lgbm_mae</t>
   </si>
@@ -40,31 +40,34 @@
     <t>len</t>
   </si>
   <si>
+    <t>lgbm_mse_org</t>
+  </si>
+  <si>
+    <t>consensus_mse_org</t>
+  </si>
+  <si>
+    <t>lgbm_r2_org</t>
+  </si>
+  <si>
     <t>lgbm_mae_org</t>
   </si>
   <si>
+    <t>consensus_medae_org</t>
+  </si>
+  <si>
     <t>lgbm_medae_org</t>
   </si>
   <si>
-    <t>consensus_mse_org</t>
-  </si>
-  <si>
     <t>consensus_mae_org</t>
   </si>
   <si>
-    <t>consensus_medae_org</t>
-  </si>
-  <si>
-    <t>lgbm_mse_org</t>
-  </si>
-  <si>
-    <t>lgbm_r2_org</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
     <t>ibes_1|fwdepsqcut-46|dense2｜compare large space</t>
+  </si>
+  <si>
+    <t>ibes_qoq_2|fwdepsqcut|q_2｜ibes_qoq_tune10_ind3</t>
   </si>
   <si>
     <t>ibes_2|ni_depthwise|xgb ind_all_tuning -sample_type industry -x_type ni_sp500</t>
@@ -518,7 +521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -603,25 +606,25 @@
         <v>14156</v>
       </c>
       <c r="J2">
+        <v>0.0004250480609163007</v>
+      </c>
+      <c r="K2">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="L2">
+        <v>0.06836645151013176</v>
+      </c>
+      <c r="M2">
         <v>0.01071193221870467</v>
-      </c>
-      <c r="K2">
-        <v>0.005638666708596741</v>
-      </c>
-      <c r="L2">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="M2">
-        <v>0.009674189396799987</v>
       </c>
       <c r="N2">
         <v>0.004818030126325817</v>
       </c>
       <c r="O2">
-        <v>0.0004250480609163007</v>
+        <v>0.005638666708596741</v>
       </c>
       <c r="P2">
-        <v>0.06836645151013176</v>
+        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -629,49 +632,49 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.005308188556537048</v>
+        <v>0.003127879691820042</v>
       </c>
       <c r="C3">
-        <v>0.005639127357765789</v>
+        <v>0.002538761048289119</v>
       </c>
       <c r="D3">
-        <v>7.028985097208806E-05</v>
+        <v>2.076719194527133E-05</v>
       </c>
       <c r="E3">
-        <v>9.102681873913914E-05</v>
+        <v>2.103311528121684E-05</v>
       </c>
       <c r="F3">
-        <v>0.4089911478654851</v>
+        <v>0.01355620914095823</v>
       </c>
       <c r="G3">
-        <v>0.2346312460124846</v>
+        <v>0.0009248228524665336</v>
       </c>
       <c r="H3">
-        <v>0.4208397194991282</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I3">
-        <v>6771</v>
+        <v>11611</v>
       </c>
       <c r="J3">
-        <v>0.005632685300523813</v>
+        <v>0.0001978384306784256</v>
       </c>
       <c r="K3">
-        <v>0.003171635367762127</v>
+        <v>0.0001631540263502446</v>
       </c>
       <c r="L3">
-        <v>0.0001037297229528328</v>
+        <v>0.04615441883950755</v>
       </c>
       <c r="M3">
-        <v>0.005813234561065725</v>
+        <v>0.00502885184437347</v>
       </c>
       <c r="N3">
-        <v>0.003193202088483064</v>
+        <v>0.001592932311570713</v>
       </c>
       <c r="O3">
-        <v>0.0001152638129503358</v>
+        <v>0.001779221775169934</v>
       </c>
       <c r="P3">
-        <v>0.3564407544954944</v>
+        <v>0.004580501696160511</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -679,49 +682,49 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.008311421494257554</v>
+        <v>0.005308188556537048</v>
       </c>
       <c r="C4">
-        <v>0.008853442839112767</v>
+        <v>0.005639127357765789</v>
       </c>
       <c r="D4">
-        <v>0.0001712304539584277</v>
+        <v>7.028985097208806E-05</v>
       </c>
       <c r="E4">
-        <v>0.0002150273861825077</v>
+        <v>9.102681873913914E-05</v>
       </c>
       <c r="F4">
-        <v>0.3115448762458137</v>
+        <v>0.4089911478654851</v>
       </c>
       <c r="G4">
-        <v>0.1354534059650468</v>
+        <v>0.2346312460124846</v>
       </c>
       <c r="H4">
-        <v>0.2582640092197723</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I4">
-        <v>42468</v>
+        <v>6771</v>
       </c>
       <c r="J4">
-        <v>0.009106885821888167</v>
+        <v>0.0001152638129503358</v>
       </c>
       <c r="K4">
-        <v>0.004616722796530505</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="L4">
-        <v>0.0003384092866814527</v>
+        <v>0.3564407544954944</v>
       </c>
       <c r="M4">
-        <v>0.009674189396799987</v>
+        <v>0.005632685300523813</v>
       </c>
       <c r="N4">
-        <v>0.004818030126325817</v>
+        <v>0.003193202088483064</v>
       </c>
       <c r="O4">
-        <v>0.000333070102780211</v>
+        <v>0.003171635367762127</v>
       </c>
       <c r="P4">
-        <v>0.269966598412229</v>
+        <v>0.005813234561065725</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -729,49 +732,49 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>0.007944638673415367</v>
+        <v>0.008311421494257554</v>
       </c>
       <c r="C5">
-        <v>0.008722720041403264</v>
+        <v>0.008853442839112767</v>
       </c>
       <c r="D5">
-        <v>0.0001442016437287739</v>
+        <v>0.0001712304539584277</v>
       </c>
       <c r="E5">
-        <v>0.0001985649052123504</v>
+        <v>0.0002150273861825077</v>
       </c>
       <c r="F5">
-        <v>0.3807705094595015</v>
+        <v>0.3115448762458137</v>
       </c>
       <c r="G5">
-        <v>0.147324247391146</v>
+        <v>0.1354534059650468</v>
       </c>
       <c r="H5">
-        <v>0.2582640092197721</v>
+        <v>0.2582640092197723</v>
       </c>
       <c r="I5">
-        <v>14156</v>
+        <v>42468</v>
       </c>
       <c r="J5">
-        <v>0.008950010380536522</v>
+        <v>0.000333070102780211</v>
       </c>
       <c r="K5">
-        <v>0.004615286290830784</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="L5">
-        <v>0.0003384092866814527</v>
+        <v>0.269966598412229</v>
       </c>
       <c r="M5">
-        <v>0.009674189396799985</v>
+        <v>0.009106885821888167</v>
       </c>
       <c r="N5">
         <v>0.004818030126325817</v>
       </c>
       <c r="O5">
-        <v>0.0003285627388197843</v>
+        <v>0.004616722796530505</v>
       </c>
       <c r="P5">
-        <v>0.2798459788092014</v>
+        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -779,19 +782,19 @@
         <v>20</v>
       </c>
       <c r="B6">
-        <v>0.008392539580425228</v>
+        <v>0.007944638673415367</v>
       </c>
       <c r="C6">
         <v>0.008722720041403264</v>
       </c>
       <c r="D6">
-        <v>0.0001662926371782633</v>
+        <v>0.0001442016437287739</v>
       </c>
       <c r="E6">
         <v>0.0001985649052123504</v>
       </c>
       <c r="F6">
-        <v>0.2859075504422648</v>
+        <v>0.3807705094595015</v>
       </c>
       <c r="G6">
         <v>0.147324247391146</v>
@@ -803,25 +806,25 @@
         <v>14156</v>
       </c>
       <c r="J6">
-        <v>0.00941140169945745</v>
+        <v>0.0003285627388197843</v>
       </c>
       <c r="K6">
-        <v>0.004590555422836876</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="L6">
-        <v>0.0003384092866814527</v>
+        <v>0.2798459788092014</v>
       </c>
       <c r="M6">
-        <v>0.009674189396799985</v>
+        <v>0.008950010380536522</v>
       </c>
       <c r="N6">
         <v>0.004818030126325817</v>
       </c>
       <c r="O6">
-        <v>0.0003713407546776094</v>
+        <v>0.004615286290830784</v>
       </c>
       <c r="P6">
-        <v>0.1860837943045432</v>
+        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -829,49 +832,49 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>0.007970745265560365</v>
+        <v>0.008392539580425228</v>
       </c>
       <c r="C7">
-        <v>0.00654101945735325</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D7">
-        <v>0.0001659654171746955</v>
+        <v>0.0001662926371782633</v>
       </c>
       <c r="E7">
-        <v>0.0001252256324013319</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F7">
-        <v>-0.0277890197779842</v>
+        <v>0.2859075504422648</v>
       </c>
       <c r="G7">
-        <v>0.224503922757791</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H7">
-        <v>0.3127047460379806</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I7">
-        <v>24768</v>
+        <v>14156</v>
       </c>
       <c r="J7">
-        <v>0.008363098231375462</v>
+        <v>0.0003713407546776094</v>
       </c>
       <c r="K7">
-        <v>0.004275415213561056</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="L7">
-        <v>0.0001796235360933539</v>
+        <v>0.1860837943045432</v>
       </c>
       <c r="M7">
-        <v>0.006875190708555331</v>
+        <v>0.00941140169945745</v>
       </c>
       <c r="N7">
-        <v>0.003559726400188349</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="O7">
-        <v>0.0002632414236722758</v>
+        <v>0.004590555422836876</v>
       </c>
       <c r="P7">
-        <v>-0.00724317687482956</v>
+        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -879,49 +882,49 @@
         <v>22</v>
       </c>
       <c r="B8">
-        <v>0.009885890648801</v>
+        <v>0.007970745265560365</v>
       </c>
       <c r="C8">
-        <v>0.009614451672116909</v>
+        <v>0.00654101945735325</v>
       </c>
       <c r="D8">
-        <v>0.0002810826792241289</v>
+        <v>0.0001659654171746955</v>
       </c>
       <c r="E8">
-        <v>0.0002968767906711129</v>
+        <v>0.0001252256324013319</v>
       </c>
       <c r="F8">
-        <v>0.2059318010033613</v>
+        <v>-0.0277890197779842</v>
       </c>
       <c r="G8">
-        <v>0.1613128950427474</v>
+        <v>0.224503922757791</v>
       </c>
       <c r="H8">
-        <v>0.2582640092197721</v>
+        <v>0.3127047460379806</v>
       </c>
       <c r="I8">
-        <v>14156</v>
+        <v>24768</v>
       </c>
       <c r="J8">
-        <v>0.009901025034115019</v>
+        <v>0.0002632414236722758</v>
       </c>
       <c r="K8">
-        <v>0.005167135423672592</v>
+        <v>0.0001796235360933539</v>
       </c>
       <c r="L8">
-        <v>0.0003384092866814527</v>
+        <v>-0.00724317687482956</v>
       </c>
       <c r="M8">
-        <v>0.009674189396799985</v>
+        <v>0.008363098231375462</v>
       </c>
       <c r="N8">
-        <v>0.004818030126325817</v>
+        <v>0.003559726400188349</v>
       </c>
       <c r="O8">
-        <v>0.0003847976244374441</v>
+        <v>0.004275415213561056</v>
       </c>
       <c r="P8">
-        <v>0.1565886089862186</v>
+        <v>0.006875190708555331</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -929,49 +932,49 @@
         <v>23</v>
       </c>
       <c r="B9">
-        <v>0.003125769257313045</v>
+        <v>0.009885890648801</v>
       </c>
       <c r="C9">
-        <v>0.00254141838673398</v>
+        <v>0.009614451672116909</v>
       </c>
       <c r="D9">
-        <v>2.166040204619485E-05</v>
+        <v>0.0002810826792241289</v>
       </c>
       <c r="E9">
-        <v>2.106152912726658E-05</v>
+        <v>0.0002968767906711129</v>
       </c>
       <c r="F9">
-        <v>-0.02738763561426372</v>
+        <v>0.2059318010033613</v>
       </c>
       <c r="G9">
-        <v>0.001017868166272584</v>
+        <v>0.1613128950427474</v>
       </c>
       <c r="H9">
-        <v>0.212555477012045</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I9">
-        <v>11542</v>
+        <v>14156</v>
       </c>
       <c r="J9">
-        <v>0.00512210974064752</v>
+        <v>0.0003847976244374441</v>
       </c>
       <c r="K9">
-        <v>0.001602037466360856</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="L9">
-        <v>0.000163888349337522</v>
+        <v>0.1565886089862186</v>
       </c>
       <c r="M9">
-        <v>0.004589584286176587</v>
+        <v>0.009901025034115019</v>
       </c>
       <c r="N9">
-        <v>0.001597174444307401</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="O9">
-        <v>0.000209188838038313</v>
+        <v>0.005167135423672592</v>
       </c>
       <c r="P9">
-        <v>-0.005102592401121431</v>
+        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -979,49 +982,49 @@
         <v>24</v>
       </c>
       <c r="B10">
-        <v>0.003208711377129972</v>
+        <v>0.003125769257313045</v>
       </c>
       <c r="C10">
-        <v>0.002538761048289119</v>
+        <v>0.00254141838673398</v>
       </c>
       <c r="D10">
-        <v>2.210896317387241E-05</v>
+        <v>2.166040204619485E-05</v>
       </c>
       <c r="E10">
-        <v>2.103311528121684E-05</v>
+        <v>2.106152912726658E-05</v>
       </c>
       <c r="F10">
-        <v>-0.05017806464506647</v>
+        <v>-0.02738763561426372</v>
       </c>
       <c r="G10">
-        <v>0.0009248228524665336</v>
+        <v>0.001017868166272584</v>
       </c>
       <c r="H10">
-        <v>0.2133795918767654</v>
+        <v>0.212555477012045</v>
       </c>
       <c r="I10">
-        <v>11611</v>
+        <v>11542</v>
       </c>
       <c r="J10">
-        <v>0.005213165544267774</v>
+        <v>0.000209188838038313</v>
       </c>
       <c r="K10">
-        <v>0.00173711317318318</v>
+        <v>0.000163888349337522</v>
       </c>
       <c r="L10">
-        <v>0.0001631540263502446</v>
+        <v>-0.005102592401121431</v>
       </c>
       <c r="M10">
-        <v>0.004580501696160511</v>
+        <v>0.00512210974064752</v>
       </c>
       <c r="N10">
-        <v>0.001592932311570713</v>
+        <v>0.001597174444307401</v>
       </c>
       <c r="O10">
-        <v>0.0002098592232396584</v>
+        <v>0.001602037466360856</v>
       </c>
       <c r="P10">
-        <v>-0.01180186309853548</v>
+        <v>0.004589584286176587</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1029,49 +1032,49 @@
         <v>25</v>
       </c>
       <c r="B11">
-        <v>0.003491208235511574</v>
+        <v>0.003208711377129972</v>
       </c>
       <c r="C11">
-        <v>0.001329144946829925</v>
+        <v>0.002538761048289119</v>
       </c>
       <c r="D11">
-        <v>1.85690054965323E-05</v>
+        <v>2.210896317387241E-05</v>
       </c>
       <c r="E11">
-        <v>9.168575316995369E-06</v>
+        <v>2.103311528121684E-05</v>
       </c>
       <c r="F11">
-        <v>-0.009024320017351872</v>
+        <v>-0.05017806464506647</v>
       </c>
       <c r="G11">
-        <v>0.501787240222058</v>
+        <v>0.0009248228524665336</v>
       </c>
       <c r="H11">
-        <v>0.6230156929756394</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I11">
-        <v>49</v>
+        <v>11611</v>
       </c>
       <c r="J11">
-        <v>0.007217175147339313</v>
+        <v>0.0002098592232396584</v>
       </c>
       <c r="K11">
-        <v>0.002972419699024923</v>
+        <v>0.0001631540263502446</v>
       </c>
       <c r="L11">
-        <v>0.0001158352549329261</v>
+        <v>-0.01180186309853548</v>
       </c>
       <c r="M11">
-        <v>0.004529835290885987</v>
+        <v>0.005213165544267774</v>
       </c>
       <c r="N11">
-        <v>0.00129198945232948</v>
+        <v>0.001592932311570713</v>
       </c>
       <c r="O11">
-        <v>0.0003123469992588732</v>
+        <v>0.00173711317318318</v>
       </c>
       <c r="P11">
-        <v>-0.01652918306199047</v>
+        <v>0.004580501696160511</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1079,49 +1082,49 @@
         <v>26</v>
       </c>
       <c r="B12">
-        <v>0.009164293356549506</v>
+        <v>0.003491208235511574</v>
       </c>
       <c r="C12">
-        <v>0.008733878054388279</v>
+        <v>0.001329144946829925</v>
       </c>
       <c r="D12">
-        <v>0.0001865208677798922</v>
+        <v>1.85690054965323E-05</v>
       </c>
       <c r="E12">
-        <v>0.0001961492659581503</v>
+        <v>9.168575316995369E-06</v>
       </c>
       <c r="F12">
-        <v>0.1708507589293765</v>
+        <v>-0.009024320017351872</v>
       </c>
       <c r="G12">
-        <v>0.1280492261183164</v>
+        <v>0.501787240222058</v>
       </c>
       <c r="H12">
-        <v>0.2582640092197721</v>
+        <v>0.6230156929756394</v>
       </c>
       <c r="I12">
-        <v>14156</v>
+        <v>49</v>
       </c>
       <c r="J12">
-        <v>0.0102119158074488</v>
+        <v>0.0003123469992588732</v>
       </c>
       <c r="K12">
-        <v>0.005239736253559311</v>
+        <v>0.0001158352549329261</v>
       </c>
       <c r="L12">
-        <v>0.0003384092866814527</v>
+        <v>-0.01652918306199047</v>
       </c>
       <c r="M12">
-        <v>0.009674189396799987</v>
+        <v>0.007217175147339313</v>
       </c>
       <c r="N12">
-        <v>0.004818030126325817</v>
+        <v>0.00129198945232948</v>
       </c>
       <c r="O12">
-        <v>0.0004006378783650764</v>
+        <v>0.002972419699024923</v>
       </c>
       <c r="P12">
-        <v>0.1218694481841025</v>
+        <v>0.004529835290885987</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1129,49 +1132,49 @@
         <v>27</v>
       </c>
       <c r="B13">
-        <v>0.005611881407010991</v>
+        <v>0.009164293356549506</v>
       </c>
       <c r="C13">
-        <v>0.005639127357765789</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D13">
-        <v>8.431607544410066E-05</v>
+        <v>0.0001865208677798922</v>
       </c>
       <c r="E13">
-        <v>9.102681873913914E-05</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F13">
-        <v>0.291056300795216</v>
+        <v>0.1708507589293765</v>
       </c>
       <c r="G13">
-        <v>0.2346312460124846</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H13">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I13">
-        <v>6771</v>
+        <v>14156</v>
       </c>
       <c r="J13">
-        <v>0.00595976388177965</v>
+        <v>0.0004006378783650764</v>
       </c>
       <c r="K13">
-        <v>0.002972129451884979</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="L13">
-        <v>0.0001037297229528328</v>
+        <v>0.1218694481841025</v>
       </c>
       <c r="M13">
-        <v>0.005813234561065725</v>
+        <v>0.0102119158074488</v>
       </c>
       <c r="N13">
-        <v>0.003193202088483064</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="O13">
-        <v>0.0001424514975481683</v>
+        <v>0.005239736253559311</v>
       </c>
       <c r="P13">
-        <v>0.2046421514566161</v>
+        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1179,22 +1182,22 @@
         <v>28</v>
       </c>
       <c r="B14">
-        <v>0.005713567326092179</v>
+        <v>0.005611881407010991</v>
       </c>
       <c r="C14">
-        <v>0.005699109365498782</v>
+        <v>0.005639127357765789</v>
       </c>
       <c r="D14">
-        <v>8.903433264960941E-05</v>
+        <v>8.431607544410066E-05</v>
       </c>
       <c r="E14">
-        <v>9.470932808225897E-05</v>
+        <v>9.102681873913914E-05</v>
       </c>
       <c r="F14">
-        <v>0.3003097955821736</v>
+        <v>0.291056300795216</v>
       </c>
       <c r="G14">
-        <v>0.2557119579146814</v>
+        <v>0.2346312460124846</v>
       </c>
       <c r="H14">
         <v>0.4208397194991282</v>
@@ -1203,25 +1206,25 @@
         <v>6771</v>
       </c>
       <c r="J14">
-        <v>0.00592641693601841</v>
+        <v>0.0001424514975481683</v>
       </c>
       <c r="K14">
-        <v>0.003005755874836842</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="L14">
-        <v>0.0001037297229528328</v>
+        <v>0.2046421514566161</v>
       </c>
       <c r="M14">
-        <v>0.005813234561065725</v>
+        <v>0.00595976388177965</v>
       </c>
       <c r="N14">
         <v>0.003193202088483064</v>
       </c>
       <c r="O14">
-        <v>0.00013855240761432</v>
+        <v>0.002972129451884979</v>
       </c>
       <c r="P14">
-        <v>0.2264121702660996</v>
+        <v>0.005813234561065725</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1229,49 +1232,49 @@
         <v>29</v>
       </c>
       <c r="B15">
-        <v>0.007927365294981236</v>
+        <v>0.005713567326092179</v>
       </c>
       <c r="C15">
-        <v>0.008722720041403264</v>
+        <v>0.005699109365498782</v>
       </c>
       <c r="D15">
-        <v>0.000143672851475712</v>
+        <v>8.903433264960941E-05</v>
       </c>
       <c r="E15">
-        <v>0.0001985649052123504</v>
+        <v>9.470932808225897E-05</v>
       </c>
       <c r="F15">
-        <v>0.3830412447229715</v>
+        <v>0.3003097955821736</v>
       </c>
       <c r="G15">
-        <v>0.147324247391146</v>
+        <v>0.2557119579146814</v>
       </c>
       <c r="H15">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I15">
-        <v>14156</v>
+        <v>6771</v>
       </c>
       <c r="J15">
-        <v>0.008942022948316988</v>
+        <v>0.00013855240761432</v>
       </c>
       <c r="K15">
-        <v>0.004617426367895965</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="L15">
-        <v>0.0003384092866814527</v>
+        <v>0.2264121702660996</v>
       </c>
       <c r="M15">
-        <v>0.009674189396799985</v>
+        <v>0.00592641693601841</v>
       </c>
       <c r="N15">
-        <v>0.004818030126325817</v>
+        <v>0.003193202088483064</v>
       </c>
       <c r="O15">
-        <v>0.0003279955215444224</v>
+        <v>0.003005755874836842</v>
       </c>
       <c r="P15">
-        <v>0.2810892232598902</v>
+        <v>0.005813234561065725</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1279,49 +1282,49 @@
         <v>30</v>
       </c>
       <c r="B16">
-        <v>0.003031636244261009</v>
+        <v>0.007927365294981236</v>
       </c>
       <c r="C16">
-        <v>0.002499571894821071</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D16">
-        <v>1.91501667802569E-05</v>
+        <v>0.000143672851475712</v>
       </c>
       <c r="E16">
-        <v>1.967007435869721E-05</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F16">
-        <v>-0.01488433510101705</v>
+        <v>0.3830412447229715</v>
       </c>
       <c r="G16">
-        <v>-0.04243741404356438</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H16">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I16">
-        <v>11611</v>
+        <v>14156</v>
       </c>
       <c r="J16">
-        <v>0.005089153979501482</v>
+        <v>0.0003279955215444224</v>
       </c>
       <c r="K16">
-        <v>0.001554417436991534</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="L16">
-        <v>0.0001631540263502446</v>
+        <v>0.2810892232598902</v>
       </c>
       <c r="M16">
-        <v>0.004580501696160511</v>
+        <v>0.008942022948316988</v>
       </c>
       <c r="N16">
-        <v>0.001592932311570713</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="O16">
-        <v>0.0002083353057278959</v>
+        <v>0.004617426367895965</v>
       </c>
       <c r="P16">
-        <v>-0.004454544482717981</v>
+        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1329,49 +1332,49 @@
         <v>31</v>
       </c>
       <c r="B17">
-        <v>0.007781992577683896</v>
+        <v>0.003031636244261009</v>
       </c>
       <c r="C17">
-        <v>0.00859065864792076</v>
+        <v>0.002499571894821071</v>
       </c>
       <c r="D17">
-        <v>0.0001409300345186765</v>
+        <v>1.91501667802569E-05</v>
       </c>
       <c r="E17">
-        <v>0.0001927871917829494</v>
+        <v>1.967007435869721E-05</v>
       </c>
       <c r="F17">
-        <v>0.3590392616833861</v>
+        <v>-0.01488433510101705</v>
       </c>
       <c r="G17">
-        <v>0.1231888844332176</v>
+        <v>-0.04243741404356438</v>
       </c>
       <c r="H17">
-        <v>0.1607683912702015</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I17">
-        <v>12165</v>
+        <v>11611</v>
       </c>
       <c r="J17">
-        <v>0.008612572238732815</v>
+        <v>0.0002083353057278959</v>
       </c>
       <c r="K17">
-        <v>0.004522763064395587</v>
+        <v>0.0001631540263502446</v>
       </c>
       <c r="L17">
-        <v>0.0002898025533356035</v>
+        <v>-0.004454544482717981</v>
       </c>
       <c r="M17">
-        <v>0.009443827890009157</v>
+        <v>0.005089153979501482</v>
       </c>
       <c r="N17">
-        <v>0.004755169990739034</v>
+        <v>0.001592932311570713</v>
       </c>
       <c r="O17">
-        <v>0.000242169264872158</v>
+        <v>0.001554417436991534</v>
       </c>
       <c r="P17">
-        <v>0.2987083812604719</v>
+        <v>0.004580501696160511</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -1379,49 +1382,49 @@
         <v>32</v>
       </c>
       <c r="B18">
-        <v>0.003103990424644728</v>
+        <v>0.007930591965804838</v>
       </c>
       <c r="C18">
-        <v>0.00254141838673398</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D18">
-        <v>2.156002471405648E-05</v>
+        <v>0.0001447739509943206</v>
       </c>
       <c r="E18">
-        <v>2.106152912726658E-05</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F18">
-        <v>-0.02262657763782516</v>
+        <v>0.3783129123939393</v>
       </c>
       <c r="G18">
-        <v>0.001017868166272584</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H18">
-        <v>0.212555477012045</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I18">
-        <v>11542</v>
+        <v>14156</v>
       </c>
       <c r="J18">
-        <v>0.00510134746390362</v>
+        <v>0.0003287617791593521</v>
       </c>
       <c r="K18">
-        <v>0.001583264354559398</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="L18">
-        <v>0.000163888349337522</v>
+        <v>0.2794097160076624</v>
       </c>
       <c r="M18">
-        <v>0.004589584286176587</v>
+        <v>0.008948225748787574</v>
       </c>
       <c r="N18">
-        <v>0.001597174444307401</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="O18">
-        <v>0.0002091701444985722</v>
+        <v>0.004643473178262874</v>
       </c>
       <c r="P18">
-        <v>-0.005012774390606101</v>
+        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -1429,49 +1432,49 @@
         <v>33</v>
       </c>
       <c r="B19">
-        <v>0.00304699828992123</v>
+        <v>0.003103990424644728</v>
       </c>
       <c r="C19">
-        <v>0.002499571894821071</v>
+        <v>0.00254141838673398</v>
       </c>
       <c r="D19">
-        <v>1.903121423403654E-05</v>
+        <v>2.156002471405648E-05</v>
       </c>
       <c r="E19">
-        <v>1.967007435869721E-05</v>
+        <v>2.106152912726658E-05</v>
       </c>
       <c r="F19">
-        <v>-0.008580312939503454</v>
+        <v>-0.02262657763782516</v>
       </c>
       <c r="G19">
-        <v>-0.04243741404356438</v>
+        <v>0.001017868166272584</v>
       </c>
       <c r="H19">
-        <v>0.2133795918767654</v>
+        <v>0.212555477012045</v>
       </c>
       <c r="I19">
-        <v>11611</v>
+        <v>11542</v>
       </c>
       <c r="J19">
-        <v>0.005107549406927882</v>
+        <v>0.0002091701444985722</v>
       </c>
       <c r="K19">
-        <v>0.001554596452837835</v>
+        <v>0.000163888349337522</v>
       </c>
       <c r="L19">
-        <v>0.0001631540263502446</v>
+        <v>-0.005012774390606101</v>
       </c>
       <c r="M19">
-        <v>0.004580501696160511</v>
+        <v>0.00510134746390362</v>
       </c>
       <c r="N19">
-        <v>0.001592932311570713</v>
+        <v>0.001597174444307401</v>
       </c>
       <c r="O19">
-        <v>0.000207986162951978</v>
+        <v>0.001583264354559398</v>
       </c>
       <c r="P19">
-        <v>-0.002771209789547591</v>
+        <v>0.004589584286176587</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1479,49 +1482,49 @@
         <v>34</v>
       </c>
       <c r="B20">
-        <v>0.006549373422714545</v>
+        <v>0.00304699828992123</v>
       </c>
       <c r="C20">
-        <v>0.005670204101840715</v>
+        <v>0.002499571894821071</v>
       </c>
       <c r="D20">
-        <v>0.0001064697656049724</v>
+        <v>1.903121423403654E-05</v>
       </c>
       <c r="E20">
-        <v>9.344840654260834E-05</v>
+        <v>1.967007435869721E-05</v>
       </c>
       <c r="F20">
-        <v>0.1346849985258249</v>
+        <v>-0.008580312939503454</v>
       </c>
       <c r="G20">
-        <v>0.2405138906269937</v>
+        <v>-0.04243741404356438</v>
       </c>
       <c r="H20">
-        <v>0.4208397194991282</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I20">
-        <v>6771</v>
+        <v>11611</v>
       </c>
       <c r="J20">
-        <v>0.006776662396495037</v>
+        <v>0.000207986162951978</v>
       </c>
       <c r="K20">
-        <v>0.003715325925925931</v>
+        <v>0.0001631540263502446</v>
       </c>
       <c r="L20">
-        <v>0.0001037297229528328</v>
+        <v>-0.002771209789547591</v>
       </c>
       <c r="M20">
-        <v>0.005813234561065723</v>
+        <v>0.005107549406927882</v>
       </c>
       <c r="N20">
-        <v>0.003193202088483064</v>
+        <v>0.001592932311570713</v>
       </c>
       <c r="O20">
-        <v>0.000160150142460433</v>
+        <v>0.001554596452837835</v>
       </c>
       <c r="P20">
-        <v>0.1058242633905934</v>
+        <v>0.004580501696160511</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1529,49 +1532,49 @@
         <v>35</v>
       </c>
       <c r="B21">
-        <v>0.002783525716284511</v>
+        <v>0.006549373422714545</v>
       </c>
       <c r="C21">
-        <v>0.002457544020376962</v>
+        <v>0.005670204101840715</v>
       </c>
       <c r="D21">
-        <v>1.713865210259099E-05</v>
+        <v>0.0001064697656049724</v>
       </c>
       <c r="E21">
-        <v>1.89022549270271E-05</v>
+        <v>9.344840654260834E-05</v>
       </c>
       <c r="F21">
-        <v>-0.05370835704473098</v>
+        <v>0.1346849985258249</v>
       </c>
       <c r="G21">
-        <v>-0.1621371309933592</v>
+        <v>0.2405138906269937</v>
       </c>
       <c r="H21">
-        <v>0.3649062991209757</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I21">
-        <v>4010</v>
+        <v>6771</v>
       </c>
       <c r="J21">
-        <v>0.004501420066184821</v>
+        <v>0.000160150142460433</v>
       </c>
       <c r="K21">
-        <v>0.001362431751651251</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="L21">
-        <v>0.0001730864695810989</v>
+        <v>0.1058242633905934</v>
       </c>
       <c r="M21">
-        <v>0.004349183403839366</v>
+        <v>0.006776662396495037</v>
       </c>
       <c r="N21">
-        <v>0.001438312583710056</v>
+        <v>0.003193202088483064</v>
       </c>
       <c r="O21">
-        <v>0.0002742305932959652</v>
+        <v>0.003715325925925931</v>
       </c>
       <c r="P21">
-        <v>-0.006214540120261569</v>
+        <v>0.005813234561065723</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1579,49 +1582,49 @@
         <v>36</v>
       </c>
       <c r="B22">
-        <v>0.00929322862430519</v>
+        <v>0.002783525716284511</v>
       </c>
       <c r="C22">
-        <v>0.008733878054388279</v>
+        <v>0.002457544020376962</v>
       </c>
       <c r="D22">
-        <v>0.000192984991667648</v>
+        <v>1.713865210259099E-05</v>
       </c>
       <c r="E22">
-        <v>0.0001961492659581503</v>
+        <v>1.89022549270271E-05</v>
       </c>
       <c r="F22">
-        <v>0.1421155108066621</v>
+        <v>-0.05370835704473098</v>
       </c>
       <c r="G22">
-        <v>0.1280492261183164</v>
+        <v>-0.1621371309933592</v>
       </c>
       <c r="H22">
-        <v>0.2582640092197721</v>
+        <v>0.3649062991209757</v>
       </c>
       <c r="I22">
-        <v>14156</v>
+        <v>4010</v>
       </c>
       <c r="J22">
-        <v>0.01035431191953904</v>
+        <v>0.0002742305932959652</v>
       </c>
       <c r="K22">
-        <v>0.005409147625572685</v>
+        <v>0.0001730864695810989</v>
       </c>
       <c r="L22">
-        <v>0.0003384092866814527</v>
+        <v>-0.006214540120261569</v>
       </c>
       <c r="M22">
-        <v>0.009674189396799987</v>
+        <v>0.004501420066184821</v>
       </c>
       <c r="N22">
-        <v>0.004818030126325817</v>
+        <v>0.001438312583710056</v>
       </c>
       <c r="O22">
-        <v>0.0004001063569688302</v>
+        <v>0.001362431751651251</v>
       </c>
       <c r="P22">
-        <v>0.1230344532976788</v>
+        <v>0.004349183403839366</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1629,49 +1632,49 @@
         <v>37</v>
       </c>
       <c r="B23">
-        <v>0.003030458698074221</v>
+        <v>0.00929322862430519</v>
       </c>
       <c r="C23">
-        <v>0.002499571894821071</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D23">
-        <v>1.91281128971015E-05</v>
+        <v>0.000192984991667648</v>
       </c>
       <c r="E23">
-        <v>1.967007435869721E-05</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F23">
-        <v>-0.01371556509502225</v>
+        <v>0.1421155108066621</v>
       </c>
       <c r="G23">
-        <v>-0.04243741404356438</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H23">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I23">
-        <v>11611</v>
+        <v>14156</v>
       </c>
       <c r="J23">
-        <v>0.005089488294347637</v>
+        <v>0.0004001063569688302</v>
       </c>
       <c r="K23">
-        <v>0.001547174514616301</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="L23">
-        <v>0.0001631540263502446</v>
+        <v>0.1230344532976788</v>
       </c>
       <c r="M23">
-        <v>0.004580501696160511</v>
+        <v>0.01035431191953904</v>
       </c>
       <c r="N23">
-        <v>0.001592932311570713</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="O23">
-        <v>0.0002081444394071696</v>
+        <v>0.005409147625572685</v>
       </c>
       <c r="P23">
-        <v>-0.00353431378743374</v>
+        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -1679,49 +1682,49 @@
         <v>38</v>
       </c>
       <c r="B24">
-        <v>0.008532806478705164</v>
+        <v>0.003030458698074221</v>
       </c>
       <c r="C24">
-        <v>0.008733878054388279</v>
+        <v>0.002499571894821071</v>
       </c>
       <c r="D24">
-        <v>0.0001656454412935777</v>
+        <v>1.91281128971015E-05</v>
       </c>
       <c r="E24">
-        <v>0.0001961492659581503</v>
+        <v>1.967007435869721E-05</v>
       </c>
       <c r="F24">
-        <v>0.2636491907304709</v>
+        <v>-0.01371556509502225</v>
       </c>
       <c r="G24">
-        <v>0.1280492261183164</v>
+        <v>-0.04243741404356438</v>
       </c>
       <c r="H24">
-        <v>0.2582640092197721</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I24">
-        <v>14156</v>
+        <v>11611</v>
       </c>
       <c r="J24">
-        <v>0.009554445336689437</v>
+        <v>0.0002081444394071696</v>
       </c>
       <c r="K24">
-        <v>0.004730871750625608</v>
+        <v>0.0001631540263502446</v>
       </c>
       <c r="L24">
-        <v>0.0003384092866814527</v>
+        <v>-0.00353431378743374</v>
       </c>
       <c r="M24">
-        <v>0.009674189396799987</v>
+        <v>0.005089488294347637</v>
       </c>
       <c r="N24">
-        <v>0.004818030126325817</v>
+        <v>0.001592932311570713</v>
       </c>
       <c r="O24">
-        <v>0.0003744000227958637</v>
+        <v>0.001547174514616301</v>
       </c>
       <c r="P24">
-        <v>0.179378395374721</v>
+        <v>0.004580501696160511</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -1729,19 +1732,19 @@
         <v>39</v>
       </c>
       <c r="B25">
-        <v>0.008529233938818522</v>
+        <v>0.008532806478705164</v>
       </c>
       <c r="C25">
         <v>0.008733878054388279</v>
       </c>
       <c r="D25">
-        <v>0.0001653251466070655</v>
+        <v>0.0001656454412935777</v>
       </c>
       <c r="E25">
         <v>0.0001961492659581503</v>
       </c>
       <c r="F25">
-        <v>0.2650730104853413</v>
+        <v>0.2636491907304709</v>
       </c>
       <c r="G25">
         <v>0.1280492261183164</v>
@@ -1753,25 +1756,25 @@
         <v>14156</v>
       </c>
       <c r="J25">
-        <v>0.009555217528480035</v>
+        <v>0.0003744000227958637</v>
       </c>
       <c r="K25">
-        <v>0.004764640177213803</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="L25">
-        <v>0.0003384092866814527</v>
+        <v>0.179378395374721</v>
       </c>
       <c r="M25">
-        <v>0.009674189396799987</v>
+        <v>0.009554445336689437</v>
       </c>
       <c r="N25">
         <v>0.004818030126325817</v>
       </c>
       <c r="O25">
-        <v>0.0003746361399868205</v>
+        <v>0.004730871750625608</v>
       </c>
       <c r="P25">
-        <v>0.1788608663781261</v>
+        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -1779,19 +1782,19 @@
         <v>40</v>
       </c>
       <c r="B26">
-        <v>0.008505250051591662</v>
+        <v>0.008529233938818522</v>
       </c>
       <c r="C26">
         <v>0.008733878054388279</v>
       </c>
       <c r="D26">
-        <v>0.0001646168902522808</v>
+        <v>0.0001653251466070655</v>
       </c>
       <c r="E26">
         <v>0.0001961492659581503</v>
       </c>
       <c r="F26">
-        <v>0.268221452941368</v>
+        <v>0.2650730104853413</v>
       </c>
       <c r="G26">
         <v>0.1280492261183164</v>
@@ -1803,25 +1806,25 @@
         <v>14156</v>
       </c>
       <c r="J26">
-        <v>0.009526287265811475</v>
+        <v>0.0003746361399868205</v>
       </c>
       <c r="K26">
-        <v>0.004756476812602748</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="L26">
-        <v>0.0003384092866814527</v>
+        <v>0.1788608663781261</v>
       </c>
       <c r="M26">
-        <v>0.009674189396799987</v>
+        <v>0.009555217528480035</v>
       </c>
       <c r="N26">
         <v>0.004818030126325817</v>
       </c>
       <c r="O26">
-        <v>0.0003736225585176234</v>
+        <v>0.004764640177213803</v>
       </c>
       <c r="P26">
-        <v>0.1810824657398455</v>
+        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -1829,49 +1832,49 @@
         <v>41</v>
       </c>
       <c r="B27">
-        <v>0.006299187529923155</v>
+        <v>0.008505250051591662</v>
       </c>
       <c r="C27">
-        <v>0.00553167406053466</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D27">
-        <v>9.00395869891457E-05</v>
+        <v>0.0001646168902522808</v>
       </c>
       <c r="E27">
-        <v>8.170381435551846E-05</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F27">
-        <v>0.1391419988807219</v>
+        <v>0.268221452941368</v>
       </c>
       <c r="G27">
-        <v>0.2188393498696173</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H27">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I27">
-        <v>6771</v>
+        <v>14156</v>
       </c>
       <c r="J27">
-        <v>0.00674135934653288</v>
+        <v>0.0003736225585176234</v>
       </c>
       <c r="K27">
-        <v>0.003667719421830667</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="L27">
-        <v>0.0001037297229528328</v>
+        <v>0.1810824657398455</v>
       </c>
       <c r="M27">
-        <v>0.005813234561065723</v>
+        <v>0.009526287265811475</v>
       </c>
       <c r="N27">
-        <v>0.003193202088483064</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="O27">
-        <v>0.0001603751212724098</v>
+        <v>0.004756476812602748</v>
       </c>
       <c r="P27">
-        <v>0.1045681259196538</v>
+        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -1879,49 +1882,49 @@
         <v>42</v>
       </c>
       <c r="B28">
-        <v>0.00869522801124366</v>
+        <v>0.006299187529923155</v>
       </c>
       <c r="C28">
-        <v>0.008722720041403264</v>
+        <v>0.00553167406053466</v>
       </c>
       <c r="D28">
-        <v>0.0001671499749450426</v>
+        <v>9.00395869891457E-05</v>
       </c>
       <c r="E28">
-        <v>0.0001985649052123504</v>
+        <v>8.170381435551846E-05</v>
       </c>
       <c r="F28">
-        <v>0.2822259777859754</v>
+        <v>0.1391419988807219</v>
       </c>
       <c r="G28">
-        <v>0.147324247391146</v>
+        <v>0.2188393498696173</v>
       </c>
       <c r="H28">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I28">
-        <v>14156</v>
+        <v>6771</v>
       </c>
       <c r="J28">
-        <v>0.009719161233546112</v>
+        <v>0.0001603751212724098</v>
       </c>
       <c r="K28">
-        <v>0.005173194757001598</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="L28">
-        <v>0.0003384092866814527</v>
+        <v>0.1045681259196538</v>
       </c>
       <c r="M28">
-        <v>0.009674189396799985</v>
+        <v>0.00674135934653288</v>
       </c>
       <c r="N28">
-        <v>0.004818030126325817</v>
+        <v>0.003193202088483064</v>
       </c>
       <c r="O28">
-        <v>0.0003635971635380399</v>
+        <v>0.003667719421830667</v>
       </c>
       <c r="P28">
-        <v>0.2030564380000814</v>
+        <v>0.005813234561065723</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -1929,19 +1932,19 @@
         <v>43</v>
       </c>
       <c r="B29">
-        <v>0.007668256776450208</v>
+        <v>0.00869522801124366</v>
       </c>
       <c r="C29">
         <v>0.008722720041403264</v>
       </c>
       <c r="D29">
-        <v>0.0001436777206558706</v>
+        <v>0.0001671499749450426</v>
       </c>
       <c r="E29">
         <v>0.0001985649052123504</v>
       </c>
       <c r="F29">
-        <v>0.3830203355303232</v>
+        <v>0.2822259777859754</v>
       </c>
       <c r="G29">
         <v>0.147324247391146</v>
@@ -1953,25 +1956,25 @@
         <v>14156</v>
       </c>
       <c r="J29">
-        <v>0.00867861064019221</v>
+        <v>0.0003635971635380399</v>
       </c>
       <c r="K29">
-        <v>0.004128330862335852</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="L29">
-        <v>0.0003384092866814527</v>
+        <v>0.2030564380000814</v>
       </c>
       <c r="M29">
-        <v>0.009674189396799985</v>
+        <v>0.009719161233546112</v>
       </c>
       <c r="N29">
         <v>0.004818030126325817</v>
       </c>
       <c r="O29">
-        <v>0.0003344607981243851</v>
+        <v>0.005173194757001598</v>
       </c>
       <c r="P29">
-        <v>0.2669184291403396</v>
+        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -1979,19 +1982,19 @@
         <v>44</v>
       </c>
       <c r="B30">
-        <v>0.00958912348219286</v>
+        <v>0.007668256776450208</v>
       </c>
       <c r="C30">
         <v>0.008722720041403264</v>
       </c>
       <c r="D30">
-        <v>0.00021842684931279</v>
+        <v>0.0001436777206558706</v>
       </c>
       <c r="E30">
         <v>0.0001985649052123504</v>
       </c>
       <c r="F30">
-        <v>0.06203325341612431</v>
+        <v>0.3830203355303232</v>
       </c>
       <c r="G30">
         <v>0.147324247391146</v>
@@ -2003,25 +2006,25 @@
         <v>14156</v>
       </c>
       <c r="J30">
-        <v>0.01064772150300563</v>
+        <v>0.0003344607981243851</v>
       </c>
       <c r="K30">
-        <v>0.005560650653515711</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="L30">
-        <v>0.0003384092866814527</v>
+        <v>0.2669184291403396</v>
       </c>
       <c r="M30">
-        <v>0.009674189396799985</v>
+        <v>0.00867861064019221</v>
       </c>
       <c r="N30">
         <v>0.004818030126325817</v>
       </c>
       <c r="O30">
-        <v>0.0004313797729252501</v>
+        <v>0.004128330862335852</v>
       </c>
       <c r="P30">
-        <v>0.05448840836791147</v>
+        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -2029,49 +2032,49 @@
         <v>45</v>
       </c>
       <c r="B31">
-        <v>0.005743153097997238</v>
+        <v>0.00958912348219286</v>
       </c>
       <c r="C31">
-        <v>0.005699109365498782</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D31">
-        <v>9.179016309205035E-05</v>
+        <v>0.00021842684931279</v>
       </c>
       <c r="E31">
-        <v>9.470932808225897E-05</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F31">
-        <v>0.2786526717712858</v>
+        <v>0.06203325341612431</v>
       </c>
       <c r="G31">
-        <v>0.2557119579146814</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H31">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I31">
-        <v>6771</v>
+        <v>14156</v>
       </c>
       <c r="J31">
-        <v>0.00595976388177965</v>
+        <v>0.0004313797729252501</v>
       </c>
       <c r="K31">
-        <v>0.002972129451884979</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="L31">
-        <v>0.0001037297229528328</v>
+        <v>0.05448840836791147</v>
       </c>
       <c r="M31">
-        <v>0.005813234561065725</v>
+        <v>0.01064772150300563</v>
       </c>
       <c r="N31">
-        <v>0.003193202088483064</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="O31">
-        <v>0.0001424514975481683</v>
+        <v>0.005560650653515711</v>
       </c>
       <c r="P31">
-        <v>0.2046421514566161</v>
+        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -2079,49 +2082,49 @@
         <v>46</v>
       </c>
       <c r="B32">
-        <v>0.009301347310769852</v>
+        <v>0.005743153097997238</v>
       </c>
       <c r="C32">
-        <v>0.008733878054388279</v>
+        <v>0.005699109365498782</v>
       </c>
       <c r="D32">
-        <v>0.0001883109214593075</v>
+        <v>9.179016309205035E-05</v>
       </c>
       <c r="E32">
-        <v>0.0001961492659581503</v>
+        <v>9.470932808225897E-05</v>
       </c>
       <c r="F32">
-        <v>0.1628933562675233</v>
+        <v>0.2786526717712858</v>
       </c>
       <c r="G32">
-        <v>0.1280492261183164</v>
+        <v>0.2557119579146814</v>
       </c>
       <c r="H32">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I32">
-        <v>14156</v>
+        <v>6771</v>
       </c>
       <c r="J32">
-        <v>0.01035467890006862</v>
+        <v>0.0001424514975481683</v>
       </c>
       <c r="K32">
-        <v>0.005399385735558927</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="L32">
-        <v>0.0003384092866814527</v>
+        <v>0.2046421514566161</v>
       </c>
       <c r="M32">
-        <v>0.009674189396799987</v>
+        <v>0.00595976388177965</v>
       </c>
       <c r="N32">
-        <v>0.004818030126325817</v>
+        <v>0.003193202088483064</v>
       </c>
       <c r="O32">
-        <v>0.0004026104577395279</v>
+        <v>0.002972129451884979</v>
       </c>
       <c r="P32">
-        <v>0.1175458874123242</v>
+        <v>0.005813234561065725</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -2129,49 +2132,49 @@
         <v>47</v>
       </c>
       <c r="B33">
-        <v>0.00303210497017975</v>
+        <v>0.009301347310769852</v>
       </c>
       <c r="C33">
-        <v>0.002499571894821071</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D33">
-        <v>1.909735738640315E-05</v>
+        <v>0.0001883109214593075</v>
       </c>
       <c r="E33">
-        <v>1.967007435869721E-05</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F33">
-        <v>-0.0120856426831728</v>
+        <v>0.1628933562675233</v>
       </c>
       <c r="G33">
-        <v>-0.04243741404356438</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H33">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I33">
-        <v>11611</v>
+        <v>14156</v>
       </c>
       <c r="J33">
-        <v>0.005090949099942899</v>
+        <v>0.0004026104577395279</v>
       </c>
       <c r="K33">
-        <v>0.001550051802718652</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="L33">
-        <v>0.0001631540263502446</v>
+        <v>0.1175458874123242</v>
       </c>
       <c r="M33">
-        <v>0.004580501696160511</v>
+        <v>0.01035467890006862</v>
       </c>
       <c r="N33">
-        <v>0.001592932311570713</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="O33">
-        <v>0.0002080153046483946</v>
+        <v>0.005399385735558927</v>
       </c>
       <c r="P33">
-        <v>-0.002911711704464803</v>
+        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -2179,49 +2182,99 @@
         <v>48</v>
       </c>
       <c r="B34">
+        <v>0.00303210497017975</v>
+      </c>
+      <c r="C34">
+        <v>0.002499571894821071</v>
+      </c>
+      <c r="D34">
+        <v>1.909735738640315E-05</v>
+      </c>
+      <c r="E34">
+        <v>1.967007435869721E-05</v>
+      </c>
+      <c r="F34">
+        <v>-0.0120856426831728</v>
+      </c>
+      <c r="G34">
+        <v>-0.04243741404356438</v>
+      </c>
+      <c r="H34">
+        <v>0.2133795918767654</v>
+      </c>
+      <c r="I34">
+        <v>11611</v>
+      </c>
+      <c r="J34">
+        <v>0.0002080153046483946</v>
+      </c>
+      <c r="K34">
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="L34">
+        <v>-0.002911711704464803</v>
+      </c>
+      <c r="M34">
+        <v>0.005090949099942899</v>
+      </c>
+      <c r="N34">
+        <v>0.001592932311570713</v>
+      </c>
+      <c r="O34">
+        <v>0.001550051802718652</v>
+      </c>
+      <c r="P34">
+        <v>0.004580501696160511</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35">
         <v>0.008142928261746932</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <v>0.008733878054388279</v>
       </c>
-      <c r="D34">
+      <c r="D35">
         <v>0.0001648112327367591</v>
       </c>
-      <c r="E34">
+      <c r="E35">
         <v>0.0001961492659581503</v>
       </c>
-      <c r="F34">
+      <c r="F35">
         <v>0.2673575339309593</v>
       </c>
-      <c r="G34">
+      <c r="G35">
         <v>0.1280492261183164</v>
       </c>
-      <c r="H34">
+      <c r="H35">
         <v>0.2582640092197721</v>
       </c>
-      <c r="I34">
+      <c r="I35">
         <v>14156</v>
       </c>
-      <c r="J34">
+      <c r="J35">
+        <v>0.0003438074749231005</v>
+      </c>
+      <c r="K35">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="L35">
+        <v>0.2464320924804251</v>
+      </c>
+      <c r="M35">
         <v>0.009263751492683912</v>
       </c>
-      <c r="K34">
+      <c r="N35">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="O35">
         <v>0.004666820467017538</v>
       </c>
-      <c r="L34">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="M34">
+      <c r="P35">
         <v>0.009674189396799987</v>
-      </c>
-      <c r="N34">
-        <v>0.004818030126325817</v>
-      </c>
-      <c r="O34">
-        <v>0.0003438074749231005</v>
-      </c>
-      <c r="P34">
-        <v>0.2464320924804251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update lgbm new config I - random half
</commit_message>
<xml_diff>
--- a/results_analysis/compare_with_ibes/#compare_all.xlsx
+++ b/results_analysis/compare_with_ibes/#compare_all.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>lgbm_mae</t>
   </si>
@@ -40,39 +40,39 @@
     <t>len</t>
   </si>
   <si>
+    <t>lgbm_r2_org</t>
+  </si>
+  <si>
+    <t>lgbm_mse_org</t>
+  </si>
+  <si>
+    <t>consensus_mae_eps</t>
+  </si>
+  <si>
+    <t>consensus_mse_org</t>
+  </si>
+  <si>
+    <t>lgbm_medae_org</t>
+  </si>
+  <si>
     <t>consensus_mae_org</t>
   </si>
   <si>
-    <t>consensus_mse_org</t>
-  </si>
-  <si>
-    <t>consensus_mae_eps</t>
+    <t>lgbm_mae_eps</t>
+  </si>
+  <si>
+    <t>lgbm_mae_org</t>
   </si>
   <si>
     <t>consensus_mape_eps</t>
   </si>
   <si>
+    <t>lgbm_mape_eps</t>
+  </si>
+  <si>
     <t>consensus_medae_org</t>
   </si>
   <si>
-    <t>lgbm_mape_eps</t>
-  </si>
-  <si>
-    <t>lgbm_r2_org</t>
-  </si>
-  <si>
-    <t>lgbm_mse_org</t>
-  </si>
-  <si>
-    <t>lgbm_medae_org</t>
-  </si>
-  <si>
-    <t>lgbm_mae_org</t>
-  </si>
-  <si>
-    <t>lgbm_mae_eps</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>ibes_2|ni|ibes_new industry_all x -mse</t>
+  </si>
+  <si>
+    <t>ibes_2|fwdepsqcut|rounding_ind_ex</t>
   </si>
   <si>
     <t>ibes_1|fwdepsqcut|ibes_entire_only ws -smaller space</t>
@@ -566,7 +569,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T46"/>
+  <dimension ref="A1:T47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -663,25 +666,25 @@
         <v>14156</v>
       </c>
       <c r="J2">
+        <v>0.06836645151013176</v>
+      </c>
+      <c r="K2">
+        <v>0.0004250480609163007</v>
+      </c>
+      <c r="M2">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="N2">
+        <v>0.005638666708596741</v>
+      </c>
+      <c r="O2">
         <v>0.009674189396799987</v>
       </c>
-      <c r="K2">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N2">
+      <c r="Q2">
+        <v>0.01071193221870467</v>
+      </c>
+      <c r="T2">
         <v>0.004818030126325816</v>
-      </c>
-      <c r="P2">
-        <v>0.06836645151013176</v>
-      </c>
-      <c r="Q2">
-        <v>0.0004250480609163007</v>
-      </c>
-      <c r="R2">
-        <v>0.005638666708596741</v>
-      </c>
-      <c r="S2">
-        <v>0.01071193221870467</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -713,25 +716,25 @@
         <v>11611</v>
       </c>
       <c r="J3">
+        <v>0.04615441883950755</v>
+      </c>
+      <c r="K3">
+        <v>0.0001978384306784256</v>
+      </c>
+      <c r="M3">
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="N3">
+        <v>0.001779221775169934</v>
+      </c>
+      <c r="O3">
         <v>0.004580501696160511</v>
       </c>
-      <c r="K3">
-        <v>0.0001631540263502446</v>
-      </c>
-      <c r="N3">
+      <c r="Q3">
+        <v>0.00502885184437347</v>
+      </c>
+      <c r="T3">
         <v>0.001592932311570713</v>
-      </c>
-      <c r="P3">
-        <v>0.04615441883950755</v>
-      </c>
-      <c r="Q3">
-        <v>0.0001978384306784256</v>
-      </c>
-      <c r="R3">
-        <v>0.001779221775169934</v>
-      </c>
-      <c r="S3">
-        <v>0.00502885184437347</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -763,25 +766,25 @@
         <v>6771</v>
       </c>
       <c r="J4">
+        <v>0.36470746642943</v>
+      </c>
+      <c r="K4">
+        <v>0.0001137832146297872</v>
+      </c>
+      <c r="M4">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="N4">
+        <v>0.003094044369724517</v>
+      </c>
+      <c r="O4">
         <v>0.005813234561065725</v>
       </c>
-      <c r="K4">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N4">
+      <c r="Q4">
+        <v>0.005606434133779571</v>
+      </c>
+      <c r="T4">
         <v>0.003193202088483064</v>
-      </c>
-      <c r="P4">
-        <v>0.36470746642943</v>
-      </c>
-      <c r="Q4">
-        <v>0.0001137832146297872</v>
-      </c>
-      <c r="R4">
-        <v>0.003094044369724517</v>
-      </c>
-      <c r="S4">
-        <v>0.005606434133779571</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -813,25 +816,25 @@
         <v>6771</v>
       </c>
       <c r="J5">
+        <v>0.3564407544954944</v>
+      </c>
+      <c r="K5">
+        <v>0.0001152638129503358</v>
+      </c>
+      <c r="M5">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="N5">
+        <v>0.003171635367762127</v>
+      </c>
+      <c r="O5">
         <v>0.005813234561065725</v>
       </c>
-      <c r="K5">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N5">
+      <c r="Q5">
+        <v>0.005632685300523813</v>
+      </c>
+      <c r="T5">
         <v>0.003193202088483064</v>
-      </c>
-      <c r="P5">
-        <v>0.3564407544954944</v>
-      </c>
-      <c r="Q5">
-        <v>0.0001152638129503358</v>
-      </c>
-      <c r="R5">
-        <v>0.003171635367762127</v>
-      </c>
-      <c r="S5">
-        <v>0.005632685300523813</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -863,25 +866,25 @@
         <v>42468</v>
       </c>
       <c r="J6">
+        <v>0.269966598412229</v>
+      </c>
+      <c r="K6">
+        <v>0.000333070102780211</v>
+      </c>
+      <c r="M6">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="N6">
+        <v>0.004616722796530505</v>
+      </c>
+      <c r="O6">
         <v>0.009674189396799987</v>
       </c>
-      <c r="K6">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N6">
+      <c r="Q6">
+        <v>0.009106885821888167</v>
+      </c>
+      <c r="T6">
         <v>0.004818030126325817</v>
-      </c>
-      <c r="P6">
-        <v>0.269966598412229</v>
-      </c>
-      <c r="Q6">
-        <v>0.000333070102780211</v>
-      </c>
-      <c r="R6">
-        <v>0.004616722796530505</v>
-      </c>
-      <c r="S6">
-        <v>0.009106885821888167</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -913,25 +916,25 @@
         <v>14156</v>
       </c>
       <c r="J7">
+        <v>0.2798459788092014</v>
+      </c>
+      <c r="K7">
+        <v>0.0003285627388197843</v>
+      </c>
+      <c r="M7">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="N7">
+        <v>0.004615286290830784</v>
+      </c>
+      <c r="O7">
         <v>0.009674189396799985</v>
       </c>
-      <c r="K7">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N7">
+      <c r="Q7">
+        <v>0.008950010380536522</v>
+      </c>
+      <c r="T7">
         <v>0.004818030126325817</v>
-      </c>
-      <c r="P7">
-        <v>0.2798459788092014</v>
-      </c>
-      <c r="Q7">
-        <v>0.0003285627388197843</v>
-      </c>
-      <c r="R7">
-        <v>0.004615286290830784</v>
-      </c>
-      <c r="S7">
-        <v>0.008950010380536522</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -963,25 +966,25 @@
         <v>14156</v>
       </c>
       <c r="J8">
+        <v>0.1860837943045432</v>
+      </c>
+      <c r="K8">
+        <v>0.0003713407546776094</v>
+      </c>
+      <c r="M8">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="N8">
+        <v>0.004590555422836876</v>
+      </c>
+      <c r="O8">
         <v>0.009674189396799985</v>
       </c>
-      <c r="K8">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N8">
+      <c r="Q8">
+        <v>0.00941140169945745</v>
+      </c>
+      <c r="T8">
         <v>0.004818030126325816</v>
-      </c>
-      <c r="P8">
-        <v>0.1860837943045432</v>
-      </c>
-      <c r="Q8">
-        <v>0.0003713407546776094</v>
-      </c>
-      <c r="R8">
-        <v>0.004590555422836876</v>
-      </c>
-      <c r="S8">
-        <v>0.00941140169945745</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -1013,25 +1016,25 @@
         <v>24768</v>
       </c>
       <c r="J9">
+        <v>-0.00724317687482956</v>
+      </c>
+      <c r="K9">
+        <v>0.0002632414236722758</v>
+      </c>
+      <c r="M9">
+        <v>0.0001796235360933539</v>
+      </c>
+      <c r="N9">
+        <v>0.004275415213561056</v>
+      </c>
+      <c r="O9">
         <v>0.006875190708555331</v>
       </c>
-      <c r="K9">
-        <v>0.0001796235360933539</v>
-      </c>
-      <c r="N9">
+      <c r="Q9">
+        <v>0.008363098231375462</v>
+      </c>
+      <c r="T9">
         <v>0.003559726400188349</v>
-      </c>
-      <c r="P9">
-        <v>-0.00724317687482956</v>
-      </c>
-      <c r="Q9">
-        <v>0.0002632414236722758</v>
-      </c>
-      <c r="R9">
-        <v>0.004275415213561056</v>
-      </c>
-      <c r="S9">
-        <v>0.008363098231375462</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -1063,25 +1066,25 @@
         <v>14156</v>
       </c>
       <c r="J10">
+        <v>0.1565886089862186</v>
+      </c>
+      <c r="K10">
+        <v>0.0003847976244374441</v>
+      </c>
+      <c r="M10">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="N10">
+        <v>0.005167135423672592</v>
+      </c>
+      <c r="O10">
         <v>0.009674189396799985</v>
       </c>
-      <c r="K10">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N10">
+      <c r="Q10">
+        <v>0.009901025034115019</v>
+      </c>
+      <c r="T10">
         <v>0.004818030126325817</v>
-      </c>
-      <c r="P10">
-        <v>0.1565886089862186</v>
-      </c>
-      <c r="Q10">
-        <v>0.0003847976244374441</v>
-      </c>
-      <c r="R10">
-        <v>0.005167135423672592</v>
-      </c>
-      <c r="S10">
-        <v>0.009901025034115019</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1113,25 +1116,25 @@
         <v>11542</v>
       </c>
       <c r="J11">
+        <v>-0.005102592401121431</v>
+      </c>
+      <c r="K11">
+        <v>0.000209188838038313</v>
+      </c>
+      <c r="M11">
+        <v>0.000163888349337522</v>
+      </c>
+      <c r="N11">
+        <v>0.001602037466360856</v>
+      </c>
+      <c r="O11">
         <v>0.004589584286176587</v>
       </c>
-      <c r="K11">
-        <v>0.000163888349337522</v>
-      </c>
-      <c r="N11">
+      <c r="Q11">
+        <v>0.00512210974064752</v>
+      </c>
+      <c r="T11">
         <v>0.001597174444307401</v>
-      </c>
-      <c r="P11">
-        <v>-0.005102592401121431</v>
-      </c>
-      <c r="Q11">
-        <v>0.000209188838038313</v>
-      </c>
-      <c r="R11">
-        <v>0.001602037466360856</v>
-      </c>
-      <c r="S11">
-        <v>0.00512210974064752</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -1163,25 +1166,25 @@
         <v>6771</v>
       </c>
       <c r="J12">
+        <v>0.3693483364419842</v>
+      </c>
+      <c r="K12">
+        <v>0.000112952017849086</v>
+      </c>
+      <c r="M12">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="N12">
+        <v>0.002682213716882752</v>
+      </c>
+      <c r="O12">
         <v>0.005813234561065725</v>
       </c>
-      <c r="K12">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N12">
+      <c r="Q12">
+        <v>0.00526064949972486</v>
+      </c>
+      <c r="T12">
         <v>0.003193202088483064</v>
-      </c>
-      <c r="P12">
-        <v>0.3693483364419842</v>
-      </c>
-      <c r="Q12">
-        <v>0.000112952017849086</v>
-      </c>
-      <c r="R12">
-        <v>0.002682213716882752</v>
-      </c>
-      <c r="S12">
-        <v>0.00526064949972486</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -1213,25 +1216,25 @@
         <v>6771</v>
       </c>
       <c r="J13">
+        <v>0.2122246979933391</v>
+      </c>
+      <c r="K13">
+        <v>0.0001410934357507483</v>
+      </c>
+      <c r="M13">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="N13">
+        <v>0.003030311329129174</v>
+      </c>
+      <c r="O13">
         <v>0.005813234561065723</v>
       </c>
-      <c r="K13">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N13">
+      <c r="Q13">
+        <v>0.006002887168865449</v>
+      </c>
+      <c r="T13">
         <v>0.003193202088483064</v>
-      </c>
-      <c r="P13">
-        <v>0.2122246979933391</v>
-      </c>
-      <c r="Q13">
-        <v>0.0001410934357507483</v>
-      </c>
-      <c r="R13">
-        <v>0.003030311329129174</v>
-      </c>
-      <c r="S13">
-        <v>0.006002887168865449</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -1263,25 +1266,25 @@
         <v>11611</v>
       </c>
       <c r="J14">
+        <v>-0.01180186309853548</v>
+      </c>
+      <c r="K14">
+        <v>0.0002098592232396584</v>
+      </c>
+      <c r="M14">
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="N14">
+        <v>0.00173711317318318</v>
+      </c>
+      <c r="O14">
         <v>0.004580501696160511</v>
       </c>
-      <c r="K14">
-        <v>0.0001631540263502446</v>
-      </c>
-      <c r="N14">
+      <c r="Q14">
+        <v>0.005213165544267774</v>
+      </c>
+      <c r="T14">
         <v>0.001592932311570713</v>
-      </c>
-      <c r="P14">
-        <v>-0.01180186309853548</v>
-      </c>
-      <c r="Q14">
-        <v>0.0002098592232396584</v>
-      </c>
-      <c r="R14">
-        <v>0.00173711317318318</v>
-      </c>
-      <c r="S14">
-        <v>0.005213165544267774</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -1313,25 +1316,25 @@
         <v>49</v>
       </c>
       <c r="J15">
+        <v>-0.01652918306199047</v>
+      </c>
+      <c r="K15">
+        <v>0.0003123469992588732</v>
+      </c>
+      <c r="M15">
+        <v>0.0001158352549329261</v>
+      </c>
+      <c r="N15">
+        <v>0.002972419699024923</v>
+      </c>
+      <c r="O15">
         <v>0.004529835290885987</v>
       </c>
-      <c r="K15">
-        <v>0.0001158352549329261</v>
-      </c>
-      <c r="N15">
+      <c r="Q15">
+        <v>0.007217175147339313</v>
+      </c>
+      <c r="T15">
         <v>0.00129198945232948</v>
-      </c>
-      <c r="P15">
-        <v>-0.01652918306199047</v>
-      </c>
-      <c r="Q15">
-        <v>0.0003123469992588732</v>
-      </c>
-      <c r="R15">
-        <v>0.002972419699024923</v>
-      </c>
-      <c r="S15">
-        <v>0.007217175147339313</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -1363,28 +1366,28 @@
         <v>14156</v>
       </c>
       <c r="J16">
+        <v>0.1218694481841025</v>
+      </c>
+      <c r="K16">
+        <v>0.0004006378783650764</v>
+      </c>
+      <c r="M16">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="N16">
+        <v>0.005239736253559311</v>
+      </c>
+      <c r="O16">
         <v>0.009674189396799987</v>
       </c>
-      <c r="K16">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N16">
+      <c r="Q16">
+        <v>0.0102119158074488</v>
+      </c>
+      <c r="T16">
         <v>0.004818030126325817</v>
       </c>
-      <c r="P16">
-        <v>0.1218694481841025</v>
-      </c>
-      <c r="Q16">
-        <v>0.0004006378783650764</v>
-      </c>
-      <c r="R16">
-        <v>0.005239736253559311</v>
-      </c>
-      <c r="S16">
-        <v>0.0102119158074488</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19">
+    </row>
+    <row r="17" spans="1:20">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -1413,28 +1416,28 @@
         <v>6771</v>
       </c>
       <c r="J17">
+        <v>0.2606707993949464</v>
+      </c>
+      <c r="K17">
+        <v>0.0001324165619288979</v>
+      </c>
+      <c r="M17">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="N17">
+        <v>0.003330775568204595</v>
+      </c>
+      <c r="O17">
         <v>0.005813234561065725</v>
       </c>
-      <c r="K17">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N17">
+      <c r="Q17">
+        <v>0.006002882908757912</v>
+      </c>
+      <c r="T17">
         <v>0.003193202088483064</v>
       </c>
-      <c r="P17">
-        <v>0.2606707993949464</v>
-      </c>
-      <c r="Q17">
-        <v>0.0001324165619288979</v>
-      </c>
-      <c r="R17">
-        <v>0.003330775568204595</v>
-      </c>
-      <c r="S17">
-        <v>0.006002882908757912</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19">
+    </row>
+    <row r="18" spans="1:20">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -1463,28 +1466,28 @@
         <v>6771</v>
       </c>
       <c r="J18">
+        <v>0.2046421514566161</v>
+      </c>
+      <c r="K18">
+        <v>0.0001424514975481683</v>
+      </c>
+      <c r="M18">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="N18">
+        <v>0.002972129451884979</v>
+      </c>
+      <c r="O18">
         <v>0.005813234561065725</v>
       </c>
-      <c r="K18">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N18">
+      <c r="Q18">
+        <v>0.00595976388177965</v>
+      </c>
+      <c r="T18">
         <v>0.003193202088483064</v>
       </c>
-      <c r="P18">
-        <v>0.2046421514566161</v>
-      </c>
-      <c r="Q18">
-        <v>0.0001424514975481683</v>
-      </c>
-      <c r="R18">
-        <v>0.002972129451884979</v>
-      </c>
-      <c r="S18">
-        <v>0.00595976388177965</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19">
+    </row>
+    <row r="19" spans="1:20">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -1513,28 +1516,28 @@
         <v>6771</v>
       </c>
       <c r="J19">
+        <v>0.2264121702660996</v>
+      </c>
+      <c r="K19">
+        <v>0.00013855240761432</v>
+      </c>
+      <c r="M19">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="N19">
+        <v>0.003005755874836842</v>
+      </c>
+      <c r="O19">
         <v>0.005813234561065725</v>
       </c>
-      <c r="K19">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N19">
+      <c r="Q19">
+        <v>0.00592641693601841</v>
+      </c>
+      <c r="T19">
         <v>0.003193202088483064</v>
       </c>
-      <c r="P19">
-        <v>0.2264121702660996</v>
-      </c>
-      <c r="Q19">
-        <v>0.00013855240761432</v>
-      </c>
-      <c r="R19">
-        <v>0.003005755874836842</v>
-      </c>
-      <c r="S19">
-        <v>0.00592641693601841</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19">
+    </row>
+    <row r="20" spans="1:20">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -1563,28 +1566,28 @@
         <v>14156</v>
       </c>
       <c r="J20">
+        <v>0.2810892232598902</v>
+      </c>
+      <c r="K20">
+        <v>0.0003279955215444224</v>
+      </c>
+      <c r="M20">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="N20">
+        <v>0.004617426367895965</v>
+      </c>
+      <c r="O20">
         <v>0.009674189396799985</v>
       </c>
-      <c r="K20">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N20">
+      <c r="Q20">
+        <v>0.008942022948316988</v>
+      </c>
+      <c r="T20">
         <v>0.004818030126325817</v>
       </c>
-      <c r="P20">
-        <v>0.2810892232598902</v>
-      </c>
-      <c r="Q20">
-        <v>0.0003279955215444224</v>
-      </c>
-      <c r="R20">
-        <v>0.004617426367895965</v>
-      </c>
-      <c r="S20">
-        <v>0.008942022948316988</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19">
+    </row>
+    <row r="21" spans="1:20">
       <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
@@ -1613,28 +1616,28 @@
         <v>11611</v>
       </c>
       <c r="J21">
+        <v>-0.004454544482717981</v>
+      </c>
+      <c r="K21">
+        <v>0.0002083353057278959</v>
+      </c>
+      <c r="M21">
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="N21">
+        <v>0.001554417436991534</v>
+      </c>
+      <c r="O21">
         <v>0.004580501696160511</v>
       </c>
-      <c r="K21">
-        <v>0.0001631540263502446</v>
-      </c>
-      <c r="N21">
+      <c r="Q21">
+        <v>0.005089153979501482</v>
+      </c>
+      <c r="T21">
         <v>0.001592932311570713</v>
       </c>
-      <c r="P21">
-        <v>-0.004454544482717981</v>
-      </c>
-      <c r="Q21">
-        <v>0.0002083353057278959</v>
-      </c>
-      <c r="R21">
-        <v>0.001554417436991534</v>
-      </c>
-      <c r="S21">
-        <v>0.005089153979501482</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19">
+    </row>
+    <row r="22" spans="1:20">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
@@ -1663,28 +1666,28 @@
         <v>14156</v>
       </c>
       <c r="J22">
+        <v>0.2865909829079945</v>
+      </c>
+      <c r="K22">
+        <v>0.0003254854012574867</v>
+      </c>
+      <c r="M22">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="N22">
+        <v>0.00456770441607247</v>
+      </c>
+      <c r="O22">
         <v>0.009674189396799985</v>
       </c>
-      <c r="K22">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N22">
+      <c r="Q22">
+        <v>0.008855143980453176</v>
+      </c>
+      <c r="T22">
         <v>0.004818030126325816</v>
       </c>
-      <c r="P22">
-        <v>0.2865909829079945</v>
-      </c>
-      <c r="Q22">
-        <v>0.0003254854012574867</v>
-      </c>
-      <c r="R22">
-        <v>0.00456770441607247</v>
-      </c>
-      <c r="S22">
-        <v>0.008855143980453176</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19">
+    </row>
+    <row r="23" spans="1:20">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -1713,28 +1716,28 @@
         <v>11542</v>
       </c>
       <c r="J23">
+        <v>-0.005012774390606101</v>
+      </c>
+      <c r="K23">
+        <v>0.0002091701444985722</v>
+      </c>
+      <c r="M23">
+        <v>0.000163888349337522</v>
+      </c>
+      <c r="N23">
+        <v>0.001583264354559398</v>
+      </c>
+      <c r="O23">
         <v>0.004589584286176587</v>
       </c>
-      <c r="K23">
-        <v>0.000163888349337522</v>
-      </c>
-      <c r="N23">
+      <c r="Q23">
+        <v>0.00510134746390362</v>
+      </c>
+      <c r="T23">
         <v>0.001597174444307401</v>
       </c>
-      <c r="P23">
-        <v>-0.005012774390606101</v>
-      </c>
-      <c r="Q23">
-        <v>0.0002091701444985722</v>
-      </c>
-      <c r="R23">
-        <v>0.001583264354559398</v>
-      </c>
-      <c r="S23">
-        <v>0.00510134746390362</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19">
+    </row>
+    <row r="24" spans="1:20">
       <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
@@ -1763,28 +1766,28 @@
         <v>6771</v>
       </c>
       <c r="J24">
+        <v>0.2028896166553128</v>
+      </c>
+      <c r="K24">
+        <v>0.0001427653829362463</v>
+      </c>
+      <c r="M24">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="N24">
+        <v>0.003125364361436701</v>
+      </c>
+      <c r="O24">
         <v>0.005813234561065723</v>
       </c>
-      <c r="K24">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N24">
+      <c r="Q24">
+        <v>0.006096382291329448</v>
+      </c>
+      <c r="T24">
         <v>0.003193202088483064</v>
       </c>
-      <c r="P24">
-        <v>0.2028896166553128</v>
-      </c>
-      <c r="Q24">
-        <v>0.0001427653829362463</v>
-      </c>
-      <c r="R24">
-        <v>0.003125364361436701</v>
-      </c>
-      <c r="S24">
-        <v>0.006096382291329448</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19">
+    </row>
+    <row r="25" spans="1:20">
       <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
@@ -1813,28 +1816,28 @@
         <v>6771</v>
       </c>
       <c r="J25">
+        <v>0.1996305390032257</v>
+      </c>
+      <c r="K25">
+        <v>0.0001433490956550128</v>
+      </c>
+      <c r="M25">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="N25">
+        <v>0.003163476470023769</v>
+      </c>
+      <c r="O25">
         <v>0.005813234561065723</v>
       </c>
-      <c r="K25">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N25">
+      <c r="Q25">
+        <v>0.00610593491672969</v>
+      </c>
+      <c r="T25">
         <v>0.003193202088483064</v>
       </c>
-      <c r="P25">
-        <v>0.1996305390032257</v>
-      </c>
-      <c r="Q25">
-        <v>0.0001433490956550128</v>
-      </c>
-      <c r="R25">
-        <v>0.003163476470023769</v>
-      </c>
-      <c r="S25">
-        <v>0.00610593491672969</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19">
+    </row>
+    <row r="26" spans="1:20">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
@@ -1863,28 +1866,28 @@
         <v>6771</v>
       </c>
       <c r="J26">
+        <v>0.2020008505541708</v>
+      </c>
+      <c r="K26">
+        <v>0.0001429245641932233</v>
+      </c>
+      <c r="M26">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="N26">
+        <v>0.003090643964573058</v>
+      </c>
+      <c r="O26">
         <v>0.005813234561065723</v>
       </c>
-      <c r="K26">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N26">
+      <c r="Q26">
+        <v>0.006067498374332903</v>
+      </c>
+      <c r="T26">
         <v>0.003193202088483064</v>
       </c>
-      <c r="P26">
-        <v>0.2020008505541708</v>
-      </c>
-      <c r="Q26">
-        <v>0.0001429245641932233</v>
-      </c>
-      <c r="R26">
-        <v>0.003090643964573058</v>
-      </c>
-      <c r="S26">
-        <v>0.006067498374332903</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19">
+    </row>
+    <row r="27" spans="1:20">
       <c r="A27" s="1" t="s">
         <v>45</v>
       </c>
@@ -1913,28 +1916,28 @@
         <v>11611</v>
       </c>
       <c r="J27">
+        <v>-0.002771209789547591</v>
+      </c>
+      <c r="K27">
+        <v>0.000207986162951978</v>
+      </c>
+      <c r="M27">
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="N27">
+        <v>0.001554596452837835</v>
+      </c>
+      <c r="O27">
         <v>0.004580501696160511</v>
       </c>
-      <c r="K27">
-        <v>0.0001631540263502446</v>
-      </c>
-      <c r="N27">
+      <c r="Q27">
+        <v>0.005107549406927882</v>
+      </c>
+      <c r="T27">
         <v>0.001592932311570713</v>
       </c>
-      <c r="P27">
-        <v>-0.002771209789547591</v>
-      </c>
-      <c r="Q27">
-        <v>0.000207986162951978</v>
-      </c>
-      <c r="R27">
-        <v>0.001554596452837835</v>
-      </c>
-      <c r="S27">
-        <v>0.005107549406927882</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19">
+    </row>
+    <row r="28" spans="1:20">
       <c r="A28" s="1" t="s">
         <v>46</v>
       </c>
@@ -1963,28 +1966,28 @@
         <v>6771</v>
       </c>
       <c r="J28">
+        <v>0.1058242633905934</v>
+      </c>
+      <c r="K28">
+        <v>0.000160150142460433</v>
+      </c>
+      <c r="M28">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="N28">
+        <v>0.003715325925925931</v>
+      </c>
+      <c r="O28">
         <v>0.005813234561065723</v>
       </c>
-      <c r="K28">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N28">
+      <c r="Q28">
+        <v>0.006776662396495037</v>
+      </c>
+      <c r="T28">
         <v>0.003193202088483064</v>
       </c>
-      <c r="P28">
-        <v>0.1058242633905934</v>
-      </c>
-      <c r="Q28">
-        <v>0.000160150142460433</v>
-      </c>
-      <c r="R28">
-        <v>0.003715325925925931</v>
-      </c>
-      <c r="S28">
-        <v>0.006776662396495037</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19">
+    </row>
+    <row r="29" spans="1:20">
       <c r="A29" s="1" t="s">
         <v>47</v>
       </c>
@@ -2013,28 +2016,28 @@
         <v>4010</v>
       </c>
       <c r="J29">
+        <v>-0.006214540120261569</v>
+      </c>
+      <c r="K29">
+        <v>0.0002742305932959652</v>
+      </c>
+      <c r="M29">
+        <v>0.0001730864695810989</v>
+      </c>
+      <c r="N29">
+        <v>0.001362431751651251</v>
+      </c>
+      <c r="O29">
         <v>0.004349183403839366</v>
       </c>
-      <c r="K29">
-        <v>0.0001730864695810989</v>
-      </c>
-      <c r="N29">
+      <c r="Q29">
+        <v>0.004501420066184821</v>
+      </c>
+      <c r="T29">
         <v>0.001438312583710056</v>
       </c>
-      <c r="P29">
-        <v>-0.006214540120261569</v>
-      </c>
-      <c r="Q29">
-        <v>0.0002742305932959652</v>
-      </c>
-      <c r="R29">
-        <v>0.001362431751651251</v>
-      </c>
-      <c r="S29">
-        <v>0.004501420066184821</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19">
+    </row>
+    <row r="30" spans="1:20">
       <c r="A30" s="1" t="s">
         <v>48</v>
       </c>
@@ -2063,28 +2066,28 @@
         <v>14156</v>
       </c>
       <c r="J30">
+        <v>0.1230344532976788</v>
+      </c>
+      <c r="K30">
+        <v>0.0004001063569688302</v>
+      </c>
+      <c r="M30">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="N30">
+        <v>0.005409147625572685</v>
+      </c>
+      <c r="O30">
         <v>0.009674189396799987</v>
       </c>
-      <c r="K30">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N30">
+      <c r="Q30">
+        <v>0.01035431191953904</v>
+      </c>
+      <c r="T30">
         <v>0.004818030126325817</v>
       </c>
-      <c r="P30">
-        <v>0.1230344532976788</v>
-      </c>
-      <c r="Q30">
-        <v>0.0004001063569688302</v>
-      </c>
-      <c r="R30">
-        <v>0.005409147625572685</v>
-      </c>
-      <c r="S30">
-        <v>0.01035431191953904</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19">
+    </row>
+    <row r="31" spans="1:20">
       <c r="A31" s="1" t="s">
         <v>49</v>
       </c>
@@ -2113,28 +2116,28 @@
         <v>11611</v>
       </c>
       <c r="J31">
+        <v>-0.00353431378743374</v>
+      </c>
+      <c r="K31">
+        <v>0.0002081444394071696</v>
+      </c>
+      <c r="M31">
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="N31">
+        <v>0.001547174514616301</v>
+      </c>
+      <c r="O31">
         <v>0.004580501696160511</v>
       </c>
-      <c r="K31">
-        <v>0.0001631540263502446</v>
-      </c>
-      <c r="N31">
+      <c r="Q31">
+        <v>0.005089488294347637</v>
+      </c>
+      <c r="T31">
         <v>0.001592932311570713</v>
       </c>
-      <c r="P31">
-        <v>-0.00353431378743374</v>
-      </c>
-      <c r="Q31">
-        <v>0.0002081444394071696</v>
-      </c>
-      <c r="R31">
-        <v>0.001547174514616301</v>
-      </c>
-      <c r="S31">
-        <v>0.005089488294347637</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19">
+    </row>
+    <row r="32" spans="1:20">
       <c r="A32" s="1" t="s">
         <v>50</v>
       </c>
@@ -2163,25 +2166,25 @@
         <v>14156</v>
       </c>
       <c r="J32">
+        <v>0.2085500335179142</v>
+      </c>
+      <c r="K32">
+        <v>0.0003610907680501377</v>
+      </c>
+      <c r="M32">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="N32">
+        <v>0.004884082851211167</v>
+      </c>
+      <c r="O32">
         <v>0.009674189396799985</v>
       </c>
-      <c r="K32">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N32">
+      <c r="Q32">
+        <v>0.009406309171688502</v>
+      </c>
+      <c r="T32">
         <v>0.004818030126325816</v>
-      </c>
-      <c r="P32">
-        <v>0.2085500335179142</v>
-      </c>
-      <c r="Q32">
-        <v>0.0003610907680501377</v>
-      </c>
-      <c r="R32">
-        <v>0.004884082851211167</v>
-      </c>
-      <c r="S32">
-        <v>0.009406309171688502</v>
       </c>
     </row>
     <row r="33" spans="1:20">
@@ -2189,22 +2192,22 @@
         <v>51</v>
       </c>
       <c r="B33">
-        <v>0.008532806478705164</v>
+        <v>0.008519531777817098</v>
       </c>
       <c r="C33">
-        <v>0.008733878054388279</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D33">
-        <v>0.0001656454412935777</v>
+        <v>0.0001673145877462598</v>
       </c>
       <c r="E33">
-        <v>0.0001961492659581503</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F33">
-        <v>0.2636491907304709</v>
+        <v>0.2815190988739301</v>
       </c>
       <c r="G33">
-        <v>0.1280492261183164</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H33">
         <v>0.2582640092197721</v>
@@ -2213,25 +2216,25 @@
         <v>14156</v>
       </c>
       <c r="J33">
-        <v>0.009674189396799987</v>
+        <v>0.1866413032030688</v>
       </c>
       <c r="K33">
+        <v>0.0003710863970746162</v>
+      </c>
+      <c r="M33">
         <v>0.0003384092866814527</v>
       </c>
       <c r="N33">
-        <v>0.004818030126325817</v>
-      </c>
-      <c r="P33">
-        <v>0.179378395374721</v>
+        <v>0.004784771004405694</v>
+      </c>
+      <c r="O33">
+        <v>0.009674189396799985</v>
       </c>
       <c r="Q33">
-        <v>0.0003744000227958637</v>
-      </c>
-      <c r="R33">
-        <v>0.004730871750625608</v>
-      </c>
-      <c r="S33">
-        <v>0.009554445336689437</v>
+        <v>0.009535796789931871</v>
+      </c>
+      <c r="T33">
+        <v>0.004818030126325816</v>
       </c>
     </row>
     <row r="34" spans="1:20">
@@ -2239,19 +2242,19 @@
         <v>52</v>
       </c>
       <c r="B34">
-        <v>0.008529233938818522</v>
+        <v>0.008532806478705164</v>
       </c>
       <c r="C34">
         <v>0.008733878054388279</v>
       </c>
       <c r="D34">
-        <v>0.0001653251466070655</v>
+        <v>0.0001656454412935777</v>
       </c>
       <c r="E34">
         <v>0.0001961492659581503</v>
       </c>
       <c r="F34">
-        <v>0.2650730104853413</v>
+        <v>0.2636491907304709</v>
       </c>
       <c r="G34">
         <v>0.1280492261183164</v>
@@ -2263,25 +2266,25 @@
         <v>14156</v>
       </c>
       <c r="J34">
+        <v>0.179378395374721</v>
+      </c>
+      <c r="K34">
+        <v>0.0003744000227958637</v>
+      </c>
+      <c r="M34">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="N34">
+        <v>0.004730871750625608</v>
+      </c>
+      <c r="O34">
         <v>0.009674189396799987</v>
       </c>
-      <c r="K34">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N34">
+      <c r="Q34">
+        <v>0.009554445336689437</v>
+      </c>
+      <c r="T34">
         <v>0.004818030126325817</v>
-      </c>
-      <c r="P34">
-        <v>0.1788608663781261</v>
-      </c>
-      <c r="Q34">
-        <v>0.0003746361399868205</v>
-      </c>
-      <c r="R34">
-        <v>0.004764640177213803</v>
-      </c>
-      <c r="S34">
-        <v>0.009555217528480035</v>
       </c>
     </row>
     <row r="35" spans="1:20">
@@ -2289,19 +2292,19 @@
         <v>53</v>
       </c>
       <c r="B35">
-        <v>0.008505250051591662</v>
+        <v>0.008529233938818522</v>
       </c>
       <c r="C35">
         <v>0.008733878054388279</v>
       </c>
       <c r="D35">
-        <v>0.0001646168902522808</v>
+        <v>0.0001653251466070655</v>
       </c>
       <c r="E35">
         <v>0.0001961492659581503</v>
       </c>
       <c r="F35">
-        <v>0.268221452941368</v>
+        <v>0.2650730104853413</v>
       </c>
       <c r="G35">
         <v>0.1280492261183164</v>
@@ -2313,25 +2316,25 @@
         <v>14156</v>
       </c>
       <c r="J35">
+        <v>0.1788608663781261</v>
+      </c>
+      <c r="K35">
+        <v>0.0003746361399868205</v>
+      </c>
+      <c r="M35">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="N35">
+        <v>0.004764640177213803</v>
+      </c>
+      <c r="O35">
         <v>0.009674189396799987</v>
       </c>
-      <c r="K35">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N35">
+      <c r="Q35">
+        <v>0.009555217528480035</v>
+      </c>
+      <c r="T35">
         <v>0.004818030126325817</v>
-      </c>
-      <c r="P35">
-        <v>0.1810824657398455</v>
-      </c>
-      <c r="Q35">
-        <v>0.0003736225585176234</v>
-      </c>
-      <c r="R35">
-        <v>0.004756476812602748</v>
-      </c>
-      <c r="S35">
-        <v>0.009526287265811475</v>
       </c>
     </row>
     <row r="36" spans="1:20">
@@ -2339,49 +2342,49 @@
         <v>54</v>
       </c>
       <c r="B36">
-        <v>0.006299187529923155</v>
+        <v>0.008505250051591662</v>
       </c>
       <c r="C36">
-        <v>0.00553167406053466</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D36">
-        <v>9.00395869891457E-05</v>
+        <v>0.0001646168902522808</v>
       </c>
       <c r="E36">
-        <v>8.170381435551846E-05</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F36">
-        <v>0.1391419988807219</v>
+        <v>0.268221452941368</v>
       </c>
       <c r="G36">
-        <v>0.2188393498696173</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H36">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I36">
-        <v>6771</v>
+        <v>14156</v>
       </c>
       <c r="J36">
-        <v>0.005813234561065723</v>
+        <v>0.1810824657398455</v>
       </c>
       <c r="K36">
-        <v>0.0001037297229528328</v>
+        <v>0.0003736225585176234</v>
+      </c>
+      <c r="M36">
+        <v>0.0003384092866814527</v>
       </c>
       <c r="N36">
-        <v>0.003193202088483064</v>
-      </c>
-      <c r="P36">
-        <v>0.1045681259196538</v>
+        <v>0.004756476812602748</v>
+      </c>
+      <c r="O36">
+        <v>0.009674189396799987</v>
       </c>
       <c r="Q36">
-        <v>0.0001603751212724098</v>
-      </c>
-      <c r="R36">
-        <v>0.003667719421830667</v>
-      </c>
-      <c r="S36">
-        <v>0.00674135934653288</v>
+        <v>0.009526287265811475</v>
+      </c>
+      <c r="T36">
+        <v>0.004818030126325817</v>
       </c>
     </row>
     <row r="37" spans="1:20">
@@ -2389,49 +2392,49 @@
         <v>55</v>
       </c>
       <c r="B37">
-        <v>0.00864935396008955</v>
+        <v>0.006299187529923155</v>
       </c>
       <c r="C37">
-        <v>0.008733878054388279</v>
+        <v>0.00553167406053466</v>
       </c>
       <c r="D37">
-        <v>0.0001602711781363747</v>
+        <v>9.00395869891457E-05</v>
       </c>
       <c r="E37">
-        <v>0.0001961492659581503</v>
+        <v>8.170381435551846E-05</v>
       </c>
       <c r="F37">
-        <v>0.2875396340419782</v>
+        <v>0.1391419988807219</v>
       </c>
       <c r="G37">
-        <v>0.1280492261183164</v>
+        <v>0.2188393498696173</v>
       </c>
       <c r="H37">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I37">
-        <v>14156</v>
+        <v>6771</v>
       </c>
       <c r="J37">
-        <v>0.009674189396799987</v>
+        <v>0.1045681259196538</v>
       </c>
       <c r="K37">
-        <v>0.0003384092866814527</v>
+        <v>0.0001603751212724098</v>
+      </c>
+      <c r="M37">
+        <v>0.0001037297229528328</v>
       </c>
       <c r="N37">
-        <v>0.004818030126325816</v>
-      </c>
-      <c r="P37">
-        <v>0.2088743260447083</v>
+        <v>0.003667719421830667</v>
+      </c>
+      <c r="O37">
+        <v>0.005813234561065723</v>
       </c>
       <c r="Q37">
-        <v>0.0003609428129771297</v>
-      </c>
-      <c r="R37">
-        <v>0.005274143159156646</v>
-      </c>
-      <c r="S37">
-        <v>0.009669808352814117</v>
+        <v>0.00674135934653288</v>
+      </c>
+      <c r="T37">
+        <v>0.003193202088483064</v>
       </c>
     </row>
     <row r="38" spans="1:20">
@@ -2439,22 +2442,22 @@
         <v>56</v>
       </c>
       <c r="B38">
-        <v>0.00869522801124366</v>
+        <v>0.00864935396008955</v>
       </c>
       <c r="C38">
-        <v>0.008722720041403264</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D38">
-        <v>0.0001671499749450426</v>
+        <v>0.0001602711781363747</v>
       </c>
       <c r="E38">
-        <v>0.0001985649052123504</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F38">
-        <v>0.2822259777859754</v>
+        <v>0.2875396340419782</v>
       </c>
       <c r="G38">
-        <v>0.147324247391146</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H38">
         <v>0.2582640092197721</v>
@@ -2463,25 +2466,25 @@
         <v>14156</v>
       </c>
       <c r="J38">
-        <v>0.009674189396799985</v>
+        <v>0.2088743260447083</v>
       </c>
       <c r="K38">
+        <v>0.0003609428129771297</v>
+      </c>
+      <c r="M38">
         <v>0.0003384092866814527</v>
       </c>
       <c r="N38">
-        <v>0.004818030126325817</v>
-      </c>
-      <c r="P38">
-        <v>0.2030564380000814</v>
+        <v>0.005274143159156646</v>
+      </c>
+      <c r="O38">
+        <v>0.009674189396799987</v>
       </c>
       <c r="Q38">
-        <v>0.0003635971635380399</v>
-      </c>
-      <c r="R38">
-        <v>0.005173194757001598</v>
-      </c>
-      <c r="S38">
-        <v>0.009719161233546112</v>
+        <v>0.009669808352814117</v>
+      </c>
+      <c r="T38">
+        <v>0.004818030126325816</v>
       </c>
     </row>
     <row r="39" spans="1:20">
@@ -2489,19 +2492,19 @@
         <v>57</v>
       </c>
       <c r="B39">
-        <v>0.007668256776450208</v>
+        <v>0.00869522801124366</v>
       </c>
       <c r="C39">
         <v>0.008722720041403264</v>
       </c>
       <c r="D39">
-        <v>0.0001436777206558706</v>
+        <v>0.0001671499749450426</v>
       </c>
       <c r="E39">
         <v>0.0001985649052123504</v>
       </c>
       <c r="F39">
-        <v>0.3830203355303232</v>
+        <v>0.2822259777859754</v>
       </c>
       <c r="G39">
         <v>0.147324247391146</v>
@@ -2513,25 +2516,25 @@
         <v>14156</v>
       </c>
       <c r="J39">
+        <v>0.2030564380000814</v>
+      </c>
+      <c r="K39">
+        <v>0.0003635971635380399</v>
+      </c>
+      <c r="M39">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="N39">
+        <v>0.005173194757001598</v>
+      </c>
+      <c r="O39">
         <v>0.009674189396799985</v>
       </c>
-      <c r="K39">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N39">
+      <c r="Q39">
+        <v>0.009719161233546112</v>
+      </c>
+      <c r="T39">
         <v>0.004818030126325817</v>
-      </c>
-      <c r="P39">
-        <v>0.2669184291403396</v>
-      </c>
-      <c r="Q39">
-        <v>0.0003344607981243851</v>
-      </c>
-      <c r="R39">
-        <v>0.004128330862335852</v>
-      </c>
-      <c r="S39">
-        <v>0.00867861064019221</v>
       </c>
     </row>
     <row r="40" spans="1:20">
@@ -2539,22 +2542,22 @@
         <v>58</v>
       </c>
       <c r="B40">
-        <v>0.01020612284563066</v>
+        <v>0.007668256776450208</v>
       </c>
       <c r="C40">
-        <v>0.009760820655321729</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D40">
-        <v>0.0002760452274294578</v>
+        <v>0.0001436777206558706</v>
       </c>
       <c r="E40">
-        <v>0.0002924361182664438</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F40">
-        <v>0.1971347954963554</v>
+        <v>0.3830203355303232</v>
       </c>
       <c r="G40">
-        <v>0.1494626221848404</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H40">
         <v>0.2582640092197721</v>
@@ -2563,25 +2566,25 @@
         <v>14156</v>
       </c>
       <c r="J40">
-        <v>0.009674189396799987</v>
+        <v>0.2669184291403396</v>
       </c>
       <c r="K40">
+        <v>0.0003344607981243851</v>
+      </c>
+      <c r="M40">
         <v>0.0003384092866814527</v>
       </c>
       <c r="N40">
-        <v>0.004818030126325816</v>
-      </c>
-      <c r="P40">
-        <v>0.1481445083553075</v>
+        <v>0.004128330862335852</v>
+      </c>
+      <c r="O40">
+        <v>0.009674189396799985</v>
       </c>
       <c r="Q40">
-        <v>0.0003886501570187028</v>
-      </c>
-      <c r="R40">
-        <v>0.005394960099510664</v>
-      </c>
-      <c r="S40">
-        <v>0.01011738460212881</v>
+        <v>0.00867861064019221</v>
+      </c>
+      <c r="T40">
+        <v>0.004818030126325817</v>
       </c>
     </row>
     <row r="41" spans="1:20">
@@ -2589,22 +2592,22 @@
         <v>59</v>
       </c>
       <c r="B41">
-        <v>0.00958912348219286</v>
+        <v>0.01020612284563066</v>
       </c>
       <c r="C41">
-        <v>0.008722720041403264</v>
+        <v>0.009760820655321729</v>
       </c>
       <c r="D41">
-        <v>0.00021842684931279</v>
+        <v>0.0002760452274294578</v>
       </c>
       <c r="E41">
-        <v>0.0001985649052123504</v>
+        <v>0.0002924361182664438</v>
       </c>
       <c r="F41">
-        <v>0.06203325341612431</v>
+        <v>0.1971347954963554</v>
       </c>
       <c r="G41">
-        <v>0.147324247391146</v>
+        <v>0.1494626221848404</v>
       </c>
       <c r="H41">
         <v>0.2582640092197721</v>
@@ -2613,25 +2616,25 @@
         <v>14156</v>
       </c>
       <c r="J41">
-        <v>0.009674189396799985</v>
+        <v>0.1481445083553075</v>
       </c>
       <c r="K41">
+        <v>0.0003886501570187028</v>
+      </c>
+      <c r="M41">
         <v>0.0003384092866814527</v>
       </c>
       <c r="N41">
-        <v>0.004818030126325817</v>
-      </c>
-      <c r="P41">
-        <v>0.05448840836791147</v>
+        <v>0.005394960099510664</v>
+      </c>
+      <c r="O41">
+        <v>0.009674189396799987</v>
       </c>
       <c r="Q41">
-        <v>0.0004313797729252501</v>
-      </c>
-      <c r="R41">
-        <v>0.005560650653515711</v>
-      </c>
-      <c r="S41">
-        <v>0.01064772150300563</v>
+        <v>0.01011738460212881</v>
+      </c>
+      <c r="T41">
+        <v>0.004818030126325816</v>
       </c>
     </row>
     <row r="42" spans="1:20">
@@ -2639,61 +2642,49 @@
         <v>60</v>
       </c>
       <c r="B42">
-        <v>0.005414655366858831</v>
+        <v>0.00958912348219286</v>
       </c>
       <c r="C42">
-        <v>0.005250633999685894</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D42">
-        <v>8.390458217824665E-05</v>
+        <v>0.00021842684931279</v>
       </c>
       <c r="E42">
-        <v>8.336263472823423E-05</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F42">
-        <v>0.2548808040617673</v>
+        <v>0.06203325341612431</v>
       </c>
       <c r="G42">
-        <v>0.2596935978056915</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H42">
-        <v>0.456874413314975</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I42">
-        <v>5153</v>
+        <v>14156</v>
       </c>
       <c r="J42">
-        <v>0.005318929375230071</v>
+        <v>0.05448840836791147</v>
       </c>
       <c r="K42">
-        <v>9.243123959608208E-05</v>
-      </c>
-      <c r="L42">
-        <v>0.4055123229186881</v>
+        <v>0.0004313797729252501</v>
       </c>
       <c r="M42">
-        <v>10.4129840341794</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="N42">
-        <v>0.002848413552158193</v>
+        <v>0.005560650653515711</v>
       </c>
       <c r="O42">
-        <v>11.43997477570016</v>
-      </c>
-      <c r="P42">
-        <v>0.1703625716885953</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="Q42">
-        <v>0.000141190946981845</v>
-      </c>
-      <c r="R42">
-        <v>0.002733726006933551</v>
-      </c>
-      <c r="S42">
-        <v>0.005626234126090045</v>
+        <v>0.01064772150300563</v>
       </c>
       <c r="T42">
-        <v>0.4113135413420823</v>
+        <v>0.004818030126325817</v>
       </c>
     </row>
     <row r="43" spans="1:20">
@@ -2701,49 +2692,61 @@
         <v>61</v>
       </c>
       <c r="B43">
-        <v>0.009301347310769852</v>
+        <v>0.005414655366858831</v>
       </c>
       <c r="C43">
-        <v>0.008733878054388279</v>
+        <v>0.005250633999685894</v>
       </c>
       <c r="D43">
-        <v>0.0001883109214593075</v>
+        <v>8.390458217824665E-05</v>
       </c>
       <c r="E43">
-        <v>0.0001961492659581503</v>
+        <v>8.336263472823423E-05</v>
       </c>
       <c r="F43">
-        <v>0.1628933562675233</v>
+        <v>0.2548808040617673</v>
       </c>
       <c r="G43">
-        <v>0.1280492261183164</v>
+        <v>0.2596935978056915</v>
       </c>
       <c r="H43">
-        <v>0.2582640092197721</v>
+        <v>0.456874413314975</v>
       </c>
       <c r="I43">
-        <v>14156</v>
+        <v>5153</v>
       </c>
       <c r="J43">
-        <v>0.009674189396799987</v>
+        <v>0.1703625716885953</v>
       </c>
       <c r="K43">
-        <v>0.0003384092866814527</v>
+        <v>0.000141190946981845</v>
+      </c>
+      <c r="L43">
+        <v>0.4055123229186881</v>
+      </c>
+      <c r="M43">
+        <v>9.243123959608208E-05</v>
       </c>
       <c r="N43">
-        <v>0.004818030126325817</v>
+        <v>0.002733726006933551</v>
+      </c>
+      <c r="O43">
+        <v>0.005318929375230071</v>
       </c>
       <c r="P43">
-        <v>0.1175458874123242</v>
+        <v>0.4113135413420823</v>
       </c>
       <c r="Q43">
-        <v>0.0004026104577395279</v>
+        <v>0.005626234126090045</v>
       </c>
       <c r="R43">
-        <v>0.005399385735558927</v>
+        <v>10.4129840341794</v>
       </c>
       <c r="S43">
-        <v>0.01035467890006862</v>
+        <v>11.43997477570016</v>
+      </c>
+      <c r="T43">
+        <v>0.002848413552158193</v>
       </c>
     </row>
     <row r="44" spans="1:20">
@@ -2751,49 +2754,49 @@
         <v>62</v>
       </c>
       <c r="B44">
-        <v>0.00303210497017975</v>
+        <v>0.009301347310769852</v>
       </c>
       <c r="C44">
-        <v>0.002499571894821071</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D44">
-        <v>1.909735738640315E-05</v>
+        <v>0.0001883109214593075</v>
       </c>
       <c r="E44">
-        <v>1.967007435869721E-05</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F44">
-        <v>-0.0120856426831728</v>
+        <v>0.1628933562675233</v>
       </c>
       <c r="G44">
-        <v>-0.04243741404356438</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H44">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I44">
-        <v>11611</v>
+        <v>14156</v>
       </c>
       <c r="J44">
-        <v>0.004580501696160511</v>
+        <v>0.1175458874123242</v>
       </c>
       <c r="K44">
-        <v>0.0001631540263502446</v>
+        <v>0.0004026104577395279</v>
+      </c>
+      <c r="M44">
+        <v>0.0003384092866814527</v>
       </c>
       <c r="N44">
-        <v>0.001592932311570713</v>
-      </c>
-      <c r="P44">
-        <v>-0.002911711704464803</v>
+        <v>0.005399385735558927</v>
+      </c>
+      <c r="O44">
+        <v>0.009674189396799987</v>
       </c>
       <c r="Q44">
-        <v>0.0002080153046483946</v>
-      </c>
-      <c r="R44">
-        <v>0.001550051802718652</v>
-      </c>
-      <c r="S44">
-        <v>0.005090949099942899</v>
+        <v>0.01035467890006862</v>
+      </c>
+      <c r="T44">
+        <v>0.004818030126325817</v>
       </c>
     </row>
     <row r="45" spans="1:20">
@@ -2801,49 +2804,49 @@
         <v>63</v>
       </c>
       <c r="B45">
-        <v>0.008142928261746932</v>
+        <v>0.00303210497017975</v>
       </c>
       <c r="C45">
-        <v>0.008733878054388279</v>
+        <v>0.002499571894821071</v>
       </c>
       <c r="D45">
-        <v>0.0001648112327367591</v>
+        <v>1.909735738640315E-05</v>
       </c>
       <c r="E45">
-        <v>0.0001961492659581503</v>
+        <v>1.967007435869721E-05</v>
       </c>
       <c r="F45">
-        <v>0.2673575339309593</v>
+        <v>-0.0120856426831728</v>
       </c>
       <c r="G45">
-        <v>0.1280492261183164</v>
+        <v>-0.04243741404356438</v>
       </c>
       <c r="H45">
-        <v>0.2582640092197721</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I45">
-        <v>14156</v>
+        <v>11611</v>
       </c>
       <c r="J45">
-        <v>0.009674189396799987</v>
+        <v>-0.002911711704464803</v>
       </c>
       <c r="K45">
-        <v>0.0003384092866814527</v>
+        <v>0.0002080153046483946</v>
+      </c>
+      <c r="M45">
+        <v>0.0001631540263502446</v>
       </c>
       <c r="N45">
-        <v>0.004818030126325817</v>
-      </c>
-      <c r="P45">
-        <v>0.2464320924804251</v>
+        <v>0.001550051802718652</v>
+      </c>
+      <c r="O45">
+        <v>0.004580501696160511</v>
       </c>
       <c r="Q45">
-        <v>0.0003438074749231005</v>
-      </c>
-      <c r="R45">
-        <v>0.004666820467017538</v>
-      </c>
-      <c r="S45">
-        <v>0.009263751492683912</v>
+        <v>0.005090949099942899</v>
+      </c>
+      <c r="T45">
+        <v>0.001592932311570713</v>
       </c>
     </row>
     <row r="46" spans="1:20">
@@ -2851,49 +2854,99 @@
         <v>64</v>
       </c>
       <c r="B46">
+        <v>0.008142928261746932</v>
+      </c>
+      <c r="C46">
+        <v>0.008733878054388279</v>
+      </c>
+      <c r="D46">
+        <v>0.0001648112327367591</v>
+      </c>
+      <c r="E46">
+        <v>0.0001961492659581503</v>
+      </c>
+      <c r="F46">
+        <v>0.2673575339309593</v>
+      </c>
+      <c r="G46">
+        <v>0.1280492261183164</v>
+      </c>
+      <c r="H46">
+        <v>0.2582640092197721</v>
+      </c>
+      <c r="I46">
+        <v>14156</v>
+      </c>
+      <c r="J46">
+        <v>0.2464320924804251</v>
+      </c>
+      <c r="K46">
+        <v>0.0003438074749231005</v>
+      </c>
+      <c r="M46">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="N46">
+        <v>0.004666820467017538</v>
+      </c>
+      <c r="O46">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="Q46">
+        <v>0.009263751492683912</v>
+      </c>
+      <c r="T46">
+        <v>0.004818030126325817</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20">
+      <c r="A47" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47">
         <v>0.01025436961368844</v>
       </c>
-      <c r="C46">
+      <c r="C47">
         <v>0.01023301201875394</v>
       </c>
-      <c r="D46">
+      <c r="D47">
         <v>0.0002841844015704704</v>
       </c>
-      <c r="E46">
+      <c r="E47">
         <v>0.0003551633527675986</v>
       </c>
-      <c r="F46">
+      <c r="F47">
         <v>0.3369590471682379</v>
       </c>
-      <c r="G46">
+      <c r="G47">
         <v>0.1713554771880856</v>
       </c>
-      <c r="H46">
+      <c r="H47">
         <v>0.4827027158358849</v>
       </c>
-      <c r="I46">
+      <c r="I47">
         <v>1267</v>
       </c>
-      <c r="J46">
+      <c r="J47">
+        <v>0.2718477491393597</v>
+      </c>
+      <c r="K47">
+        <v>0.0006028948928221208</v>
+      </c>
+      <c r="M47">
+        <v>0.0004283113735138171</v>
+      </c>
+      <c r="N47">
+        <v>0.005379622896887214</v>
+      </c>
+      <c r="O47">
         <v>0.01026809155717979</v>
       </c>
-      <c r="K46">
-        <v>0.0004283113735138171</v>
-      </c>
-      <c r="N46">
+      <c r="Q47">
+        <v>0.0102050584404969</v>
+      </c>
+      <c r="T47">
         <v>0.004670472236637264</v>
-      </c>
-      <c r="P46">
-        <v>0.2718477491393597</v>
-      </c>
-      <c r="Q46">
-        <v>0.0006028948928221208</v>
-      </c>
-      <c r="R46">
-        <v>0.005379622896887214</v>
-      </c>
-      <c r="S46">
-        <v>0.0102050584404969</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. update lgbm new config I - random half 2. update consensus
</commit_message>
<xml_diff>
--- a/results_analysis/compare_with_ibes/#compare_all.xlsx
+++ b/results_analysis/compare_with_ibes/#compare_all.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>lgbm_mae</t>
   </si>
@@ -40,39 +40,39 @@
     <t>len</t>
   </si>
   <si>
+    <t>consensus_mape_eps</t>
+  </si>
+  <si>
+    <t>consensus_mae_eps</t>
+  </si>
+  <si>
+    <t>consensus_mse_org</t>
+  </si>
+  <si>
+    <t>lgbm_mae_eps</t>
+  </si>
+  <si>
+    <t>lgbm_mape_eps</t>
+  </si>
+  <si>
     <t>lgbm_r2_org</t>
   </si>
   <si>
+    <t>consensus_medae_org</t>
+  </si>
+  <si>
+    <t>lgbm_mae_org</t>
+  </si>
+  <si>
+    <t>lgbm_medae_org</t>
+  </si>
+  <si>
     <t>lgbm_mse_org</t>
   </si>
   <si>
-    <t>consensus_mae_eps</t>
-  </si>
-  <si>
-    <t>consensus_mse_org</t>
-  </si>
-  <si>
-    <t>lgbm_medae_org</t>
-  </si>
-  <si>
     <t>consensus_mae_org</t>
   </si>
   <si>
-    <t>lgbm_mae_eps</t>
-  </si>
-  <si>
-    <t>lgbm_mae_org</t>
-  </si>
-  <si>
-    <t>consensus_mape_eps</t>
-  </si>
-  <si>
-    <t>lgbm_mape_eps</t>
-  </si>
-  <si>
-    <t>consensus_medae_org</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -118,6 +118,15 @@
     <t>ibes_qoq_2|ni|q_2｜ibes_qoq</t>
   </si>
   <si>
+    <t>ibes_1|fwdepsqcut|cnn_rnn｜without ibes -2</t>
+  </si>
+  <si>
+    <t>ibes_1|ni-industry_code|cnn_rnn｜without ibes -2</t>
+  </si>
+  <si>
+    <t>ibes_1|ni-sector_code|cnn_rnn｜without ibes -2</t>
+  </si>
+  <si>
     <t>ibes_1|fwdepsqcut-46|dense2｜all x 0 -fix space</t>
   </si>
   <si>
@@ -163,6 +172,9 @@
     <t>ibes_1|fwdepsqcut-46|dense2｜mini_tune15_re -code 0 -exclude_fwd True</t>
   </si>
   <si>
+    <t>ibes_1|fwdepsqcut|cnn_rnn｜small_training_True_0</t>
+  </si>
+  <si>
     <t>ibes_qoq_1|fwdepsqcut|q_1｜ibes_qoqcut8_entire</t>
   </si>
   <si>
@@ -200,6 +212,9 @@
   </si>
   <si>
     <t>ibes_2|fwdepsqcut|ibes_industry -sp500</t>
+  </si>
+  <si>
+    <t>ibes_1|fwdepsqcut-46|dense2｜large_big_allx -code 0 -exclude_fwd True</t>
   </si>
   <si>
     <t>ibes_1|fwdepsqcut-46|dense2｜new with indi code -fix space</t>
@@ -569,7 +584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T47"/>
+  <dimension ref="A1:T52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -665,26 +680,26 @@
       <c r="I2">
         <v>14156</v>
       </c>
-      <c r="J2">
+      <c r="L2">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="O2">
         <v>0.06836645151013176</v>
       </c>
-      <c r="K2">
-        <v>0.0004250480609163007</v>
-      </c>
-      <c r="M2">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N2">
-        <v>0.005638666708596741</v>
-      </c>
-      <c r="O2">
-        <v>0.009674189396799987</v>
+      <c r="P2">
+        <v>0.004818030126325816</v>
       </c>
       <c r="Q2">
         <v>0.01071193221870467</v>
       </c>
+      <c r="R2">
+        <v>0.005638666708596741</v>
+      </c>
+      <c r="S2">
+        <v>0.0004250480609163007</v>
+      </c>
       <c r="T2">
-        <v>0.004818030126325816</v>
+        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -715,26 +730,26 @@
       <c r="I3">
         <v>11611</v>
       </c>
-      <c r="J3">
+      <c r="L3">
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="O3">
         <v>0.04615441883950755</v>
       </c>
-      <c r="K3">
-        <v>0.0001978384306784256</v>
-      </c>
-      <c r="M3">
-        <v>0.0001631540263502446</v>
-      </c>
-      <c r="N3">
-        <v>0.001779221775169934</v>
-      </c>
-      <c r="O3">
-        <v>0.004580501696160511</v>
+      <c r="P3">
+        <v>0.001592932311570713</v>
       </c>
       <c r="Q3">
         <v>0.00502885184437347</v>
       </c>
+      <c r="R3">
+        <v>0.001779221775169934</v>
+      </c>
+      <c r="S3">
+        <v>0.0001978384306784256</v>
+      </c>
       <c r="T3">
-        <v>0.001592932311570713</v>
+        <v>0.004580501696160511</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -765,26 +780,26 @@
       <c r="I4">
         <v>6771</v>
       </c>
-      <c r="J4">
+      <c r="L4">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="O4">
         <v>0.36470746642943</v>
       </c>
-      <c r="K4">
-        <v>0.0001137832146297872</v>
-      </c>
-      <c r="M4">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N4">
-        <v>0.003094044369724517</v>
-      </c>
-      <c r="O4">
-        <v>0.005813234561065725</v>
+      <c r="P4">
+        <v>0.003193202088483064</v>
       </c>
       <c r="Q4">
         <v>0.005606434133779571</v>
       </c>
+      <c r="R4">
+        <v>0.003094044369724517</v>
+      </c>
+      <c r="S4">
+        <v>0.0001137832146297872</v>
+      </c>
       <c r="T4">
-        <v>0.003193202088483064</v>
+        <v>0.005813234561065725</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -815,26 +830,26 @@
       <c r="I5">
         <v>6771</v>
       </c>
-      <c r="J5">
+      <c r="L5">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="O5">
         <v>0.3564407544954944</v>
       </c>
-      <c r="K5">
-        <v>0.0001152638129503358</v>
-      </c>
-      <c r="M5">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N5">
-        <v>0.003171635367762127</v>
-      </c>
-      <c r="O5">
-        <v>0.005813234561065725</v>
+      <c r="P5">
+        <v>0.003193202088483064</v>
       </c>
       <c r="Q5">
         <v>0.005632685300523813</v>
       </c>
+      <c r="R5">
+        <v>0.003171635367762127</v>
+      </c>
+      <c r="S5">
+        <v>0.0001152638129503358</v>
+      </c>
       <c r="T5">
-        <v>0.003193202088483064</v>
+        <v>0.005813234561065725</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -865,26 +880,26 @@
       <c r="I6">
         <v>42468</v>
       </c>
-      <c r="J6">
+      <c r="L6">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="O6">
         <v>0.269966598412229</v>
       </c>
-      <c r="K6">
-        <v>0.000333070102780211</v>
-      </c>
-      <c r="M6">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N6">
-        <v>0.004616722796530505</v>
-      </c>
-      <c r="O6">
-        <v>0.009674189396799987</v>
+      <c r="P6">
+        <v>0.004818030126325817</v>
       </c>
       <c r="Q6">
         <v>0.009106885821888167</v>
       </c>
+      <c r="R6">
+        <v>0.004616722796530505</v>
+      </c>
+      <c r="S6">
+        <v>0.000333070102780211</v>
+      </c>
       <c r="T6">
-        <v>0.004818030126325817</v>
+        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -915,26 +930,26 @@
       <c r="I7">
         <v>14156</v>
       </c>
-      <c r="J7">
+      <c r="L7">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="O7">
         <v>0.2798459788092014</v>
       </c>
-      <c r="K7">
-        <v>0.0003285627388197843</v>
-      </c>
-      <c r="M7">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N7">
-        <v>0.004615286290830784</v>
-      </c>
-      <c r="O7">
-        <v>0.009674189396799985</v>
+      <c r="P7">
+        <v>0.004818030126325817</v>
       </c>
       <c r="Q7">
         <v>0.008950010380536522</v>
       </c>
+      <c r="R7">
+        <v>0.004615286290830784</v>
+      </c>
+      <c r="S7">
+        <v>0.0003285627388197843</v>
+      </c>
       <c r="T7">
-        <v>0.004818030126325817</v>
+        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -965,26 +980,26 @@
       <c r="I8">
         <v>14156</v>
       </c>
-      <c r="J8">
+      <c r="L8">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="O8">
         <v>0.1860837943045432</v>
       </c>
-      <c r="K8">
-        <v>0.0003713407546776094</v>
-      </c>
-      <c r="M8">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N8">
-        <v>0.004590555422836876</v>
-      </c>
-      <c r="O8">
-        <v>0.009674189396799985</v>
+      <c r="P8">
+        <v>0.004818030126325816</v>
       </c>
       <c r="Q8">
         <v>0.00941140169945745</v>
       </c>
+      <c r="R8">
+        <v>0.004590555422836876</v>
+      </c>
+      <c r="S8">
+        <v>0.0003713407546776094</v>
+      </c>
       <c r="T8">
-        <v>0.004818030126325816</v>
+        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -1015,26 +1030,26 @@
       <c r="I9">
         <v>24768</v>
       </c>
-      <c r="J9">
+      <c r="L9">
+        <v>0.0001796235360933539</v>
+      </c>
+      <c r="O9">
         <v>-0.00724317687482956</v>
       </c>
-      <c r="K9">
-        <v>0.0002632414236722758</v>
-      </c>
-      <c r="M9">
-        <v>0.0001796235360933539</v>
-      </c>
-      <c r="N9">
-        <v>0.004275415213561056</v>
-      </c>
-      <c r="O9">
-        <v>0.006875190708555331</v>
+      <c r="P9">
+        <v>0.003559726400188349</v>
       </c>
       <c r="Q9">
         <v>0.008363098231375462</v>
       </c>
+      <c r="R9">
+        <v>0.004275415213561056</v>
+      </c>
+      <c r="S9">
+        <v>0.0002632414236722758</v>
+      </c>
       <c r="T9">
-        <v>0.003559726400188349</v>
+        <v>0.006875190708555331</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -1065,26 +1080,26 @@
       <c r="I10">
         <v>14156</v>
       </c>
-      <c r="J10">
+      <c r="L10">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="O10">
         <v>0.1565886089862186</v>
       </c>
-      <c r="K10">
-        <v>0.0003847976244374441</v>
-      </c>
-      <c r="M10">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N10">
-        <v>0.005167135423672592</v>
-      </c>
-      <c r="O10">
-        <v>0.009674189396799985</v>
+      <c r="P10">
+        <v>0.004818030126325816</v>
       </c>
       <c r="Q10">
         <v>0.009901025034115019</v>
       </c>
+      <c r="R10">
+        <v>0.005167135423672592</v>
+      </c>
+      <c r="S10">
+        <v>0.0003847976244374441</v>
+      </c>
       <c r="T10">
-        <v>0.004818030126325817</v>
+        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1115,26 +1130,26 @@
       <c r="I11">
         <v>11542</v>
       </c>
-      <c r="J11">
+      <c r="L11">
+        <v>0.000163888349337522</v>
+      </c>
+      <c r="O11">
         <v>-0.005102592401121431</v>
       </c>
-      <c r="K11">
-        <v>0.000209188838038313</v>
-      </c>
-      <c r="M11">
-        <v>0.000163888349337522</v>
-      </c>
-      <c r="N11">
-        <v>0.001602037466360856</v>
-      </c>
-      <c r="O11">
-        <v>0.004589584286176587</v>
+      <c r="P11">
+        <v>0.001597174444307401</v>
       </c>
       <c r="Q11">
         <v>0.00512210974064752</v>
       </c>
+      <c r="R11">
+        <v>0.001602037466360856</v>
+      </c>
+      <c r="S11">
+        <v>0.000209188838038313</v>
+      </c>
       <c r="T11">
-        <v>0.001597174444307401</v>
+        <v>0.004589584286176587</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -1165,26 +1180,26 @@
       <c r="I12">
         <v>6771</v>
       </c>
-      <c r="J12">
+      <c r="L12">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="O12">
         <v>0.3693483364419842</v>
       </c>
-      <c r="K12">
-        <v>0.000112952017849086</v>
-      </c>
-      <c r="M12">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N12">
-        <v>0.002682213716882752</v>
-      </c>
-      <c r="O12">
-        <v>0.005813234561065725</v>
+      <c r="P12">
+        <v>0.003193202088483064</v>
       </c>
       <c r="Q12">
         <v>0.00526064949972486</v>
       </c>
+      <c r="R12">
+        <v>0.002682213716882752</v>
+      </c>
+      <c r="S12">
+        <v>0.000112952017849086</v>
+      </c>
       <c r="T12">
-        <v>0.003193202088483064</v>
+        <v>0.005813234561065725</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -1215,26 +1230,26 @@
       <c r="I13">
         <v>6771</v>
       </c>
-      <c r="J13">
+      <c r="L13">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="O13">
         <v>0.2122246979933391</v>
       </c>
-      <c r="K13">
-        <v>0.0001410934357507483</v>
-      </c>
-      <c r="M13">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N13">
-        <v>0.003030311329129174</v>
-      </c>
-      <c r="O13">
-        <v>0.005813234561065723</v>
+      <c r="P13">
+        <v>0.003193202088483064</v>
       </c>
       <c r="Q13">
         <v>0.006002887168865449</v>
       </c>
+      <c r="R13">
+        <v>0.003030311329129174</v>
+      </c>
+      <c r="S13">
+        <v>0.0001410934357507483</v>
+      </c>
       <c r="T13">
-        <v>0.003193202088483064</v>
+        <v>0.005813234561065723</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -1265,26 +1280,26 @@
       <c r="I14">
         <v>11611</v>
       </c>
-      <c r="J14">
+      <c r="L14">
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="O14">
         <v>-0.01180186309853548</v>
       </c>
-      <c r="K14">
-        <v>0.0002098592232396584</v>
-      </c>
-      <c r="M14">
-        <v>0.0001631540263502446</v>
-      </c>
-      <c r="N14">
-        <v>0.00173711317318318</v>
-      </c>
-      <c r="O14">
-        <v>0.004580501696160511</v>
+      <c r="P14">
+        <v>0.001592932311570713</v>
       </c>
       <c r="Q14">
         <v>0.005213165544267774</v>
       </c>
+      <c r="R14">
+        <v>0.00173711317318318</v>
+      </c>
+      <c r="S14">
+        <v>0.0002098592232396584</v>
+      </c>
       <c r="T14">
-        <v>0.001592932311570713</v>
+        <v>0.004580501696160511</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -1315,26 +1330,26 @@
       <c r="I15">
         <v>49</v>
       </c>
-      <c r="J15">
+      <c r="L15">
+        <v>0.0001158352549329261</v>
+      </c>
+      <c r="O15">
         <v>-0.01652918306199047</v>
       </c>
-      <c r="K15">
-        <v>0.0003123469992588732</v>
-      </c>
-      <c r="M15">
-        <v>0.0001158352549329261</v>
-      </c>
-      <c r="N15">
-        <v>0.002972419699024923</v>
-      </c>
-      <c r="O15">
-        <v>0.004529835290885987</v>
+      <c r="P15">
+        <v>0.00129198945232948</v>
       </c>
       <c r="Q15">
         <v>0.007217175147339313</v>
       </c>
+      <c r="R15">
+        <v>0.002972419699024923</v>
+      </c>
+      <c r="S15">
+        <v>0.0003123469992588732</v>
+      </c>
       <c r="T15">
-        <v>0.00129198945232948</v>
+        <v>0.004529835290885987</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -1342,49 +1357,49 @@
         <v>34</v>
       </c>
       <c r="B16">
-        <v>0.009164293356549506</v>
+        <v>0.01042798137117382</v>
       </c>
       <c r="C16">
-        <v>0.008733878054388279</v>
+        <v>0.009812042985245533</v>
       </c>
       <c r="D16">
-        <v>0.0001865208677798922</v>
+        <v>0.0002839828498694114</v>
       </c>
       <c r="E16">
-        <v>0.0001961492659581503</v>
+        <v>0.000297330738550053</v>
       </c>
       <c r="F16">
-        <v>0.1708507589293765</v>
+        <v>0.1884050333044567</v>
       </c>
       <c r="G16">
-        <v>0.1280492261183164</v>
+        <v>0.1502580843805948</v>
       </c>
       <c r="H16">
-        <v>0.2582640092197721</v>
+        <v>0.2597560818810524</v>
       </c>
       <c r="I16">
-        <v>14156</v>
-      </c>
-      <c r="J16">
-        <v>0.1218694481841025</v>
-      </c>
-      <c r="K16">
-        <v>0.0004006378783650764</v>
-      </c>
-      <c r="M16">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N16">
-        <v>0.005239736253559311</v>
+        <v>12741</v>
+      </c>
+      <c r="L16">
+        <v>0.0003441387227458278</v>
       </c>
       <c r="O16">
-        <v>0.009674189396799987</v>
+        <v>0.1379172254546043</v>
+      </c>
+      <c r="P16">
+        <v>0.004797770485226469</v>
       </c>
       <c r="Q16">
-        <v>0.0102119158074488</v>
+        <v>0.01033009227796955</v>
+      </c>
+      <c r="R16">
+        <v>0.005554310648909318</v>
+      </c>
+      <c r="S16">
+        <v>0.0004007814960332574</v>
       </c>
       <c r="T16">
-        <v>0.004818030126325817</v>
+        <v>0.009714954248817111</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -1392,49 +1407,49 @@
         <v>35</v>
       </c>
       <c r="B17">
-        <v>0.005791630591612971</v>
+        <v>0.00997695293896445</v>
       </c>
       <c r="C17">
-        <v>0.005699109365498782</v>
+        <v>0.009631259951277263</v>
       </c>
       <c r="D17">
-        <v>8.698446620952695E-05</v>
+        <v>0.0002746516022984678</v>
       </c>
       <c r="E17">
-        <v>9.470932808225897E-05</v>
+        <v>0.000318358280400409</v>
       </c>
       <c r="F17">
-        <v>0.3164189910555092</v>
+        <v>0.272470124651383</v>
       </c>
       <c r="G17">
-        <v>0.2557119579146814</v>
+        <v>0.156694670201814</v>
       </c>
       <c r="H17">
-        <v>0.4208397194991282</v>
+        <v>0.4558883625799528</v>
       </c>
       <c r="I17">
-        <v>6771</v>
-      </c>
-      <c r="J17">
-        <v>0.2606707993949464</v>
-      </c>
-      <c r="K17">
-        <v>0.0001324165619288979</v>
-      </c>
-      <c r="M17">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N17">
-        <v>0.003330775568204595</v>
+        <v>1284</v>
+      </c>
+      <c r="L17">
+        <v>0.0002640644396388745</v>
       </c>
       <c r="O17">
-        <v>0.005813234561065725</v>
+        <v>0.2289566739349258</v>
+      </c>
+      <c r="P17">
+        <v>0.004252957223118693</v>
       </c>
       <c r="Q17">
-        <v>0.006002882908757912</v>
+        <v>0.009685349739034687</v>
+      </c>
+      <c r="R17">
+        <v>0.005106524251936465</v>
+      </c>
+      <c r="S17">
+        <v>0.0003741973334738424</v>
       </c>
       <c r="T17">
-        <v>0.003193202088483064</v>
+        <v>0.009204693368560462</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -1442,49 +1457,49 @@
         <v>36</v>
       </c>
       <c r="B18">
-        <v>0.005611881407010991</v>
+        <v>0.0102733372090916</v>
       </c>
       <c r="C18">
-        <v>0.005639127357765789</v>
+        <v>0.00987889837479569</v>
       </c>
       <c r="D18">
-        <v>8.431607544410066E-05</v>
+        <v>0.0002816309717823605</v>
       </c>
       <c r="E18">
-        <v>9.102681873913914E-05</v>
+        <v>0.0003034120436381377</v>
       </c>
       <c r="F18">
-        <v>0.291056300795216</v>
+        <v>0.204771852061556</v>
       </c>
       <c r="G18">
-        <v>0.2346312460124846</v>
+        <v>0.1432696624324651</v>
       </c>
       <c r="H18">
-        <v>0.4208397194991282</v>
+        <v>0.2595879210340796</v>
       </c>
       <c r="I18">
-        <v>6771</v>
-      </c>
-      <c r="J18">
-        <v>0.2046421514566161</v>
-      </c>
-      <c r="K18">
-        <v>0.0001424514975481683</v>
-      </c>
-      <c r="M18">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N18">
-        <v>0.002972129451884979</v>
+        <v>12051</v>
+      </c>
+      <c r="L18">
+        <v>0.0003482779314587717</v>
       </c>
       <c r="O18">
-        <v>0.005813234561065725</v>
+        <v>0.1478874304814285</v>
+      </c>
+      <c r="P18">
+        <v>0.004769747765218425</v>
       </c>
       <c r="Q18">
-        <v>0.00595976388177965</v>
+        <v>0.01017444484578581</v>
+      </c>
+      <c r="R18">
+        <v>0.005371111699895803</v>
+      </c>
+      <c r="S18">
+        <v>0.0004008200453677453</v>
       </c>
       <c r="T18">
-        <v>0.003193202088483064</v>
+        <v>0.009769435123820693</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -1492,49 +1507,49 @@
         <v>37</v>
       </c>
       <c r="B19">
-        <v>0.005713567326092179</v>
+        <v>0.009164293356549506</v>
       </c>
       <c r="C19">
-        <v>0.005699109365498782</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D19">
-        <v>8.903433264960941E-05</v>
+        <v>0.0001865208677798922</v>
       </c>
       <c r="E19">
-        <v>9.470932808225897E-05</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F19">
-        <v>0.3003097955821736</v>
+        <v>0.1708507589293765</v>
       </c>
       <c r="G19">
-        <v>0.2557119579146814</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H19">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I19">
-        <v>6771</v>
-      </c>
-      <c r="J19">
-        <v>0.2264121702660996</v>
-      </c>
-      <c r="K19">
-        <v>0.00013855240761432</v>
-      </c>
-      <c r="M19">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N19">
-        <v>0.003005755874836842</v>
+        <v>14156</v>
+      </c>
+      <c r="L19">
+        <v>0.0003384092866814527</v>
       </c>
       <c r="O19">
-        <v>0.005813234561065725</v>
+        <v>0.1218694481841025</v>
+      </c>
+      <c r="P19">
+        <v>0.004818030126325817</v>
       </c>
       <c r="Q19">
-        <v>0.00592641693601841</v>
+        <v>0.0102119158074488</v>
+      </c>
+      <c r="R19">
+        <v>0.005239736253559311</v>
+      </c>
+      <c r="S19">
+        <v>0.0004006378783650764</v>
       </c>
       <c r="T19">
-        <v>0.003193202088483064</v>
+        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -1542,49 +1557,49 @@
         <v>38</v>
       </c>
       <c r="B20">
-        <v>0.007927365294981236</v>
+        <v>0.005791630591612971</v>
       </c>
       <c r="C20">
-        <v>0.008722720041403264</v>
+        <v>0.005699109365498782</v>
       </c>
       <c r="D20">
-        <v>0.000143672851475712</v>
+        <v>8.698446620952695E-05</v>
       </c>
       <c r="E20">
-        <v>0.0001985649052123504</v>
+        <v>9.470932808225897E-05</v>
       </c>
       <c r="F20">
-        <v>0.3830412447229715</v>
+        <v>0.3164189910555092</v>
       </c>
       <c r="G20">
-        <v>0.147324247391146</v>
+        <v>0.2557119579146814</v>
       </c>
       <c r="H20">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I20">
-        <v>14156</v>
-      </c>
-      <c r="J20">
-        <v>0.2810892232598902</v>
-      </c>
-      <c r="K20">
-        <v>0.0003279955215444224</v>
-      </c>
-      <c r="M20">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N20">
-        <v>0.004617426367895965</v>
+        <v>6771</v>
+      </c>
+      <c r="L20">
+        <v>0.0001037297229528328</v>
       </c>
       <c r="O20">
-        <v>0.009674189396799985</v>
+        <v>0.2606707993949464</v>
+      </c>
+      <c r="P20">
+        <v>0.003193202088483064</v>
       </c>
       <c r="Q20">
-        <v>0.008942022948316988</v>
+        <v>0.006002882908757912</v>
+      </c>
+      <c r="R20">
+        <v>0.003330775568204595</v>
+      </c>
+      <c r="S20">
+        <v>0.0001324165619288979</v>
       </c>
       <c r="T20">
-        <v>0.004818030126325817</v>
+        <v>0.005813234561065725</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -1592,49 +1607,49 @@
         <v>39</v>
       </c>
       <c r="B21">
-        <v>0.003031636244261009</v>
+        <v>0.005611881407010991</v>
       </c>
       <c r="C21">
-        <v>0.002499571894821071</v>
+        <v>0.005639127357765789</v>
       </c>
       <c r="D21">
-        <v>1.91501667802569E-05</v>
+        <v>8.431607544410066E-05</v>
       </c>
       <c r="E21">
-        <v>1.967007435869721E-05</v>
+        <v>9.102681873913914E-05</v>
       </c>
       <c r="F21">
-        <v>-0.01488433510101705</v>
+        <v>0.291056300795216</v>
       </c>
       <c r="G21">
-        <v>-0.04243741404356438</v>
+        <v>0.2346312460124846</v>
       </c>
       <c r="H21">
-        <v>0.2133795918767654</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I21">
-        <v>11611</v>
-      </c>
-      <c r="J21">
-        <v>-0.004454544482717981</v>
-      </c>
-      <c r="K21">
-        <v>0.0002083353057278959</v>
-      </c>
-      <c r="M21">
-        <v>0.0001631540263502446</v>
-      </c>
-      <c r="N21">
-        <v>0.001554417436991534</v>
+        <v>6771</v>
+      </c>
+      <c r="L21">
+        <v>0.0001037297229528328</v>
       </c>
       <c r="O21">
-        <v>0.004580501696160511</v>
+        <v>0.2046421514566161</v>
+      </c>
+      <c r="P21">
+        <v>0.003193202088483064</v>
       </c>
       <c r="Q21">
-        <v>0.005089153979501482</v>
+        <v>0.00595976388177965</v>
+      </c>
+      <c r="R21">
+        <v>0.002972129451884979</v>
+      </c>
+      <c r="S21">
+        <v>0.0001424514975481683</v>
       </c>
       <c r="T21">
-        <v>0.001592932311570713</v>
+        <v>0.005813234561065725</v>
       </c>
     </row>
     <row r="22" spans="1:20">
@@ -1642,49 +1657,49 @@
         <v>40</v>
       </c>
       <c r="B22">
-        <v>0.00784507820846319</v>
+        <v>0.005713567326092179</v>
       </c>
       <c r="C22">
-        <v>0.008722720041403264</v>
+        <v>0.005699109365498782</v>
       </c>
       <c r="D22">
-        <v>0.0001417160098566256</v>
+        <v>8.903433264960941E-05</v>
       </c>
       <c r="E22">
-        <v>0.0001985649052123504</v>
+        <v>9.470932808225897E-05</v>
       </c>
       <c r="F22">
-        <v>0.3914442976114285</v>
+        <v>0.3003097955821736</v>
       </c>
       <c r="G22">
-        <v>0.147324247391146</v>
+        <v>0.2557119579146814</v>
       </c>
       <c r="H22">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I22">
-        <v>14156</v>
-      </c>
-      <c r="J22">
-        <v>0.2865909829079945</v>
-      </c>
-      <c r="K22">
-        <v>0.0003254854012574867</v>
-      </c>
-      <c r="M22">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N22">
-        <v>0.00456770441607247</v>
+        <v>6771</v>
+      </c>
+      <c r="L22">
+        <v>0.0001037297229528328</v>
       </c>
       <c r="O22">
-        <v>0.009674189396799985</v>
+        <v>0.2264121702660996</v>
+      </c>
+      <c r="P22">
+        <v>0.003193202088483064</v>
       </c>
       <c r="Q22">
-        <v>0.008855143980453176</v>
+        <v>0.00592641693601841</v>
+      </c>
+      <c r="R22">
+        <v>0.003005755874836842</v>
+      </c>
+      <c r="S22">
+        <v>0.00013855240761432</v>
       </c>
       <c r="T22">
-        <v>0.004818030126325816</v>
+        <v>0.005813234561065725</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -1692,49 +1707,49 @@
         <v>41</v>
       </c>
       <c r="B23">
-        <v>0.003103990424644728</v>
+        <v>0.007927365294981236</v>
       </c>
       <c r="C23">
-        <v>0.00254141838673398</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D23">
-        <v>2.156002471405648E-05</v>
+        <v>0.000143672851475712</v>
       </c>
       <c r="E23">
-        <v>2.106152912726658E-05</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F23">
-        <v>-0.02262657763782516</v>
+        <v>0.3830412447229715</v>
       </c>
       <c r="G23">
-        <v>0.001017868166272584</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H23">
-        <v>0.212555477012045</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I23">
-        <v>11542</v>
-      </c>
-      <c r="J23">
-        <v>-0.005012774390606101</v>
-      </c>
-      <c r="K23">
-        <v>0.0002091701444985722</v>
-      </c>
-      <c r="M23">
-        <v>0.000163888349337522</v>
-      </c>
-      <c r="N23">
-        <v>0.001583264354559398</v>
+        <v>14156</v>
+      </c>
+      <c r="L23">
+        <v>0.0003384092866814527</v>
       </c>
       <c r="O23">
-        <v>0.004589584286176587</v>
+        <v>0.2810892232598902</v>
+      </c>
+      <c r="P23">
+        <v>0.004818030126325817</v>
       </c>
       <c r="Q23">
-        <v>0.00510134746390362</v>
+        <v>0.008942022948316988</v>
+      </c>
+      <c r="R23">
+        <v>0.004617426367895965</v>
+      </c>
+      <c r="S23">
+        <v>0.0003279955215444224</v>
       </c>
       <c r="T23">
-        <v>0.001597174444307401</v>
+        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="24" spans="1:20">
@@ -1742,49 +1757,49 @@
         <v>42</v>
       </c>
       <c r="B24">
-        <v>0.005895505445859815</v>
+        <v>0.003031636244261009</v>
       </c>
       <c r="C24">
-        <v>0.005670204101840715</v>
+        <v>0.002499571894821071</v>
       </c>
       <c r="D24">
-        <v>9.166134936686534E-05</v>
+        <v>1.91501667802569E-05</v>
       </c>
       <c r="E24">
-        <v>9.344840654260834E-05</v>
+        <v>1.967007435869721E-05</v>
       </c>
       <c r="F24">
-        <v>0.255037895389058</v>
+        <v>-0.01488433510101705</v>
       </c>
       <c r="G24">
-        <v>0.2405138906269937</v>
+        <v>-0.04243741404356438</v>
       </c>
       <c r="H24">
-        <v>0.4208397194991282</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I24">
-        <v>6771</v>
-      </c>
-      <c r="J24">
-        <v>0.2028896166553128</v>
-      </c>
-      <c r="K24">
-        <v>0.0001427653829362463</v>
-      </c>
-      <c r="M24">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N24">
-        <v>0.003125364361436701</v>
+        <v>11611</v>
+      </c>
+      <c r="L24">
+        <v>0.0001631540263502446</v>
       </c>
       <c r="O24">
-        <v>0.005813234561065723</v>
+        <v>-0.004454544482717981</v>
+      </c>
+      <c r="P24">
+        <v>0.001592932311570713</v>
       </c>
       <c r="Q24">
-        <v>0.006096382291329448</v>
+        <v>0.005089153979501482</v>
+      </c>
+      <c r="R24">
+        <v>0.001554417436991534</v>
+      </c>
+      <c r="S24">
+        <v>0.0002083353057278959</v>
       </c>
       <c r="T24">
-        <v>0.003193202088483064</v>
+        <v>0.004580501696160511</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -1792,49 +1807,49 @@
         <v>43</v>
       </c>
       <c r="B25">
-        <v>0.005903838435270049</v>
+        <v>0.00784507820846319</v>
       </c>
       <c r="C25">
-        <v>0.005670204101840715</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D25">
-        <v>9.181732856753832E-05</v>
+        <v>0.0001417160098566256</v>
       </c>
       <c r="E25">
-        <v>9.344840654260834E-05</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F25">
-        <v>0.2537702008328302</v>
+        <v>0.3914442976114285</v>
       </c>
       <c r="G25">
-        <v>0.2405138906269937</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H25">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I25">
-        <v>6771</v>
-      </c>
-      <c r="J25">
-        <v>0.1996305390032257</v>
-      </c>
-      <c r="K25">
-        <v>0.0001433490956550128</v>
-      </c>
-      <c r="M25">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N25">
-        <v>0.003163476470023769</v>
+        <v>14156</v>
+      </c>
+      <c r="L25">
+        <v>0.0003384092866814527</v>
       </c>
       <c r="O25">
-        <v>0.005813234561065723</v>
+        <v>0.2865909829079945</v>
+      </c>
+      <c r="P25">
+        <v>0.004818030126325816</v>
       </c>
       <c r="Q25">
-        <v>0.00610593491672969</v>
+        <v>0.008855143980453176</v>
+      </c>
+      <c r="R25">
+        <v>0.00456770441607247</v>
+      </c>
+      <c r="S25">
+        <v>0.0003254854012574867</v>
       </c>
       <c r="T25">
-        <v>0.003193202088483064</v>
+        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="26" spans="1:20">
@@ -1842,49 +1857,49 @@
         <v>44</v>
       </c>
       <c r="B26">
-        <v>0.005871671098387516</v>
+        <v>0.003103990424644728</v>
       </c>
       <c r="C26">
-        <v>0.005670204101840715</v>
+        <v>0.00254141838673398</v>
       </c>
       <c r="D26">
-        <v>9.132537185586264E-05</v>
+        <v>2.156002471405648E-05</v>
       </c>
       <c r="E26">
-        <v>9.344840654260834E-05</v>
+        <v>2.106152912726658E-05</v>
       </c>
       <c r="F26">
-        <v>0.2577684957503591</v>
+        <v>-0.02262657763782516</v>
       </c>
       <c r="G26">
-        <v>0.2405138906269937</v>
+        <v>0.001017868166272584</v>
       </c>
       <c r="H26">
-        <v>0.4208397194991282</v>
+        <v>0.212555477012045</v>
       </c>
       <c r="I26">
-        <v>6771</v>
-      </c>
-      <c r="J26">
-        <v>0.2020008505541708</v>
-      </c>
-      <c r="K26">
-        <v>0.0001429245641932233</v>
-      </c>
-      <c r="M26">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N26">
-        <v>0.003090643964573058</v>
+        <v>11542</v>
+      </c>
+      <c r="L26">
+        <v>0.000163888349337522</v>
       </c>
       <c r="O26">
-        <v>0.005813234561065723</v>
+        <v>-0.005012774390606101</v>
+      </c>
+      <c r="P26">
+        <v>0.001597174444307401</v>
       </c>
       <c r="Q26">
-        <v>0.006067498374332903</v>
+        <v>0.00510134746390362</v>
+      </c>
+      <c r="R26">
+        <v>0.001583264354559398</v>
+      </c>
+      <c r="S26">
+        <v>0.0002091701444985722</v>
       </c>
       <c r="T26">
-        <v>0.003193202088483064</v>
+        <v>0.004589584286176587</v>
       </c>
     </row>
     <row r="27" spans="1:20">
@@ -1892,49 +1907,49 @@
         <v>45</v>
       </c>
       <c r="B27">
-        <v>0.00304699828992123</v>
+        <v>0.005895505445859815</v>
       </c>
       <c r="C27">
-        <v>0.002499571894821071</v>
+        <v>0.005670204101840715</v>
       </c>
       <c r="D27">
-        <v>1.903121423403654E-05</v>
+        <v>9.166134936686534E-05</v>
       </c>
       <c r="E27">
-        <v>1.967007435869721E-05</v>
+        <v>9.344840654260834E-05</v>
       </c>
       <c r="F27">
-        <v>-0.008580312939503454</v>
+        <v>0.255037895389058</v>
       </c>
       <c r="G27">
-        <v>-0.04243741404356438</v>
+        <v>0.2405138906269937</v>
       </c>
       <c r="H27">
-        <v>0.2133795918767654</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I27">
-        <v>11611</v>
-      </c>
-      <c r="J27">
-        <v>-0.002771209789547591</v>
-      </c>
-      <c r="K27">
-        <v>0.000207986162951978</v>
-      </c>
-      <c r="M27">
-        <v>0.0001631540263502446</v>
-      </c>
-      <c r="N27">
-        <v>0.001554596452837835</v>
+        <v>6771</v>
+      </c>
+      <c r="L27">
+        <v>0.0001037297229528328</v>
       </c>
       <c r="O27">
-        <v>0.004580501696160511</v>
+        <v>0.2028896166553128</v>
+      </c>
+      <c r="P27">
+        <v>0.003193202088483064</v>
       </c>
       <c r="Q27">
-        <v>0.005107549406927882</v>
+        <v>0.006096382291329448</v>
+      </c>
+      <c r="R27">
+        <v>0.003125364361436701</v>
+      </c>
+      <c r="S27">
+        <v>0.0001427653829362463</v>
       </c>
       <c r="T27">
-        <v>0.001592932311570713</v>
+        <v>0.005813234561065723</v>
       </c>
     </row>
     <row r="28" spans="1:20">
@@ -1942,19 +1957,19 @@
         <v>46</v>
       </c>
       <c r="B28">
-        <v>0.006549373422714545</v>
+        <v>0.005903838435270049</v>
       </c>
       <c r="C28">
         <v>0.005670204101840715</v>
       </c>
       <c r="D28">
-        <v>0.0001064697656049724</v>
+        <v>9.181732856753832E-05</v>
       </c>
       <c r="E28">
         <v>9.344840654260834E-05</v>
       </c>
       <c r="F28">
-        <v>0.1346849985258249</v>
+        <v>0.2537702008328302</v>
       </c>
       <c r="G28">
         <v>0.2405138906269937</v>
@@ -1965,26 +1980,26 @@
       <c r="I28">
         <v>6771</v>
       </c>
-      <c r="J28">
-        <v>0.1058242633905934</v>
-      </c>
-      <c r="K28">
-        <v>0.000160150142460433</v>
-      </c>
-      <c r="M28">
+      <c r="L28">
         <v>0.0001037297229528328</v>
       </c>
-      <c r="N28">
-        <v>0.003715325925925931</v>
-      </c>
       <c r="O28">
+        <v>0.1996305390032257</v>
+      </c>
+      <c r="P28">
+        <v>0.003193202088483064</v>
+      </c>
+      <c r="Q28">
+        <v>0.00610593491672969</v>
+      </c>
+      <c r="R28">
+        <v>0.003163476470023769</v>
+      </c>
+      <c r="S28">
+        <v>0.0001433490956550128</v>
+      </c>
+      <c r="T28">
         <v>0.005813234561065723</v>
-      </c>
-      <c r="Q28">
-        <v>0.006776662396495037</v>
-      </c>
-      <c r="T28">
-        <v>0.003193202088483064</v>
       </c>
     </row>
     <row r="29" spans="1:20">
@@ -1992,49 +2007,49 @@
         <v>47</v>
       </c>
       <c r="B29">
-        <v>0.002783525716284511</v>
+        <v>0.005871671098387516</v>
       </c>
       <c r="C29">
-        <v>0.002457544020376962</v>
+        <v>0.005670204101840715</v>
       </c>
       <c r="D29">
-        <v>1.713865210259099E-05</v>
+        <v>9.132537185586264E-05</v>
       </c>
       <c r="E29">
-        <v>1.89022549270271E-05</v>
+        <v>9.344840654260834E-05</v>
       </c>
       <c r="F29">
-        <v>-0.05370835704473098</v>
+        <v>0.2577684957503591</v>
       </c>
       <c r="G29">
-        <v>-0.1621371309933592</v>
+        <v>0.2405138906269937</v>
       </c>
       <c r="H29">
-        <v>0.3649062991209757</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I29">
-        <v>4010</v>
-      </c>
-      <c r="J29">
-        <v>-0.006214540120261569</v>
-      </c>
-      <c r="K29">
-        <v>0.0002742305932959652</v>
-      </c>
-      <c r="M29">
-        <v>0.0001730864695810989</v>
-      </c>
-      <c r="N29">
-        <v>0.001362431751651251</v>
+        <v>6771</v>
+      </c>
+      <c r="L29">
+        <v>0.0001037297229528328</v>
       </c>
       <c r="O29">
-        <v>0.004349183403839366</v>
+        <v>0.2020008505541708</v>
+      </c>
+      <c r="P29">
+        <v>0.003193202088483064</v>
       </c>
       <c r="Q29">
-        <v>0.004501420066184821</v>
+        <v>0.006067498374332903</v>
+      </c>
+      <c r="R29">
+        <v>0.003090643964573058</v>
+      </c>
+      <c r="S29">
+        <v>0.0001429245641932233</v>
       </c>
       <c r="T29">
-        <v>0.001438312583710056</v>
+        <v>0.005813234561065723</v>
       </c>
     </row>
     <row r="30" spans="1:20">
@@ -2042,49 +2057,49 @@
         <v>48</v>
       </c>
       <c r="B30">
-        <v>0.00929322862430519</v>
+        <v>0.00304699828992123</v>
       </c>
       <c r="C30">
-        <v>0.008733878054388279</v>
+        <v>0.002499571894821071</v>
       </c>
       <c r="D30">
-        <v>0.000192984991667648</v>
+        <v>1.903121423403654E-05</v>
       </c>
       <c r="E30">
-        <v>0.0001961492659581503</v>
+        <v>1.967007435869721E-05</v>
       </c>
       <c r="F30">
-        <v>0.1421155108066621</v>
+        <v>-0.008580312939503454</v>
       </c>
       <c r="G30">
-        <v>0.1280492261183164</v>
+        <v>-0.04243741404356438</v>
       </c>
       <c r="H30">
-        <v>0.2582640092197721</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I30">
-        <v>14156</v>
-      </c>
-      <c r="J30">
-        <v>0.1230344532976788</v>
-      </c>
-      <c r="K30">
-        <v>0.0004001063569688302</v>
-      </c>
-      <c r="M30">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N30">
-        <v>0.005409147625572685</v>
+        <v>11611</v>
+      </c>
+      <c r="L30">
+        <v>0.0001631540263502446</v>
       </c>
       <c r="O30">
-        <v>0.009674189396799987</v>
+        <v>-0.002771209789547591</v>
+      </c>
+      <c r="P30">
+        <v>0.001592932311570713</v>
       </c>
       <c r="Q30">
-        <v>0.01035431191953904</v>
+        <v>0.005107549406927882</v>
+      </c>
+      <c r="R30">
+        <v>0.001554596452837835</v>
+      </c>
+      <c r="S30">
+        <v>0.000207986162951978</v>
       </c>
       <c r="T30">
-        <v>0.004818030126325817</v>
+        <v>0.004580501696160511</v>
       </c>
     </row>
     <row r="31" spans="1:20">
@@ -2092,49 +2107,49 @@
         <v>49</v>
       </c>
       <c r="B31">
-        <v>0.003030458698074221</v>
+        <v>0.006549373422714545</v>
       </c>
       <c r="C31">
-        <v>0.002499571894821071</v>
+        <v>0.005670204101840715</v>
       </c>
       <c r="D31">
-        <v>1.91281128971015E-05</v>
+        <v>0.0001064697656049724</v>
       </c>
       <c r="E31">
-        <v>1.967007435869721E-05</v>
+        <v>9.344840654260834E-05</v>
       </c>
       <c r="F31">
-        <v>-0.01371556509502225</v>
+        <v>0.1346849985258249</v>
       </c>
       <c r="G31">
-        <v>-0.04243741404356438</v>
+        <v>0.2405138906269937</v>
       </c>
       <c r="H31">
-        <v>0.2133795918767654</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I31">
-        <v>11611</v>
-      </c>
-      <c r="J31">
-        <v>-0.00353431378743374</v>
-      </c>
-      <c r="K31">
-        <v>0.0002081444394071696</v>
-      </c>
-      <c r="M31">
-        <v>0.0001631540263502446</v>
-      </c>
-      <c r="N31">
-        <v>0.001547174514616301</v>
+        <v>6771</v>
+      </c>
+      <c r="L31">
+        <v>0.0001037297229528328</v>
       </c>
       <c r="O31">
-        <v>0.004580501696160511</v>
+        <v>0.1058242633905934</v>
+      </c>
+      <c r="P31">
+        <v>0.003193202088483064</v>
       </c>
       <c r="Q31">
-        <v>0.005089488294347637</v>
+        <v>0.006776662396495037</v>
+      </c>
+      <c r="R31">
+        <v>0.003715325925925931</v>
+      </c>
+      <c r="S31">
+        <v>0.000160150142460433</v>
       </c>
       <c r="T31">
-        <v>0.001592932311570713</v>
+        <v>0.005813234561065723</v>
       </c>
     </row>
     <row r="32" spans="1:20">
@@ -2142,49 +2157,49 @@
         <v>50</v>
       </c>
       <c r="B32">
-        <v>0.008384122629515654</v>
+        <v>0.002783525716284511</v>
       </c>
       <c r="C32">
-        <v>0.008722720041403264</v>
+        <v>0.002457544020376962</v>
       </c>
       <c r="D32">
-        <v>0.0001620814063416336</v>
+        <v>1.713865210259099E-05</v>
       </c>
       <c r="E32">
-        <v>0.0001985649052123504</v>
+        <v>1.89022549270271E-05</v>
       </c>
       <c r="F32">
-        <v>0.3039913826239528</v>
+        <v>-0.05370835704473098</v>
       </c>
       <c r="G32">
-        <v>0.147324247391146</v>
+        <v>-0.1621371309933592</v>
       </c>
       <c r="H32">
-        <v>0.2582640092197721</v>
+        <v>0.3649062991209757</v>
       </c>
       <c r="I32">
-        <v>14156</v>
-      </c>
-      <c r="J32">
-        <v>0.2085500335179142</v>
-      </c>
-      <c r="K32">
-        <v>0.0003610907680501377</v>
-      </c>
-      <c r="M32">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N32">
-        <v>0.004884082851211167</v>
+        <v>4010</v>
+      </c>
+      <c r="L32">
+        <v>0.0001730864695810989</v>
       </c>
       <c r="O32">
-        <v>0.009674189396799985</v>
+        <v>-0.006214540120261569</v>
+      </c>
+      <c r="P32">
+        <v>0.001438312583710056</v>
       </c>
       <c r="Q32">
-        <v>0.009406309171688502</v>
+        <v>0.004501420066184821</v>
+      </c>
+      <c r="R32">
+        <v>0.001362431751651251</v>
+      </c>
+      <c r="S32">
+        <v>0.0002742305932959652</v>
       </c>
       <c r="T32">
-        <v>0.004818030126325816</v>
+        <v>0.004349183403839366</v>
       </c>
     </row>
     <row r="33" spans="1:20">
@@ -2192,22 +2207,22 @@
         <v>51</v>
       </c>
       <c r="B33">
-        <v>0.008519531777817098</v>
+        <v>0.00929322862430519</v>
       </c>
       <c r="C33">
-        <v>0.008722720041403264</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D33">
-        <v>0.0001673145877462598</v>
+        <v>0.000192984991667648</v>
       </c>
       <c r="E33">
-        <v>0.0001985649052123504</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F33">
-        <v>0.2815190988739301</v>
+        <v>0.1421155108066621</v>
       </c>
       <c r="G33">
-        <v>0.147324247391146</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H33">
         <v>0.2582640092197721</v>
@@ -2215,26 +2230,26 @@
       <c r="I33">
         <v>14156</v>
       </c>
-      <c r="J33">
-        <v>0.1866413032030688</v>
-      </c>
-      <c r="K33">
-        <v>0.0003710863970746162</v>
-      </c>
-      <c r="M33">
+      <c r="L33">
         <v>0.0003384092866814527</v>
       </c>
-      <c r="N33">
-        <v>0.004784771004405694</v>
-      </c>
       <c r="O33">
-        <v>0.009674189396799985</v>
+        <v>0.1230344532976788</v>
+      </c>
+      <c r="P33">
+        <v>0.004818030126325817</v>
       </c>
       <c r="Q33">
-        <v>0.009535796789931871</v>
+        <v>0.01035431191953904</v>
+      </c>
+      <c r="R33">
+        <v>0.005409147625572685</v>
+      </c>
+      <c r="S33">
+        <v>0.0004001063569688302</v>
       </c>
       <c r="T33">
-        <v>0.004818030126325816</v>
+        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="34" spans="1:20">
@@ -2242,49 +2257,49 @@
         <v>52</v>
       </c>
       <c r="B34">
-        <v>0.008532806478705164</v>
+        <v>0.01016347810751514</v>
       </c>
       <c r="C34">
-        <v>0.008733878054388279</v>
+        <v>0.009447153043753395</v>
       </c>
       <c r="D34">
-        <v>0.0001656454412935777</v>
+        <v>0.0002829041504470825</v>
       </c>
       <c r="E34">
-        <v>0.0001961492659581503</v>
+        <v>0.0002806495860517923</v>
       </c>
       <c r="F34">
-        <v>0.2636491907304709</v>
+        <v>0.1619293810393613</v>
       </c>
       <c r="G34">
-        <v>0.1280492261183164</v>
+        <v>0.1686082656554458</v>
       </c>
       <c r="H34">
-        <v>0.2582640092197721</v>
+        <v>0.3904390743053188</v>
       </c>
       <c r="I34">
-        <v>14156</v>
-      </c>
-      <c r="J34">
-        <v>0.179378395374721</v>
-      </c>
-      <c r="K34">
-        <v>0.0003744000227958637</v>
-      </c>
-      <c r="M34">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N34">
-        <v>0.004730871750625608</v>
+        <v>4699</v>
+      </c>
+      <c r="L34">
+        <v>0.0003220429185286173</v>
       </c>
       <c r="O34">
-        <v>0.009674189396799987</v>
+        <v>0.1094051116331665</v>
+      </c>
+      <c r="P34">
+        <v>0.004731165595531388</v>
       </c>
       <c r="Q34">
-        <v>0.009554445336689437</v>
+        <v>0.01022526679210232</v>
+      </c>
+      <c r="R34">
+        <v>0.005350192890365459</v>
+      </c>
+      <c r="S34">
+        <v>0.0004705186388866096</v>
       </c>
       <c r="T34">
-        <v>0.004818030126325817</v>
+        <v>0.009384601794708014</v>
       </c>
     </row>
     <row r="35" spans="1:20">
@@ -2292,49 +2307,49 @@
         <v>53</v>
       </c>
       <c r="B35">
-        <v>0.008529233938818522</v>
+        <v>0.003030458698074221</v>
       </c>
       <c r="C35">
-        <v>0.008733878054388279</v>
+        <v>0.002499571894821071</v>
       </c>
       <c r="D35">
-        <v>0.0001653251466070655</v>
+        <v>1.91281128971015E-05</v>
       </c>
       <c r="E35">
-        <v>0.0001961492659581503</v>
+        <v>1.967007435869721E-05</v>
       </c>
       <c r="F35">
-        <v>0.2650730104853413</v>
+        <v>-0.01371556509502225</v>
       </c>
       <c r="G35">
-        <v>0.1280492261183164</v>
+        <v>-0.04243741404356438</v>
       </c>
       <c r="H35">
-        <v>0.2582640092197721</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I35">
-        <v>14156</v>
-      </c>
-      <c r="J35">
-        <v>0.1788608663781261</v>
-      </c>
-      <c r="K35">
-        <v>0.0003746361399868205</v>
-      </c>
-      <c r="M35">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N35">
-        <v>0.004764640177213803</v>
+        <v>11611</v>
+      </c>
+      <c r="L35">
+        <v>0.0001631540263502446</v>
       </c>
       <c r="O35">
-        <v>0.009674189396799987</v>
+        <v>-0.00353431378743374</v>
+      </c>
+      <c r="P35">
+        <v>0.001592932311570713</v>
       </c>
       <c r="Q35">
-        <v>0.009555217528480035</v>
+        <v>0.005089488294347637</v>
+      </c>
+      <c r="R35">
+        <v>0.001547174514616301</v>
+      </c>
+      <c r="S35">
+        <v>0.0002081444394071696</v>
       </c>
       <c r="T35">
-        <v>0.004818030126325817</v>
+        <v>0.004580501696160511</v>
       </c>
     </row>
     <row r="36" spans="1:20">
@@ -2342,22 +2357,22 @@
         <v>54</v>
       </c>
       <c r="B36">
-        <v>0.008505250051591662</v>
+        <v>0.008384122629515654</v>
       </c>
       <c r="C36">
-        <v>0.008733878054388279</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D36">
-        <v>0.0001646168902522808</v>
+        <v>0.0001620814063416336</v>
       </c>
       <c r="E36">
-        <v>0.0001961492659581503</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F36">
-        <v>0.268221452941368</v>
+        <v>0.3039913826239528</v>
       </c>
       <c r="G36">
-        <v>0.1280492261183164</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H36">
         <v>0.2582640092197721</v>
@@ -2365,26 +2380,26 @@
       <c r="I36">
         <v>14156</v>
       </c>
-      <c r="J36">
-        <v>0.1810824657398455</v>
-      </c>
-      <c r="K36">
-        <v>0.0003736225585176234</v>
-      </c>
-      <c r="M36">
+      <c r="L36">
         <v>0.0003384092866814527</v>
       </c>
-      <c r="N36">
-        <v>0.004756476812602748</v>
-      </c>
       <c r="O36">
-        <v>0.009674189396799987</v>
+        <v>0.2085500335179142</v>
+      </c>
+      <c r="P36">
+        <v>0.004818030126325816</v>
       </c>
       <c r="Q36">
-        <v>0.009526287265811475</v>
+        <v>0.009406309171688502</v>
+      </c>
+      <c r="R36">
+        <v>0.004884082851211167</v>
+      </c>
+      <c r="S36">
+        <v>0.0003610907680501377</v>
       </c>
       <c r="T36">
-        <v>0.004818030126325817</v>
+        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="37" spans="1:20">
@@ -2392,49 +2407,49 @@
         <v>55</v>
       </c>
       <c r="B37">
-        <v>0.006299187529923155</v>
+        <v>0.008519531777817098</v>
       </c>
       <c r="C37">
-        <v>0.00553167406053466</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D37">
-        <v>9.00395869891457E-05</v>
+        <v>0.0001673145877462598</v>
       </c>
       <c r="E37">
-        <v>8.170381435551846E-05</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F37">
-        <v>0.1391419988807219</v>
+        <v>0.2815190988739301</v>
       </c>
       <c r="G37">
-        <v>0.2188393498696173</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H37">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I37">
-        <v>6771</v>
-      </c>
-      <c r="J37">
-        <v>0.1045681259196538</v>
-      </c>
-      <c r="K37">
-        <v>0.0001603751212724098</v>
-      </c>
-      <c r="M37">
-        <v>0.0001037297229528328</v>
-      </c>
-      <c r="N37">
-        <v>0.003667719421830667</v>
+        <v>14156</v>
+      </c>
+      <c r="L37">
+        <v>0.0003384092866814527</v>
       </c>
       <c r="O37">
-        <v>0.005813234561065723</v>
+        <v>0.1866413032030688</v>
+      </c>
+      <c r="P37">
+        <v>0.004818030126325816</v>
       </c>
       <c r="Q37">
-        <v>0.00674135934653288</v>
+        <v>0.009535796789931871</v>
+      </c>
+      <c r="R37">
+        <v>0.004784771004405694</v>
+      </c>
+      <c r="S37">
+        <v>0.0003710863970746162</v>
       </c>
       <c r="T37">
-        <v>0.003193202088483064</v>
+        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="38" spans="1:20">
@@ -2442,19 +2457,19 @@
         <v>56</v>
       </c>
       <c r="B38">
-        <v>0.00864935396008955</v>
+        <v>0.008532806478705164</v>
       </c>
       <c r="C38">
         <v>0.008733878054388279</v>
       </c>
       <c r="D38">
-        <v>0.0001602711781363747</v>
+        <v>0.0001656454412935777</v>
       </c>
       <c r="E38">
         <v>0.0001961492659581503</v>
       </c>
       <c r="F38">
-        <v>0.2875396340419782</v>
+        <v>0.2636491907304709</v>
       </c>
       <c r="G38">
         <v>0.1280492261183164</v>
@@ -2465,26 +2480,26 @@
       <c r="I38">
         <v>14156</v>
       </c>
-      <c r="J38">
-        <v>0.2088743260447083</v>
-      </c>
-      <c r="K38">
-        <v>0.0003609428129771297</v>
-      </c>
-      <c r="M38">
+      <c r="L38">
         <v>0.0003384092866814527</v>
       </c>
-      <c r="N38">
-        <v>0.005274143159156646</v>
-      </c>
       <c r="O38">
+        <v>0.179378395374721</v>
+      </c>
+      <c r="P38">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="Q38">
+        <v>0.009554445336689437</v>
+      </c>
+      <c r="R38">
+        <v>0.004730871750625608</v>
+      </c>
+      <c r="S38">
+        <v>0.0003744000227958637</v>
+      </c>
+      <c r="T38">
         <v>0.009674189396799987</v>
-      </c>
-      <c r="Q38">
-        <v>0.009669808352814117</v>
-      </c>
-      <c r="T38">
-        <v>0.004818030126325816</v>
       </c>
     </row>
     <row r="39" spans="1:20">
@@ -2492,22 +2507,22 @@
         <v>57</v>
       </c>
       <c r="B39">
-        <v>0.00869522801124366</v>
+        <v>0.008529233938818522</v>
       </c>
       <c r="C39">
-        <v>0.008722720041403264</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D39">
-        <v>0.0001671499749450426</v>
+        <v>0.0001653251466070655</v>
       </c>
       <c r="E39">
-        <v>0.0001985649052123504</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F39">
-        <v>0.2822259777859754</v>
+        <v>0.2650730104853413</v>
       </c>
       <c r="G39">
-        <v>0.147324247391146</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H39">
         <v>0.2582640092197721</v>
@@ -2515,26 +2530,26 @@
       <c r="I39">
         <v>14156</v>
       </c>
-      <c r="J39">
-        <v>0.2030564380000814</v>
-      </c>
-      <c r="K39">
-        <v>0.0003635971635380399</v>
-      </c>
-      <c r="M39">
+      <c r="L39">
         <v>0.0003384092866814527</v>
       </c>
-      <c r="N39">
-        <v>0.005173194757001598</v>
-      </c>
       <c r="O39">
-        <v>0.009674189396799985</v>
+        <v>0.1788608663781261</v>
+      </c>
+      <c r="P39">
+        <v>0.004818030126325817</v>
       </c>
       <c r="Q39">
-        <v>0.009719161233546112</v>
+        <v>0.009555217528480035</v>
+      </c>
+      <c r="R39">
+        <v>0.004764640177213803</v>
+      </c>
+      <c r="S39">
+        <v>0.0003746361399868205</v>
       </c>
       <c r="T39">
-        <v>0.004818030126325817</v>
+        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="40" spans="1:20">
@@ -2542,22 +2557,22 @@
         <v>58</v>
       </c>
       <c r="B40">
-        <v>0.007668256776450208</v>
+        <v>0.008505250051591662</v>
       </c>
       <c r="C40">
-        <v>0.008722720041403264</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D40">
-        <v>0.0001436777206558706</v>
+        <v>0.0001646168902522808</v>
       </c>
       <c r="E40">
-        <v>0.0001985649052123504</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F40">
-        <v>0.3830203355303232</v>
+        <v>0.268221452941368</v>
       </c>
       <c r="G40">
-        <v>0.147324247391146</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H40">
         <v>0.2582640092197721</v>
@@ -2565,26 +2580,26 @@
       <c r="I40">
         <v>14156</v>
       </c>
-      <c r="J40">
-        <v>0.2669184291403396</v>
-      </c>
-      <c r="K40">
-        <v>0.0003344607981243851</v>
-      </c>
-      <c r="M40">
+      <c r="L40">
         <v>0.0003384092866814527</v>
       </c>
-      <c r="N40">
-        <v>0.004128330862335852</v>
-      </c>
       <c r="O40">
-        <v>0.009674189396799985</v>
+        <v>0.1810824657398455</v>
+      </c>
+      <c r="P40">
+        <v>0.004818030126325817</v>
       </c>
       <c r="Q40">
-        <v>0.00867861064019221</v>
+        <v>0.009526287265811475</v>
+      </c>
+      <c r="R40">
+        <v>0.004756476812602748</v>
+      </c>
+      <c r="S40">
+        <v>0.0003736225585176234</v>
       </c>
       <c r="T40">
-        <v>0.004818030126325817</v>
+        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="41" spans="1:20">
@@ -2592,49 +2607,49 @@
         <v>59</v>
       </c>
       <c r="B41">
-        <v>0.01020612284563066</v>
+        <v>0.006299187529923155</v>
       </c>
       <c r="C41">
-        <v>0.009760820655321729</v>
+        <v>0.00553167406053466</v>
       </c>
       <c r="D41">
-        <v>0.0002760452274294578</v>
+        <v>9.00395869891457E-05</v>
       </c>
       <c r="E41">
-        <v>0.0002924361182664438</v>
+        <v>8.170381435551846E-05</v>
       </c>
       <c r="F41">
-        <v>0.1971347954963554</v>
+        <v>0.1391419988807219</v>
       </c>
       <c r="G41">
-        <v>0.1494626221848404</v>
+        <v>0.2188393498696173</v>
       </c>
       <c r="H41">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I41">
-        <v>14156</v>
-      </c>
-      <c r="J41">
-        <v>0.1481445083553075</v>
-      </c>
-      <c r="K41">
-        <v>0.0003886501570187028</v>
-      </c>
-      <c r="M41">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="N41">
-        <v>0.005394960099510664</v>
+        <v>6771</v>
+      </c>
+      <c r="L41">
+        <v>0.0001037297229528328</v>
       </c>
       <c r="O41">
-        <v>0.009674189396799987</v>
+        <v>0.1045681259196538</v>
+      </c>
+      <c r="P41">
+        <v>0.003193202088483064</v>
       </c>
       <c r="Q41">
-        <v>0.01011738460212881</v>
+        <v>0.00674135934653288</v>
+      </c>
+      <c r="R41">
+        <v>0.003667719421830667</v>
+      </c>
+      <c r="S41">
+        <v>0.0001603751212724098</v>
       </c>
       <c r="T41">
-        <v>0.004818030126325816</v>
+        <v>0.005813234561065723</v>
       </c>
     </row>
     <row r="42" spans="1:20">
@@ -2642,22 +2657,22 @@
         <v>60</v>
       </c>
       <c r="B42">
-        <v>0.00958912348219286</v>
+        <v>0.00864935396008955</v>
       </c>
       <c r="C42">
-        <v>0.008722720041403264</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D42">
-        <v>0.00021842684931279</v>
+        <v>0.0001602711781363747</v>
       </c>
       <c r="E42">
-        <v>0.0001985649052123504</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F42">
-        <v>0.06203325341612431</v>
+        <v>0.2875396340419782</v>
       </c>
       <c r="G42">
-        <v>0.147324247391146</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H42">
         <v>0.2582640092197721</v>
@@ -2665,26 +2680,26 @@
       <c r="I42">
         <v>14156</v>
       </c>
-      <c r="J42">
-        <v>0.05448840836791147</v>
-      </c>
-      <c r="K42">
-        <v>0.0004313797729252501</v>
-      </c>
-      <c r="M42">
+      <c r="L42">
         <v>0.0003384092866814527</v>
       </c>
-      <c r="N42">
-        <v>0.005560650653515711</v>
-      </c>
       <c r="O42">
-        <v>0.009674189396799985</v>
+        <v>0.2088743260447083</v>
+      </c>
+      <c r="P42">
+        <v>0.004818030126325816</v>
       </c>
       <c r="Q42">
-        <v>0.01064772150300563</v>
+        <v>0.009669808352814117</v>
+      </c>
+      <c r="R42">
+        <v>0.005274143159156646</v>
+      </c>
+      <c r="S42">
+        <v>0.0003609428129771297</v>
       </c>
       <c r="T42">
-        <v>0.004818030126325817</v>
+        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="43" spans="1:20">
@@ -2692,61 +2707,49 @@
         <v>61</v>
       </c>
       <c r="B43">
-        <v>0.005414655366858831</v>
+        <v>0.00869522801124366</v>
       </c>
       <c r="C43">
-        <v>0.005250633999685894</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D43">
-        <v>8.390458217824665E-05</v>
+        <v>0.0001671499749450426</v>
       </c>
       <c r="E43">
-        <v>8.336263472823423E-05</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F43">
-        <v>0.2548808040617673</v>
+        <v>0.2822259777859754</v>
       </c>
       <c r="G43">
-        <v>0.2596935978056915</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H43">
-        <v>0.456874413314975</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I43">
-        <v>5153</v>
-      </c>
-      <c r="J43">
-        <v>0.1703625716885953</v>
-      </c>
-      <c r="K43">
-        <v>0.000141190946981845</v>
+        <v>14156</v>
       </c>
       <c r="L43">
-        <v>0.4055123229186881</v>
-      </c>
-      <c r="M43">
-        <v>9.243123959608208E-05</v>
-      </c>
-      <c r="N43">
-        <v>0.002733726006933551</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="O43">
-        <v>0.005318929375230071</v>
+        <v>0.2030564380000814</v>
       </c>
       <c r="P43">
-        <v>0.4113135413420823</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="Q43">
-        <v>0.005626234126090045</v>
+        <v>0.009719161233546112</v>
       </c>
       <c r="R43">
-        <v>10.4129840341794</v>
+        <v>0.005173194757001598</v>
       </c>
       <c r="S43">
-        <v>11.43997477570016</v>
+        <v>0.0003635971635380399</v>
       </c>
       <c r="T43">
-        <v>0.002848413552158193</v>
+        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="44" spans="1:20">
@@ -2754,22 +2757,22 @@
         <v>62</v>
       </c>
       <c r="B44">
-        <v>0.009301347310769852</v>
+        <v>0.007668256776450208</v>
       </c>
       <c r="C44">
-        <v>0.008733878054388279</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D44">
-        <v>0.0001883109214593075</v>
+        <v>0.0001436777206558706</v>
       </c>
       <c r="E44">
-        <v>0.0001961492659581503</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F44">
-        <v>0.1628933562675233</v>
+        <v>0.3830203355303232</v>
       </c>
       <c r="G44">
-        <v>0.1280492261183164</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H44">
         <v>0.2582640092197721</v>
@@ -2777,26 +2780,26 @@
       <c r="I44">
         <v>14156</v>
       </c>
-      <c r="J44">
-        <v>0.1175458874123242</v>
-      </c>
-      <c r="K44">
-        <v>0.0004026104577395279</v>
-      </c>
-      <c r="M44">
+      <c r="L44">
         <v>0.0003384092866814527</v>
       </c>
-      <c r="N44">
-        <v>0.005399385735558927</v>
-      </c>
       <c r="O44">
-        <v>0.009674189396799987</v>
+        <v>0.2669184291403396</v>
+      </c>
+      <c r="P44">
+        <v>0.004818030126325817</v>
       </c>
       <c r="Q44">
-        <v>0.01035467890006862</v>
+        <v>0.00867861064019221</v>
+      </c>
+      <c r="R44">
+        <v>0.004128330862335852</v>
+      </c>
+      <c r="S44">
+        <v>0.0003344607981243851</v>
       </c>
       <c r="T44">
-        <v>0.004818030126325817</v>
+        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="45" spans="1:20">
@@ -2804,49 +2807,49 @@
         <v>63</v>
       </c>
       <c r="B45">
-        <v>0.00303210497017975</v>
+        <v>0.01020612284563066</v>
       </c>
       <c r="C45">
-        <v>0.002499571894821071</v>
+        <v>0.009760820655321729</v>
       </c>
       <c r="D45">
-        <v>1.909735738640315E-05</v>
+        <v>0.0002760452274294578</v>
       </c>
       <c r="E45">
-        <v>1.967007435869721E-05</v>
+        <v>0.0002924361182664438</v>
       </c>
       <c r="F45">
-        <v>-0.0120856426831728</v>
+        <v>0.1971347954963554</v>
       </c>
       <c r="G45">
-        <v>-0.04243741404356438</v>
+        <v>0.1494626221848404</v>
       </c>
       <c r="H45">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I45">
-        <v>11611</v>
-      </c>
-      <c r="J45">
-        <v>-0.002911711704464803</v>
-      </c>
-      <c r="K45">
-        <v>0.0002080153046483946</v>
-      </c>
-      <c r="M45">
-        <v>0.0001631540263502446</v>
-      </c>
-      <c r="N45">
-        <v>0.001550051802718652</v>
+        <v>14156</v>
+      </c>
+      <c r="L45">
+        <v>0.0003384092866814527</v>
       </c>
       <c r="O45">
-        <v>0.004580501696160511</v>
+        <v>0.1481445083553075</v>
+      </c>
+      <c r="P45">
+        <v>0.004818030126325816</v>
       </c>
       <c r="Q45">
-        <v>0.005090949099942899</v>
+        <v>0.01011738460212881</v>
+      </c>
+      <c r="R45">
+        <v>0.005394960099510664</v>
+      </c>
+      <c r="S45">
+        <v>0.0003886501570187028</v>
       </c>
       <c r="T45">
-        <v>0.001592932311570713</v>
+        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="46" spans="1:20">
@@ -2854,22 +2857,22 @@
         <v>64</v>
       </c>
       <c r="B46">
-        <v>0.008142928261746932</v>
+        <v>0.00958912348219286</v>
       </c>
       <c r="C46">
-        <v>0.008733878054388279</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D46">
-        <v>0.0001648112327367591</v>
+        <v>0.00021842684931279</v>
       </c>
       <c r="E46">
-        <v>0.0001961492659581503</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F46">
-        <v>0.2673575339309593</v>
+        <v>0.06203325341612431</v>
       </c>
       <c r="G46">
-        <v>0.1280492261183164</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H46">
         <v>0.2582640092197721</v>
@@ -2877,26 +2880,26 @@
       <c r="I46">
         <v>14156</v>
       </c>
-      <c r="J46">
-        <v>0.2464320924804251</v>
-      </c>
-      <c r="K46">
-        <v>0.0003438074749231005</v>
-      </c>
-      <c r="M46">
+      <c r="L46">
         <v>0.0003384092866814527</v>
       </c>
-      <c r="N46">
-        <v>0.004666820467017538</v>
-      </c>
       <c r="O46">
-        <v>0.009674189396799987</v>
+        <v>0.05448840836791147</v>
+      </c>
+      <c r="P46">
+        <v>0.004818030126325817</v>
       </c>
       <c r="Q46">
-        <v>0.009263751492683912</v>
+        <v>0.01064772150300563</v>
+      </c>
+      <c r="R46">
+        <v>0.005560650653515711</v>
+      </c>
+      <c r="S46">
+        <v>0.0004313797729252501</v>
       </c>
       <c r="T46">
-        <v>0.004818030126325817</v>
+        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="47" spans="1:20">
@@ -2904,49 +2907,311 @@
         <v>65</v>
       </c>
       <c r="B47">
+        <v>0.005414655366858831</v>
+      </c>
+      <c r="C47">
+        <v>0.005250633999685894</v>
+      </c>
+      <c r="D47">
+        <v>8.390458217824665E-05</v>
+      </c>
+      <c r="E47">
+        <v>8.336263472823423E-05</v>
+      </c>
+      <c r="F47">
+        <v>0.2548808040617673</v>
+      </c>
+      <c r="G47">
+        <v>0.2596935978056915</v>
+      </c>
+      <c r="H47">
+        <v>0.456874413314975</v>
+      </c>
+      <c r="I47">
+        <v>5153</v>
+      </c>
+      <c r="J47">
+        <v>10.4129840341794</v>
+      </c>
+      <c r="K47">
+        <v>0.4055123229186881</v>
+      </c>
+      <c r="L47">
+        <v>9.243123959608208E-05</v>
+      </c>
+      <c r="M47">
+        <v>0.4113135413420823</v>
+      </c>
+      <c r="N47">
+        <v>11.43997477570016</v>
+      </c>
+      <c r="O47">
+        <v>0.1703625716885953</v>
+      </c>
+      <c r="P47">
+        <v>0.002848413552158193</v>
+      </c>
+      <c r="Q47">
+        <v>0.005626234126090045</v>
+      </c>
+      <c r="R47">
+        <v>0.002733726006933551</v>
+      </c>
+      <c r="S47">
+        <v>0.000141190946981845</v>
+      </c>
+      <c r="T47">
+        <v>0.005318929375230071</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20">
+      <c r="A48" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48">
+        <v>0.00955739351620514</v>
+      </c>
+      <c r="C48">
+        <v>0.008733878054388279</v>
+      </c>
+      <c r="D48">
+        <v>0.0001939926155429641</v>
+      </c>
+      <c r="E48">
+        <v>0.0001961492659581503</v>
+      </c>
+      <c r="F48">
+        <v>0.137636277027368</v>
+      </c>
+      <c r="G48">
+        <v>0.1280492261183164</v>
+      </c>
+      <c r="H48">
+        <v>0.2582640092197721</v>
+      </c>
+      <c r="I48">
+        <v>14156</v>
+      </c>
+      <c r="L48">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="O48">
+        <v>0.09278621544819221</v>
+      </c>
+      <c r="P48">
+        <v>0.004818030126325816</v>
+      </c>
+      <c r="Q48">
+        <v>0.01060174085834054</v>
+      </c>
+      <c r="R48">
+        <v>0.005675761589993111</v>
+      </c>
+      <c r="S48">
+        <v>0.0004139067990685161</v>
+      </c>
+      <c r="T48">
+        <v>0.009674189396799987</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20">
+      <c r="A49" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49">
+        <v>0.009301347310769852</v>
+      </c>
+      <c r="C49">
+        <v>0.008733878054388279</v>
+      </c>
+      <c r="D49">
+        <v>0.0001883109214593075</v>
+      </c>
+      <c r="E49">
+        <v>0.0001961492659581503</v>
+      </c>
+      <c r="F49">
+        <v>0.1628933562675233</v>
+      </c>
+      <c r="G49">
+        <v>0.1280492261183164</v>
+      </c>
+      <c r="H49">
+        <v>0.2582640092197721</v>
+      </c>
+      <c r="I49">
+        <v>14156</v>
+      </c>
+      <c r="L49">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="O49">
+        <v>0.1175458874123242</v>
+      </c>
+      <c r="P49">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="Q49">
+        <v>0.01035467890006862</v>
+      </c>
+      <c r="R49">
+        <v>0.005399385735558927</v>
+      </c>
+      <c r="S49">
+        <v>0.0004026104577395279</v>
+      </c>
+      <c r="T49">
+        <v>0.009674189396799987</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20">
+      <c r="A50" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50">
+        <v>0.00303210497017975</v>
+      </c>
+      <c r="C50">
+        <v>0.002499571894821071</v>
+      </c>
+      <c r="D50">
+        <v>1.909735738640315E-05</v>
+      </c>
+      <c r="E50">
+        <v>1.967007435869721E-05</v>
+      </c>
+      <c r="F50">
+        <v>-0.0120856426831728</v>
+      </c>
+      <c r="G50">
+        <v>-0.04243741404356438</v>
+      </c>
+      <c r="H50">
+        <v>0.2133795918767654</v>
+      </c>
+      <c r="I50">
+        <v>11611</v>
+      </c>
+      <c r="L50">
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="O50">
+        <v>-0.002911711704464803</v>
+      </c>
+      <c r="P50">
+        <v>0.001592932311570713</v>
+      </c>
+      <c r="Q50">
+        <v>0.005090949099942899</v>
+      </c>
+      <c r="R50">
+        <v>0.001550051802718652</v>
+      </c>
+      <c r="S50">
+        <v>0.0002080153046483946</v>
+      </c>
+      <c r="T50">
+        <v>0.004580501696160511</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20">
+      <c r="A51" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B51">
+        <v>0.008142928261746932</v>
+      </c>
+      <c r="C51">
+        <v>0.008733878054388279</v>
+      </c>
+      <c r="D51">
+        <v>0.0001648112327367591</v>
+      </c>
+      <c r="E51">
+        <v>0.0001961492659581503</v>
+      </c>
+      <c r="F51">
+        <v>0.2673575339309593</v>
+      </c>
+      <c r="G51">
+        <v>0.1280492261183164</v>
+      </c>
+      <c r="H51">
+        <v>0.2582640092197721</v>
+      </c>
+      <c r="I51">
+        <v>14156</v>
+      </c>
+      <c r="L51">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="O51">
+        <v>0.2464320924804251</v>
+      </c>
+      <c r="P51">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="Q51">
+        <v>0.009263751492683912</v>
+      </c>
+      <c r="R51">
+        <v>0.004666820467017538</v>
+      </c>
+      <c r="S51">
+        <v>0.0003438074749231005</v>
+      </c>
+      <c r="T51">
+        <v>0.009674189396799987</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20">
+      <c r="A52" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52">
         <v>0.01025436961368844</v>
       </c>
-      <c r="C47">
+      <c r="C52">
         <v>0.01023301201875394</v>
       </c>
-      <c r="D47">
+      <c r="D52">
         <v>0.0002841844015704704</v>
       </c>
-      <c r="E47">
+      <c r="E52">
         <v>0.0003551633527675986</v>
       </c>
-      <c r="F47">
+      <c r="F52">
         <v>0.3369590471682379</v>
       </c>
-      <c r="G47">
+      <c r="G52">
         <v>0.1713554771880856</v>
       </c>
-      <c r="H47">
+      <c r="H52">
         <v>0.4827027158358849</v>
       </c>
-      <c r="I47">
+      <c r="I52">
         <v>1267</v>
       </c>
-      <c r="J47">
+      <c r="L52">
+        <v>0.0004283113735138171</v>
+      </c>
+      <c r="O52">
         <v>0.2718477491393597</v>
       </c>
-      <c r="K47">
+      <c r="P52">
+        <v>0.004670472236637264</v>
+      </c>
+      <c r="Q52">
+        <v>0.0102050584404969</v>
+      </c>
+      <c r="R52">
+        <v>0.005379622896887214</v>
+      </c>
+      <c r="S52">
         <v>0.0006028948928221208</v>
       </c>
-      <c r="M47">
-        <v>0.0004283113735138171</v>
-      </c>
-      <c r="N47">
-        <v>0.005379622896887214</v>
-      </c>
-      <c r="O47">
+      <c r="T52">
         <v>0.01026809155717979</v>
-      </c>
-      <c r="Q47">
-        <v>0.0102050584404969</v>
-      </c>
-      <c r="T47">
-        <v>0.004670472236637264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update load_data_lgbm IIIb country partition
</commit_message>
<xml_diff>
--- a/results_analysis/compare_with_ibes/#compare_all.xlsx
+++ b/results_analysis/compare_with_ibes/#compare_all.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>lgbm_mae</t>
   </si>
@@ -40,39 +40,39 @@
     <t>len</t>
   </si>
   <si>
+    <t>consensus_mae_eps</t>
+  </si>
+  <si>
+    <t>lgbm_mse_org</t>
+  </si>
+  <si>
     <t>consensus_mape_eps</t>
   </si>
   <si>
-    <t>consensus_mae_eps</t>
-  </si>
-  <si>
     <t>consensus_mse_org</t>
   </si>
   <si>
+    <t>lgbm_mape_eps</t>
+  </si>
+  <si>
+    <t>lgbm_mae_org</t>
+  </si>
+  <si>
+    <t>lgbm_medae_org</t>
+  </si>
+  <si>
+    <t>consensus_mae_org</t>
+  </si>
+  <si>
     <t>lgbm_mae_eps</t>
   </si>
   <si>
-    <t>lgbm_mape_eps</t>
-  </si>
-  <si>
     <t>lgbm_r2_org</t>
   </si>
   <si>
     <t>consensus_medae_org</t>
   </si>
   <si>
-    <t>lgbm_mae_org</t>
-  </si>
-  <si>
-    <t>lgbm_medae_org</t>
-  </si>
-  <si>
-    <t>lgbm_mse_org</t>
-  </si>
-  <si>
-    <t>consensus_mae_org</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>ibes_1|ni|rnn_top｜top15_lgbm</t>
+  </si>
+  <si>
+    <t>ibes_1|fwdepsqcut-46|dense2｜small_new_config_1 -code 0 -exclude_fwd True</t>
   </si>
 </sst>
 </file>
@@ -584,7 +587,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T52"/>
+  <dimension ref="A1:T53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -680,26 +683,26 @@
       <c r="I2">
         <v>14156</v>
       </c>
-      <c r="L2">
+      <c r="K2">
+        <v>0.0004250480609163007</v>
+      </c>
+      <c r="M2">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O2">
+        <v>0.01071193221870467</v>
+      </c>
+      <c r="P2">
+        <v>0.005638666708596741</v>
+      </c>
+      <c r="Q2">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="S2">
         <v>0.06836645151013176</v>
       </c>
-      <c r="P2">
+      <c r="T2">
         <v>0.004818030126325816</v>
-      </c>
-      <c r="Q2">
-        <v>0.01071193221870467</v>
-      </c>
-      <c r="R2">
-        <v>0.005638666708596741</v>
-      </c>
-      <c r="S2">
-        <v>0.0004250480609163007</v>
-      </c>
-      <c r="T2">
-        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -730,26 +733,26 @@
       <c r="I3">
         <v>11611</v>
       </c>
-      <c r="L3">
+      <c r="K3">
+        <v>0.0001978384306784256</v>
+      </c>
+      <c r="M3">
         <v>0.0001631540263502446</v>
       </c>
       <c r="O3">
+        <v>0.00502885184437347</v>
+      </c>
+      <c r="P3">
+        <v>0.001779221775169934</v>
+      </c>
+      <c r="Q3">
+        <v>0.004580501696160511</v>
+      </c>
+      <c r="S3">
         <v>0.04615441883950755</v>
       </c>
-      <c r="P3">
+      <c r="T3">
         <v>0.001592932311570713</v>
-      </c>
-      <c r="Q3">
-        <v>0.00502885184437347</v>
-      </c>
-      <c r="R3">
-        <v>0.001779221775169934</v>
-      </c>
-      <c r="S3">
-        <v>0.0001978384306784256</v>
-      </c>
-      <c r="T3">
-        <v>0.004580501696160511</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -780,26 +783,26 @@
       <c r="I4">
         <v>6771</v>
       </c>
-      <c r="L4">
+      <c r="K4">
+        <v>0.0001137832146297872</v>
+      </c>
+      <c r="M4">
         <v>0.0001037297229528328</v>
       </c>
       <c r="O4">
+        <v>0.005606434133779571</v>
+      </c>
+      <c r="P4">
+        <v>0.003094044369724517</v>
+      </c>
+      <c r="Q4">
+        <v>0.005813234561065725</v>
+      </c>
+      <c r="S4">
         <v>0.36470746642943</v>
       </c>
-      <c r="P4">
+      <c r="T4">
         <v>0.003193202088483064</v>
-      </c>
-      <c r="Q4">
-        <v>0.005606434133779571</v>
-      </c>
-      <c r="R4">
-        <v>0.003094044369724517</v>
-      </c>
-      <c r="S4">
-        <v>0.0001137832146297872</v>
-      </c>
-      <c r="T4">
-        <v>0.005813234561065725</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -830,26 +833,26 @@
       <c r="I5">
         <v>6771</v>
       </c>
-      <c r="L5">
+      <c r="K5">
+        <v>0.0001152638129503358</v>
+      </c>
+      <c r="M5">
         <v>0.0001037297229528328</v>
       </c>
       <c r="O5">
+        <v>0.005632685300523813</v>
+      </c>
+      <c r="P5">
+        <v>0.003171635367762127</v>
+      </c>
+      <c r="Q5">
+        <v>0.005813234561065725</v>
+      </c>
+      <c r="S5">
         <v>0.3564407544954944</v>
       </c>
-      <c r="P5">
+      <c r="T5">
         <v>0.003193202088483064</v>
-      </c>
-      <c r="Q5">
-        <v>0.005632685300523813</v>
-      </c>
-      <c r="R5">
-        <v>0.003171635367762127</v>
-      </c>
-      <c r="S5">
-        <v>0.0001152638129503358</v>
-      </c>
-      <c r="T5">
-        <v>0.005813234561065725</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -880,26 +883,26 @@
       <c r="I6">
         <v>42468</v>
       </c>
-      <c r="L6">
+      <c r="K6">
+        <v>0.000333070102780211</v>
+      </c>
+      <c r="M6">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O6">
+        <v>0.009106885821888167</v>
+      </c>
+      <c r="P6">
+        <v>0.004616722796530505</v>
+      </c>
+      <c r="Q6">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="S6">
         <v>0.269966598412229</v>
       </c>
-      <c r="P6">
+      <c r="T6">
         <v>0.004818030126325817</v>
-      </c>
-      <c r="Q6">
-        <v>0.009106885821888167</v>
-      </c>
-      <c r="R6">
-        <v>0.004616722796530505</v>
-      </c>
-      <c r="S6">
-        <v>0.000333070102780211</v>
-      </c>
-      <c r="T6">
-        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -930,26 +933,26 @@
       <c r="I7">
         <v>14156</v>
       </c>
-      <c r="L7">
+      <c r="K7">
+        <v>0.0003285627388197843</v>
+      </c>
+      <c r="M7">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O7">
+        <v>0.008950010380536522</v>
+      </c>
+      <c r="P7">
+        <v>0.004615286290830784</v>
+      </c>
+      <c r="Q7">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="S7">
         <v>0.2798459788092014</v>
       </c>
-      <c r="P7">
+      <c r="T7">
         <v>0.004818030126325817</v>
-      </c>
-      <c r="Q7">
-        <v>0.008950010380536522</v>
-      </c>
-      <c r="R7">
-        <v>0.004615286290830784</v>
-      </c>
-      <c r="S7">
-        <v>0.0003285627388197843</v>
-      </c>
-      <c r="T7">
-        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -980,26 +983,26 @@
       <c r="I8">
         <v>14156</v>
       </c>
-      <c r="L8">
+      <c r="K8">
+        <v>0.0003713407546776094</v>
+      </c>
+      <c r="M8">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O8">
+        <v>0.00941140169945745</v>
+      </c>
+      <c r="P8">
+        <v>0.004590555422836876</v>
+      </c>
+      <c r="Q8">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="S8">
         <v>0.1860837943045432</v>
       </c>
-      <c r="P8">
+      <c r="T8">
         <v>0.004818030126325816</v>
-      </c>
-      <c r="Q8">
-        <v>0.00941140169945745</v>
-      </c>
-      <c r="R8">
-        <v>0.004590555422836876</v>
-      </c>
-      <c r="S8">
-        <v>0.0003713407546776094</v>
-      </c>
-      <c r="T8">
-        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -1030,26 +1033,26 @@
       <c r="I9">
         <v>24768</v>
       </c>
-      <c r="L9">
+      <c r="K9">
+        <v>0.0002632414236722758</v>
+      </c>
+      <c r="M9">
         <v>0.0001796235360933539</v>
       </c>
       <c r="O9">
+        <v>0.008363098231375462</v>
+      </c>
+      <c r="P9">
+        <v>0.004275415213561056</v>
+      </c>
+      <c r="Q9">
+        <v>0.006875190708555331</v>
+      </c>
+      <c r="S9">
         <v>-0.00724317687482956</v>
       </c>
-      <c r="P9">
+      <c r="T9">
         <v>0.003559726400188349</v>
-      </c>
-      <c r="Q9">
-        <v>0.008363098231375462</v>
-      </c>
-      <c r="R9">
-        <v>0.004275415213561056</v>
-      </c>
-      <c r="S9">
-        <v>0.0002632414236722758</v>
-      </c>
-      <c r="T9">
-        <v>0.006875190708555331</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -1080,26 +1083,26 @@
       <c r="I10">
         <v>14156</v>
       </c>
-      <c r="L10">
+      <c r="K10">
+        <v>0.0003847976244374441</v>
+      </c>
+      <c r="M10">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O10">
+        <v>0.009901025034115019</v>
+      </c>
+      <c r="P10">
+        <v>0.005167135423672592</v>
+      </c>
+      <c r="Q10">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="S10">
         <v>0.1565886089862186</v>
       </c>
-      <c r="P10">
+      <c r="T10">
         <v>0.004818030126325816</v>
-      </c>
-      <c r="Q10">
-        <v>0.009901025034115019</v>
-      </c>
-      <c r="R10">
-        <v>0.005167135423672592</v>
-      </c>
-      <c r="S10">
-        <v>0.0003847976244374441</v>
-      </c>
-      <c r="T10">
-        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1130,26 +1133,26 @@
       <c r="I11">
         <v>11542</v>
       </c>
-      <c r="L11">
+      <c r="K11">
+        <v>0.000209188838038313</v>
+      </c>
+      <c r="M11">
         <v>0.000163888349337522</v>
       </c>
       <c r="O11">
+        <v>0.00512210974064752</v>
+      </c>
+      <c r="P11">
+        <v>0.001602037466360856</v>
+      </c>
+      <c r="Q11">
+        <v>0.004589584286176587</v>
+      </c>
+      <c r="S11">
         <v>-0.005102592401121431</v>
       </c>
-      <c r="P11">
+      <c r="T11">
         <v>0.001597174444307401</v>
-      </c>
-      <c r="Q11">
-        <v>0.00512210974064752</v>
-      </c>
-      <c r="R11">
-        <v>0.001602037466360856</v>
-      </c>
-      <c r="S11">
-        <v>0.000209188838038313</v>
-      </c>
-      <c r="T11">
-        <v>0.004589584286176587</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -1180,26 +1183,26 @@
       <c r="I12">
         <v>6771</v>
       </c>
-      <c r="L12">
+      <c r="K12">
+        <v>0.000112952017849086</v>
+      </c>
+      <c r="M12">
         <v>0.0001037297229528328</v>
       </c>
       <c r="O12">
+        <v>0.00526064949972486</v>
+      </c>
+      <c r="P12">
+        <v>0.002682213716882752</v>
+      </c>
+      <c r="Q12">
+        <v>0.005813234561065725</v>
+      </c>
+      <c r="S12">
         <v>0.3693483364419842</v>
       </c>
-      <c r="P12">
+      <c r="T12">
         <v>0.003193202088483064</v>
-      </c>
-      <c r="Q12">
-        <v>0.00526064949972486</v>
-      </c>
-      <c r="R12">
-        <v>0.002682213716882752</v>
-      </c>
-      <c r="S12">
-        <v>0.000112952017849086</v>
-      </c>
-      <c r="T12">
-        <v>0.005813234561065725</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -1230,26 +1233,26 @@
       <c r="I13">
         <v>6771</v>
       </c>
-      <c r="L13">
+      <c r="K13">
+        <v>0.0001410934357507483</v>
+      </c>
+      <c r="M13">
         <v>0.0001037297229528328</v>
       </c>
       <c r="O13">
+        <v>0.006002887168865449</v>
+      </c>
+      <c r="P13">
+        <v>0.003030311329129174</v>
+      </c>
+      <c r="Q13">
+        <v>0.005813234561065723</v>
+      </c>
+      <c r="S13">
         <v>0.2122246979933391</v>
       </c>
-      <c r="P13">
+      <c r="T13">
         <v>0.003193202088483064</v>
-      </c>
-      <c r="Q13">
-        <v>0.006002887168865449</v>
-      </c>
-      <c r="R13">
-        <v>0.003030311329129174</v>
-      </c>
-      <c r="S13">
-        <v>0.0001410934357507483</v>
-      </c>
-      <c r="T13">
-        <v>0.005813234561065723</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -1280,26 +1283,26 @@
       <c r="I14">
         <v>11611</v>
       </c>
-      <c r="L14">
+      <c r="K14">
+        <v>0.0002098592232396584</v>
+      </c>
+      <c r="M14">
         <v>0.0001631540263502446</v>
       </c>
       <c r="O14">
+        <v>0.005213165544267774</v>
+      </c>
+      <c r="P14">
+        <v>0.00173711317318318</v>
+      </c>
+      <c r="Q14">
+        <v>0.004580501696160511</v>
+      </c>
+      <c r="S14">
         <v>-0.01180186309853548</v>
       </c>
-      <c r="P14">
+      <c r="T14">
         <v>0.001592932311570713</v>
-      </c>
-      <c r="Q14">
-        <v>0.005213165544267774</v>
-      </c>
-      <c r="R14">
-        <v>0.00173711317318318</v>
-      </c>
-      <c r="S14">
-        <v>0.0002098592232396584</v>
-      </c>
-      <c r="T14">
-        <v>0.004580501696160511</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -1330,26 +1333,26 @@
       <c r="I15">
         <v>49</v>
       </c>
-      <c r="L15">
+      <c r="K15">
+        <v>0.0003123469992588732</v>
+      </c>
+      <c r="M15">
         <v>0.0001158352549329261</v>
       </c>
       <c r="O15">
+        <v>0.007217175147339313</v>
+      </c>
+      <c r="P15">
+        <v>0.002972419699024923</v>
+      </c>
+      <c r="Q15">
+        <v>0.004529835290885987</v>
+      </c>
+      <c r="S15">
         <v>-0.01652918306199047</v>
       </c>
-      <c r="P15">
+      <c r="T15">
         <v>0.00129198945232948</v>
-      </c>
-      <c r="Q15">
-        <v>0.007217175147339313</v>
-      </c>
-      <c r="R15">
-        <v>0.002972419699024923</v>
-      </c>
-      <c r="S15">
-        <v>0.0003123469992588732</v>
-      </c>
-      <c r="T15">
-        <v>0.004529835290885987</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -1380,26 +1383,26 @@
       <c r="I16">
         <v>12741</v>
       </c>
-      <c r="L16">
+      <c r="K16">
+        <v>0.0004007814960332574</v>
+      </c>
+      <c r="M16">
         <v>0.0003441387227458278</v>
       </c>
       <c r="O16">
+        <v>0.01033009227796955</v>
+      </c>
+      <c r="P16">
+        <v>0.005554310648909318</v>
+      </c>
+      <c r="Q16">
+        <v>0.009714954248817111</v>
+      </c>
+      <c r="S16">
         <v>0.1379172254546043</v>
       </c>
-      <c r="P16">
+      <c r="T16">
         <v>0.004797770485226469</v>
-      </c>
-      <c r="Q16">
-        <v>0.01033009227796955</v>
-      </c>
-      <c r="R16">
-        <v>0.005554310648909318</v>
-      </c>
-      <c r="S16">
-        <v>0.0004007814960332574</v>
-      </c>
-      <c r="T16">
-        <v>0.009714954248817111</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -1430,26 +1433,26 @@
       <c r="I17">
         <v>1284</v>
       </c>
-      <c r="L17">
+      <c r="K17">
+        <v>0.0003741973334738424</v>
+      </c>
+      <c r="M17">
         <v>0.0002640644396388745</v>
       </c>
       <c r="O17">
+        <v>0.009685349739034687</v>
+      </c>
+      <c r="P17">
+        <v>0.005106524251936465</v>
+      </c>
+      <c r="Q17">
+        <v>0.009204693368560462</v>
+      </c>
+      <c r="S17">
         <v>0.2289566739349258</v>
       </c>
-      <c r="P17">
+      <c r="T17">
         <v>0.004252957223118693</v>
-      </c>
-      <c r="Q17">
-        <v>0.009685349739034687</v>
-      </c>
-      <c r="R17">
-        <v>0.005106524251936465</v>
-      </c>
-      <c r="S17">
-        <v>0.0003741973334738424</v>
-      </c>
-      <c r="T17">
-        <v>0.009204693368560462</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -1480,26 +1483,26 @@
       <c r="I18">
         <v>12051</v>
       </c>
-      <c r="L18">
+      <c r="K18">
+        <v>0.0004008200453677453</v>
+      </c>
+      <c r="M18">
         <v>0.0003482779314587717</v>
       </c>
       <c r="O18">
+        <v>0.01017444484578581</v>
+      </c>
+      <c r="P18">
+        <v>0.005371111699895803</v>
+      </c>
+      <c r="Q18">
+        <v>0.009769435123820693</v>
+      </c>
+      <c r="S18">
         <v>0.1478874304814285</v>
       </c>
-      <c r="P18">
+      <c r="T18">
         <v>0.004769747765218425</v>
-      </c>
-      <c r="Q18">
-        <v>0.01017444484578581</v>
-      </c>
-      <c r="R18">
-        <v>0.005371111699895803</v>
-      </c>
-      <c r="S18">
-        <v>0.0004008200453677453</v>
-      </c>
-      <c r="T18">
-        <v>0.009769435123820693</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -1530,26 +1533,26 @@
       <c r="I19">
         <v>14156</v>
       </c>
-      <c r="L19">
+      <c r="K19">
+        <v>0.0004006378783650764</v>
+      </c>
+      <c r="M19">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O19">
+        <v>0.0102119158074488</v>
+      </c>
+      <c r="P19">
+        <v>0.005239736253559311</v>
+      </c>
+      <c r="Q19">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="S19">
         <v>0.1218694481841025</v>
       </c>
-      <c r="P19">
+      <c r="T19">
         <v>0.004818030126325817</v>
-      </c>
-      <c r="Q19">
-        <v>0.0102119158074488</v>
-      </c>
-      <c r="R19">
-        <v>0.005239736253559311</v>
-      </c>
-      <c r="S19">
-        <v>0.0004006378783650764</v>
-      </c>
-      <c r="T19">
-        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -1580,26 +1583,26 @@
       <c r="I20">
         <v>6771</v>
       </c>
-      <c r="L20">
+      <c r="K20">
+        <v>0.0001324165619288979</v>
+      </c>
+      <c r="M20">
         <v>0.0001037297229528328</v>
       </c>
       <c r="O20">
+        <v>0.006002882908757912</v>
+      </c>
+      <c r="P20">
+        <v>0.003330775568204595</v>
+      </c>
+      <c r="Q20">
+        <v>0.005813234561065725</v>
+      </c>
+      <c r="S20">
         <v>0.2606707993949464</v>
       </c>
-      <c r="P20">
+      <c r="T20">
         <v>0.003193202088483064</v>
-      </c>
-      <c r="Q20">
-        <v>0.006002882908757912</v>
-      </c>
-      <c r="R20">
-        <v>0.003330775568204595</v>
-      </c>
-      <c r="S20">
-        <v>0.0001324165619288979</v>
-      </c>
-      <c r="T20">
-        <v>0.005813234561065725</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -1630,26 +1633,26 @@
       <c r="I21">
         <v>6771</v>
       </c>
-      <c r="L21">
+      <c r="K21">
+        <v>0.0001424514975481683</v>
+      </c>
+      <c r="M21">
         <v>0.0001037297229528328</v>
       </c>
       <c r="O21">
+        <v>0.00595976388177965</v>
+      </c>
+      <c r="P21">
+        <v>0.002972129451884979</v>
+      </c>
+      <c r="Q21">
+        <v>0.005813234561065725</v>
+      </c>
+      <c r="S21">
         <v>0.2046421514566161</v>
       </c>
-      <c r="P21">
+      <c r="T21">
         <v>0.003193202088483064</v>
-      </c>
-      <c r="Q21">
-        <v>0.00595976388177965</v>
-      </c>
-      <c r="R21">
-        <v>0.002972129451884979</v>
-      </c>
-      <c r="S21">
-        <v>0.0001424514975481683</v>
-      </c>
-      <c r="T21">
-        <v>0.005813234561065725</v>
       </c>
     </row>
     <row r="22" spans="1:20">
@@ -1680,26 +1683,26 @@
       <c r="I22">
         <v>6771</v>
       </c>
-      <c r="L22">
+      <c r="K22">
+        <v>0.00013855240761432</v>
+      </c>
+      <c r="M22">
         <v>0.0001037297229528328</v>
       </c>
       <c r="O22">
+        <v>0.00592641693601841</v>
+      </c>
+      <c r="P22">
+        <v>0.003005755874836842</v>
+      </c>
+      <c r="Q22">
+        <v>0.005813234561065725</v>
+      </c>
+      <c r="S22">
         <v>0.2264121702660996</v>
       </c>
-      <c r="P22">
+      <c r="T22">
         <v>0.003193202088483064</v>
-      </c>
-      <c r="Q22">
-        <v>0.00592641693601841</v>
-      </c>
-      <c r="R22">
-        <v>0.003005755874836842</v>
-      </c>
-      <c r="S22">
-        <v>0.00013855240761432</v>
-      </c>
-      <c r="T22">
-        <v>0.005813234561065725</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -1730,26 +1733,26 @@
       <c r="I23">
         <v>14156</v>
       </c>
-      <c r="L23">
+      <c r="K23">
+        <v>0.0003279955215444224</v>
+      </c>
+      <c r="M23">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O23">
+        <v>0.008942022948316988</v>
+      </c>
+      <c r="P23">
+        <v>0.004617426367895965</v>
+      </c>
+      <c r="Q23">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="S23">
         <v>0.2810892232598902</v>
       </c>
-      <c r="P23">
+      <c r="T23">
         <v>0.004818030126325817</v>
-      </c>
-      <c r="Q23">
-        <v>0.008942022948316988</v>
-      </c>
-      <c r="R23">
-        <v>0.004617426367895965</v>
-      </c>
-      <c r="S23">
-        <v>0.0003279955215444224</v>
-      </c>
-      <c r="T23">
-        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="24" spans="1:20">
@@ -1780,26 +1783,26 @@
       <c r="I24">
         <v>11611</v>
       </c>
-      <c r="L24">
+      <c r="K24">
+        <v>0.0002083353057278959</v>
+      </c>
+      <c r="M24">
         <v>0.0001631540263502446</v>
       </c>
       <c r="O24">
+        <v>0.005089153979501482</v>
+      </c>
+      <c r="P24">
+        <v>0.001554417436991534</v>
+      </c>
+      <c r="Q24">
+        <v>0.004580501696160511</v>
+      </c>
+      <c r="S24">
         <v>-0.004454544482717981</v>
       </c>
-      <c r="P24">
+      <c r="T24">
         <v>0.001592932311570713</v>
-      </c>
-      <c r="Q24">
-        <v>0.005089153979501482</v>
-      </c>
-      <c r="R24">
-        <v>0.001554417436991534</v>
-      </c>
-      <c r="S24">
-        <v>0.0002083353057278959</v>
-      </c>
-      <c r="T24">
-        <v>0.004580501696160511</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -1830,26 +1833,26 @@
       <c r="I25">
         <v>14156</v>
       </c>
-      <c r="L25">
+      <c r="K25">
+        <v>0.0003254854012574867</v>
+      </c>
+      <c r="M25">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O25">
+        <v>0.008855143980453176</v>
+      </c>
+      <c r="P25">
+        <v>0.00456770441607247</v>
+      </c>
+      <c r="Q25">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="S25">
         <v>0.2865909829079945</v>
       </c>
-      <c r="P25">
+      <c r="T25">
         <v>0.004818030126325816</v>
-      </c>
-      <c r="Q25">
-        <v>0.008855143980453176</v>
-      </c>
-      <c r="R25">
-        <v>0.00456770441607247</v>
-      </c>
-      <c r="S25">
-        <v>0.0003254854012574867</v>
-      </c>
-      <c r="T25">
-        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="26" spans="1:20">
@@ -1880,26 +1883,26 @@
       <c r="I26">
         <v>11542</v>
       </c>
-      <c r="L26">
+      <c r="K26">
+        <v>0.0002091701444985722</v>
+      </c>
+      <c r="M26">
         <v>0.000163888349337522</v>
       </c>
       <c r="O26">
+        <v>0.00510134746390362</v>
+      </c>
+      <c r="P26">
+        <v>0.001583264354559398</v>
+      </c>
+      <c r="Q26">
+        <v>0.004589584286176587</v>
+      </c>
+      <c r="S26">
         <v>-0.005012774390606101</v>
       </c>
-      <c r="P26">
+      <c r="T26">
         <v>0.001597174444307401</v>
-      </c>
-      <c r="Q26">
-        <v>0.00510134746390362</v>
-      </c>
-      <c r="R26">
-        <v>0.001583264354559398</v>
-      </c>
-      <c r="S26">
-        <v>0.0002091701444985722</v>
-      </c>
-      <c r="T26">
-        <v>0.004589584286176587</v>
       </c>
     </row>
     <row r="27" spans="1:20">
@@ -1930,26 +1933,26 @@
       <c r="I27">
         <v>6771</v>
       </c>
-      <c r="L27">
+      <c r="K27">
+        <v>0.0001427653829362463</v>
+      </c>
+      <c r="M27">
         <v>0.0001037297229528328</v>
       </c>
       <c r="O27">
+        <v>0.006096382291329448</v>
+      </c>
+      <c r="P27">
+        <v>0.003125364361436701</v>
+      </c>
+      <c r="Q27">
+        <v>0.005813234561065723</v>
+      </c>
+      <c r="S27">
         <v>0.2028896166553128</v>
       </c>
-      <c r="P27">
+      <c r="T27">
         <v>0.003193202088483064</v>
-      </c>
-      <c r="Q27">
-        <v>0.006096382291329448</v>
-      </c>
-      <c r="R27">
-        <v>0.003125364361436701</v>
-      </c>
-      <c r="S27">
-        <v>0.0001427653829362463</v>
-      </c>
-      <c r="T27">
-        <v>0.005813234561065723</v>
       </c>
     </row>
     <row r="28" spans="1:20">
@@ -1980,26 +1983,26 @@
       <c r="I28">
         <v>6771</v>
       </c>
-      <c r="L28">
+      <c r="K28">
+        <v>0.0001433490956550128</v>
+      </c>
+      <c r="M28">
         <v>0.0001037297229528328</v>
       </c>
       <c r="O28">
+        <v>0.00610593491672969</v>
+      </c>
+      <c r="P28">
+        <v>0.003163476470023769</v>
+      </c>
+      <c r="Q28">
+        <v>0.005813234561065723</v>
+      </c>
+      <c r="S28">
         <v>0.1996305390032257</v>
       </c>
-      <c r="P28">
+      <c r="T28">
         <v>0.003193202088483064</v>
-      </c>
-      <c r="Q28">
-        <v>0.00610593491672969</v>
-      </c>
-      <c r="R28">
-        <v>0.003163476470023769</v>
-      </c>
-      <c r="S28">
-        <v>0.0001433490956550128</v>
-      </c>
-      <c r="T28">
-        <v>0.005813234561065723</v>
       </c>
     </row>
     <row r="29" spans="1:20">
@@ -2030,26 +2033,26 @@
       <c r="I29">
         <v>6771</v>
       </c>
-      <c r="L29">
+      <c r="K29">
+        <v>0.0001429245641932233</v>
+      </c>
+      <c r="M29">
         <v>0.0001037297229528328</v>
       </c>
       <c r="O29">
+        <v>0.006067498374332903</v>
+      </c>
+      <c r="P29">
+        <v>0.003090643964573058</v>
+      </c>
+      <c r="Q29">
+        <v>0.005813234561065723</v>
+      </c>
+      <c r="S29">
         <v>0.2020008505541708</v>
       </c>
-      <c r="P29">
+      <c r="T29">
         <v>0.003193202088483064</v>
-      </c>
-      <c r="Q29">
-        <v>0.006067498374332903</v>
-      </c>
-      <c r="R29">
-        <v>0.003090643964573058</v>
-      </c>
-      <c r="S29">
-        <v>0.0001429245641932233</v>
-      </c>
-      <c r="T29">
-        <v>0.005813234561065723</v>
       </c>
     </row>
     <row r="30" spans="1:20">
@@ -2080,26 +2083,26 @@
       <c r="I30">
         <v>11611</v>
       </c>
-      <c r="L30">
+      <c r="K30">
+        <v>0.000207986162951978</v>
+      </c>
+      <c r="M30">
         <v>0.0001631540263502446</v>
       </c>
       <c r="O30">
+        <v>0.005107549406927882</v>
+      </c>
+      <c r="P30">
+        <v>0.001554596452837835</v>
+      </c>
+      <c r="Q30">
+        <v>0.004580501696160511</v>
+      </c>
+      <c r="S30">
         <v>-0.002771209789547591</v>
       </c>
-      <c r="P30">
+      <c r="T30">
         <v>0.001592932311570713</v>
-      </c>
-      <c r="Q30">
-        <v>0.005107549406927882</v>
-      </c>
-      <c r="R30">
-        <v>0.001554596452837835</v>
-      </c>
-      <c r="S30">
-        <v>0.000207986162951978</v>
-      </c>
-      <c r="T30">
-        <v>0.004580501696160511</v>
       </c>
     </row>
     <row r="31" spans="1:20">
@@ -2130,26 +2133,26 @@
       <c r="I31">
         <v>6771</v>
       </c>
-      <c r="L31">
+      <c r="K31">
+        <v>0.000160150142460433</v>
+      </c>
+      <c r="M31">
         <v>0.0001037297229528328</v>
       </c>
       <c r="O31">
+        <v>0.006776662396495037</v>
+      </c>
+      <c r="P31">
+        <v>0.003715325925925931</v>
+      </c>
+      <c r="Q31">
+        <v>0.005813234561065723</v>
+      </c>
+      <c r="S31">
         <v>0.1058242633905934</v>
       </c>
-      <c r="P31">
+      <c r="T31">
         <v>0.003193202088483064</v>
-      </c>
-      <c r="Q31">
-        <v>0.006776662396495037</v>
-      </c>
-      <c r="R31">
-        <v>0.003715325925925931</v>
-      </c>
-      <c r="S31">
-        <v>0.000160150142460433</v>
-      </c>
-      <c r="T31">
-        <v>0.005813234561065723</v>
       </c>
     </row>
     <row r="32" spans="1:20">
@@ -2180,26 +2183,26 @@
       <c r="I32">
         <v>4010</v>
       </c>
-      <c r="L32">
+      <c r="K32">
+        <v>0.0002742305932959652</v>
+      </c>
+      <c r="M32">
         <v>0.0001730864695810989</v>
       </c>
       <c r="O32">
+        <v>0.004501420066184821</v>
+      </c>
+      <c r="P32">
+        <v>0.001362431751651251</v>
+      </c>
+      <c r="Q32">
+        <v>0.004349183403839366</v>
+      </c>
+      <c r="S32">
         <v>-0.006214540120261569</v>
       </c>
-      <c r="P32">
+      <c r="T32">
         <v>0.001438312583710056</v>
-      </c>
-      <c r="Q32">
-        <v>0.004501420066184821</v>
-      </c>
-      <c r="R32">
-        <v>0.001362431751651251</v>
-      </c>
-      <c r="S32">
-        <v>0.0002742305932959652</v>
-      </c>
-      <c r="T32">
-        <v>0.004349183403839366</v>
       </c>
     </row>
     <row r="33" spans="1:20">
@@ -2230,26 +2233,26 @@
       <c r="I33">
         <v>14156</v>
       </c>
-      <c r="L33">
+      <c r="K33">
+        <v>0.0004001063569688302</v>
+      </c>
+      <c r="M33">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O33">
+        <v>0.01035431191953904</v>
+      </c>
+      <c r="P33">
+        <v>0.005409147625572685</v>
+      </c>
+      <c r="Q33">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="S33">
         <v>0.1230344532976788</v>
       </c>
-      <c r="P33">
+      <c r="T33">
         <v>0.004818030126325817</v>
-      </c>
-      <c r="Q33">
-        <v>0.01035431191953904</v>
-      </c>
-      <c r="R33">
-        <v>0.005409147625572685</v>
-      </c>
-      <c r="S33">
-        <v>0.0004001063569688302</v>
-      </c>
-      <c r="T33">
-        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="34" spans="1:20">
@@ -2280,26 +2283,26 @@
       <c r="I34">
         <v>4699</v>
       </c>
-      <c r="L34">
+      <c r="K34">
+        <v>0.0004705186388866096</v>
+      </c>
+      <c r="M34">
         <v>0.0003220429185286173</v>
       </c>
       <c r="O34">
+        <v>0.01022526679210232</v>
+      </c>
+      <c r="P34">
+        <v>0.005350192890365459</v>
+      </c>
+      <c r="Q34">
+        <v>0.009384601794708014</v>
+      </c>
+      <c r="S34">
         <v>0.1094051116331665</v>
       </c>
-      <c r="P34">
+      <c r="T34">
         <v>0.004731165595531388</v>
-      </c>
-      <c r="Q34">
-        <v>0.01022526679210232</v>
-      </c>
-      <c r="R34">
-        <v>0.005350192890365459</v>
-      </c>
-      <c r="S34">
-        <v>0.0004705186388866096</v>
-      </c>
-      <c r="T34">
-        <v>0.009384601794708014</v>
       </c>
     </row>
     <row r="35" spans="1:20">
@@ -2330,26 +2333,26 @@
       <c r="I35">
         <v>11611</v>
       </c>
-      <c r="L35">
+      <c r="K35">
+        <v>0.0002081444394071696</v>
+      </c>
+      <c r="M35">
         <v>0.0001631540263502446</v>
       </c>
       <c r="O35">
+        <v>0.005089488294347637</v>
+      </c>
+      <c r="P35">
+        <v>0.001547174514616301</v>
+      </c>
+      <c r="Q35">
+        <v>0.004580501696160511</v>
+      </c>
+      <c r="S35">
         <v>-0.00353431378743374</v>
       </c>
-      <c r="P35">
+      <c r="T35">
         <v>0.001592932311570713</v>
-      </c>
-      <c r="Q35">
-        <v>0.005089488294347637</v>
-      </c>
-      <c r="R35">
-        <v>0.001547174514616301</v>
-      </c>
-      <c r="S35">
-        <v>0.0002081444394071696</v>
-      </c>
-      <c r="T35">
-        <v>0.004580501696160511</v>
       </c>
     </row>
     <row r="36" spans="1:20">
@@ -2380,26 +2383,26 @@
       <c r="I36">
         <v>14156</v>
       </c>
-      <c r="L36">
+      <c r="K36">
+        <v>0.0003610907680501377</v>
+      </c>
+      <c r="M36">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O36">
+        <v>0.009406309171688502</v>
+      </c>
+      <c r="P36">
+        <v>0.004884082851211167</v>
+      </c>
+      <c r="Q36">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="S36">
         <v>0.2085500335179142</v>
       </c>
-      <c r="P36">
+      <c r="T36">
         <v>0.004818030126325816</v>
-      </c>
-      <c r="Q36">
-        <v>0.009406309171688502</v>
-      </c>
-      <c r="R36">
-        <v>0.004884082851211167</v>
-      </c>
-      <c r="S36">
-        <v>0.0003610907680501377</v>
-      </c>
-      <c r="T36">
-        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="37" spans="1:20">
@@ -2430,26 +2433,26 @@
       <c r="I37">
         <v>14156</v>
       </c>
-      <c r="L37">
+      <c r="K37">
+        <v>0.0003710863970746162</v>
+      </c>
+      <c r="M37">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O37">
+        <v>0.009535796789931871</v>
+      </c>
+      <c r="P37">
+        <v>0.004784771004405694</v>
+      </c>
+      <c r="Q37">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="S37">
         <v>0.1866413032030688</v>
       </c>
-      <c r="P37">
+      <c r="T37">
         <v>0.004818030126325816</v>
-      </c>
-      <c r="Q37">
-        <v>0.009535796789931871</v>
-      </c>
-      <c r="R37">
-        <v>0.004784771004405694</v>
-      </c>
-      <c r="S37">
-        <v>0.0003710863970746162</v>
-      </c>
-      <c r="T37">
-        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="38" spans="1:20">
@@ -2480,26 +2483,26 @@
       <c r="I38">
         <v>14156</v>
       </c>
-      <c r="L38">
+      <c r="K38">
+        <v>0.0003744000227958637</v>
+      </c>
+      <c r="M38">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O38">
+        <v>0.009554445336689437</v>
+      </c>
+      <c r="P38">
+        <v>0.004730871750625608</v>
+      </c>
+      <c r="Q38">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="S38">
         <v>0.179378395374721</v>
       </c>
-      <c r="P38">
+      <c r="T38">
         <v>0.004818030126325817</v>
-      </c>
-      <c r="Q38">
-        <v>0.009554445336689437</v>
-      </c>
-      <c r="R38">
-        <v>0.004730871750625608</v>
-      </c>
-      <c r="S38">
-        <v>0.0003744000227958637</v>
-      </c>
-      <c r="T38">
-        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="39" spans="1:20">
@@ -2530,26 +2533,26 @@
       <c r="I39">
         <v>14156</v>
       </c>
-      <c r="L39">
+      <c r="K39">
+        <v>0.0003746361399868205</v>
+      </c>
+      <c r="M39">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O39">
+        <v>0.009555217528480035</v>
+      </c>
+      <c r="P39">
+        <v>0.004764640177213803</v>
+      </c>
+      <c r="Q39">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="S39">
         <v>0.1788608663781261</v>
       </c>
-      <c r="P39">
+      <c r="T39">
         <v>0.004818030126325817</v>
-      </c>
-      <c r="Q39">
-        <v>0.009555217528480035</v>
-      </c>
-      <c r="R39">
-        <v>0.004764640177213803</v>
-      </c>
-      <c r="S39">
-        <v>0.0003746361399868205</v>
-      </c>
-      <c r="T39">
-        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="40" spans="1:20">
@@ -2580,26 +2583,26 @@
       <c r="I40">
         <v>14156</v>
       </c>
-      <c r="L40">
+      <c r="K40">
+        <v>0.0003736225585176234</v>
+      </c>
+      <c r="M40">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O40">
+        <v>0.009526287265811475</v>
+      </c>
+      <c r="P40">
+        <v>0.004756476812602748</v>
+      </c>
+      <c r="Q40">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="S40">
         <v>0.1810824657398455</v>
       </c>
-      <c r="P40">
+      <c r="T40">
         <v>0.004818030126325817</v>
-      </c>
-      <c r="Q40">
-        <v>0.009526287265811475</v>
-      </c>
-      <c r="R40">
-        <v>0.004756476812602748</v>
-      </c>
-      <c r="S40">
-        <v>0.0003736225585176234</v>
-      </c>
-      <c r="T40">
-        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="41" spans="1:20">
@@ -2630,26 +2633,26 @@
       <c r="I41">
         <v>6771</v>
       </c>
-      <c r="L41">
+      <c r="K41">
+        <v>0.0001603751212724098</v>
+      </c>
+      <c r="M41">
         <v>0.0001037297229528328</v>
       </c>
       <c r="O41">
+        <v>0.00674135934653288</v>
+      </c>
+      <c r="P41">
+        <v>0.003667719421830667</v>
+      </c>
+      <c r="Q41">
+        <v>0.005813234561065723</v>
+      </c>
+      <c r="S41">
         <v>0.1045681259196538</v>
       </c>
-      <c r="P41">
+      <c r="T41">
         <v>0.003193202088483064</v>
-      </c>
-      <c r="Q41">
-        <v>0.00674135934653288</v>
-      </c>
-      <c r="R41">
-        <v>0.003667719421830667</v>
-      </c>
-      <c r="S41">
-        <v>0.0001603751212724098</v>
-      </c>
-      <c r="T41">
-        <v>0.005813234561065723</v>
       </c>
     </row>
     <row r="42" spans="1:20">
@@ -2680,26 +2683,26 @@
       <c r="I42">
         <v>14156</v>
       </c>
-      <c r="L42">
+      <c r="K42">
+        <v>0.0003609428129771297</v>
+      </c>
+      <c r="M42">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O42">
+        <v>0.009669808352814117</v>
+      </c>
+      <c r="P42">
+        <v>0.005274143159156646</v>
+      </c>
+      <c r="Q42">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="S42">
         <v>0.2088743260447083</v>
       </c>
-      <c r="P42">
+      <c r="T42">
         <v>0.004818030126325816</v>
-      </c>
-      <c r="Q42">
-        <v>0.009669808352814117</v>
-      </c>
-      <c r="R42">
-        <v>0.005274143159156646</v>
-      </c>
-      <c r="S42">
-        <v>0.0003609428129771297</v>
-      </c>
-      <c r="T42">
-        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="43" spans="1:20">
@@ -2730,26 +2733,26 @@
       <c r="I43">
         <v>14156</v>
       </c>
-      <c r="L43">
+      <c r="K43">
+        <v>0.0003635971635380399</v>
+      </c>
+      <c r="M43">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O43">
+        <v>0.009719161233546112</v>
+      </c>
+      <c r="P43">
+        <v>0.005173194757001598</v>
+      </c>
+      <c r="Q43">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="S43">
         <v>0.2030564380000814</v>
       </c>
-      <c r="P43">
+      <c r="T43">
         <v>0.004818030126325817</v>
-      </c>
-      <c r="Q43">
-        <v>0.009719161233546112</v>
-      </c>
-      <c r="R43">
-        <v>0.005173194757001598</v>
-      </c>
-      <c r="S43">
-        <v>0.0003635971635380399</v>
-      </c>
-      <c r="T43">
-        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="44" spans="1:20">
@@ -2780,26 +2783,26 @@
       <c r="I44">
         <v>14156</v>
       </c>
-      <c r="L44">
+      <c r="K44">
+        <v>0.0003344607981243851</v>
+      </c>
+      <c r="M44">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O44">
+        <v>0.00867861064019221</v>
+      </c>
+      <c r="P44">
+        <v>0.004128330862335852</v>
+      </c>
+      <c r="Q44">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="S44">
         <v>0.2669184291403396</v>
       </c>
-      <c r="P44">
+      <c r="T44">
         <v>0.004818030126325817</v>
-      </c>
-      <c r="Q44">
-        <v>0.00867861064019221</v>
-      </c>
-      <c r="R44">
-        <v>0.004128330862335852</v>
-      </c>
-      <c r="S44">
-        <v>0.0003344607981243851</v>
-      </c>
-      <c r="T44">
-        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="45" spans="1:20">
@@ -2830,26 +2833,26 @@
       <c r="I45">
         <v>14156</v>
       </c>
-      <c r="L45">
+      <c r="K45">
+        <v>0.0003886501570187028</v>
+      </c>
+      <c r="M45">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O45">
+        <v>0.01011738460212881</v>
+      </c>
+      <c r="P45">
+        <v>0.005394960099510664</v>
+      </c>
+      <c r="Q45">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="S45">
         <v>0.1481445083553075</v>
       </c>
-      <c r="P45">
+      <c r="T45">
         <v>0.004818030126325816</v>
-      </c>
-      <c r="Q45">
-        <v>0.01011738460212881</v>
-      </c>
-      <c r="R45">
-        <v>0.005394960099510664</v>
-      </c>
-      <c r="S45">
-        <v>0.0003886501570187028</v>
-      </c>
-      <c r="T45">
-        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="46" spans="1:20">
@@ -2880,26 +2883,26 @@
       <c r="I46">
         <v>14156</v>
       </c>
-      <c r="L46">
+      <c r="K46">
+        <v>0.0004313797729252501</v>
+      </c>
+      <c r="M46">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O46">
+        <v>0.01064772150300563</v>
+      </c>
+      <c r="P46">
+        <v>0.005560650653515711</v>
+      </c>
+      <c r="Q46">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="S46">
         <v>0.05448840836791147</v>
       </c>
-      <c r="P46">
+      <c r="T46">
         <v>0.004818030126325817</v>
-      </c>
-      <c r="Q46">
-        <v>0.01064772150300563</v>
-      </c>
-      <c r="R46">
-        <v>0.005560650653515711</v>
-      </c>
-      <c r="S46">
-        <v>0.0004313797729252501</v>
-      </c>
-      <c r="T46">
-        <v>0.009674189396799985</v>
       </c>
     </row>
     <row r="47" spans="1:20">
@@ -2931,37 +2934,37 @@
         <v>5153</v>
       </c>
       <c r="J47">
+        <v>0.4055123229186881</v>
+      </c>
+      <c r="K47">
+        <v>0.000141190946981845</v>
+      </c>
+      <c r="L47">
         <v>10.4129840341794</v>
       </c>
-      <c r="K47">
-        <v>0.4055123229186881</v>
-      </c>
-      <c r="L47">
+      <c r="M47">
         <v>9.243123959608208E-05</v>
-      </c>
-      <c r="M47">
-        <v>0.4113135413420823</v>
       </c>
       <c r="N47">
         <v>11.43997477570016</v>
       </c>
       <c r="O47">
+        <v>0.005626234126090045</v>
+      </c>
+      <c r="P47">
+        <v>0.002733726006933551</v>
+      </c>
+      <c r="Q47">
+        <v>0.005318929375230071</v>
+      </c>
+      <c r="R47">
+        <v>0.4113135413420823</v>
+      </c>
+      <c r="S47">
         <v>0.1703625716885953</v>
       </c>
-      <c r="P47">
+      <c r="T47">
         <v>0.002848413552158193</v>
-      </c>
-      <c r="Q47">
-        <v>0.005626234126090045</v>
-      </c>
-      <c r="R47">
-        <v>0.002733726006933551</v>
-      </c>
-      <c r="S47">
-        <v>0.000141190946981845</v>
-      </c>
-      <c r="T47">
-        <v>0.005318929375230071</v>
       </c>
     </row>
     <row r="48" spans="1:20">
@@ -2992,26 +2995,26 @@
       <c r="I48">
         <v>14156</v>
       </c>
-      <c r="L48">
+      <c r="K48">
+        <v>0.0004139067990685161</v>
+      </c>
+      <c r="M48">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O48">
+        <v>0.01060174085834054</v>
+      </c>
+      <c r="P48">
+        <v>0.005675761589993111</v>
+      </c>
+      <c r="Q48">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="S48">
         <v>0.09278621544819221</v>
       </c>
-      <c r="P48">
+      <c r="T48">
         <v>0.004818030126325816</v>
-      </c>
-      <c r="Q48">
-        <v>0.01060174085834054</v>
-      </c>
-      <c r="R48">
-        <v>0.005675761589993111</v>
-      </c>
-      <c r="S48">
-        <v>0.0004139067990685161</v>
-      </c>
-      <c r="T48">
-        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="49" spans="1:20">
@@ -3042,26 +3045,26 @@
       <c r="I49">
         <v>14156</v>
       </c>
-      <c r="L49">
+      <c r="K49">
+        <v>0.0004026104577395279</v>
+      </c>
+      <c r="M49">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O49">
+        <v>0.01035467890006862</v>
+      </c>
+      <c r="P49">
+        <v>0.005399385735558927</v>
+      </c>
+      <c r="Q49">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="S49">
         <v>0.1175458874123242</v>
       </c>
-      <c r="P49">
+      <c r="T49">
         <v>0.004818030126325817</v>
-      </c>
-      <c r="Q49">
-        <v>0.01035467890006862</v>
-      </c>
-      <c r="R49">
-        <v>0.005399385735558927</v>
-      </c>
-      <c r="S49">
-        <v>0.0004026104577395279</v>
-      </c>
-      <c r="T49">
-        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="50" spans="1:20">
@@ -3092,26 +3095,26 @@
       <c r="I50">
         <v>11611</v>
       </c>
-      <c r="L50">
+      <c r="K50">
+        <v>0.0002080153046483946</v>
+      </c>
+      <c r="M50">
         <v>0.0001631540263502446</v>
       </c>
       <c r="O50">
+        <v>0.005090949099942899</v>
+      </c>
+      <c r="P50">
+        <v>0.001550051802718652</v>
+      </c>
+      <c r="Q50">
+        <v>0.004580501696160511</v>
+      </c>
+      <c r="S50">
         <v>-0.002911711704464803</v>
       </c>
-      <c r="P50">
+      <c r="T50">
         <v>0.001592932311570713</v>
-      </c>
-      <c r="Q50">
-        <v>0.005090949099942899</v>
-      </c>
-      <c r="R50">
-        <v>0.001550051802718652</v>
-      </c>
-      <c r="S50">
-        <v>0.0002080153046483946</v>
-      </c>
-      <c r="T50">
-        <v>0.004580501696160511</v>
       </c>
     </row>
     <row r="51" spans="1:20">
@@ -3142,26 +3145,26 @@
       <c r="I51">
         <v>14156</v>
       </c>
-      <c r="L51">
+      <c r="K51">
+        <v>0.0003438074749231005</v>
+      </c>
+      <c r="M51">
         <v>0.0003384092866814527</v>
       </c>
       <c r="O51">
+        <v>0.009263751492683912</v>
+      </c>
+      <c r="P51">
+        <v>0.004666820467017538</v>
+      </c>
+      <c r="Q51">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="S51">
         <v>0.2464320924804251</v>
       </c>
-      <c r="P51">
+      <c r="T51">
         <v>0.004818030126325817</v>
-      </c>
-      <c r="Q51">
-        <v>0.009263751492683912</v>
-      </c>
-      <c r="R51">
-        <v>0.004666820467017538</v>
-      </c>
-      <c r="S51">
-        <v>0.0003438074749231005</v>
-      </c>
-      <c r="T51">
-        <v>0.009674189396799987</v>
       </c>
     </row>
     <row r="52" spans="1:20">
@@ -3192,26 +3195,76 @@
       <c r="I52">
         <v>1267</v>
       </c>
-      <c r="L52">
+      <c r="K52">
+        <v>0.0006028948928221208</v>
+      </c>
+      <c r="M52">
         <v>0.0004283113735138171</v>
       </c>
       <c r="O52">
+        <v>0.0102050584404969</v>
+      </c>
+      <c r="P52">
+        <v>0.005379622896887214</v>
+      </c>
+      <c r="Q52">
+        <v>0.01026809155717979</v>
+      </c>
+      <c r="S52">
         <v>0.2718477491393597</v>
       </c>
-      <c r="P52">
+      <c r="T52">
         <v>0.004670472236637264</v>
       </c>
-      <c r="Q52">
-        <v>0.0102050584404969</v>
-      </c>
-      <c r="R52">
-        <v>0.005379622896887214</v>
-      </c>
-      <c r="S52">
-        <v>0.0006028948928221208</v>
-      </c>
-      <c r="T52">
-        <v>0.01026809155717979</v>
+    </row>
+    <row r="53" spans="1:20">
+      <c r="A53" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53">
+        <v>0.009592505378186515</v>
+      </c>
+      <c r="C53">
+        <v>0.008764961593413305</v>
+      </c>
+      <c r="D53">
+        <v>0.0001961445305465736</v>
+      </c>
+      <c r="E53">
+        <v>0.0001968262288307614</v>
+      </c>
+      <c r="F53">
+        <v>0.122423362108982</v>
+      </c>
+      <c r="G53">
+        <v>0.1193733535942066</v>
+      </c>
+      <c r="H53">
+        <v>0.2253493365624453</v>
+      </c>
+      <c r="I53">
+        <v>7054</v>
+      </c>
+      <c r="K53">
+        <v>0.0003426357597594948</v>
+      </c>
+      <c r="M53">
+        <v>0.0002911643753660776</v>
+      </c>
+      <c r="O53">
+        <v>0.01043843340429874</v>
+      </c>
+      <c r="P53">
+        <v>0.005648699862893431</v>
+      </c>
+      <c r="Q53">
+        <v>0.009545579499406483</v>
+      </c>
+      <c r="S53">
+        <v>0.08840833195541187</v>
+      </c>
+      <c r="T53">
+        <v>0.004876716066832584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update xgboost new space
</commit_message>
<xml_diff>
--- a/results_analysis/compare_with_ibes/#compare_all.xlsx
+++ b/results_analysis/compare_with_ibes/#compare_all.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>lgbm_mae</t>
   </si>
@@ -43,36 +43,36 @@
     <t>consensus_mae_eps</t>
   </si>
   <si>
+    <t>lgbm_mape_eps</t>
+  </si>
+  <si>
+    <t>consensus_mae_org</t>
+  </si>
+  <si>
+    <t>consensus_mape_eps</t>
+  </si>
+  <si>
+    <t>consensus_medae_org</t>
+  </si>
+  <si>
+    <t>lgbm_mae_org</t>
+  </si>
+  <si>
+    <t>lgbm_r2_org</t>
+  </si>
+  <si>
+    <t>consensus_mse_org</t>
+  </si>
+  <si>
     <t>lgbm_mse_org</t>
   </si>
   <si>
-    <t>consensus_mape_eps</t>
-  </si>
-  <si>
-    <t>consensus_mse_org</t>
-  </si>
-  <si>
-    <t>lgbm_mape_eps</t>
-  </si>
-  <si>
-    <t>lgbm_mae_org</t>
-  </si>
-  <si>
     <t>lgbm_medae_org</t>
   </si>
   <si>
-    <t>consensus_mae_org</t>
-  </si>
-  <si>
     <t>lgbm_mae_eps</t>
   </si>
   <si>
-    <t>lgbm_r2_org</t>
-  </si>
-  <si>
-    <t>consensus_medae_org</t>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>ibes_2|ni_depthwise|xgb ind_all_tuning -sample_type industry -x_type ni</t>
+  </si>
+  <si>
+    <t>ibes_2|fwdepsqcut|optimize_r2_industry</t>
   </si>
   <si>
     <t>ibes_2|fwdepsqcut|ibes_new industry_only ws -indi space3</t>
@@ -587,7 +590,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T53"/>
+  <dimension ref="A1:T54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -683,26 +686,26 @@
       <c r="I2">
         <v>14156</v>
       </c>
-      <c r="K2">
-        <v>0.0004250480609163007</v>
-      </c>
-      <c r="M2">
-        <v>0.0003384092866814527</v>
+      <c r="L2">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="N2">
+        <v>0.004818030126325816</v>
       </c>
       <c r="O2">
         <v>0.01071193221870467</v>
       </c>
       <c r="P2">
+        <v>0.06836645151013176</v>
+      </c>
+      <c r="Q2">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="R2">
+        <v>0.0004250480609163007</v>
+      </c>
+      <c r="S2">
         <v>0.005638666708596741</v>
-      </c>
-      <c r="Q2">
-        <v>0.009674189396799987</v>
-      </c>
-      <c r="S2">
-        <v>0.06836645151013176</v>
-      </c>
-      <c r="T2">
-        <v>0.004818030126325816</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -733,26 +736,26 @@
       <c r="I3">
         <v>11611</v>
       </c>
-      <c r="K3">
-        <v>0.0001978384306784256</v>
-      </c>
-      <c r="M3">
-        <v>0.0001631540263502446</v>
+      <c r="L3">
+        <v>0.004580501696160511</v>
+      </c>
+      <c r="N3">
+        <v>0.001592932311570713</v>
       </c>
       <c r="O3">
         <v>0.00502885184437347</v>
       </c>
       <c r="P3">
+        <v>0.04615441883950755</v>
+      </c>
+      <c r="Q3">
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="R3">
+        <v>0.0001978384306784256</v>
+      </c>
+      <c r="S3">
         <v>0.001779221775169934</v>
-      </c>
-      <c r="Q3">
-        <v>0.004580501696160511</v>
-      </c>
-      <c r="S3">
-        <v>0.04615441883950755</v>
-      </c>
-      <c r="T3">
-        <v>0.001592932311570713</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -783,26 +786,26 @@
       <c r="I4">
         <v>6771</v>
       </c>
-      <c r="K4">
-        <v>0.0001137832146297872</v>
-      </c>
-      <c r="M4">
-        <v>0.0001037297229528328</v>
+      <c r="L4">
+        <v>0.005813234561065725</v>
+      </c>
+      <c r="N4">
+        <v>0.003193202088483064</v>
       </c>
       <c r="O4">
         <v>0.005606434133779571</v>
       </c>
       <c r="P4">
+        <v>0.36470746642943</v>
+      </c>
+      <c r="Q4">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="R4">
+        <v>0.0001137832146297872</v>
+      </c>
+      <c r="S4">
         <v>0.003094044369724517</v>
-      </c>
-      <c r="Q4">
-        <v>0.005813234561065725</v>
-      </c>
-      <c r="S4">
-        <v>0.36470746642943</v>
-      </c>
-      <c r="T4">
-        <v>0.003193202088483064</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -833,26 +836,26 @@
       <c r="I5">
         <v>6771</v>
       </c>
-      <c r="K5">
-        <v>0.0001152638129503358</v>
-      </c>
-      <c r="M5">
-        <v>0.0001037297229528328</v>
+      <c r="L5">
+        <v>0.005813234561065725</v>
+      </c>
+      <c r="N5">
+        <v>0.003193202088483064</v>
       </c>
       <c r="O5">
         <v>0.005632685300523813</v>
       </c>
       <c r="P5">
+        <v>0.3564407544954944</v>
+      </c>
+      <c r="Q5">
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="R5">
+        <v>0.0001152638129503358</v>
+      </c>
+      <c r="S5">
         <v>0.003171635367762127</v>
-      </c>
-      <c r="Q5">
-        <v>0.005813234561065725</v>
-      </c>
-      <c r="S5">
-        <v>0.3564407544954944</v>
-      </c>
-      <c r="T5">
-        <v>0.003193202088483064</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -883,26 +886,26 @@
       <c r="I6">
         <v>42468</v>
       </c>
-      <c r="K6">
-        <v>0.000333070102780211</v>
-      </c>
-      <c r="M6">
-        <v>0.0003384092866814527</v>
+      <c r="L6">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="N6">
+        <v>0.004818030126325817</v>
       </c>
       <c r="O6">
         <v>0.009106885821888167</v>
       </c>
       <c r="P6">
+        <v>0.269966598412229</v>
+      </c>
+      <c r="Q6">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="R6">
+        <v>0.000333070102780211</v>
+      </c>
+      <c r="S6">
         <v>0.004616722796530505</v>
-      </c>
-      <c r="Q6">
-        <v>0.009674189396799987</v>
-      </c>
-      <c r="S6">
-        <v>0.269966598412229</v>
-      </c>
-      <c r="T6">
-        <v>0.004818030126325817</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -933,26 +936,26 @@
       <c r="I7">
         <v>14156</v>
       </c>
-      <c r="K7">
-        <v>0.0003285627388197843</v>
-      </c>
-      <c r="M7">
-        <v>0.0003384092866814527</v>
+      <c r="L7">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="N7">
+        <v>0.004818030126325817</v>
       </c>
       <c r="O7">
         <v>0.008950010380536522</v>
       </c>
       <c r="P7">
+        <v>0.2798459788092014</v>
+      </c>
+      <c r="Q7">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="R7">
+        <v>0.0003285627388197843</v>
+      </c>
+      <c r="S7">
         <v>0.004615286290830784</v>
-      </c>
-      <c r="Q7">
-        <v>0.009674189396799985</v>
-      </c>
-      <c r="S7">
-        <v>0.2798459788092014</v>
-      </c>
-      <c r="T7">
-        <v>0.004818030126325817</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -960,49 +963,49 @@
         <v>26</v>
       </c>
       <c r="B8">
-        <v>0.008392539580425228</v>
+        <v>0.007217625299424186</v>
       </c>
       <c r="C8">
-        <v>0.008722720041403264</v>
+        <v>0.007503385771072112</v>
       </c>
       <c r="D8">
-        <v>0.0001662926371782633</v>
+        <v>0.000121552070520227</v>
       </c>
       <c r="E8">
-        <v>0.0001985649052123504</v>
+        <v>0.0001421229460831389</v>
       </c>
       <c r="F8">
-        <v>0.2859075504422648</v>
+        <v>0.2901272390281715</v>
       </c>
       <c r="G8">
-        <v>0.147324247391146</v>
+        <v>0.1699918586191453</v>
       </c>
       <c r="H8">
-        <v>0.2582640092197721</v>
+        <v>0.2364760695203898</v>
       </c>
       <c r="I8">
-        <v>14156</v>
-      </c>
-      <c r="K8">
-        <v>0.0003713407546776094</v>
-      </c>
-      <c r="M8">
-        <v>0.0003384092866814527</v>
+        <v>5254</v>
+      </c>
+      <c r="L8">
+        <v>0.007921255031590064</v>
+      </c>
+      <c r="N8">
+        <v>0.004527241212605013</v>
       </c>
       <c r="O8">
-        <v>0.00941140169945745</v>
+        <v>0.007677919171285994</v>
       </c>
       <c r="P8">
-        <v>0.004590555422836876</v>
+        <v>0.2347147170485431</v>
       </c>
       <c r="Q8">
-        <v>0.009674189396799985</v>
+        <v>0.0001858662918611346</v>
+      </c>
+      <c r="R8">
+        <v>0.0001862950617261432</v>
       </c>
       <c r="S8">
-        <v>0.1860837943045432</v>
-      </c>
-      <c r="T8">
-        <v>0.004818030126325816</v>
+        <v>0.004259528456878571</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -1010,49 +1013,49 @@
         <v>27</v>
       </c>
       <c r="B9">
-        <v>0.007970745265560365</v>
+        <v>0.008392539580425228</v>
       </c>
       <c r="C9">
-        <v>0.00654101945735325</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D9">
-        <v>0.0001659654171746955</v>
+        <v>0.0001662926371782633</v>
       </c>
       <c r="E9">
-        <v>0.0001252256324013319</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F9">
-        <v>-0.0277890197779842</v>
+        <v>0.2859075504422648</v>
       </c>
       <c r="G9">
-        <v>0.224503922757791</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H9">
-        <v>0.3127047460379806</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I9">
-        <v>24768</v>
-      </c>
-      <c r="K9">
-        <v>0.0002632414236722758</v>
-      </c>
-      <c r="M9">
-        <v>0.0001796235360933539</v>
+        <v>14156</v>
+      </c>
+      <c r="L9">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="N9">
+        <v>0.004818030126325816</v>
       </c>
       <c r="O9">
-        <v>0.008363098231375462</v>
+        <v>0.00941140169945745</v>
       </c>
       <c r="P9">
-        <v>0.004275415213561056</v>
+        <v>0.1860837943045432</v>
       </c>
       <c r="Q9">
-        <v>0.006875190708555331</v>
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="R9">
+        <v>0.0003713407546776094</v>
       </c>
       <c r="S9">
-        <v>-0.00724317687482956</v>
-      </c>
-      <c r="T9">
-        <v>0.003559726400188349</v>
+        <v>0.004590555422836876</v>
       </c>
     </row>
     <row r="10" spans="1:20">
@@ -1060,49 +1063,49 @@
         <v>28</v>
       </c>
       <c r="B10">
-        <v>0.009885890648801</v>
+        <v>0.007970745265560365</v>
       </c>
       <c r="C10">
-        <v>0.009614451672116909</v>
+        <v>0.00654101945735325</v>
       </c>
       <c r="D10">
-        <v>0.0002810826792241289</v>
+        <v>0.0001659654171746955</v>
       </c>
       <c r="E10">
-        <v>0.0002968767906711129</v>
+        <v>0.0001252256324013319</v>
       </c>
       <c r="F10">
-        <v>0.2059318010033613</v>
+        <v>-0.0277890197779842</v>
       </c>
       <c r="G10">
-        <v>0.1613128950427474</v>
+        <v>0.224503922757791</v>
       </c>
       <c r="H10">
-        <v>0.2582640092197721</v>
+        <v>0.3127047460379806</v>
       </c>
       <c r="I10">
-        <v>14156</v>
-      </c>
-      <c r="K10">
-        <v>0.0003847976244374441</v>
-      </c>
-      <c r="M10">
-        <v>0.0003384092866814527</v>
+        <v>24768</v>
+      </c>
+      <c r="L10">
+        <v>0.006875190708555331</v>
+      </c>
+      <c r="N10">
+        <v>0.003559726400188349</v>
       </c>
       <c r="O10">
-        <v>0.009901025034115019</v>
+        <v>0.008363098231375462</v>
       </c>
       <c r="P10">
-        <v>0.005167135423672592</v>
+        <v>-0.00724317687482956</v>
       </c>
       <c r="Q10">
-        <v>0.009674189396799985</v>
+        <v>0.0001796235360933539</v>
+      </c>
+      <c r="R10">
+        <v>0.0002632414236722758</v>
       </c>
       <c r="S10">
-        <v>0.1565886089862186</v>
-      </c>
-      <c r="T10">
-        <v>0.004818030126325816</v>
+        <v>0.004275415213561056</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1110,49 +1113,49 @@
         <v>29</v>
       </c>
       <c r="B11">
-        <v>0.003125769257313045</v>
+        <v>0.009885890648801</v>
       </c>
       <c r="C11">
-        <v>0.00254141838673398</v>
+        <v>0.009614451672116909</v>
       </c>
       <c r="D11">
-        <v>2.166040204619485E-05</v>
+        <v>0.0002810826792241289</v>
       </c>
       <c r="E11">
-        <v>2.106152912726658E-05</v>
+        <v>0.0002968767906711129</v>
       </c>
       <c r="F11">
-        <v>-0.02738763561426372</v>
+        <v>0.2059318010033613</v>
       </c>
       <c r="G11">
-        <v>0.001017868166272584</v>
+        <v>0.1613128950427474</v>
       </c>
       <c r="H11">
-        <v>0.212555477012045</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I11">
-        <v>11542</v>
-      </c>
-      <c r="K11">
-        <v>0.000209188838038313</v>
-      </c>
-      <c r="M11">
-        <v>0.000163888349337522</v>
+        <v>14156</v>
+      </c>
+      <c r="L11">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="N11">
+        <v>0.004818030126325816</v>
       </c>
       <c r="O11">
-        <v>0.00512210974064752</v>
+        <v>0.009901025034115019</v>
       </c>
       <c r="P11">
-        <v>0.001602037466360856</v>
+        <v>0.1565886089862186</v>
       </c>
       <c r="Q11">
-        <v>0.004589584286176587</v>
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="R11">
+        <v>0.0003847976244374441</v>
       </c>
       <c r="S11">
-        <v>-0.005102592401121431</v>
-      </c>
-      <c r="T11">
-        <v>0.001597174444307401</v>
+        <v>0.005167135423672592</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -1160,49 +1163,49 @@
         <v>30</v>
       </c>
       <c r="B12">
-        <v>0.005058551760597552</v>
+        <v>0.003125769257313045</v>
       </c>
       <c r="C12">
-        <v>0.005699109365498782</v>
+        <v>0.00254141838673398</v>
       </c>
       <c r="D12">
-        <v>7.085921366241217E-05</v>
+        <v>2.166040204619485E-05</v>
       </c>
       <c r="E12">
-        <v>9.470932808225897E-05</v>
+        <v>2.106152912726658E-05</v>
       </c>
       <c r="F12">
-        <v>0.4431418058979847</v>
+        <v>-0.02738763561426372</v>
       </c>
       <c r="G12">
-        <v>0.2557119579146814</v>
+        <v>0.001017868166272584</v>
       </c>
       <c r="H12">
-        <v>0.4208397194991282</v>
+        <v>0.212555477012045</v>
       </c>
       <c r="I12">
-        <v>6771</v>
-      </c>
-      <c r="K12">
-        <v>0.000112952017849086</v>
-      </c>
-      <c r="M12">
-        <v>0.0001037297229528328</v>
+        <v>11542</v>
+      </c>
+      <c r="L12">
+        <v>0.004589584286176587</v>
+      </c>
+      <c r="N12">
+        <v>0.001597174444307401</v>
       </c>
       <c r="O12">
-        <v>0.00526064949972486</v>
+        <v>0.00512210974064752</v>
       </c>
       <c r="P12">
-        <v>0.002682213716882752</v>
+        <v>-0.005102592401121431</v>
       </c>
       <c r="Q12">
-        <v>0.005813234561065725</v>
+        <v>0.000163888349337522</v>
+      </c>
+      <c r="R12">
+        <v>0.000209188838038313</v>
       </c>
       <c r="S12">
-        <v>0.3693483364419842</v>
-      </c>
-      <c r="T12">
-        <v>0.003193202088483064</v>
+        <v>0.001602037466360856</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -1210,22 +1213,22 @@
         <v>31</v>
       </c>
       <c r="B13">
-        <v>0.005806826536720938</v>
+        <v>0.005058551760597552</v>
       </c>
       <c r="C13">
-        <v>0.005670204101840715</v>
+        <v>0.005699109365498782</v>
       </c>
       <c r="D13">
-        <v>8.986367404537444E-05</v>
+        <v>7.085921366241217E-05</v>
       </c>
       <c r="E13">
-        <v>9.344840654260834E-05</v>
+        <v>9.470932808225897E-05</v>
       </c>
       <c r="F13">
-        <v>0.2696481973337195</v>
+        <v>0.4431418058979847</v>
       </c>
       <c r="G13">
-        <v>0.2405138906269937</v>
+        <v>0.2557119579146814</v>
       </c>
       <c r="H13">
         <v>0.4208397194991282</v>
@@ -1233,26 +1236,26 @@
       <c r="I13">
         <v>6771</v>
       </c>
-      <c r="K13">
-        <v>0.0001410934357507483</v>
-      </c>
-      <c r="M13">
+      <c r="L13">
+        <v>0.005813234561065725</v>
+      </c>
+      <c r="N13">
+        <v>0.003193202088483064</v>
+      </c>
+      <c r="O13">
+        <v>0.00526064949972486</v>
+      </c>
+      <c r="P13">
+        <v>0.3693483364419842</v>
+      </c>
+      <c r="Q13">
         <v>0.0001037297229528328</v>
       </c>
-      <c r="O13">
-        <v>0.006002887168865449</v>
-      </c>
-      <c r="P13">
-        <v>0.003030311329129174</v>
-      </c>
-      <c r="Q13">
-        <v>0.005813234561065723</v>
+      <c r="R13">
+        <v>0.000112952017849086</v>
       </c>
       <c r="S13">
-        <v>0.2122246979933391</v>
-      </c>
-      <c r="T13">
-        <v>0.003193202088483064</v>
+        <v>0.002682213716882752</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -1260,49 +1263,49 @@
         <v>32</v>
       </c>
       <c r="B14">
-        <v>0.003208711377129972</v>
+        <v>0.005806826536720938</v>
       </c>
       <c r="C14">
-        <v>0.002538761048289119</v>
+        <v>0.005670204101840715</v>
       </c>
       <c r="D14">
-        <v>2.210896317387241E-05</v>
+        <v>8.986367404537444E-05</v>
       </c>
       <c r="E14">
-        <v>2.103311528121684E-05</v>
+        <v>9.344840654260834E-05</v>
       </c>
       <c r="F14">
-        <v>-0.05017806464506647</v>
+        <v>0.2696481973337195</v>
       </c>
       <c r="G14">
-        <v>0.0009248228524665336</v>
+        <v>0.2405138906269937</v>
       </c>
       <c r="H14">
-        <v>0.2133795918767654</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I14">
-        <v>11611</v>
-      </c>
-      <c r="K14">
-        <v>0.0002098592232396584</v>
-      </c>
-      <c r="M14">
-        <v>0.0001631540263502446</v>
+        <v>6771</v>
+      </c>
+      <c r="L14">
+        <v>0.005813234561065723</v>
+      </c>
+      <c r="N14">
+        <v>0.003193202088483064</v>
       </c>
       <c r="O14">
-        <v>0.005213165544267774</v>
+        <v>0.006002887168865449</v>
       </c>
       <c r="P14">
-        <v>0.00173711317318318</v>
+        <v>0.2122246979933391</v>
       </c>
       <c r="Q14">
-        <v>0.004580501696160511</v>
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="R14">
+        <v>0.0001410934357507483</v>
       </c>
       <c r="S14">
-        <v>-0.01180186309853548</v>
-      </c>
-      <c r="T14">
-        <v>0.001592932311570713</v>
+        <v>0.003030311329129174</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -1310,49 +1313,49 @@
         <v>33</v>
       </c>
       <c r="B15">
-        <v>0.003491208235511574</v>
+        <v>0.003208711377129972</v>
       </c>
       <c r="C15">
-        <v>0.001329144946829925</v>
+        <v>0.002538761048289119</v>
       </c>
       <c r="D15">
-        <v>1.85690054965323E-05</v>
+        <v>2.210896317387241E-05</v>
       </c>
       <c r="E15">
-        <v>9.168575316995369E-06</v>
+        <v>2.103311528121684E-05</v>
       </c>
       <c r="F15">
-        <v>-0.009024320017351872</v>
+        <v>-0.05017806464506647</v>
       </c>
       <c r="G15">
-        <v>0.501787240222058</v>
+        <v>0.0009248228524665336</v>
       </c>
       <c r="H15">
-        <v>0.6230156929756394</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I15">
-        <v>49</v>
-      </c>
-      <c r="K15">
-        <v>0.0003123469992588732</v>
-      </c>
-      <c r="M15">
-        <v>0.0001158352549329261</v>
+        <v>11611</v>
+      </c>
+      <c r="L15">
+        <v>0.004580501696160511</v>
+      </c>
+      <c r="N15">
+        <v>0.001592932311570713</v>
       </c>
       <c r="O15">
-        <v>0.007217175147339313</v>
+        <v>0.005213165544267774</v>
       </c>
       <c r="P15">
-        <v>0.002972419699024923</v>
+        <v>-0.01180186309853548</v>
       </c>
       <c r="Q15">
-        <v>0.004529835290885987</v>
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="R15">
+        <v>0.0002098592232396584</v>
       </c>
       <c r="S15">
-        <v>-0.01652918306199047</v>
-      </c>
-      <c r="T15">
-        <v>0.00129198945232948</v>
+        <v>0.00173711317318318</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -1360,272 +1363,272 @@
         <v>34</v>
       </c>
       <c r="B16">
-        <v>0.01042798137117382</v>
+        <v>0.003491208235511574</v>
       </c>
       <c r="C16">
-        <v>0.009812042985245533</v>
+        <v>0.001329144946829925</v>
       </c>
       <c r="D16">
-        <v>0.0002839828498694114</v>
+        <v>1.85690054965323E-05</v>
       </c>
       <c r="E16">
-        <v>0.000297330738550053</v>
+        <v>9.168575316995369E-06</v>
       </c>
       <c r="F16">
-        <v>0.1884050333044567</v>
+        <v>-0.009024320017351872</v>
       </c>
       <c r="G16">
-        <v>0.1502580843805948</v>
+        <v>0.501787240222058</v>
       </c>
       <c r="H16">
-        <v>0.2597560818810524</v>
+        <v>0.6230156929756394</v>
       </c>
       <c r="I16">
-        <v>12741</v>
-      </c>
-      <c r="K16">
-        <v>0.0004007814960332574</v>
-      </c>
-      <c r="M16">
-        <v>0.0003441387227458278</v>
+        <v>49</v>
+      </c>
+      <c r="L16">
+        <v>0.004529835290885987</v>
+      </c>
+      <c r="N16">
+        <v>0.00129198945232948</v>
       </c>
       <c r="O16">
-        <v>0.01033009227796955</v>
+        <v>0.007217175147339313</v>
       </c>
       <c r="P16">
-        <v>0.005554310648909318</v>
+        <v>-0.01652918306199047</v>
       </c>
       <c r="Q16">
-        <v>0.009714954248817111</v>
+        <v>0.0001158352549329261</v>
+      </c>
+      <c r="R16">
+        <v>0.0003123469992588732</v>
       </c>
       <c r="S16">
-        <v>0.1379172254546043</v>
-      </c>
-      <c r="T16">
-        <v>0.004797770485226469</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20">
+        <v>0.002972419699024923</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B17">
-        <v>0.00997695293896445</v>
+        <v>0.01042798137117382</v>
       </c>
       <c r="C17">
-        <v>0.009631259951277263</v>
+        <v>0.009812042985245533</v>
       </c>
       <c r="D17">
-        <v>0.0002746516022984678</v>
+        <v>0.0002839828498694114</v>
       </c>
       <c r="E17">
-        <v>0.000318358280400409</v>
+        <v>0.000297330738550053</v>
       </c>
       <c r="F17">
-        <v>0.272470124651383</v>
+        <v>0.1884050333044567</v>
       </c>
       <c r="G17">
-        <v>0.156694670201814</v>
+        <v>0.1502580843805948</v>
       </c>
       <c r="H17">
-        <v>0.4558883625799528</v>
+        <v>0.2597560818810524</v>
       </c>
       <c r="I17">
-        <v>1284</v>
-      </c>
-      <c r="K17">
-        <v>0.0003741973334738424</v>
-      </c>
-      <c r="M17">
-        <v>0.0002640644396388745</v>
+        <v>12741</v>
+      </c>
+      <c r="L17">
+        <v>0.009714954248817111</v>
+      </c>
+      <c r="N17">
+        <v>0.004797770485226469</v>
       </c>
       <c r="O17">
-        <v>0.009685349739034687</v>
+        <v>0.01033009227796955</v>
       </c>
       <c r="P17">
-        <v>0.005106524251936465</v>
+        <v>0.1379172254546043</v>
       </c>
       <c r="Q17">
-        <v>0.009204693368560462</v>
+        <v>0.0003441387227458278</v>
+      </c>
+      <c r="R17">
+        <v>0.0004007814960332574</v>
       </c>
       <c r="S17">
-        <v>0.2289566739349258</v>
-      </c>
-      <c r="T17">
-        <v>0.004252957223118693</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20">
+        <v>0.005554310648909318</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B18">
-        <v>0.0102733372090916</v>
+        <v>0.00997695293896445</v>
       </c>
       <c r="C18">
-        <v>0.00987889837479569</v>
+        <v>0.009631259951277263</v>
       </c>
       <c r="D18">
-        <v>0.0002816309717823605</v>
+        <v>0.0002746516022984678</v>
       </c>
       <c r="E18">
-        <v>0.0003034120436381377</v>
+        <v>0.000318358280400409</v>
       </c>
       <c r="F18">
-        <v>0.204771852061556</v>
+        <v>0.272470124651383</v>
       </c>
       <c r="G18">
-        <v>0.1432696624324651</v>
+        <v>0.156694670201814</v>
       </c>
       <c r="H18">
-        <v>0.2595879210340796</v>
+        <v>0.4558883625799528</v>
       </c>
       <c r="I18">
-        <v>12051</v>
-      </c>
-      <c r="K18">
-        <v>0.0004008200453677453</v>
-      </c>
-      <c r="M18">
-        <v>0.0003482779314587717</v>
+        <v>1284</v>
+      </c>
+      <c r="L18">
+        <v>0.009204693368560462</v>
+      </c>
+      <c r="N18">
+        <v>0.004252957223118693</v>
       </c>
       <c r="O18">
-        <v>0.01017444484578581</v>
+        <v>0.009685349739034687</v>
       </c>
       <c r="P18">
-        <v>0.005371111699895803</v>
+        <v>0.2289566739349258</v>
       </c>
       <c r="Q18">
-        <v>0.009769435123820693</v>
+        <v>0.0002640644396388745</v>
+      </c>
+      <c r="R18">
+        <v>0.0003741973334738424</v>
       </c>
       <c r="S18">
-        <v>0.1478874304814285</v>
-      </c>
-      <c r="T18">
-        <v>0.004769747765218425</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
+        <v>0.005106524251936465</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B19">
-        <v>0.009164293356549506</v>
+        <v>0.0102733372090916</v>
       </c>
       <c r="C19">
-        <v>0.008733878054388279</v>
+        <v>0.00987889837479569</v>
       </c>
       <c r="D19">
-        <v>0.0001865208677798922</v>
+        <v>0.0002816309717823605</v>
       </c>
       <c r="E19">
-        <v>0.0001961492659581503</v>
+        <v>0.0003034120436381377</v>
       </c>
       <c r="F19">
-        <v>0.1708507589293765</v>
+        <v>0.204771852061556</v>
       </c>
       <c r="G19">
-        <v>0.1280492261183164</v>
+        <v>0.1432696624324651</v>
       </c>
       <c r="H19">
-        <v>0.2582640092197721</v>
+        <v>0.2595879210340796</v>
       </c>
       <c r="I19">
-        <v>14156</v>
-      </c>
-      <c r="K19">
-        <v>0.0004006378783650764</v>
-      </c>
-      <c r="M19">
-        <v>0.0003384092866814527</v>
+        <v>12051</v>
+      </c>
+      <c r="L19">
+        <v>0.009769435123820693</v>
+      </c>
+      <c r="N19">
+        <v>0.004769747765218425</v>
       </c>
       <c r="O19">
-        <v>0.0102119158074488</v>
+        <v>0.01017444484578581</v>
       </c>
       <c r="P19">
-        <v>0.005239736253559311</v>
+        <v>0.1478874304814285</v>
       </c>
       <c r="Q19">
-        <v>0.009674189396799987</v>
+        <v>0.0003482779314587717</v>
+      </c>
+      <c r="R19">
+        <v>0.0004008200453677453</v>
       </c>
       <c r="S19">
-        <v>0.1218694481841025</v>
-      </c>
-      <c r="T19">
-        <v>0.004818030126325817</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20">
+        <v>0.005371111699895803</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B20">
-        <v>0.005791630591612971</v>
+        <v>0.009164293356549506</v>
       </c>
       <c r="C20">
-        <v>0.005699109365498782</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D20">
-        <v>8.698446620952695E-05</v>
+        <v>0.0001865208677798922</v>
       </c>
       <c r="E20">
-        <v>9.470932808225897E-05</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F20">
-        <v>0.3164189910555092</v>
+        <v>0.1708507589293765</v>
       </c>
       <c r="G20">
-        <v>0.2557119579146814</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H20">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I20">
-        <v>6771</v>
-      </c>
-      <c r="K20">
-        <v>0.0001324165619288979</v>
-      </c>
-      <c r="M20">
-        <v>0.0001037297229528328</v>
+        <v>14156</v>
+      </c>
+      <c r="L20">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="N20">
+        <v>0.004818030126325817</v>
       </c>
       <c r="O20">
-        <v>0.006002882908757912</v>
+        <v>0.0102119158074488</v>
       </c>
       <c r="P20">
-        <v>0.003330775568204595</v>
+        <v>0.1218694481841025</v>
       </c>
       <c r="Q20">
-        <v>0.005813234561065725</v>
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="R20">
+        <v>0.0004006378783650764</v>
       </c>
       <c r="S20">
-        <v>0.2606707993949464</v>
-      </c>
-      <c r="T20">
-        <v>0.003193202088483064</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20">
+        <v>0.005239736253559311</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B21">
-        <v>0.005611881407010991</v>
+        <v>0.005791630591612971</v>
       </c>
       <c r="C21">
-        <v>0.005639127357765789</v>
+        <v>0.005699109365498782</v>
       </c>
       <c r="D21">
-        <v>8.431607544410066E-05</v>
+        <v>8.698446620952695E-05</v>
       </c>
       <c r="E21">
-        <v>9.102681873913914E-05</v>
+        <v>9.470932808225897E-05</v>
       </c>
       <c r="F21">
-        <v>0.291056300795216</v>
+        <v>0.3164189910555092</v>
       </c>
       <c r="G21">
-        <v>0.2346312460124846</v>
+        <v>0.2557119579146814</v>
       </c>
       <c r="H21">
         <v>0.4208397194991282</v>
@@ -1633,49 +1636,49 @@
       <c r="I21">
         <v>6771</v>
       </c>
-      <c r="K21">
-        <v>0.0001424514975481683</v>
-      </c>
-      <c r="M21">
+      <c r="L21">
+        <v>0.005813234561065725</v>
+      </c>
+      <c r="N21">
+        <v>0.003193202088483064</v>
+      </c>
+      <c r="O21">
+        <v>0.006002882908757912</v>
+      </c>
+      <c r="P21">
+        <v>0.2606707993949464</v>
+      </c>
+      <c r="Q21">
         <v>0.0001037297229528328</v>
       </c>
-      <c r="O21">
-        <v>0.00595976388177965</v>
-      </c>
-      <c r="P21">
-        <v>0.002972129451884979</v>
-      </c>
-      <c r="Q21">
-        <v>0.005813234561065725</v>
+      <c r="R21">
+        <v>0.0001324165619288979</v>
       </c>
       <c r="S21">
-        <v>0.2046421514566161</v>
-      </c>
-      <c r="T21">
-        <v>0.003193202088483064</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20">
+        <v>0.003330775568204595</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B22">
-        <v>0.005713567326092179</v>
+        <v>0.005611881407010991</v>
       </c>
       <c r="C22">
-        <v>0.005699109365498782</v>
+        <v>0.005639127357765789</v>
       </c>
       <c r="D22">
-        <v>8.903433264960941E-05</v>
+        <v>8.431607544410066E-05</v>
       </c>
       <c r="E22">
-        <v>9.470932808225897E-05</v>
+        <v>9.102681873913914E-05</v>
       </c>
       <c r="F22">
-        <v>0.3003097955821736</v>
+        <v>0.291056300795216</v>
       </c>
       <c r="G22">
-        <v>0.2557119579146814</v>
+        <v>0.2346312460124846</v>
       </c>
       <c r="H22">
         <v>0.4208397194991282</v>
@@ -1683,296 +1686,296 @@
       <c r="I22">
         <v>6771</v>
       </c>
-      <c r="K22">
-        <v>0.00013855240761432</v>
-      </c>
-      <c r="M22">
+      <c r="L22">
+        <v>0.005813234561065725</v>
+      </c>
+      <c r="N22">
+        <v>0.003193202088483064</v>
+      </c>
+      <c r="O22">
+        <v>0.00595976388177965</v>
+      </c>
+      <c r="P22">
+        <v>0.2046421514566161</v>
+      </c>
+      <c r="Q22">
         <v>0.0001037297229528328</v>
       </c>
-      <c r="O22">
-        <v>0.00592641693601841</v>
-      </c>
-      <c r="P22">
-        <v>0.003005755874836842</v>
-      </c>
-      <c r="Q22">
-        <v>0.005813234561065725</v>
+      <c r="R22">
+        <v>0.0001424514975481683</v>
       </c>
       <c r="S22">
-        <v>0.2264121702660996</v>
-      </c>
-      <c r="T22">
-        <v>0.003193202088483064</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20">
+        <v>0.002972129451884979</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B23">
-        <v>0.007927365294981236</v>
+        <v>0.005713567326092179</v>
       </c>
       <c r="C23">
-        <v>0.008722720041403264</v>
+        <v>0.005699109365498782</v>
       </c>
       <c r="D23">
-        <v>0.000143672851475712</v>
+        <v>8.903433264960941E-05</v>
       </c>
       <c r="E23">
-        <v>0.0001985649052123504</v>
+        <v>9.470932808225897E-05</v>
       </c>
       <c r="F23">
-        <v>0.3830412447229715</v>
+        <v>0.3003097955821736</v>
       </c>
       <c r="G23">
-        <v>0.147324247391146</v>
+        <v>0.2557119579146814</v>
       </c>
       <c r="H23">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I23">
-        <v>14156</v>
-      </c>
-      <c r="K23">
-        <v>0.0003279955215444224</v>
-      </c>
-      <c r="M23">
-        <v>0.0003384092866814527</v>
+        <v>6771</v>
+      </c>
+      <c r="L23">
+        <v>0.005813234561065725</v>
+      </c>
+      <c r="N23">
+        <v>0.003193202088483064</v>
       </c>
       <c r="O23">
-        <v>0.008942022948316988</v>
+        <v>0.00592641693601841</v>
       </c>
       <c r="P23">
-        <v>0.004617426367895965</v>
+        <v>0.2264121702660996</v>
       </c>
       <c r="Q23">
-        <v>0.009674189396799985</v>
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="R23">
+        <v>0.00013855240761432</v>
       </c>
       <c r="S23">
-        <v>0.2810892232598902</v>
-      </c>
-      <c r="T23">
-        <v>0.004818030126325817</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20">
+        <v>0.003005755874836842</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B24">
-        <v>0.003031636244261009</v>
+        <v>0.007927365294981236</v>
       </c>
       <c r="C24">
-        <v>0.002499571894821071</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D24">
-        <v>1.91501667802569E-05</v>
+        <v>0.000143672851475712</v>
       </c>
       <c r="E24">
-        <v>1.967007435869721E-05</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F24">
-        <v>-0.01488433510101705</v>
+        <v>0.3830412447229715</v>
       </c>
       <c r="G24">
-        <v>-0.04243741404356438</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H24">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I24">
-        <v>11611</v>
-      </c>
-      <c r="K24">
-        <v>0.0002083353057278959</v>
-      </c>
-      <c r="M24">
-        <v>0.0001631540263502446</v>
+        <v>14156</v>
+      </c>
+      <c r="L24">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="N24">
+        <v>0.004818030126325817</v>
       </c>
       <c r="O24">
-        <v>0.005089153979501482</v>
+        <v>0.008942022948316988</v>
       </c>
       <c r="P24">
-        <v>0.001554417436991534</v>
+        <v>0.2810892232598902</v>
       </c>
       <c r="Q24">
-        <v>0.004580501696160511</v>
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="R24">
+        <v>0.0003279955215444224</v>
       </c>
       <c r="S24">
-        <v>-0.004454544482717981</v>
-      </c>
-      <c r="T24">
-        <v>0.001592932311570713</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20">
+        <v>0.004617426367895965</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B25">
-        <v>0.00784507820846319</v>
+        <v>0.003031636244261009</v>
       </c>
       <c r="C25">
-        <v>0.008722720041403264</v>
+        <v>0.002499571894821071</v>
       </c>
       <c r="D25">
-        <v>0.0001417160098566256</v>
+        <v>1.91501667802569E-05</v>
       </c>
       <c r="E25">
-        <v>0.0001985649052123504</v>
+        <v>1.967007435869721E-05</v>
       </c>
       <c r="F25">
-        <v>0.3914442976114285</v>
+        <v>-0.01488433510101705</v>
       </c>
       <c r="G25">
-        <v>0.147324247391146</v>
+        <v>-0.04243741404356438</v>
       </c>
       <c r="H25">
-        <v>0.2582640092197721</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I25">
-        <v>14156</v>
-      </c>
-      <c r="K25">
-        <v>0.0003254854012574867</v>
-      </c>
-      <c r="M25">
-        <v>0.0003384092866814527</v>
+        <v>11611</v>
+      </c>
+      <c r="L25">
+        <v>0.004580501696160511</v>
+      </c>
+      <c r="N25">
+        <v>0.001592932311570713</v>
       </c>
       <c r="O25">
-        <v>0.008855143980453176</v>
+        <v>0.005089153979501482</v>
       </c>
       <c r="P25">
-        <v>0.00456770441607247</v>
+        <v>-0.004454544482717981</v>
       </c>
       <c r="Q25">
-        <v>0.009674189396799985</v>
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="R25">
+        <v>0.0002083353057278959</v>
       </c>
       <c r="S25">
-        <v>0.2865909829079945</v>
-      </c>
-      <c r="T25">
-        <v>0.004818030126325816</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20">
+        <v>0.001554417436991534</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B26">
-        <v>0.003103990424644728</v>
+        <v>0.00784507820846319</v>
       </c>
       <c r="C26">
-        <v>0.00254141838673398</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D26">
-        <v>2.156002471405648E-05</v>
+        <v>0.0001417160098566256</v>
       </c>
       <c r="E26">
-        <v>2.106152912726658E-05</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F26">
-        <v>-0.02262657763782516</v>
+        <v>0.3914442976114285</v>
       </c>
       <c r="G26">
-        <v>0.001017868166272584</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H26">
-        <v>0.212555477012045</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I26">
-        <v>11542</v>
-      </c>
-      <c r="K26">
-        <v>0.0002091701444985722</v>
-      </c>
-      <c r="M26">
-        <v>0.000163888349337522</v>
+        <v>14156</v>
+      </c>
+      <c r="L26">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="N26">
+        <v>0.004818030126325816</v>
       </c>
       <c r="O26">
-        <v>0.00510134746390362</v>
+        <v>0.008855143980453176</v>
       </c>
       <c r="P26">
-        <v>0.001583264354559398</v>
+        <v>0.2865909829079945</v>
       </c>
       <c r="Q26">
-        <v>0.004589584286176587</v>
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="R26">
+        <v>0.0003254854012574867</v>
       </c>
       <c r="S26">
-        <v>-0.005012774390606101</v>
-      </c>
-      <c r="T26">
-        <v>0.001597174444307401</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20">
+        <v>0.00456770441607247</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B27">
-        <v>0.005895505445859815</v>
+        <v>0.003103990424644728</v>
       </c>
       <c r="C27">
-        <v>0.005670204101840715</v>
+        <v>0.00254141838673398</v>
       </c>
       <c r="D27">
-        <v>9.166134936686534E-05</v>
+        <v>2.156002471405648E-05</v>
       </c>
       <c r="E27">
-        <v>9.344840654260834E-05</v>
+        <v>2.106152912726658E-05</v>
       </c>
       <c r="F27">
-        <v>0.255037895389058</v>
+        <v>-0.02262657763782516</v>
       </c>
       <c r="G27">
-        <v>0.2405138906269937</v>
+        <v>0.001017868166272584</v>
       </c>
       <c r="H27">
-        <v>0.4208397194991282</v>
+        <v>0.212555477012045</v>
       </c>
       <c r="I27">
-        <v>6771</v>
-      </c>
-      <c r="K27">
-        <v>0.0001427653829362463</v>
-      </c>
-      <c r="M27">
-        <v>0.0001037297229528328</v>
+        <v>11542</v>
+      </c>
+      <c r="L27">
+        <v>0.004589584286176587</v>
+      </c>
+      <c r="N27">
+        <v>0.001597174444307401</v>
       </c>
       <c r="O27">
-        <v>0.006096382291329448</v>
+        <v>0.00510134746390362</v>
       </c>
       <c r="P27">
-        <v>0.003125364361436701</v>
+        <v>-0.005012774390606101</v>
       </c>
       <c r="Q27">
-        <v>0.005813234561065723</v>
+        <v>0.000163888349337522</v>
+      </c>
+      <c r="R27">
+        <v>0.0002091701444985722</v>
       </c>
       <c r="S27">
-        <v>0.2028896166553128</v>
-      </c>
-      <c r="T27">
-        <v>0.003193202088483064</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20">
+        <v>0.001583264354559398</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B28">
-        <v>0.005903838435270049</v>
+        <v>0.005895505445859815</v>
       </c>
       <c r="C28">
         <v>0.005670204101840715</v>
       </c>
       <c r="D28">
-        <v>9.181732856753832E-05</v>
+        <v>9.166134936686534E-05</v>
       </c>
       <c r="E28">
         <v>9.344840654260834E-05</v>
       </c>
       <c r="F28">
-        <v>0.2537702008328302</v>
+        <v>0.255037895389058</v>
       </c>
       <c r="G28">
         <v>0.2405138906269937</v>
@@ -1983,46 +1986,46 @@
       <c r="I28">
         <v>6771</v>
       </c>
-      <c r="K28">
-        <v>0.0001433490956550128</v>
-      </c>
-      <c r="M28">
+      <c r="L28">
+        <v>0.005813234561065723</v>
+      </c>
+      <c r="N28">
+        <v>0.003193202088483064</v>
+      </c>
+      <c r="O28">
+        <v>0.006096382291329448</v>
+      </c>
+      <c r="P28">
+        <v>0.2028896166553128</v>
+      </c>
+      <c r="Q28">
         <v>0.0001037297229528328</v>
       </c>
-      <c r="O28">
-        <v>0.00610593491672969</v>
-      </c>
-      <c r="P28">
-        <v>0.003163476470023769</v>
-      </c>
-      <c r="Q28">
-        <v>0.005813234561065723</v>
+      <c r="R28">
+        <v>0.0001427653829362463</v>
       </c>
       <c r="S28">
-        <v>0.1996305390032257</v>
-      </c>
-      <c r="T28">
-        <v>0.003193202088483064</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20">
+        <v>0.003125364361436701</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B29">
-        <v>0.005871671098387516</v>
+        <v>0.005903838435270049</v>
       </c>
       <c r="C29">
         <v>0.005670204101840715</v>
       </c>
       <c r="D29">
-        <v>9.132537185586264E-05</v>
+        <v>9.181732856753832E-05</v>
       </c>
       <c r="E29">
         <v>9.344840654260834E-05</v>
       </c>
       <c r="F29">
-        <v>0.2577684957503591</v>
+        <v>0.2537702008328302</v>
       </c>
       <c r="G29">
         <v>0.2405138906269937</v>
@@ -2033,176 +2036,176 @@
       <c r="I29">
         <v>6771</v>
       </c>
-      <c r="K29">
-        <v>0.0001429245641932233</v>
-      </c>
-      <c r="M29">
+      <c r="L29">
+        <v>0.005813234561065723</v>
+      </c>
+      <c r="N29">
+        <v>0.003193202088483064</v>
+      </c>
+      <c r="O29">
+        <v>0.00610593491672969</v>
+      </c>
+      <c r="P29">
+        <v>0.1996305390032257</v>
+      </c>
+      <c r="Q29">
         <v>0.0001037297229528328</v>
       </c>
-      <c r="O29">
-        <v>0.006067498374332903</v>
-      </c>
-      <c r="P29">
-        <v>0.003090643964573058</v>
-      </c>
-      <c r="Q29">
-        <v>0.005813234561065723</v>
+      <c r="R29">
+        <v>0.0001433490956550128</v>
       </c>
       <c r="S29">
-        <v>0.2020008505541708</v>
-      </c>
-      <c r="T29">
-        <v>0.003193202088483064</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20">
+        <v>0.003163476470023769</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B30">
-        <v>0.00304699828992123</v>
+        <v>0.005871671098387516</v>
       </c>
       <c r="C30">
-        <v>0.002499571894821071</v>
+        <v>0.005670204101840715</v>
       </c>
       <c r="D30">
-        <v>1.903121423403654E-05</v>
+        <v>9.132537185586264E-05</v>
       </c>
       <c r="E30">
-        <v>1.967007435869721E-05</v>
+        <v>9.344840654260834E-05</v>
       </c>
       <c r="F30">
-        <v>-0.008580312939503454</v>
+        <v>0.2577684957503591</v>
       </c>
       <c r="G30">
-        <v>-0.04243741404356438</v>
+        <v>0.2405138906269937</v>
       </c>
       <c r="H30">
-        <v>0.2133795918767654</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I30">
-        <v>11611</v>
-      </c>
-      <c r="K30">
-        <v>0.000207986162951978</v>
-      </c>
-      <c r="M30">
-        <v>0.0001631540263502446</v>
+        <v>6771</v>
+      </c>
+      <c r="L30">
+        <v>0.005813234561065723</v>
+      </c>
+      <c r="N30">
+        <v>0.003193202088483064</v>
       </c>
       <c r="O30">
-        <v>0.005107549406927882</v>
+        <v>0.006067498374332903</v>
       </c>
       <c r="P30">
-        <v>0.001554596452837835</v>
+        <v>0.2020008505541708</v>
       </c>
       <c r="Q30">
-        <v>0.004580501696160511</v>
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="R30">
+        <v>0.0001429245641932233</v>
       </c>
       <c r="S30">
-        <v>-0.002771209789547591</v>
-      </c>
-      <c r="T30">
-        <v>0.001592932311570713</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20">
+        <v>0.003090643964573058</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B31">
-        <v>0.006549373422714545</v>
+        <v>0.00304699828992123</v>
       </c>
       <c r="C31">
-        <v>0.005670204101840715</v>
+        <v>0.002499571894821071</v>
       </c>
       <c r="D31">
-        <v>0.0001064697656049724</v>
+        <v>1.903121423403654E-05</v>
       </c>
       <c r="E31">
-        <v>9.344840654260834E-05</v>
+        <v>1.967007435869721E-05</v>
       </c>
       <c r="F31">
-        <v>0.1346849985258249</v>
+        <v>-0.008580312939503454</v>
       </c>
       <c r="G31">
-        <v>0.2405138906269937</v>
+        <v>-0.04243741404356438</v>
       </c>
       <c r="H31">
-        <v>0.4208397194991282</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I31">
-        <v>6771</v>
-      </c>
-      <c r="K31">
-        <v>0.000160150142460433</v>
-      </c>
-      <c r="M31">
-        <v>0.0001037297229528328</v>
+        <v>11611</v>
+      </c>
+      <c r="L31">
+        <v>0.004580501696160511</v>
+      </c>
+      <c r="N31">
+        <v>0.001592932311570713</v>
       </c>
       <c r="O31">
-        <v>0.006776662396495037</v>
+        <v>0.005107549406927882</v>
       </c>
       <c r="P31">
-        <v>0.003715325925925931</v>
+        <v>-0.002771209789547591</v>
       </c>
       <c r="Q31">
-        <v>0.005813234561065723</v>
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="R31">
+        <v>0.000207986162951978</v>
       </c>
       <c r="S31">
-        <v>0.1058242633905934</v>
-      </c>
-      <c r="T31">
-        <v>0.003193202088483064</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20">
+        <v>0.001554596452837835</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B32">
-        <v>0.002783525716284511</v>
+        <v>0.006549373422714545</v>
       </c>
       <c r="C32">
-        <v>0.002457544020376962</v>
+        <v>0.005670204101840715</v>
       </c>
       <c r="D32">
-        <v>1.713865210259099E-05</v>
+        <v>0.0001064697656049724</v>
       </c>
       <c r="E32">
-        <v>1.89022549270271E-05</v>
+        <v>9.344840654260834E-05</v>
       </c>
       <c r="F32">
-        <v>-0.05370835704473098</v>
+        <v>0.1346849985258249</v>
       </c>
       <c r="G32">
-        <v>-0.1621371309933592</v>
+        <v>0.2405138906269937</v>
       </c>
       <c r="H32">
-        <v>0.3649062991209757</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I32">
-        <v>4010</v>
-      </c>
-      <c r="K32">
-        <v>0.0002742305932959652</v>
-      </c>
-      <c r="M32">
-        <v>0.0001730864695810989</v>
+        <v>6771</v>
+      </c>
+      <c r="L32">
+        <v>0.005813234561065723</v>
+      </c>
+      <c r="N32">
+        <v>0.003193202088483064</v>
       </c>
       <c r="O32">
-        <v>0.004501420066184821</v>
+        <v>0.006776662396495037</v>
       </c>
       <c r="P32">
-        <v>0.001362431751651251</v>
+        <v>0.1058242633905934</v>
       </c>
       <c r="Q32">
-        <v>0.004349183403839366</v>
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="R32">
+        <v>0.000160150142460433</v>
       </c>
       <c r="S32">
-        <v>-0.006214540120261569</v>
-      </c>
-      <c r="T32">
-        <v>0.001438312583710056</v>
+        <v>0.003715325925925931</v>
       </c>
     </row>
     <row r="33" spans="1:20">
@@ -2210,49 +2213,49 @@
         <v>51</v>
       </c>
       <c r="B33">
-        <v>0.00929322862430519</v>
+        <v>0.002783525716284511</v>
       </c>
       <c r="C33">
-        <v>0.008733878054388279</v>
+        <v>0.002457544020376962</v>
       </c>
       <c r="D33">
-        <v>0.000192984991667648</v>
+        <v>1.713865210259099E-05</v>
       </c>
       <c r="E33">
-        <v>0.0001961492659581503</v>
+        <v>1.89022549270271E-05</v>
       </c>
       <c r="F33">
-        <v>0.1421155108066621</v>
+        <v>-0.05370835704473098</v>
       </c>
       <c r="G33">
-        <v>0.1280492261183164</v>
+        <v>-0.1621371309933592</v>
       </c>
       <c r="H33">
-        <v>0.2582640092197721</v>
+        <v>0.3649062991209757</v>
       </c>
       <c r="I33">
-        <v>14156</v>
-      </c>
-      <c r="K33">
-        <v>0.0004001063569688302</v>
-      </c>
-      <c r="M33">
-        <v>0.0003384092866814527</v>
+        <v>4010</v>
+      </c>
+      <c r="L33">
+        <v>0.004349183403839366</v>
+      </c>
+      <c r="N33">
+        <v>0.001438312583710056</v>
       </c>
       <c r="O33">
-        <v>0.01035431191953904</v>
+        <v>0.004501420066184821</v>
       </c>
       <c r="P33">
-        <v>0.005409147625572685</v>
+        <v>-0.006214540120261569</v>
       </c>
       <c r="Q33">
-        <v>0.009674189396799987</v>
+        <v>0.0001730864695810989</v>
+      </c>
+      <c r="R33">
+        <v>0.0002742305932959652</v>
       </c>
       <c r="S33">
-        <v>0.1230344532976788</v>
-      </c>
-      <c r="T33">
-        <v>0.004818030126325817</v>
+        <v>0.001362431751651251</v>
       </c>
     </row>
     <row r="34" spans="1:20">
@@ -2260,49 +2263,49 @@
         <v>52</v>
       </c>
       <c r="B34">
-        <v>0.01016347810751514</v>
+        <v>0.00929322862430519</v>
       </c>
       <c r="C34">
-        <v>0.009447153043753395</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D34">
-        <v>0.0002829041504470825</v>
+        <v>0.000192984991667648</v>
       </c>
       <c r="E34">
-        <v>0.0002806495860517923</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F34">
-        <v>0.1619293810393613</v>
+        <v>0.1421155108066621</v>
       </c>
       <c r="G34">
-        <v>0.1686082656554458</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H34">
-        <v>0.3904390743053188</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I34">
-        <v>4699</v>
-      </c>
-      <c r="K34">
-        <v>0.0004705186388866096</v>
-      </c>
-      <c r="M34">
-        <v>0.0003220429185286173</v>
+        <v>14156</v>
+      </c>
+      <c r="L34">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="N34">
+        <v>0.004818030126325817</v>
       </c>
       <c r="O34">
-        <v>0.01022526679210232</v>
+        <v>0.01035431191953904</v>
       </c>
       <c r="P34">
-        <v>0.005350192890365459</v>
+        <v>0.1230344532976788</v>
       </c>
       <c r="Q34">
-        <v>0.009384601794708014</v>
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="R34">
+        <v>0.0004001063569688302</v>
       </c>
       <c r="S34">
-        <v>0.1094051116331665</v>
-      </c>
-      <c r="T34">
-        <v>0.004731165595531388</v>
+        <v>0.005409147625572685</v>
       </c>
     </row>
     <row r="35" spans="1:20">
@@ -2310,49 +2313,49 @@
         <v>53</v>
       </c>
       <c r="B35">
-        <v>0.003030458698074221</v>
+        <v>0.01016347810751514</v>
       </c>
       <c r="C35">
-        <v>0.002499571894821071</v>
+        <v>0.009447153043753395</v>
       </c>
       <c r="D35">
-        <v>1.91281128971015E-05</v>
+        <v>0.0002829041504470825</v>
       </c>
       <c r="E35">
-        <v>1.967007435869721E-05</v>
+        <v>0.0002806495860517923</v>
       </c>
       <c r="F35">
-        <v>-0.01371556509502225</v>
+        <v>0.1619293810393613</v>
       </c>
       <c r="G35">
-        <v>-0.04243741404356438</v>
+        <v>0.1686082656554458</v>
       </c>
       <c r="H35">
-        <v>0.2133795918767654</v>
+        <v>0.3904390743053188</v>
       </c>
       <c r="I35">
-        <v>11611</v>
-      </c>
-      <c r="K35">
-        <v>0.0002081444394071696</v>
-      </c>
-      <c r="M35">
-        <v>0.0001631540263502446</v>
+        <v>4699</v>
+      </c>
+      <c r="L35">
+        <v>0.009384601794708014</v>
+      </c>
+      <c r="N35">
+        <v>0.004731165595531388</v>
       </c>
       <c r="O35">
-        <v>0.005089488294347637</v>
+        <v>0.01022526679210232</v>
       </c>
       <c r="P35">
-        <v>0.001547174514616301</v>
+        <v>0.1094051116331665</v>
       </c>
       <c r="Q35">
-        <v>0.004580501696160511</v>
+        <v>0.0003220429185286173</v>
+      </c>
+      <c r="R35">
+        <v>0.0004705186388866096</v>
       </c>
       <c r="S35">
-        <v>-0.00353431378743374</v>
-      </c>
-      <c r="T35">
-        <v>0.001592932311570713</v>
+        <v>0.005350192890365459</v>
       </c>
     </row>
     <row r="36" spans="1:20">
@@ -2360,49 +2363,49 @@
         <v>54</v>
       </c>
       <c r="B36">
-        <v>0.008384122629515654</v>
+        <v>0.003030458698074221</v>
       </c>
       <c r="C36">
-        <v>0.008722720041403264</v>
+        <v>0.002499571894821071</v>
       </c>
       <c r="D36">
-        <v>0.0001620814063416336</v>
+        <v>1.91281128971015E-05</v>
       </c>
       <c r="E36">
-        <v>0.0001985649052123504</v>
+        <v>1.967007435869721E-05</v>
       </c>
       <c r="F36">
-        <v>0.3039913826239528</v>
+        <v>-0.01371556509502225</v>
       </c>
       <c r="G36">
-        <v>0.147324247391146</v>
+        <v>-0.04243741404356438</v>
       </c>
       <c r="H36">
-        <v>0.2582640092197721</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I36">
-        <v>14156</v>
-      </c>
-      <c r="K36">
-        <v>0.0003610907680501377</v>
-      </c>
-      <c r="M36">
-        <v>0.0003384092866814527</v>
+        <v>11611</v>
+      </c>
+      <c r="L36">
+        <v>0.004580501696160511</v>
+      </c>
+      <c r="N36">
+        <v>0.001592932311570713</v>
       </c>
       <c r="O36">
-        <v>0.009406309171688502</v>
+        <v>0.005089488294347637</v>
       </c>
       <c r="P36">
-        <v>0.004884082851211167</v>
+        <v>-0.00353431378743374</v>
       </c>
       <c r="Q36">
-        <v>0.009674189396799985</v>
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="R36">
+        <v>0.0002081444394071696</v>
       </c>
       <c r="S36">
-        <v>0.2085500335179142</v>
-      </c>
-      <c r="T36">
-        <v>0.004818030126325816</v>
+        <v>0.001547174514616301</v>
       </c>
     </row>
     <row r="37" spans="1:20">
@@ -2410,19 +2413,19 @@
         <v>55</v>
       </c>
       <c r="B37">
-        <v>0.008519531777817098</v>
+        <v>0.008384122629515654</v>
       </c>
       <c r="C37">
         <v>0.008722720041403264</v>
       </c>
       <c r="D37">
-        <v>0.0001673145877462598</v>
+        <v>0.0001620814063416336</v>
       </c>
       <c r="E37">
         <v>0.0001985649052123504</v>
       </c>
       <c r="F37">
-        <v>0.2815190988739301</v>
+        <v>0.3039913826239528</v>
       </c>
       <c r="G37">
         <v>0.147324247391146</v>
@@ -2433,26 +2436,26 @@
       <c r="I37">
         <v>14156</v>
       </c>
-      <c r="K37">
-        <v>0.0003710863970746162</v>
-      </c>
-      <c r="M37">
+      <c r="L37">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="N37">
+        <v>0.004818030126325816</v>
+      </c>
+      <c r="O37">
+        <v>0.009406309171688502</v>
+      </c>
+      <c r="P37">
+        <v>0.2085500335179142</v>
+      </c>
+      <c r="Q37">
         <v>0.0003384092866814527</v>
       </c>
-      <c r="O37">
-        <v>0.009535796789931871</v>
-      </c>
-      <c r="P37">
-        <v>0.004784771004405694</v>
-      </c>
-      <c r="Q37">
-        <v>0.009674189396799985</v>
+      <c r="R37">
+        <v>0.0003610907680501377</v>
       </c>
       <c r="S37">
-        <v>0.1866413032030688</v>
-      </c>
-      <c r="T37">
-        <v>0.004818030126325816</v>
+        <v>0.004884082851211167</v>
       </c>
     </row>
     <row r="38" spans="1:20">
@@ -2460,22 +2463,22 @@
         <v>56</v>
       </c>
       <c r="B38">
-        <v>0.008532806478705164</v>
+        <v>0.008519531777817098</v>
       </c>
       <c r="C38">
-        <v>0.008733878054388279</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D38">
-        <v>0.0001656454412935777</v>
+        <v>0.0001673145877462598</v>
       </c>
       <c r="E38">
-        <v>0.0001961492659581503</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F38">
-        <v>0.2636491907304709</v>
+        <v>0.2815190988739301</v>
       </c>
       <c r="G38">
-        <v>0.1280492261183164</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H38">
         <v>0.2582640092197721</v>
@@ -2483,26 +2486,26 @@
       <c r="I38">
         <v>14156</v>
       </c>
-      <c r="K38">
-        <v>0.0003744000227958637</v>
-      </c>
-      <c r="M38">
+      <c r="L38">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="N38">
+        <v>0.004818030126325816</v>
+      </c>
+      <c r="O38">
+        <v>0.009535796789931871</v>
+      </c>
+      <c r="P38">
+        <v>0.1866413032030688</v>
+      </c>
+      <c r="Q38">
         <v>0.0003384092866814527</v>
       </c>
-      <c r="O38">
-        <v>0.009554445336689437</v>
-      </c>
-      <c r="P38">
-        <v>0.004730871750625608</v>
-      </c>
-      <c r="Q38">
-        <v>0.009674189396799987</v>
+      <c r="R38">
+        <v>0.0003710863970746162</v>
       </c>
       <c r="S38">
-        <v>0.179378395374721</v>
-      </c>
-      <c r="T38">
-        <v>0.004818030126325817</v>
+        <v>0.004784771004405694</v>
       </c>
     </row>
     <row r="39" spans="1:20">
@@ -2510,19 +2513,19 @@
         <v>57</v>
       </c>
       <c r="B39">
-        <v>0.008529233938818522</v>
+        <v>0.008532806478705164</v>
       </c>
       <c r="C39">
         <v>0.008733878054388279</v>
       </c>
       <c r="D39">
-        <v>0.0001653251466070655</v>
+        <v>0.0001656454412935777</v>
       </c>
       <c r="E39">
         <v>0.0001961492659581503</v>
       </c>
       <c r="F39">
-        <v>0.2650730104853413</v>
+        <v>0.2636491907304709</v>
       </c>
       <c r="G39">
         <v>0.1280492261183164</v>
@@ -2533,26 +2536,26 @@
       <c r="I39">
         <v>14156</v>
       </c>
-      <c r="K39">
-        <v>0.0003746361399868205</v>
-      </c>
-      <c r="M39">
+      <c r="L39">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="N39">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="O39">
+        <v>0.009554445336689437</v>
+      </c>
+      <c r="P39">
+        <v>0.179378395374721</v>
+      </c>
+      <c r="Q39">
         <v>0.0003384092866814527</v>
       </c>
-      <c r="O39">
-        <v>0.009555217528480035</v>
-      </c>
-      <c r="P39">
-        <v>0.004764640177213803</v>
-      </c>
-      <c r="Q39">
-        <v>0.009674189396799987</v>
+      <c r="R39">
+        <v>0.0003744000227958637</v>
       </c>
       <c r="S39">
-        <v>0.1788608663781261</v>
-      </c>
-      <c r="T39">
-        <v>0.004818030126325817</v>
+        <v>0.004730871750625608</v>
       </c>
     </row>
     <row r="40" spans="1:20">
@@ -2560,19 +2563,19 @@
         <v>58</v>
       </c>
       <c r="B40">
-        <v>0.008505250051591662</v>
+        <v>0.008529233938818522</v>
       </c>
       <c r="C40">
         <v>0.008733878054388279</v>
       </c>
       <c r="D40">
-        <v>0.0001646168902522808</v>
+        <v>0.0001653251466070655</v>
       </c>
       <c r="E40">
         <v>0.0001961492659581503</v>
       </c>
       <c r="F40">
-        <v>0.268221452941368</v>
+        <v>0.2650730104853413</v>
       </c>
       <c r="G40">
         <v>0.1280492261183164</v>
@@ -2583,26 +2586,26 @@
       <c r="I40">
         <v>14156</v>
       </c>
-      <c r="K40">
-        <v>0.0003736225585176234</v>
-      </c>
-      <c r="M40">
+      <c r="L40">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="N40">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="O40">
+        <v>0.009555217528480035</v>
+      </c>
+      <c r="P40">
+        <v>0.1788608663781261</v>
+      </c>
+      <c r="Q40">
         <v>0.0003384092866814527</v>
       </c>
-      <c r="O40">
-        <v>0.009526287265811475</v>
-      </c>
-      <c r="P40">
-        <v>0.004756476812602748</v>
-      </c>
-      <c r="Q40">
-        <v>0.009674189396799987</v>
+      <c r="R40">
+        <v>0.0003746361399868205</v>
       </c>
       <c r="S40">
-        <v>0.1810824657398455</v>
-      </c>
-      <c r="T40">
-        <v>0.004818030126325817</v>
+        <v>0.004764640177213803</v>
       </c>
     </row>
     <row r="41" spans="1:20">
@@ -2610,49 +2613,49 @@
         <v>59</v>
       </c>
       <c r="B41">
-        <v>0.006299187529923155</v>
+        <v>0.008505250051591662</v>
       </c>
       <c r="C41">
-        <v>0.00553167406053466</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D41">
-        <v>9.00395869891457E-05</v>
+        <v>0.0001646168902522808</v>
       </c>
       <c r="E41">
-        <v>8.170381435551846E-05</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F41">
-        <v>0.1391419988807219</v>
+        <v>0.268221452941368</v>
       </c>
       <c r="G41">
-        <v>0.2188393498696173</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H41">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I41">
-        <v>6771</v>
-      </c>
-      <c r="K41">
-        <v>0.0001603751212724098</v>
-      </c>
-      <c r="M41">
-        <v>0.0001037297229528328</v>
+        <v>14156</v>
+      </c>
+      <c r="L41">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="N41">
+        <v>0.004818030126325817</v>
       </c>
       <c r="O41">
-        <v>0.00674135934653288</v>
+        <v>0.009526287265811475</v>
       </c>
       <c r="P41">
-        <v>0.003667719421830667</v>
+        <v>0.1810824657398455</v>
       </c>
       <c r="Q41">
-        <v>0.005813234561065723</v>
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="R41">
+        <v>0.0003736225585176234</v>
       </c>
       <c r="S41">
-        <v>0.1045681259196538</v>
-      </c>
-      <c r="T41">
-        <v>0.003193202088483064</v>
+        <v>0.004756476812602748</v>
       </c>
     </row>
     <row r="42" spans="1:20">
@@ -2660,49 +2663,49 @@
         <v>60</v>
       </c>
       <c r="B42">
-        <v>0.00864935396008955</v>
+        <v>0.006299187529923155</v>
       </c>
       <c r="C42">
-        <v>0.008733878054388279</v>
+        <v>0.00553167406053466</v>
       </c>
       <c r="D42">
-        <v>0.0001602711781363747</v>
+        <v>9.00395869891457E-05</v>
       </c>
       <c r="E42">
-        <v>0.0001961492659581503</v>
+        <v>8.170381435551846E-05</v>
       </c>
       <c r="F42">
-        <v>0.2875396340419782</v>
+        <v>0.1391419988807219</v>
       </c>
       <c r="G42">
-        <v>0.1280492261183164</v>
+        <v>0.2188393498696173</v>
       </c>
       <c r="H42">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I42">
-        <v>14156</v>
-      </c>
-      <c r="K42">
-        <v>0.0003609428129771297</v>
-      </c>
-      <c r="M42">
-        <v>0.0003384092866814527</v>
+        <v>6771</v>
+      </c>
+      <c r="L42">
+        <v>0.005813234561065723</v>
+      </c>
+      <c r="N42">
+        <v>0.003193202088483064</v>
       </c>
       <c r="O42">
-        <v>0.009669808352814117</v>
+        <v>0.00674135934653288</v>
       </c>
       <c r="P42">
-        <v>0.005274143159156646</v>
+        <v>0.1045681259196538</v>
       </c>
       <c r="Q42">
-        <v>0.009674189396799987</v>
+        <v>0.0001037297229528328</v>
+      </c>
+      <c r="R42">
+        <v>0.0001603751212724098</v>
       </c>
       <c r="S42">
-        <v>0.2088743260447083</v>
-      </c>
-      <c r="T42">
-        <v>0.004818030126325816</v>
+        <v>0.003667719421830667</v>
       </c>
     </row>
     <row r="43" spans="1:20">
@@ -2710,22 +2713,22 @@
         <v>61</v>
       </c>
       <c r="B43">
-        <v>0.00869522801124366</v>
+        <v>0.00864935396008955</v>
       </c>
       <c r="C43">
-        <v>0.008722720041403264</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D43">
-        <v>0.0001671499749450426</v>
+        <v>0.0001602711781363747</v>
       </c>
       <c r="E43">
-        <v>0.0001985649052123504</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F43">
-        <v>0.2822259777859754</v>
+        <v>0.2875396340419782</v>
       </c>
       <c r="G43">
-        <v>0.147324247391146</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H43">
         <v>0.2582640092197721</v>
@@ -2733,26 +2736,26 @@
       <c r="I43">
         <v>14156</v>
       </c>
-      <c r="K43">
-        <v>0.0003635971635380399</v>
-      </c>
-      <c r="M43">
+      <c r="L43">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="N43">
+        <v>0.004818030126325816</v>
+      </c>
+      <c r="O43">
+        <v>0.009669808352814117</v>
+      </c>
+      <c r="P43">
+        <v>0.2088743260447083</v>
+      </c>
+      <c r="Q43">
         <v>0.0003384092866814527</v>
       </c>
-      <c r="O43">
-        <v>0.009719161233546112</v>
-      </c>
-      <c r="P43">
-        <v>0.005173194757001598</v>
-      </c>
-      <c r="Q43">
-        <v>0.009674189396799985</v>
+      <c r="R43">
+        <v>0.0003609428129771297</v>
       </c>
       <c r="S43">
-        <v>0.2030564380000814</v>
-      </c>
-      <c r="T43">
-        <v>0.004818030126325817</v>
+        <v>0.005274143159156646</v>
       </c>
     </row>
     <row r="44" spans="1:20">
@@ -2760,19 +2763,19 @@
         <v>62</v>
       </c>
       <c r="B44">
-        <v>0.007668256776450208</v>
+        <v>0.00869522801124366</v>
       </c>
       <c r="C44">
         <v>0.008722720041403264</v>
       </c>
       <c r="D44">
-        <v>0.0001436777206558706</v>
+        <v>0.0001671499749450426</v>
       </c>
       <c r="E44">
         <v>0.0001985649052123504</v>
       </c>
       <c r="F44">
-        <v>0.3830203355303232</v>
+        <v>0.2822259777859754</v>
       </c>
       <c r="G44">
         <v>0.147324247391146</v>
@@ -2783,26 +2786,26 @@
       <c r="I44">
         <v>14156</v>
       </c>
-      <c r="K44">
-        <v>0.0003344607981243851</v>
-      </c>
-      <c r="M44">
+      <c r="L44">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="N44">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="O44">
+        <v>0.009719161233546112</v>
+      </c>
+      <c r="P44">
+        <v>0.2030564380000814</v>
+      </c>
+      <c r="Q44">
         <v>0.0003384092866814527</v>
       </c>
-      <c r="O44">
-        <v>0.00867861064019221</v>
-      </c>
-      <c r="P44">
-        <v>0.004128330862335852</v>
-      </c>
-      <c r="Q44">
-        <v>0.009674189396799985</v>
+      <c r="R44">
+        <v>0.0003635971635380399</v>
       </c>
       <c r="S44">
-        <v>0.2669184291403396</v>
-      </c>
-      <c r="T44">
-        <v>0.004818030126325817</v>
+        <v>0.005173194757001598</v>
       </c>
     </row>
     <row r="45" spans="1:20">
@@ -2810,22 +2813,22 @@
         <v>63</v>
       </c>
       <c r="B45">
-        <v>0.01020612284563066</v>
+        <v>0.007668256776450208</v>
       </c>
       <c r="C45">
-        <v>0.009760820655321729</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D45">
-        <v>0.0002760452274294578</v>
+        <v>0.0001436777206558706</v>
       </c>
       <c r="E45">
-        <v>0.0002924361182664438</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F45">
-        <v>0.1971347954963554</v>
+        <v>0.3830203355303232</v>
       </c>
       <c r="G45">
-        <v>0.1494626221848404</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H45">
         <v>0.2582640092197721</v>
@@ -2833,26 +2836,26 @@
       <c r="I45">
         <v>14156</v>
       </c>
-      <c r="K45">
-        <v>0.0003886501570187028</v>
-      </c>
-      <c r="M45">
+      <c r="L45">
+        <v>0.009674189396799985</v>
+      </c>
+      <c r="N45">
+        <v>0.004818030126325817</v>
+      </c>
+      <c r="O45">
+        <v>0.00867861064019221</v>
+      </c>
+      <c r="P45">
+        <v>0.2669184291403396</v>
+      </c>
+      <c r="Q45">
         <v>0.0003384092866814527</v>
       </c>
-      <c r="O45">
-        <v>0.01011738460212881</v>
-      </c>
-      <c r="P45">
-        <v>0.005394960099510664</v>
-      </c>
-      <c r="Q45">
-        <v>0.009674189396799987</v>
+      <c r="R45">
+        <v>0.0003344607981243851</v>
       </c>
       <c r="S45">
-        <v>0.1481445083553075</v>
-      </c>
-      <c r="T45">
-        <v>0.004818030126325816</v>
+        <v>0.004128330862335852</v>
       </c>
     </row>
     <row r="46" spans="1:20">
@@ -2860,22 +2863,22 @@
         <v>64</v>
       </c>
       <c r="B46">
-        <v>0.00958912348219286</v>
+        <v>0.01020612284563066</v>
       </c>
       <c r="C46">
-        <v>0.008722720041403264</v>
+        <v>0.009760820655321729</v>
       </c>
       <c r="D46">
-        <v>0.00021842684931279</v>
+        <v>0.0002760452274294578</v>
       </c>
       <c r="E46">
-        <v>0.0001985649052123504</v>
+        <v>0.0002924361182664438</v>
       </c>
       <c r="F46">
-        <v>0.06203325341612431</v>
+        <v>0.1971347954963554</v>
       </c>
       <c r="G46">
-        <v>0.147324247391146</v>
+        <v>0.1494626221848404</v>
       </c>
       <c r="H46">
         <v>0.2582640092197721</v>
@@ -2883,26 +2886,26 @@
       <c r="I46">
         <v>14156</v>
       </c>
-      <c r="K46">
-        <v>0.0004313797729252501</v>
-      </c>
-      <c r="M46">
+      <c r="L46">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="N46">
+        <v>0.004818030126325816</v>
+      </c>
+      <c r="O46">
+        <v>0.01011738460212881</v>
+      </c>
+      <c r="P46">
+        <v>0.1481445083553075</v>
+      </c>
+      <c r="Q46">
         <v>0.0003384092866814527</v>
       </c>
-      <c r="O46">
-        <v>0.01064772150300563</v>
-      </c>
-      <c r="P46">
-        <v>0.005560650653515711</v>
-      </c>
-      <c r="Q46">
-        <v>0.009674189396799985</v>
+      <c r="R46">
+        <v>0.0003886501570187028</v>
       </c>
       <c r="S46">
-        <v>0.05448840836791147</v>
-      </c>
-      <c r="T46">
-        <v>0.004818030126325817</v>
+        <v>0.005394960099510664</v>
       </c>
     </row>
     <row r="47" spans="1:20">
@@ -2910,61 +2913,49 @@
         <v>65</v>
       </c>
       <c r="B47">
-        <v>0.005414655366858831</v>
+        <v>0.00958912348219286</v>
       </c>
       <c r="C47">
-        <v>0.005250633999685894</v>
+        <v>0.008722720041403264</v>
       </c>
       <c r="D47">
-        <v>8.390458217824665E-05</v>
+        <v>0.00021842684931279</v>
       </c>
       <c r="E47">
-        <v>8.336263472823423E-05</v>
+        <v>0.0001985649052123504</v>
       </c>
       <c r="F47">
-        <v>0.2548808040617673</v>
+        <v>0.06203325341612431</v>
       </c>
       <c r="G47">
-        <v>0.2596935978056915</v>
+        <v>0.147324247391146</v>
       </c>
       <c r="H47">
-        <v>0.456874413314975</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I47">
-        <v>5153</v>
-      </c>
-      <c r="J47">
-        <v>0.4055123229186881</v>
-      </c>
-      <c r="K47">
-        <v>0.000141190946981845</v>
+        <v>14156</v>
       </c>
       <c r="L47">
-        <v>10.4129840341794</v>
-      </c>
-      <c r="M47">
-        <v>9.243123959608208E-05</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="N47">
-        <v>11.43997477570016</v>
+        <v>0.004818030126325817</v>
       </c>
       <c r="O47">
-        <v>0.005626234126090045</v>
+        <v>0.01064772150300563</v>
       </c>
       <c r="P47">
-        <v>0.002733726006933551</v>
+        <v>0.05448840836791147</v>
       </c>
       <c r="Q47">
-        <v>0.005318929375230071</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="R47">
-        <v>0.4113135413420823</v>
+        <v>0.0004313797729252501</v>
       </c>
       <c r="S47">
-        <v>0.1703625716885953</v>
-      </c>
-      <c r="T47">
-        <v>0.002848413552158193</v>
+        <v>0.005560650653515711</v>
       </c>
     </row>
     <row r="48" spans="1:20">
@@ -2972,69 +2963,81 @@
         <v>66</v>
       </c>
       <c r="B48">
-        <v>0.00955739351620514</v>
+        <v>0.005414655366858831</v>
       </c>
       <c r="C48">
-        <v>0.008733878054388279</v>
+        <v>0.005250633999685894</v>
       </c>
       <c r="D48">
-        <v>0.0001939926155429641</v>
+        <v>8.390458217824665E-05</v>
       </c>
       <c r="E48">
-        <v>0.0001961492659581503</v>
+        <v>8.336263472823423E-05</v>
       </c>
       <c r="F48">
-        <v>0.137636277027368</v>
+        <v>0.2548808040617673</v>
       </c>
       <c r="G48">
-        <v>0.1280492261183164</v>
+        <v>0.2596935978056915</v>
       </c>
       <c r="H48">
-        <v>0.2582640092197721</v>
+        <v>0.456874413314975</v>
       </c>
       <c r="I48">
-        <v>14156</v>
+        <v>5153</v>
+      </c>
+      <c r="J48">
+        <v>0.4055123229186881</v>
       </c>
       <c r="K48">
-        <v>0.0004139067990685161</v>
+        <v>11.43997477570016</v>
+      </c>
+      <c r="L48">
+        <v>0.005318929375230071</v>
       </c>
       <c r="M48">
-        <v>0.0003384092866814527</v>
+        <v>10.4129840341794</v>
+      </c>
+      <c r="N48">
+        <v>0.002848413552158193</v>
       </c>
       <c r="O48">
-        <v>0.01060174085834054</v>
+        <v>0.005626234126090045</v>
       </c>
       <c r="P48">
-        <v>0.005675761589993111</v>
+        <v>0.1703625716885953</v>
       </c>
       <c r="Q48">
-        <v>0.009674189396799987</v>
+        <v>9.243123959608208E-05</v>
+      </c>
+      <c r="R48">
+        <v>0.000141190946981845</v>
       </c>
       <c r="S48">
-        <v>0.09278621544819221</v>
+        <v>0.002733726006933551</v>
       </c>
       <c r="T48">
-        <v>0.004818030126325816</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20">
+        <v>0.4113135413420823</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19">
       <c r="A49" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B49">
-        <v>0.009301347310769852</v>
+        <v>0.00955739351620514</v>
       </c>
       <c r="C49">
         <v>0.008733878054388279</v>
       </c>
       <c r="D49">
-        <v>0.0001883109214593075</v>
+        <v>0.0001939926155429641</v>
       </c>
       <c r="E49">
         <v>0.0001961492659581503</v>
       </c>
       <c r="F49">
-        <v>0.1628933562675233</v>
+        <v>0.137636277027368</v>
       </c>
       <c r="G49">
         <v>0.1280492261183164</v>
@@ -3045,226 +3048,276 @@
       <c r="I49">
         <v>14156</v>
       </c>
-      <c r="K49">
-        <v>0.0004026104577395279</v>
-      </c>
-      <c r="M49">
+      <c r="L49">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="N49">
+        <v>0.004818030126325816</v>
+      </c>
+      <c r="O49">
+        <v>0.01060174085834054</v>
+      </c>
+      <c r="P49">
+        <v>0.09278621544819221</v>
+      </c>
+      <c r="Q49">
         <v>0.0003384092866814527</v>
       </c>
-      <c r="O49">
-        <v>0.01035467890006862</v>
-      </c>
-      <c r="P49">
-        <v>0.005399385735558927</v>
-      </c>
-      <c r="Q49">
-        <v>0.009674189396799987</v>
+      <c r="R49">
+        <v>0.0004139067990685161</v>
       </c>
       <c r="S49">
-        <v>0.1175458874123242</v>
-      </c>
-      <c r="T49">
-        <v>0.004818030126325817</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20">
+        <v>0.005675761589993111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19">
       <c r="A50" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B50">
-        <v>0.00303210497017975</v>
+        <v>0.009301347310769852</v>
       </c>
       <c r="C50">
-        <v>0.002499571894821071</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D50">
-        <v>1.909735738640315E-05</v>
+        <v>0.0001883109214593075</v>
       </c>
       <c r="E50">
-        <v>1.967007435869721E-05</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F50">
-        <v>-0.0120856426831728</v>
+        <v>0.1628933562675233</v>
       </c>
       <c r="G50">
-        <v>-0.04243741404356438</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H50">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I50">
-        <v>11611</v>
-      </c>
-      <c r="K50">
-        <v>0.0002080153046483946</v>
-      </c>
-      <c r="M50">
-        <v>0.0001631540263502446</v>
+        <v>14156</v>
+      </c>
+      <c r="L50">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="N50">
+        <v>0.004818030126325817</v>
       </c>
       <c r="O50">
-        <v>0.005090949099942899</v>
+        <v>0.01035467890006862</v>
       </c>
       <c r="P50">
-        <v>0.001550051802718652</v>
+        <v>0.1175458874123242</v>
       </c>
       <c r="Q50">
-        <v>0.004580501696160511</v>
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="R50">
+        <v>0.0004026104577395279</v>
       </c>
       <c r="S50">
-        <v>-0.002911711704464803</v>
-      </c>
-      <c r="T50">
-        <v>0.001592932311570713</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20">
+        <v>0.005399385735558927</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19">
       <c r="A51" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B51">
-        <v>0.008142928261746932</v>
+        <v>0.00303210497017975</v>
       </c>
       <c r="C51">
-        <v>0.008733878054388279</v>
+        <v>0.002499571894821071</v>
       </c>
       <c r="D51">
-        <v>0.0001648112327367591</v>
+        <v>1.909735738640315E-05</v>
       </c>
       <c r="E51">
-        <v>0.0001961492659581503</v>
+        <v>1.967007435869721E-05</v>
       </c>
       <c r="F51">
-        <v>0.2673575339309593</v>
+        <v>-0.0120856426831728</v>
       </c>
       <c r="G51">
-        <v>0.1280492261183164</v>
+        <v>-0.04243741404356438</v>
       </c>
       <c r="H51">
-        <v>0.2582640092197721</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I51">
-        <v>14156</v>
-      </c>
-      <c r="K51">
-        <v>0.0003438074749231005</v>
-      </c>
-      <c r="M51">
-        <v>0.0003384092866814527</v>
+        <v>11611</v>
+      </c>
+      <c r="L51">
+        <v>0.004580501696160511</v>
+      </c>
+      <c r="N51">
+        <v>0.001592932311570713</v>
       </c>
       <c r="O51">
-        <v>0.009263751492683912</v>
+        <v>0.005090949099942899</v>
       </c>
       <c r="P51">
-        <v>0.004666820467017538</v>
+        <v>-0.002911711704464803</v>
       </c>
       <c r="Q51">
-        <v>0.009674189396799987</v>
+        <v>0.0001631540263502446</v>
+      </c>
+      <c r="R51">
+        <v>0.0002080153046483946</v>
       </c>
       <c r="S51">
-        <v>0.2464320924804251</v>
-      </c>
-      <c r="T51">
-        <v>0.004818030126325817</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20">
+        <v>0.001550051802718652</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19">
       <c r="A52" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B52">
-        <v>0.01025436961368844</v>
+        <v>0.008142928261746932</v>
       </c>
       <c r="C52">
-        <v>0.01023301201875394</v>
+        <v>0.008733878054388279</v>
       </c>
       <c r="D52">
-        <v>0.0002841844015704704</v>
+        <v>0.0001648112327367591</v>
       </c>
       <c r="E52">
-        <v>0.0003551633527675986</v>
+        <v>0.0001961492659581503</v>
       </c>
       <c r="F52">
-        <v>0.3369590471682379</v>
+        <v>0.2673575339309593</v>
       </c>
       <c r="G52">
-        <v>0.1713554771880856</v>
+        <v>0.1280492261183164</v>
       </c>
       <c r="H52">
-        <v>0.4827027158358849</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I52">
-        <v>1267</v>
-      </c>
-      <c r="K52">
-        <v>0.0006028948928221208</v>
-      </c>
-      <c r="M52">
-        <v>0.0004283113735138171</v>
+        <v>14156</v>
+      </c>
+      <c r="L52">
+        <v>0.009674189396799987</v>
+      </c>
+      <c r="N52">
+        <v>0.004818030126325817</v>
       </c>
       <c r="O52">
-        <v>0.0102050584404969</v>
+        <v>0.009263751492683912</v>
       </c>
       <c r="P52">
-        <v>0.005379622896887214</v>
+        <v>0.2464320924804251</v>
       </c>
       <c r="Q52">
-        <v>0.01026809155717979</v>
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="R52">
+        <v>0.0003438074749231005</v>
       </c>
       <c r="S52">
-        <v>0.2718477491393597</v>
-      </c>
-      <c r="T52">
-        <v>0.004670472236637264</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20">
+        <v>0.004666820467017538</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19">
       <c r="A53" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B53">
+        <v>0.01025436961368844</v>
+      </c>
+      <c r="C53">
+        <v>0.01023301201875394</v>
+      </c>
+      <c r="D53">
+        <v>0.0002841844015704704</v>
+      </c>
+      <c r="E53">
+        <v>0.0003551633527675986</v>
+      </c>
+      <c r="F53">
+        <v>0.3369590471682379</v>
+      </c>
+      <c r="G53">
+        <v>0.1713554771880856</v>
+      </c>
+      <c r="H53">
+        <v>0.4827027158358849</v>
+      </c>
+      <c r="I53">
+        <v>1267</v>
+      </c>
+      <c r="L53">
+        <v>0.01026809155717979</v>
+      </c>
+      <c r="N53">
+        <v>0.004670472236637264</v>
+      </c>
+      <c r="O53">
+        <v>0.0102050584404969</v>
+      </c>
+      <c r="P53">
+        <v>0.2718477491393597</v>
+      </c>
+      <c r="Q53">
+        <v>0.0004283113735138171</v>
+      </c>
+      <c r="R53">
+        <v>0.0006028948928221208</v>
+      </c>
+      <c r="S53">
+        <v>0.005379622896887214</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19">
+      <c r="A54" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B54">
         <v>0.009592505378186515</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <v>0.008764961593413305</v>
       </c>
-      <c r="D53">
+      <c r="D54">
         <v>0.0001961445305465736</v>
       </c>
-      <c r="E53">
+      <c r="E54">
         <v>0.0001968262288307614</v>
       </c>
-      <c r="F53">
+      <c r="F54">
         <v>0.122423362108982</v>
       </c>
-      <c r="G53">
+      <c r="G54">
         <v>0.1193733535942066</v>
       </c>
-      <c r="H53">
+      <c r="H54">
         <v>0.2253493365624453</v>
       </c>
-      <c r="I53">
+      <c r="I54">
         <v>7054</v>
       </c>
-      <c r="K53">
+      <c r="L54">
+        <v>0.009545579499406483</v>
+      </c>
+      <c r="N54">
+        <v>0.004876716066832584</v>
+      </c>
+      <c r="O54">
+        <v>0.01043843340429874</v>
+      </c>
+      <c r="P54">
+        <v>0.08840833195541187</v>
+      </c>
+      <c r="Q54">
+        <v>0.0002911643753660776</v>
+      </c>
+      <c r="R54">
         <v>0.0003426357597594948</v>
       </c>
-      <c r="M53">
-        <v>0.0002911643753660776</v>
-      </c>
-      <c r="O53">
-        <v>0.01043843340429874</v>
-      </c>
-      <c r="P53">
+      <c r="S54">
         <v>0.005648699862893431</v>
-      </c>
-      <c r="Q53">
-        <v>0.009545579499406483</v>
-      </c>
-      <c r="S53">
-        <v>0.08840833195541187</v>
-      </c>
-      <c r="T53">
-        <v>0.004876716066832584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update lgbm mse space
</commit_message>
<xml_diff>
--- a/results_analysis/compare_with_ibes/#compare_all.xlsx
+++ b/results_analysis/compare_with_ibes/#compare_all.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>lgbm_mae_org</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>ibes_qoq_2|fwdepsqcut|q_2｜ibes_qoq_tune10_ind</t>
+  </si>
+  <si>
+    <t>ibes_2|fwdepsqcut|tune_mse_ind</t>
   </si>
   <si>
     <t>ibes_qoq_1|fwdepsqcut|q_1｜ibes_qoq</t>
@@ -560,7 +563,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1354,28 +1357,28 @@
         <v>34</v>
       </c>
       <c r="B28">
-        <v>0.005107549406927882</v>
+        <v>0.01003309392811347</v>
       </c>
       <c r="C28">
-        <v>0.004580501696160511</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="D28">
-        <v>0.000207986162951978</v>
+        <v>0.0003930561638032175</v>
       </c>
       <c r="E28">
-        <v>0.0001631540263502446</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F28">
-        <v>-0.002771209789547591</v>
+        <v>0.138487285766222</v>
       </c>
       <c r="G28">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H28">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I28">
-        <v>11611</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1383,28 +1386,28 @@
         <v>35</v>
       </c>
       <c r="B29">
-        <v>0.006776662396495037</v>
+        <v>0.005107549406927882</v>
       </c>
       <c r="C29">
-        <v>0.005813234561065723</v>
+        <v>0.004580501696160511</v>
       </c>
       <c r="D29">
-        <v>0.000160150142460433</v>
+        <v>0.000207986162951978</v>
       </c>
       <c r="E29">
-        <v>0.0001037297229528328</v>
+        <v>0.0001631540263502446</v>
       </c>
       <c r="F29">
-        <v>0.1058242633905934</v>
+        <v>-0.002771209789547591</v>
       </c>
       <c r="G29">
-        <v>0.4208397194991282</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="H29">
-        <v>0.4208397194991282</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I29">
-        <v>6771</v>
+        <v>11611</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1412,28 +1415,28 @@
         <v>36</v>
       </c>
       <c r="B30">
-        <v>0.01005761747872771</v>
+        <v>0.006776662396495037</v>
       </c>
       <c r="C30">
-        <v>0.009674189396799987</v>
+        <v>0.005813234561065723</v>
       </c>
       <c r="D30">
-        <v>0.0003817896694842294</v>
+        <v>0.000160150142460433</v>
       </c>
       <c r="E30">
-        <v>0.0003384092866814527</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="F30">
-        <v>0.1631815381263255</v>
+        <v>0.1058242633905934</v>
       </c>
       <c r="G30">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="H30">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I30">
-        <v>14156</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1441,28 +1444,28 @@
         <v>37</v>
       </c>
       <c r="B31">
-        <v>0.004501420066184821</v>
+        <v>0.01005761747872771</v>
       </c>
       <c r="C31">
-        <v>0.004349183403839366</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="D31">
-        <v>0.0002742305932959652</v>
+        <v>0.0003817896694842294</v>
       </c>
       <c r="E31">
-        <v>0.0001730864695810989</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F31">
-        <v>-0.006214540120261569</v>
+        <v>0.1631815381263255</v>
       </c>
       <c r="G31">
-        <v>0.3649062991209757</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H31">
-        <v>0.3649062991209757</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I31">
-        <v>4010</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1470,28 +1473,28 @@
         <v>38</v>
       </c>
       <c r="B32">
-        <v>0.009396936069700112</v>
+        <v>0.004501420066184821</v>
       </c>
       <c r="C32">
-        <v>0.009729123728171802</v>
+        <v>0.004349183403839366</v>
       </c>
       <c r="D32">
-        <v>0.0003716511763370566</v>
+        <v>0.0002742305932959652</v>
       </c>
       <c r="E32">
-        <v>0.0003414259156749913</v>
+        <v>0.0001730864695810989</v>
       </c>
       <c r="F32">
-        <v>0.1928904449236721</v>
+        <v>-0.006214540120261569</v>
       </c>
       <c r="G32">
-        <v>0.2585302120985278</v>
+        <v>0.3649062991209757</v>
       </c>
       <c r="H32">
-        <v>0.2585302120985278</v>
+        <v>0.3649062991209757</v>
       </c>
       <c r="I32">
-        <v>14000</v>
+        <v>4010</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1499,28 +1502,28 @@
         <v>39</v>
       </c>
       <c r="B33">
-        <v>0.01035431191953904</v>
+        <v>0.009396936069700112</v>
       </c>
       <c r="C33">
-        <v>0.009674189396799987</v>
+        <v>0.009729123728171802</v>
       </c>
       <c r="D33">
-        <v>0.0004001063569688302</v>
+        <v>0.0003716511763370566</v>
       </c>
       <c r="E33">
-        <v>0.0003384092866814527</v>
+        <v>0.0003414259156749913</v>
       </c>
       <c r="F33">
-        <v>0.1230344532976788</v>
+        <v>0.1928904449236721</v>
       </c>
       <c r="G33">
-        <v>0.2582640092197721</v>
+        <v>0.2585302120985278</v>
       </c>
       <c r="H33">
-        <v>0.2582640092197721</v>
+        <v>0.2585302120985278</v>
       </c>
       <c r="I33">
-        <v>14156</v>
+        <v>14000</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1528,28 +1531,28 @@
         <v>40</v>
       </c>
       <c r="B34">
-        <v>0.01022526679210232</v>
+        <v>0.01035431191953904</v>
       </c>
       <c r="C34">
-        <v>0.009384601794708014</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="D34">
-        <v>0.0004705186388866096</v>
+        <v>0.0004001063569688302</v>
       </c>
       <c r="E34">
-        <v>0.0003220429185286173</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F34">
-        <v>0.1094051116331665</v>
+        <v>0.1230344532976788</v>
       </c>
       <c r="G34">
-        <v>0.3904390743053188</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H34">
-        <v>0.3904390743053188</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I34">
-        <v>4699</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1557,28 +1560,28 @@
         <v>41</v>
       </c>
       <c r="B35">
-        <v>0.005089488294347637</v>
+        <v>0.01022526679210232</v>
       </c>
       <c r="C35">
-        <v>0.004580501696160511</v>
+        <v>0.009384601794708014</v>
       </c>
       <c r="D35">
-        <v>0.0002081444394071696</v>
+        <v>0.0004705186388866096</v>
       </c>
       <c r="E35">
-        <v>0.0001631540263502446</v>
+        <v>0.0003220429185286173</v>
       </c>
       <c r="F35">
-        <v>-0.00353431378743374</v>
+        <v>0.1094051116331665</v>
       </c>
       <c r="G35">
-        <v>0.2133795918767654</v>
+        <v>0.3904390743053188</v>
       </c>
       <c r="H35">
-        <v>0.2133795918767654</v>
+        <v>0.3904390743053188</v>
       </c>
       <c r="I35">
-        <v>11611</v>
+        <v>4699</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1586,28 +1589,28 @@
         <v>42</v>
       </c>
       <c r="B36">
-        <v>0.009406309171688502</v>
+        <v>0.005089488294347637</v>
       </c>
       <c r="C36">
-        <v>0.009674189396799985</v>
+        <v>0.004580501696160511</v>
       </c>
       <c r="D36">
-        <v>0.0003610907680501377</v>
+        <v>0.0002081444394071696</v>
       </c>
       <c r="E36">
-        <v>0.0003384092866814527</v>
+        <v>0.0001631540263502446</v>
       </c>
       <c r="F36">
-        <v>0.2085500335179142</v>
+        <v>-0.00353431378743374</v>
       </c>
       <c r="G36">
-        <v>0.2582640092197721</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="H36">
-        <v>0.2582640092197721</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I36">
-        <v>14156</v>
+        <v>11611</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1615,19 +1618,19 @@
         <v>43</v>
       </c>
       <c r="B37">
-        <v>0.009535796789931871</v>
+        <v>0.009406309171688502</v>
       </c>
       <c r="C37">
         <v>0.009674189396799985</v>
       </c>
       <c r="D37">
-        <v>0.0003710863970746162</v>
+        <v>0.0003610907680501377</v>
       </c>
       <c r="E37">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F37">
-        <v>0.1866413032030688</v>
+        <v>0.2085500335179142</v>
       </c>
       <c r="G37">
         <v>0.2582640092197721</v>
@@ -1644,19 +1647,19 @@
         <v>44</v>
       </c>
       <c r="B38">
-        <v>0.009554445336689437</v>
+        <v>0.009535796789931871</v>
       </c>
       <c r="C38">
-        <v>0.009674189396799987</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="D38">
-        <v>0.0003744000227958637</v>
+        <v>0.0003710863970746162</v>
       </c>
       <c r="E38">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F38">
-        <v>0.179378395374721</v>
+        <v>0.1866413032030688</v>
       </c>
       <c r="G38">
         <v>0.2582640092197721</v>
@@ -1673,19 +1676,19 @@
         <v>45</v>
       </c>
       <c r="B39">
-        <v>0.009555217528480035</v>
+        <v>0.009554445336689437</v>
       </c>
       <c r="C39">
         <v>0.009674189396799987</v>
       </c>
       <c r="D39">
-        <v>0.0003746361399868205</v>
+        <v>0.0003744000227958637</v>
       </c>
       <c r="E39">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F39">
-        <v>0.1788608663781261</v>
+        <v>0.179378395374721</v>
       </c>
       <c r="G39">
         <v>0.2582640092197721</v>
@@ -1702,19 +1705,19 @@
         <v>46</v>
       </c>
       <c r="B40">
-        <v>0.009526287265811475</v>
+        <v>0.009555217528480035</v>
       </c>
       <c r="C40">
         <v>0.009674189396799987</v>
       </c>
       <c r="D40">
-        <v>0.0003736225585176234</v>
+        <v>0.0003746361399868205</v>
       </c>
       <c r="E40">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F40">
-        <v>0.1810824657398455</v>
+        <v>0.1788608663781261</v>
       </c>
       <c r="G40">
         <v>0.2582640092197721</v>
@@ -1731,28 +1734,28 @@
         <v>47</v>
       </c>
       <c r="B41">
-        <v>0.00674135934653288</v>
+        <v>0.009526287265811475</v>
       </c>
       <c r="C41">
-        <v>0.005813234561065723</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="D41">
-        <v>0.0001603751212724098</v>
+        <v>0.0003736225585176234</v>
       </c>
       <c r="E41">
-        <v>0.0001037297229528328</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F41">
-        <v>0.1045681259196538</v>
+        <v>0.1810824657398455</v>
       </c>
       <c r="G41">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H41">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I41">
-        <v>6771</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1760,28 +1763,28 @@
         <v>48</v>
       </c>
       <c r="B42">
-        <v>0.009669808352814117</v>
+        <v>0.00674135934653288</v>
       </c>
       <c r="C42">
-        <v>0.009674189396799987</v>
+        <v>0.005813234561065723</v>
       </c>
       <c r="D42">
-        <v>0.0003609428129771297</v>
+        <v>0.0001603751212724098</v>
       </c>
       <c r="E42">
-        <v>0.0003384092866814527</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="F42">
-        <v>0.2088743260447083</v>
+        <v>0.1045681259196538</v>
       </c>
       <c r="G42">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="H42">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I42">
-        <v>14156</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1789,19 +1792,19 @@
         <v>49</v>
       </c>
       <c r="B43">
-        <v>0.009547987620144199</v>
+        <v>0.009669808352814117</v>
       </c>
       <c r="C43">
-        <v>0.009674189396799985</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="D43">
-        <v>0.0003609514012730195</v>
+        <v>0.0003609428129771297</v>
       </c>
       <c r="E43">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F43">
-        <v>0.2088555019508919</v>
+        <v>0.2088743260447083</v>
       </c>
       <c r="G43">
         <v>0.2582640092197721</v>
@@ -1818,19 +1821,19 @@
         <v>50</v>
       </c>
       <c r="B44">
-        <v>0.009719161233546112</v>
+        <v>0.009547987620144199</v>
       </c>
       <c r="C44">
         <v>0.009674189396799985</v>
       </c>
       <c r="D44">
-        <v>0.0003635971635380399</v>
+        <v>0.0003609514012730195</v>
       </c>
       <c r="E44">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F44">
-        <v>0.2030564380000814</v>
+        <v>0.2088555019508919</v>
       </c>
       <c r="G44">
         <v>0.2582640092197721</v>
@@ -1847,19 +1850,19 @@
         <v>51</v>
       </c>
       <c r="B45">
-        <v>0.009501857293097325</v>
+        <v>0.009719161233546112</v>
       </c>
       <c r="C45">
         <v>0.009674189396799985</v>
       </c>
       <c r="D45">
-        <v>0.0003602535480745813</v>
+        <v>0.0003635971635380399</v>
       </c>
       <c r="E45">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F45">
-        <v>0.2103850782773533</v>
+        <v>0.2030564380000814</v>
       </c>
       <c r="G45">
         <v>0.2582640092197721</v>
@@ -1876,19 +1879,19 @@
         <v>52</v>
       </c>
       <c r="B46">
-        <v>0.00867861064019221</v>
+        <v>0.009501857293097325</v>
       </c>
       <c r="C46">
         <v>0.009674189396799985</v>
       </c>
       <c r="D46">
-        <v>0.0003344607981243851</v>
+        <v>0.0003602535480745813</v>
       </c>
       <c r="E46">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F46">
-        <v>0.2669184291403396</v>
+        <v>0.2103850782773533</v>
       </c>
       <c r="G46">
         <v>0.2582640092197721</v>
@@ -1905,19 +1908,19 @@
         <v>53</v>
       </c>
       <c r="B47">
-        <v>0.01011738460212881</v>
+        <v>0.00867861064019221</v>
       </c>
       <c r="C47">
-        <v>0.009674189396799987</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="D47">
-        <v>0.0003886501570187028</v>
+        <v>0.0003344607981243851</v>
       </c>
       <c r="E47">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F47">
-        <v>0.1481445083553075</v>
+        <v>0.2669184291403396</v>
       </c>
       <c r="G47">
         <v>0.2582640092197721</v>
@@ -1934,19 +1937,19 @@
         <v>54</v>
       </c>
       <c r="B48">
-        <v>0.01064772150300563</v>
+        <v>0.01011738460212881</v>
       </c>
       <c r="C48">
-        <v>0.009674189396799985</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="D48">
-        <v>0.0004313797729252501</v>
+        <v>0.0003886501570187028</v>
       </c>
       <c r="E48">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F48">
-        <v>0.05448840836791147</v>
+        <v>0.1481445083553075</v>
       </c>
       <c r="G48">
         <v>0.2582640092197721</v>
@@ -1963,28 +1966,28 @@
         <v>55</v>
       </c>
       <c r="B49">
-        <v>0.005626234126090045</v>
+        <v>0.01064772150300563</v>
       </c>
       <c r="C49">
-        <v>0.005318929375230071</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="D49">
-        <v>0.000141190946981845</v>
+        <v>0.0004313797729252501</v>
       </c>
       <c r="E49">
-        <v>9.243123959608208E-05</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F49">
-        <v>0.1703625716885953</v>
+        <v>0.05448840836791147</v>
       </c>
       <c r="G49">
-        <v>0.456874413314975</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H49">
-        <v>0.456874413314975</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I49">
-        <v>5153</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1992,28 +1995,28 @@
         <v>56</v>
       </c>
       <c r="B50">
-        <v>0.01060174085834054</v>
+        <v>0.005626234126090045</v>
       </c>
       <c r="C50">
-        <v>0.009674189396799987</v>
+        <v>0.005318929375230071</v>
       </c>
       <c r="D50">
-        <v>0.0004139067990685161</v>
+        <v>0.000141190946981845</v>
       </c>
       <c r="E50">
-        <v>0.0003384092866814527</v>
+        <v>9.243123959608208E-05</v>
       </c>
       <c r="F50">
-        <v>0.09278621544819221</v>
+        <v>0.1703625716885953</v>
       </c>
       <c r="G50">
-        <v>0.2582640092197721</v>
+        <v>0.456874413314975</v>
       </c>
       <c r="H50">
-        <v>0.2582640092197721</v>
+        <v>0.456874413314975</v>
       </c>
       <c r="I50">
-        <v>14156</v>
+        <v>5153</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2021,19 +2024,19 @@
         <v>57</v>
       </c>
       <c r="B51">
-        <v>0.01035467890006862</v>
+        <v>0.01060174085834054</v>
       </c>
       <c r="C51">
         <v>0.009674189396799987</v>
       </c>
       <c r="D51">
-        <v>0.0004026104577395279</v>
+        <v>0.0004139067990685161</v>
       </c>
       <c r="E51">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F51">
-        <v>0.1175458874123242</v>
+        <v>0.09278621544819221</v>
       </c>
       <c r="G51">
         <v>0.2582640092197721</v>
@@ -2050,28 +2053,28 @@
         <v>58</v>
       </c>
       <c r="B52">
-        <v>0.005090949099942899</v>
+        <v>0.01035467890006862</v>
       </c>
       <c r="C52">
-        <v>0.004580501696160511</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="D52">
-        <v>0.0002080153046483946</v>
+        <v>0.0004026104577395279</v>
       </c>
       <c r="E52">
-        <v>0.0001631540263502446</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F52">
-        <v>-0.002911711704464803</v>
+        <v>0.1175458874123242</v>
       </c>
       <c r="G52">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H52">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I52">
-        <v>11611</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2079,28 +2082,28 @@
         <v>59</v>
       </c>
       <c r="B53">
-        <v>0.009263751492683912</v>
+        <v>0.005090949099942899</v>
       </c>
       <c r="C53">
-        <v>0.009674189396799987</v>
+        <v>0.004580501696160511</v>
       </c>
       <c r="D53">
-        <v>0.0003438074749231005</v>
+        <v>0.0002080153046483946</v>
       </c>
       <c r="E53">
-        <v>0.0003384092866814527</v>
+        <v>0.0001631540263502446</v>
       </c>
       <c r="F53">
-        <v>0.2464320924804251</v>
+        <v>-0.002911711704464803</v>
       </c>
       <c r="G53">
-        <v>0.2582640092197721</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="H53">
-        <v>0.2582640092197721</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I53">
-        <v>14156</v>
+        <v>11611</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -2108,28 +2111,28 @@
         <v>60</v>
       </c>
       <c r="B54">
-        <v>0.00950560728094302</v>
+        <v>0.009263751492683912</v>
       </c>
       <c r="C54">
-        <v>0.00969865279856456</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="D54">
-        <v>0.0003676303455898381</v>
+        <v>0.0003438074749231005</v>
       </c>
       <c r="E54">
-        <v>0.0003326480833522705</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F54">
-        <v>0.277134584732579</v>
+        <v>0.2464320924804251</v>
       </c>
       <c r="G54">
-        <v>0.3459196233527754</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H54">
-        <v>0.3459196233527754</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I54">
-        <v>5919</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2137,28 +2140,28 @@
         <v>61</v>
       </c>
       <c r="B55">
-        <v>0.01043843340429874</v>
+        <v>0.00950560728094302</v>
       </c>
       <c r="C55">
-        <v>0.009545579499406483</v>
+        <v>0.00969865279856456</v>
       </c>
       <c r="D55">
-        <v>0.0003426357597594948</v>
+        <v>0.0003676303455898381</v>
       </c>
       <c r="E55">
-        <v>0.0002911643753660776</v>
+        <v>0.0003326480833522705</v>
       </c>
       <c r="F55">
-        <v>0.08840833195541187</v>
+        <v>0.277134584732579</v>
       </c>
       <c r="G55">
-        <v>0.2253493365624453</v>
+        <v>0.3459196233527754</v>
       </c>
       <c r="H55">
-        <v>0.2253493365624453</v>
+        <v>0.3459196233527754</v>
       </c>
       <c r="I55">
-        <v>7054</v>
+        <v>5919</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2166,27 +2169,56 @@
         <v>62</v>
       </c>
       <c r="B56">
+        <v>0.01043843340429874</v>
+      </c>
+      <c r="C56">
+        <v>0.009545579499406483</v>
+      </c>
+      <c r="D56">
+        <v>0.0003426357597594948</v>
+      </c>
+      <c r="E56">
+        <v>0.0002911643753660776</v>
+      </c>
+      <c r="F56">
+        <v>0.08840833195541187</v>
+      </c>
+      <c r="G56">
+        <v>0.2253493365624453</v>
+      </c>
+      <c r="H56">
+        <v>0.2253493365624453</v>
+      </c>
+      <c r="I56">
+        <v>7054</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57">
         <v>0.009547617558891911</v>
       </c>
-      <c r="C56">
+      <c r="C57">
         <v>0.009674189396799985</v>
       </c>
-      <c r="D56">
+      <c r="D57">
         <v>0.000360031497755876</v>
       </c>
-      <c r="E56">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="F56">
+      <c r="E57">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="F57">
         <v>0.2108717750662125</v>
       </c>
-      <c r="G56">
-        <v>0.2582640092197721</v>
-      </c>
-      <c r="H56">
-        <v>0.2582640092197721</v>
-      </c>
-      <c r="I56">
+      <c r="G57">
+        <v>0.2582640092197721</v>
+      </c>
+      <c r="H57">
+        <v>0.2582640092197721</v>
+      </c>
+      <c r="I57">
         <v>14156</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update xgb mse space
</commit_message>
<xml_diff>
--- a/results_analysis/compare_with_ibes/#compare_all.xlsx
+++ b/results_analysis/compare_with_ibes/#compare_all.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
   <si>
     <t>lgbm_mae_org</t>
   </si>
@@ -46,6 +46,9 @@
     <t>ibes_qoq_2|fwdepsqcut|q_2｜ibes_qoq_tune10_ind3</t>
   </si>
   <si>
+    <t>ibes_2|fwdepsqcut|tune_mse_ind2</t>
+  </si>
+  <si>
     <t>ibes_2|fwdepsqcut|mse_ex_ind_tune1</t>
   </si>
   <si>
@@ -131,6 +134,9 @@
   </si>
   <si>
     <t>ibes_qoq_1|fwdepsqcut|q_1｜ibes_qoq_filter</t>
+  </si>
+  <si>
+    <t>ibes_2|fwdepsqcut|mse_ex_ind_tune5</t>
   </si>
   <si>
     <t>ibes_1|fwdepsqcut|country_entire</t>
@@ -563,7 +569,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -661,19 +667,19 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>0.009762703396109433</v>
+        <v>0.00942898486482744</v>
       </c>
       <c r="C4">
         <v>0.009674189396799985</v>
       </c>
       <c r="D4">
-        <v>0.0003668610048628526</v>
+        <v>0.000357156486123264</v>
       </c>
       <c r="E4">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F4">
-        <v>0.1959026491589134</v>
+        <v>0.2171733149049446</v>
       </c>
       <c r="G4">
         <v>0.2582640092197721</v>
@@ -690,28 +696,28 @@
         <v>11</v>
       </c>
       <c r="B5">
-        <v>0.005606434133779571</v>
+        <v>0.009762703396109433</v>
       </c>
       <c r="C5">
-        <v>0.005813234561065725</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="D5">
-        <v>0.0001137832146297872</v>
+        <v>0.0003668610048628526</v>
       </c>
       <c r="E5">
-        <v>0.0001037297229528328</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F5">
-        <v>0.36470746642943</v>
+        <v>0.1959026491589134</v>
       </c>
       <c r="G5">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H5">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I5">
-        <v>6771</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -719,28 +725,28 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>0.01049901448336211</v>
+        <v>0.005606434133779571</v>
       </c>
       <c r="C6">
-        <v>0.009674189396799987</v>
+        <v>0.005813234561065725</v>
       </c>
       <c r="D6">
-        <v>0.0004050244790002472</v>
+        <v>0.0001137832146297872</v>
       </c>
       <c r="E6">
-        <v>0.0003384092866814527</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="F6">
-        <v>0.1122547605962045</v>
+        <v>0.36470746642943</v>
       </c>
       <c r="G6">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="H6">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I6">
-        <v>14156</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -748,28 +754,28 @@
         <v>13</v>
       </c>
       <c r="B7">
-        <v>0.005632685300523813</v>
+        <v>0.01049901448336211</v>
       </c>
       <c r="C7">
-        <v>0.005813234561065725</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="D7">
-        <v>0.0001152638129503358</v>
+        <v>0.0004050244790002472</v>
       </c>
       <c r="E7">
-        <v>0.0001037297229528328</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F7">
-        <v>0.3564407544954944</v>
+        <v>0.1122547605962045</v>
       </c>
       <c r="G7">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H7">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I7">
-        <v>6771</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -777,28 +783,28 @@
         <v>14</v>
       </c>
       <c r="B8">
-        <v>0.009106885821888167</v>
+        <v>0.005632685300523813</v>
       </c>
       <c r="C8">
-        <v>0.009674189396799987</v>
+        <v>0.005813234561065725</v>
       </c>
       <c r="D8">
-        <v>0.000333070102780211</v>
+        <v>0.0001152638129503358</v>
       </c>
       <c r="E8">
-        <v>0.0003384092866814527</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="F8">
-        <v>0.269966598412229</v>
+        <v>0.3564407544954944</v>
       </c>
       <c r="G8">
-        <v>0.2582640092197723</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="H8">
-        <v>0.2582640092197723</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I8">
-        <v>42468</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -806,28 +812,28 @@
         <v>15</v>
       </c>
       <c r="B9">
-        <v>0.008950010380536522</v>
+        <v>0.009106885821888167</v>
       </c>
       <c r="C9">
-        <v>0.009674189396799985</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="D9">
-        <v>0.0003285627388197843</v>
+        <v>0.000333070102780211</v>
       </c>
       <c r="E9">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F9">
-        <v>0.2798459788092014</v>
+        <v>0.269966598412229</v>
       </c>
       <c r="G9">
-        <v>0.2582640092197721</v>
+        <v>0.2582640092197723</v>
       </c>
       <c r="H9">
-        <v>0.2582640092197721</v>
+        <v>0.2582640092197723</v>
       </c>
       <c r="I9">
-        <v>14156</v>
+        <v>42468</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -835,28 +841,28 @@
         <v>16</v>
       </c>
       <c r="B10">
-        <v>0.007677919171285994</v>
+        <v>0.008950010380536522</v>
       </c>
       <c r="C10">
-        <v>0.007921255031590064</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="D10">
-        <v>0.0001862950617261432</v>
+        <v>0.0003285627388197843</v>
       </c>
       <c r="E10">
-        <v>0.0001858662918611346</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F10">
-        <v>0.2347147170485431</v>
+        <v>0.2798459788092014</v>
       </c>
       <c r="G10">
-        <v>0.2364760695203898</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H10">
-        <v>0.2364760695203898</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I10">
-        <v>5254</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -864,28 +870,28 @@
         <v>17</v>
       </c>
       <c r="B11">
-        <v>0.00941140169945745</v>
+        <v>0.007677919171285994</v>
       </c>
       <c r="C11">
-        <v>0.009674189396799985</v>
+        <v>0.007921255031590064</v>
       </c>
       <c r="D11">
-        <v>0.0003713407546776094</v>
+        <v>0.0001862950617261432</v>
       </c>
       <c r="E11">
-        <v>0.0003384092866814527</v>
+        <v>0.0001858662918611346</v>
       </c>
       <c r="F11">
-        <v>0.1860837943045432</v>
+        <v>0.2347147170485431</v>
       </c>
       <c r="G11">
-        <v>0.2582640092197721</v>
+        <v>0.2364760695203898</v>
       </c>
       <c r="H11">
-        <v>0.2582640092197721</v>
+        <v>0.2364760695203898</v>
       </c>
       <c r="I11">
-        <v>14156</v>
+        <v>5254</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -893,28 +899,28 @@
         <v>18</v>
       </c>
       <c r="B12">
-        <v>0.008363098231375462</v>
+        <v>0.00941140169945745</v>
       </c>
       <c r="C12">
-        <v>0.006875190708555331</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="D12">
-        <v>0.0002632414236722758</v>
+        <v>0.0003713407546776094</v>
       </c>
       <c r="E12">
-        <v>0.0001796235360933539</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F12">
-        <v>-0.00724317687482956</v>
+        <v>0.1860837943045432</v>
       </c>
       <c r="G12">
-        <v>0.3127047460379806</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H12">
-        <v>0.3127047460379806</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I12">
-        <v>24768</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -922,28 +928,28 @@
         <v>19</v>
       </c>
       <c r="B13">
-        <v>0.009901025034115019</v>
+        <v>0.008363098231375462</v>
       </c>
       <c r="C13">
-        <v>0.009674189396799985</v>
+        <v>0.006875190708555331</v>
       </c>
       <c r="D13">
-        <v>0.0003847976244374441</v>
+        <v>0.0002632414236722758</v>
       </c>
       <c r="E13">
-        <v>0.0003384092866814527</v>
+        <v>0.0001796235360933539</v>
       </c>
       <c r="F13">
-        <v>0.1565886089862186</v>
+        <v>-0.00724317687482956</v>
       </c>
       <c r="G13">
-        <v>0.2582640092197721</v>
+        <v>0.3127047460379806</v>
       </c>
       <c r="H13">
-        <v>0.2582640092197721</v>
+        <v>0.3127047460379806</v>
       </c>
       <c r="I13">
-        <v>14156</v>
+        <v>24768</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -951,28 +957,28 @@
         <v>20</v>
       </c>
       <c r="B14">
-        <v>0.00512210974064752</v>
+        <v>0.009901025034115019</v>
       </c>
       <c r="C14">
-        <v>0.004589584286176587</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="D14">
-        <v>0.000209188838038313</v>
+        <v>0.0003847976244374441</v>
       </c>
       <c r="E14">
-        <v>0.000163888349337522</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F14">
-        <v>-0.005102592401121431</v>
+        <v>0.1565886089862186</v>
       </c>
       <c r="G14">
-        <v>0.212555477012045</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H14">
-        <v>0.212555477012045</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I14">
-        <v>11542</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -980,28 +986,28 @@
         <v>21</v>
       </c>
       <c r="B15">
-        <v>0.00526064949972486</v>
+        <v>0.00512210974064752</v>
       </c>
       <c r="C15">
-        <v>0.005813234561065725</v>
+        <v>0.004589584286176587</v>
       </c>
       <c r="D15">
-        <v>0.000112952017849086</v>
+        <v>0.000209188838038313</v>
       </c>
       <c r="E15">
-        <v>0.0001037297229528328</v>
+        <v>0.000163888349337522</v>
       </c>
       <c r="F15">
-        <v>0.3693483364419842</v>
+        <v>-0.005102592401121431</v>
       </c>
       <c r="G15">
-        <v>0.4208397194991282</v>
+        <v>0.212555477012045</v>
       </c>
       <c r="H15">
-        <v>0.4208397194991282</v>
+        <v>0.212555477012045</v>
       </c>
       <c r="I15">
-        <v>6771</v>
+        <v>11542</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1009,28 +1015,28 @@
         <v>22</v>
       </c>
       <c r="B16">
-        <v>0.005213165544267774</v>
+        <v>0.00526064949972486</v>
       </c>
       <c r="C16">
-        <v>0.004580501696160511</v>
+        <v>0.005813234561065725</v>
       </c>
       <c r="D16">
-        <v>0.0002098592232396584</v>
+        <v>0.000112952017849086</v>
       </c>
       <c r="E16">
-        <v>0.0001631540263502446</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="F16">
-        <v>-0.01180186309853548</v>
+        <v>0.3693483364419842</v>
       </c>
       <c r="G16">
-        <v>0.2133795918767654</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="H16">
-        <v>0.2133795918767654</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I16">
-        <v>11611</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1038,28 +1044,28 @@
         <v>23</v>
       </c>
       <c r="B17">
-        <v>0.007217175147339313</v>
+        <v>0.005213165544267774</v>
       </c>
       <c r="C17">
-        <v>0.004529835290885987</v>
+        <v>0.004580501696160511</v>
       </c>
       <c r="D17">
-        <v>0.0003123469992588732</v>
+        <v>0.0002098592232396584</v>
       </c>
       <c r="E17">
-        <v>0.0001158352549329261</v>
+        <v>0.0001631540263502446</v>
       </c>
       <c r="F17">
-        <v>-0.01652918306199047</v>
+        <v>-0.01180186309853548</v>
       </c>
       <c r="G17">
-        <v>0.6230156929756394</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="H17">
-        <v>0.6230156929756394</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I17">
-        <v>49</v>
+        <v>11611</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1067,28 +1073,28 @@
         <v>24</v>
       </c>
       <c r="B18">
-        <v>0.009820067619913343</v>
+        <v>0.007217175147339313</v>
       </c>
       <c r="C18">
-        <v>0.009674189396799985</v>
+        <v>0.004529835290885987</v>
       </c>
       <c r="D18">
-        <v>0.0003683547284434392</v>
+        <v>0.0003123469992588732</v>
       </c>
       <c r="E18">
-        <v>0.0003384092866814527</v>
+        <v>0.0001158352549329261</v>
       </c>
       <c r="F18">
-        <v>0.192628659396803</v>
+        <v>-0.01652918306199047</v>
       </c>
       <c r="G18">
-        <v>0.2582640092197721</v>
+        <v>0.6230156929756394</v>
       </c>
       <c r="H18">
-        <v>0.2582640092197721</v>
+        <v>0.6230156929756394</v>
       </c>
       <c r="I18">
-        <v>14156</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1096,19 +1102,19 @@
         <v>25</v>
       </c>
       <c r="B19">
-        <v>0.0102119158074488</v>
+        <v>0.009820067619913343</v>
       </c>
       <c r="C19">
-        <v>0.009674189396799987</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="D19">
-        <v>0.0004006378783650764</v>
+        <v>0.0003683547284434392</v>
       </c>
       <c r="E19">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F19">
-        <v>0.1218694481841025</v>
+        <v>0.192628659396803</v>
       </c>
       <c r="G19">
         <v>0.2582640092197721</v>
@@ -1125,19 +1131,19 @@
         <v>26</v>
       </c>
       <c r="B20">
-        <v>0.009343230463755783</v>
+        <v>0.0102119158074488</v>
       </c>
       <c r="C20">
         <v>0.009674189396799987</v>
       </c>
       <c r="D20">
-        <v>0.0003680598885844467</v>
+        <v>0.0004006378783650764</v>
       </c>
       <c r="E20">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F20">
-        <v>0.1932748985620336</v>
+        <v>0.1218694481841025</v>
       </c>
       <c r="G20">
         <v>0.2582640092197721</v>
@@ -1154,28 +1160,28 @@
         <v>27</v>
       </c>
       <c r="B21">
-        <v>0.006002882908757912</v>
+        <v>0.009343230463755783</v>
       </c>
       <c r="C21">
-        <v>0.005813234561065725</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="D21">
-        <v>0.0001324165619288979</v>
+        <v>0.0003680598885844467</v>
       </c>
       <c r="E21">
-        <v>0.0001037297229528328</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F21">
-        <v>0.2606707993949464</v>
+        <v>0.1932748985620336</v>
       </c>
       <c r="G21">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H21">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I21">
-        <v>6771</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1183,19 +1189,19 @@
         <v>28</v>
       </c>
       <c r="B22">
-        <v>0.00595976388177965</v>
+        <v>0.006002882908757912</v>
       </c>
       <c r="C22">
         <v>0.005813234561065725</v>
       </c>
       <c r="D22">
-        <v>0.0001424514975481683</v>
+        <v>0.0001324165619288979</v>
       </c>
       <c r="E22">
         <v>0.0001037297229528328</v>
       </c>
       <c r="F22">
-        <v>0.2046421514566161</v>
+        <v>0.2606707993949464</v>
       </c>
       <c r="G22">
         <v>0.4208397194991282</v>
@@ -1212,19 +1218,19 @@
         <v>29</v>
       </c>
       <c r="B23">
-        <v>0.00592641693601841</v>
+        <v>0.00595976388177965</v>
       </c>
       <c r="C23">
         <v>0.005813234561065725</v>
       </c>
       <c r="D23">
-        <v>0.00013855240761432</v>
+        <v>0.0001424514975481683</v>
       </c>
       <c r="E23">
         <v>0.0001037297229528328</v>
       </c>
       <c r="F23">
-        <v>0.2264121702660996</v>
+        <v>0.2046421514566161</v>
       </c>
       <c r="G23">
         <v>0.4208397194991282</v>
@@ -1241,28 +1247,28 @@
         <v>30</v>
       </c>
       <c r="B24">
-        <v>0.008942022948316988</v>
+        <v>0.00592641693601841</v>
       </c>
       <c r="C24">
-        <v>0.009674189396799985</v>
+        <v>0.005813234561065725</v>
       </c>
       <c r="D24">
-        <v>0.0003279955215444224</v>
+        <v>0.00013855240761432</v>
       </c>
       <c r="E24">
-        <v>0.0003384092866814527</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="F24">
-        <v>0.2810892232598902</v>
+        <v>0.2264121702660996</v>
       </c>
       <c r="G24">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="H24">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I24">
-        <v>14156</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1270,28 +1276,28 @@
         <v>31</v>
       </c>
       <c r="B25">
-        <v>0.005089153979501482</v>
+        <v>0.008942022948316988</v>
       </c>
       <c r="C25">
-        <v>0.004580501696160511</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="D25">
-        <v>0.0002083353057278959</v>
+        <v>0.0003279955215444224</v>
       </c>
       <c r="E25">
-        <v>0.0001631540263502446</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F25">
-        <v>-0.004454544482717981</v>
+        <v>0.2810892232598902</v>
       </c>
       <c r="G25">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H25">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I25">
-        <v>11611</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1299,28 +1305,28 @@
         <v>32</v>
       </c>
       <c r="B26">
-        <v>0.008855143980453176</v>
+        <v>0.005089153979501482</v>
       </c>
       <c r="C26">
-        <v>0.009674189396799985</v>
+        <v>0.004580501696160511</v>
       </c>
       <c r="D26">
-        <v>0.0003254854012574867</v>
+        <v>0.0002083353057278959</v>
       </c>
       <c r="E26">
-        <v>0.0003384092866814527</v>
+        <v>0.0001631540263502446</v>
       </c>
       <c r="F26">
-        <v>0.2865909829079945</v>
+        <v>-0.004454544482717981</v>
       </c>
       <c r="G26">
-        <v>0.2582640092197721</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="H26">
-        <v>0.2582640092197721</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I26">
-        <v>14156</v>
+        <v>11611</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1328,28 +1334,28 @@
         <v>33</v>
       </c>
       <c r="B27">
-        <v>0.00510134746390362</v>
+        <v>0.008855143980453176</v>
       </c>
       <c r="C27">
-        <v>0.004589584286176587</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="D27">
-        <v>0.0002091701444985722</v>
+        <v>0.0003254854012574867</v>
       </c>
       <c r="E27">
-        <v>0.000163888349337522</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F27">
-        <v>-0.005012774390606101</v>
+        <v>0.2865909829079945</v>
       </c>
       <c r="G27">
-        <v>0.212555477012045</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H27">
-        <v>0.212555477012045</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I27">
-        <v>11542</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1357,28 +1363,28 @@
         <v>34</v>
       </c>
       <c r="B28">
-        <v>0.01003309392811347</v>
+        <v>0.00510134746390362</v>
       </c>
       <c r="C28">
-        <v>0.009674189396799985</v>
+        <v>0.004589584286176587</v>
       </c>
       <c r="D28">
-        <v>0.0003930561638032175</v>
+        <v>0.0002091701444985722</v>
       </c>
       <c r="E28">
-        <v>0.0003384092866814527</v>
+        <v>0.000163888349337522</v>
       </c>
       <c r="F28">
-        <v>0.138487285766222</v>
+        <v>-0.005012774390606101</v>
       </c>
       <c r="G28">
-        <v>0.2582640092197721</v>
+        <v>0.212555477012045</v>
       </c>
       <c r="H28">
-        <v>0.2582640092197721</v>
+        <v>0.212555477012045</v>
       </c>
       <c r="I28">
-        <v>14156</v>
+        <v>11542</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1386,28 +1392,28 @@
         <v>35</v>
       </c>
       <c r="B29">
-        <v>0.005107549406927882</v>
+        <v>0.01003309392811347</v>
       </c>
       <c r="C29">
-        <v>0.004580501696160511</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="D29">
-        <v>0.000207986162951978</v>
+        <v>0.0003930561638032175</v>
       </c>
       <c r="E29">
-        <v>0.0001631540263502446</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F29">
-        <v>-0.002771209789547591</v>
+        <v>0.138487285766222</v>
       </c>
       <c r="G29">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H29">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I29">
-        <v>11611</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1415,28 +1421,28 @@
         <v>36</v>
       </c>
       <c r="B30">
-        <v>0.006776662396495037</v>
+        <v>0.005107549406927882</v>
       </c>
       <c r="C30">
-        <v>0.005813234561065723</v>
+        <v>0.004580501696160511</v>
       </c>
       <c r="D30">
-        <v>0.000160150142460433</v>
+        <v>0.000207986162951978</v>
       </c>
       <c r="E30">
-        <v>0.0001037297229528328</v>
+        <v>0.0001631540263502446</v>
       </c>
       <c r="F30">
-        <v>0.1058242633905934</v>
+        <v>-0.002771209789547591</v>
       </c>
       <c r="G30">
-        <v>0.4208397194991282</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="H30">
-        <v>0.4208397194991282</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I30">
-        <v>6771</v>
+        <v>11611</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1444,28 +1450,28 @@
         <v>37</v>
       </c>
       <c r="B31">
-        <v>0.01005761747872771</v>
+        <v>0.006776662396495037</v>
       </c>
       <c r="C31">
-        <v>0.009674189396799987</v>
+        <v>0.005813234561065723</v>
       </c>
       <c r="D31">
-        <v>0.0003817896694842294</v>
+        <v>0.000160150142460433</v>
       </c>
       <c r="E31">
-        <v>0.0003384092866814527</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="F31">
-        <v>0.1631815381263255</v>
+        <v>0.1058242633905934</v>
       </c>
       <c r="G31">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="H31">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I31">
-        <v>14156</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1473,28 +1479,28 @@
         <v>38</v>
       </c>
       <c r="B32">
-        <v>0.004501420066184821</v>
+        <v>0.01005761747872771</v>
       </c>
       <c r="C32">
-        <v>0.004349183403839366</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="D32">
-        <v>0.0002742305932959652</v>
+        <v>0.0003817896694842294</v>
       </c>
       <c r="E32">
-        <v>0.0001730864695810989</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F32">
-        <v>-0.006214540120261569</v>
+        <v>0.1631815381263255</v>
       </c>
       <c r="G32">
-        <v>0.3649062991209757</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H32">
-        <v>0.3649062991209757</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I32">
-        <v>4010</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1502,28 +1508,28 @@
         <v>39</v>
       </c>
       <c r="B33">
-        <v>0.009396936069700112</v>
+        <v>0.004501420066184821</v>
       </c>
       <c r="C33">
-        <v>0.009729123728171802</v>
+        <v>0.004349183403839366</v>
       </c>
       <c r="D33">
-        <v>0.0003716511763370566</v>
+        <v>0.0002742305932959652</v>
       </c>
       <c r="E33">
-        <v>0.0003414259156749913</v>
+        <v>0.0001730864695810989</v>
       </c>
       <c r="F33">
-        <v>0.1928904449236721</v>
+        <v>-0.006214540120261569</v>
       </c>
       <c r="G33">
-        <v>0.2585302120985278</v>
+        <v>0.3649062991209757</v>
       </c>
       <c r="H33">
-        <v>0.2585302120985278</v>
+        <v>0.3649062991209757</v>
       </c>
       <c r="I33">
-        <v>14000</v>
+        <v>4010</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1531,19 +1537,19 @@
         <v>40</v>
       </c>
       <c r="B34">
-        <v>0.01035431191953904</v>
+        <v>0.00949661439173217</v>
       </c>
       <c r="C34">
-        <v>0.009674189396799987</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="D34">
-        <v>0.0004001063569688302</v>
+        <v>0.0003579073820851387</v>
       </c>
       <c r="E34">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F34">
-        <v>0.1230344532976788</v>
+        <v>0.2155274778012536</v>
       </c>
       <c r="G34">
         <v>0.2582640092197721</v>
@@ -1560,28 +1566,28 @@
         <v>41</v>
       </c>
       <c r="B35">
-        <v>0.01022526679210232</v>
+        <v>0.009396936069700112</v>
       </c>
       <c r="C35">
-        <v>0.009384601794708014</v>
+        <v>0.009729123728171802</v>
       </c>
       <c r="D35">
-        <v>0.0004705186388866096</v>
+        <v>0.0003716511763370566</v>
       </c>
       <c r="E35">
-        <v>0.0003220429185286173</v>
+        <v>0.0003414259156749913</v>
       </c>
       <c r="F35">
-        <v>0.1094051116331665</v>
+        <v>0.1928904449236721</v>
       </c>
       <c r="G35">
-        <v>0.3904390743053188</v>
+        <v>0.2585302120985278</v>
       </c>
       <c r="H35">
-        <v>0.3904390743053188</v>
+        <v>0.2585302120985278</v>
       </c>
       <c r="I35">
-        <v>4699</v>
+        <v>14000</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1589,28 +1595,28 @@
         <v>42</v>
       </c>
       <c r="B36">
-        <v>0.005089488294347637</v>
+        <v>0.01035431191953904</v>
       </c>
       <c r="C36">
-        <v>0.004580501696160511</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="D36">
-        <v>0.0002081444394071696</v>
+        <v>0.0004001063569688302</v>
       </c>
       <c r="E36">
-        <v>0.0001631540263502446</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F36">
-        <v>-0.00353431378743374</v>
+        <v>0.1230344532976788</v>
       </c>
       <c r="G36">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H36">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I36">
-        <v>11611</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1618,28 +1624,28 @@
         <v>43</v>
       </c>
       <c r="B37">
-        <v>0.009406309171688502</v>
+        <v>0.01022526679210232</v>
       </c>
       <c r="C37">
-        <v>0.009674189396799985</v>
+        <v>0.009384601794708014</v>
       </c>
       <c r="D37">
-        <v>0.0003610907680501377</v>
+        <v>0.0004705186388866096</v>
       </c>
       <c r="E37">
-        <v>0.0003384092866814527</v>
+        <v>0.0003220429185286173</v>
       </c>
       <c r="F37">
-        <v>0.2085500335179142</v>
+        <v>0.1094051116331665</v>
       </c>
       <c r="G37">
-        <v>0.2582640092197721</v>
+        <v>0.3904390743053188</v>
       </c>
       <c r="H37">
-        <v>0.2582640092197721</v>
+        <v>0.3904390743053188</v>
       </c>
       <c r="I37">
-        <v>14156</v>
+        <v>4699</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1647,28 +1653,28 @@
         <v>44</v>
       </c>
       <c r="B38">
-        <v>0.009535796789931871</v>
+        <v>0.005089488294347637</v>
       </c>
       <c r="C38">
-        <v>0.009674189396799985</v>
+        <v>0.004580501696160511</v>
       </c>
       <c r="D38">
-        <v>0.0003710863970746162</v>
+        <v>0.0002081444394071696</v>
       </c>
       <c r="E38">
-        <v>0.0003384092866814527</v>
+        <v>0.0001631540263502446</v>
       </c>
       <c r="F38">
-        <v>0.1866413032030688</v>
+        <v>-0.00353431378743374</v>
       </c>
       <c r="G38">
-        <v>0.2582640092197721</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="H38">
-        <v>0.2582640092197721</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I38">
-        <v>14156</v>
+        <v>11611</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1676,19 +1682,19 @@
         <v>45</v>
       </c>
       <c r="B39">
-        <v>0.009554445336689437</v>
+        <v>0.009406309171688502</v>
       </c>
       <c r="C39">
-        <v>0.009674189396799987</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="D39">
-        <v>0.0003744000227958637</v>
+        <v>0.0003610907680501377</v>
       </c>
       <c r="E39">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F39">
-        <v>0.179378395374721</v>
+        <v>0.2085500335179142</v>
       </c>
       <c r="G39">
         <v>0.2582640092197721</v>
@@ -1705,19 +1711,19 @@
         <v>46</v>
       </c>
       <c r="B40">
-        <v>0.009555217528480035</v>
+        <v>0.009535796789931871</v>
       </c>
       <c r="C40">
-        <v>0.009674189396799987</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="D40">
-        <v>0.0003746361399868205</v>
+        <v>0.0003710863970746162</v>
       </c>
       <c r="E40">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F40">
-        <v>0.1788608663781261</v>
+        <v>0.1866413032030688</v>
       </c>
       <c r="G40">
         <v>0.2582640092197721</v>
@@ -1734,19 +1740,19 @@
         <v>47</v>
       </c>
       <c r="B41">
-        <v>0.009526287265811475</v>
+        <v>0.009554445336689437</v>
       </c>
       <c r="C41">
         <v>0.009674189396799987</v>
       </c>
       <c r="D41">
-        <v>0.0003736225585176234</v>
+        <v>0.0003744000227958637</v>
       </c>
       <c r="E41">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F41">
-        <v>0.1810824657398455</v>
+        <v>0.179378395374721</v>
       </c>
       <c r="G41">
         <v>0.2582640092197721</v>
@@ -1763,28 +1769,28 @@
         <v>48</v>
       </c>
       <c r="B42">
-        <v>0.00674135934653288</v>
+        <v>0.009555217528480035</v>
       </c>
       <c r="C42">
-        <v>0.005813234561065723</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="D42">
-        <v>0.0001603751212724098</v>
+        <v>0.0003746361399868205</v>
       </c>
       <c r="E42">
-        <v>0.0001037297229528328</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F42">
-        <v>0.1045681259196538</v>
+        <v>0.1788608663781261</v>
       </c>
       <c r="G42">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H42">
-        <v>0.4208397194991282</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I42">
-        <v>6771</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1792,19 +1798,19 @@
         <v>49</v>
       </c>
       <c r="B43">
-        <v>0.009669808352814117</v>
+        <v>0.009526287265811475</v>
       </c>
       <c r="C43">
         <v>0.009674189396799987</v>
       </c>
       <c r="D43">
-        <v>0.0003609428129771297</v>
+        <v>0.0003736225585176234</v>
       </c>
       <c r="E43">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F43">
-        <v>0.2088743260447083</v>
+        <v>0.1810824657398455</v>
       </c>
       <c r="G43">
         <v>0.2582640092197721</v>
@@ -1821,28 +1827,28 @@
         <v>50</v>
       </c>
       <c r="B44">
-        <v>0.009547987620144199</v>
+        <v>0.00674135934653288</v>
       </c>
       <c r="C44">
-        <v>0.009674189396799985</v>
+        <v>0.005813234561065723</v>
       </c>
       <c r="D44">
-        <v>0.0003609514012730195</v>
+        <v>0.0001603751212724098</v>
       </c>
       <c r="E44">
-        <v>0.0003384092866814527</v>
+        <v>0.0001037297229528328</v>
       </c>
       <c r="F44">
-        <v>0.2088555019508919</v>
+        <v>0.1045681259196538</v>
       </c>
       <c r="G44">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="H44">
-        <v>0.2582640092197721</v>
+        <v>0.4208397194991282</v>
       </c>
       <c r="I44">
-        <v>14156</v>
+        <v>6771</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1850,19 +1856,19 @@
         <v>51</v>
       </c>
       <c r="B45">
-        <v>0.009719161233546112</v>
+        <v>0.009669808352814117</v>
       </c>
       <c r="C45">
-        <v>0.009674189396799985</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="D45">
-        <v>0.0003635971635380399</v>
+        <v>0.0003609428129771297</v>
       </c>
       <c r="E45">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F45">
-        <v>0.2030564380000814</v>
+        <v>0.2088743260447083</v>
       </c>
       <c r="G45">
         <v>0.2582640092197721</v>
@@ -1879,19 +1885,19 @@
         <v>52</v>
       </c>
       <c r="B46">
-        <v>0.009501857293097325</v>
+        <v>0.009547987620144199</v>
       </c>
       <c r="C46">
         <v>0.009674189396799985</v>
       </c>
       <c r="D46">
-        <v>0.0003602535480745813</v>
+        <v>0.0003609514012730195</v>
       </c>
       <c r="E46">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F46">
-        <v>0.2103850782773533</v>
+        <v>0.2088555019508919</v>
       </c>
       <c r="G46">
         <v>0.2582640092197721</v>
@@ -1908,19 +1914,19 @@
         <v>53</v>
       </c>
       <c r="B47">
-        <v>0.00867861064019221</v>
+        <v>0.009719161233546112</v>
       </c>
       <c r="C47">
         <v>0.009674189396799985</v>
       </c>
       <c r="D47">
-        <v>0.0003344607981243851</v>
+        <v>0.0003635971635380399</v>
       </c>
       <c r="E47">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F47">
-        <v>0.2669184291403396</v>
+        <v>0.2030564380000814</v>
       </c>
       <c r="G47">
         <v>0.2582640092197721</v>
@@ -1937,19 +1943,19 @@
         <v>54</v>
       </c>
       <c r="B48">
-        <v>0.01011738460212881</v>
+        <v>0.009501857293097325</v>
       </c>
       <c r="C48">
-        <v>0.009674189396799987</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="D48">
-        <v>0.0003886501570187028</v>
+        <v>0.0003602535480745813</v>
       </c>
       <c r="E48">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F48">
-        <v>0.1481445083553075</v>
+        <v>0.2103850782773533</v>
       </c>
       <c r="G48">
         <v>0.2582640092197721</v>
@@ -1966,19 +1972,19 @@
         <v>55</v>
       </c>
       <c r="B49">
-        <v>0.01064772150300563</v>
+        <v>0.00867861064019221</v>
       </c>
       <c r="C49">
         <v>0.009674189396799985</v>
       </c>
       <c r="D49">
-        <v>0.0004313797729252501</v>
+        <v>0.0003344607981243851</v>
       </c>
       <c r="E49">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F49">
-        <v>0.05448840836791147</v>
+        <v>0.2669184291403396</v>
       </c>
       <c r="G49">
         <v>0.2582640092197721</v>
@@ -1995,28 +2001,28 @@
         <v>56</v>
       </c>
       <c r="B50">
-        <v>0.005626234126090045</v>
+        <v>0.01011738460212881</v>
       </c>
       <c r="C50">
-        <v>0.005318929375230071</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="D50">
-        <v>0.000141190946981845</v>
+        <v>0.0003886501570187028</v>
       </c>
       <c r="E50">
-        <v>9.243123959608208E-05</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F50">
-        <v>0.1703625716885953</v>
+        <v>0.1481445083553075</v>
       </c>
       <c r="G50">
-        <v>0.456874413314975</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H50">
-        <v>0.456874413314975</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I50">
-        <v>5153</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2024,19 +2030,19 @@
         <v>57</v>
       </c>
       <c r="B51">
-        <v>0.01060174085834054</v>
+        <v>0.01064772150300563</v>
       </c>
       <c r="C51">
-        <v>0.009674189396799987</v>
+        <v>0.009674189396799985</v>
       </c>
       <c r="D51">
-        <v>0.0004139067990685161</v>
+        <v>0.0004313797729252501</v>
       </c>
       <c r="E51">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F51">
-        <v>0.09278621544819221</v>
+        <v>0.05448840836791147</v>
       </c>
       <c r="G51">
         <v>0.2582640092197721</v>
@@ -2053,28 +2059,28 @@
         <v>58</v>
       </c>
       <c r="B52">
-        <v>0.01035467890006862</v>
+        <v>0.005626234126090045</v>
       </c>
       <c r="C52">
-        <v>0.009674189396799987</v>
+        <v>0.005318929375230071</v>
       </c>
       <c r="D52">
-        <v>0.0004026104577395279</v>
+        <v>0.000141190946981845</v>
       </c>
       <c r="E52">
-        <v>0.0003384092866814527</v>
+        <v>9.243123959608208E-05</v>
       </c>
       <c r="F52">
-        <v>0.1175458874123242</v>
+        <v>0.1703625716885953</v>
       </c>
       <c r="G52">
-        <v>0.2582640092197721</v>
+        <v>0.456874413314975</v>
       </c>
       <c r="H52">
-        <v>0.2582640092197721</v>
+        <v>0.456874413314975</v>
       </c>
       <c r="I52">
-        <v>14156</v>
+        <v>5153</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2082,28 +2088,28 @@
         <v>59</v>
       </c>
       <c r="B53">
-        <v>0.005090949099942899</v>
+        <v>0.01060174085834054</v>
       </c>
       <c r="C53">
-        <v>0.004580501696160511</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="D53">
-        <v>0.0002080153046483946</v>
+        <v>0.0004139067990685161</v>
       </c>
       <c r="E53">
-        <v>0.0001631540263502446</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F53">
-        <v>-0.002911711704464803</v>
+        <v>0.09278621544819221</v>
       </c>
       <c r="G53">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H53">
-        <v>0.2133795918767654</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I53">
-        <v>11611</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -2111,19 +2117,19 @@
         <v>60</v>
       </c>
       <c r="B54">
-        <v>0.009263751492683912</v>
+        <v>0.01035467890006862</v>
       </c>
       <c r="C54">
         <v>0.009674189396799987</v>
       </c>
       <c r="D54">
-        <v>0.0003438074749231005</v>
+        <v>0.0004026104577395279</v>
       </c>
       <c r="E54">
         <v>0.0003384092866814527</v>
       </c>
       <c r="F54">
-        <v>0.2464320924804251</v>
+        <v>0.1175458874123242</v>
       </c>
       <c r="G54">
         <v>0.2582640092197721</v>
@@ -2140,28 +2146,28 @@
         <v>61</v>
       </c>
       <c r="B55">
-        <v>0.00950560728094302</v>
+        <v>0.005090949099942899</v>
       </c>
       <c r="C55">
-        <v>0.00969865279856456</v>
+        <v>0.004580501696160511</v>
       </c>
       <c r="D55">
-        <v>0.0003676303455898381</v>
+        <v>0.0002080153046483946</v>
       </c>
       <c r="E55">
-        <v>0.0003326480833522705</v>
+        <v>0.0001631540263502446</v>
       </c>
       <c r="F55">
-        <v>0.277134584732579</v>
+        <v>-0.002911711704464803</v>
       </c>
       <c r="G55">
-        <v>0.3459196233527754</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="H55">
-        <v>0.3459196233527754</v>
+        <v>0.2133795918767654</v>
       </c>
       <c r="I55">
-        <v>5919</v>
+        <v>11611</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2169,28 +2175,28 @@
         <v>62</v>
       </c>
       <c r="B56">
-        <v>0.01043843340429874</v>
+        <v>0.009263751492683912</v>
       </c>
       <c r="C56">
-        <v>0.009545579499406483</v>
+        <v>0.009674189396799987</v>
       </c>
       <c r="D56">
-        <v>0.0003426357597594948</v>
+        <v>0.0003438074749231005</v>
       </c>
       <c r="E56">
-        <v>0.0002911643753660776</v>
+        <v>0.0003384092866814527</v>
       </c>
       <c r="F56">
-        <v>0.08840833195541187</v>
+        <v>0.2464320924804251</v>
       </c>
       <c r="G56">
-        <v>0.2253493365624453</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="H56">
-        <v>0.2253493365624453</v>
+        <v>0.2582640092197721</v>
       </c>
       <c r="I56">
-        <v>7054</v>
+        <v>14156</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -2198,27 +2204,85 @@
         <v>63</v>
       </c>
       <c r="B57">
+        <v>0.00950560728094302</v>
+      </c>
+      <c r="C57">
+        <v>0.00969865279856456</v>
+      </c>
+      <c r="D57">
+        <v>0.0003676303455898381</v>
+      </c>
+      <c r="E57">
+        <v>0.0003326480833522705</v>
+      </c>
+      <c r="F57">
+        <v>0.277134584732579</v>
+      </c>
+      <c r="G57">
+        <v>0.3459196233527754</v>
+      </c>
+      <c r="H57">
+        <v>0.3459196233527754</v>
+      </c>
+      <c r="I57">
+        <v>5919</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B58">
+        <v>0.01043843340429874</v>
+      </c>
+      <c r="C58">
+        <v>0.009545579499406483</v>
+      </c>
+      <c r="D58">
+        <v>0.0003426357597594948</v>
+      </c>
+      <c r="E58">
+        <v>0.0002911643753660776</v>
+      </c>
+      <c r="F58">
+        <v>0.08840833195541187</v>
+      </c>
+      <c r="G58">
+        <v>0.2253493365624453</v>
+      </c>
+      <c r="H58">
+        <v>0.2253493365624453</v>
+      </c>
+      <c r="I58">
+        <v>7054</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59">
         <v>0.009547617558891911</v>
       </c>
-      <c r="C57">
+      <c r="C59">
         <v>0.009674189396799985</v>
       </c>
-      <c r="D57">
+      <c r="D59">
         <v>0.000360031497755876</v>
       </c>
-      <c r="E57">
-        <v>0.0003384092866814527</v>
-      </c>
-      <c r="F57">
+      <c r="E59">
+        <v>0.0003384092866814527</v>
+      </c>
+      <c r="F59">
         <v>0.2108717750662125</v>
       </c>
-      <c r="G57">
-        <v>0.2582640092197721</v>
-      </c>
-      <c r="H57">
-        <v>0.2582640092197721</v>
-      </c>
-      <c r="I57">
+      <c r="G59">
+        <v>0.2582640092197721</v>
+      </c>
+      <c r="H59">
+        <v>0.2582640092197721</v>
+      </c>
+      <c r="I59">
         <v>14156</v>
       </c>
     </row>

</xml_diff>